<commit_message>
Atualização no ex028 e planilha
</commit_message>
<xml_diff>
--- a/detalhesPython.xlsx
+++ b/detalhesPython.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\thiag\Documents\EstudosT\python\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8991F8DB-33CB-4E23-9731-265808DA6A5E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1CE66AC9-C27E-4DF0-8BD3-822512DF9B48}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{ECBDB9F7-0FAD-476C-A4A4-7948F29B869E}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="246" uniqueCount="231">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="270" uniqueCount="252">
   <si>
     <t>Descrição</t>
   </si>
@@ -10625,13 +10625,623 @@
       </rPr>
       <t>(nome))</t>
     </r>
+  </si>
+  <si>
+    <t>ex028</t>
+  </si>
+  <si>
+    <t>Escreva um programa que faça o computador “pensar” em um número inteiro entre 0 e 5 e peça para o usuário tentar descobrir qual foi o número escolhido pelo computador. O programa deverá escrever na tela se o usuário venceu ou perdeu.</t>
+  </si>
+  <si>
+    <r>
+      <t>from</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> random </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>import</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> randint</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>from</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> time </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>import</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> sleep</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">computador </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>=</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF67E480"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>randint</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>(</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF78D1E1"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>0</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF78D1E1"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>5</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">) </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF5A4B81"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>#faz o computador pensar</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>print</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>(</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE7DE79"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>'=-^-'</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>*</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF78D1E1"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>14</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>print</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>(</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE7DE79"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>'Vou pensar em um número entre 0 e 5. Tente adivinhar...'</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">jogador </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>=</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color rgb="FF988BC7"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>int</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>(</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF988BC7"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>input</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>(</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE7DE79"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>'Qual número eu pensei? '</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">)) </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF5A4B81"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>#jogador tenta adivinhar</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>print</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>(</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE7DE79"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>'Pensando...'</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>sleep</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>(</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF78D1E1"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>2</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>if</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> jogador </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>==</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> computador:</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">    </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF988BC7"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>print</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>(</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE7DE79"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>'Parabéns! Você consegui me vencer!'</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>else</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>:</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">    </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF988BC7"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>print</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>(</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE7DE79"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">'Ganhei! Eu pensei no número </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF78D1E1"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>{}</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE7DE79"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> e não no </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF78D1E1"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>{}</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE7DE79"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>.'</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF67E480"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>format</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>(computador, jogador))</t>
+    </r>
+  </si>
+  <si>
+    <t>randint pra fazer o computador escolher um número aleatório</t>
+  </si>
+  <si>
+    <t>sleep pra dar um delay entre uma linha e a outra..</t>
+  </si>
+  <si>
+    <t>escolher</t>
+  </si>
+  <si>
+    <t>randint</t>
+  </si>
+  <si>
+    <t>delay</t>
+  </si>
+  <si>
+    <t>tempo</t>
+  </si>
+  <si>
+    <t>sleep</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="13" x14ac:knownFonts="1">
+  <fonts count="14" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -10715,6 +11325,12 @@
     <font>
       <sz val="11"/>
       <color theme="0"/>
+      <name val="Consolas"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF5A4B81"/>
       <name val="Consolas"/>
       <family val="3"/>
     </font>
@@ -11059,7 +11675,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="45">
+  <cellXfs count="44">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -11185,9 +11801,6 @@
     </xf>
     <xf numFmtId="0" fontId="11" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -11503,9 +12116,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{73331524-72FC-41A3-82E6-4326A0999772}">
-  <dimension ref="A1:E274"/>
+  <dimension ref="A1:E295"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A274" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B276" sqref="B276"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -11552,7 +12167,7 @@
     </row>
     <row r="7" spans="1:2" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="19"/>
-      <c r="B7" s="44"/>
+      <c r="B7" s="20"/>
     </row>
     <row r="8" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="41" t="s">
@@ -11596,7 +12211,7 @@
     </row>
     <row r="15" spans="1:2" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="19"/>
-      <c r="B15" s="44"/>
+      <c r="B15" s="20"/>
     </row>
     <row r="16" spans="1:2" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="41" t="s">
@@ -11670,7 +12285,7 @@
     </row>
     <row r="28" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A28" s="19"/>
-      <c r="B28" s="44"/>
+      <c r="B28" s="20"/>
     </row>
     <row r="29" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A29" s="41" t="s">
@@ -11714,7 +12329,7 @@
     </row>
     <row r="36" spans="1:2" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A36" s="19"/>
-      <c r="B36" s="44"/>
+      <c r="B36" s="20"/>
     </row>
     <row r="37" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A37" s="41" t="s">
@@ -11776,7 +12391,7 @@
     </row>
     <row r="47" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A47" s="19"/>
-      <c r="B47" s="44"/>
+      <c r="B47" s="20"/>
     </row>
     <row r="48" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A48" s="41" t="s">
@@ -11820,7 +12435,7 @@
     </row>
     <row r="55" spans="1:2" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A55" s="19"/>
-      <c r="B55" s="44"/>
+      <c r="B55" s="20"/>
     </row>
     <row r="56" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A56" s="41" t="s">
@@ -11864,7 +12479,7 @@
     </row>
     <row r="63" spans="1:2" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A63" s="19"/>
-      <c r="B63" s="44"/>
+      <c r="B63" s="20"/>
     </row>
     <row r="64" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A64" s="41" t="s">
@@ -11956,11 +12571,11 @@
     </row>
     <row r="79" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A79" s="19"/>
-      <c r="B79" s="44"/>
+      <c r="B79" s="20"/>
     </row>
     <row r="80" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A80" s="19"/>
-      <c r="B80" s="44"/>
+      <c r="B80" s="20"/>
     </row>
     <row r="81" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A81" s="41" t="s">
@@ -11998,7 +12613,7 @@
     </row>
     <row r="87" spans="1:2" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A87" s="19"/>
-      <c r="B87" s="44"/>
+      <c r="B87" s="20"/>
     </row>
     <row r="88" spans="1:2" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A88" s="41" t="s">
@@ -12048,7 +12663,7 @@
     </row>
     <row r="96" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A96" s="19"/>
-      <c r="B96" s="44"/>
+      <c r="B96" s="20"/>
     </row>
     <row r="97" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A97" s="41" t="s">
@@ -13128,19 +13743,144 @@
       <c r="A274" s="43"/>
       <c r="B274" s="18"/>
     </row>
+    <row r="275" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="276" spans="1:2" ht="30.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A276" s="41" t="s">
+        <v>231</v>
+      </c>
+      <c r="B276" s="31" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="277" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A277" s="42"/>
+      <c r="B277" s="7"/>
+    </row>
+    <row r="278" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A278" s="42"/>
+      <c r="B278" s="34" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="279" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A279" s="42"/>
+      <c r="B279" s="34" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="280" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A280" s="42"/>
+      <c r="B280" s="7" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="281" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A281" s="42"/>
+      <c r="B281" s="11" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="282" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A282" s="42"/>
+      <c r="B282" s="11" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="283" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A283" s="42"/>
+      <c r="B283" s="11" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="284" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A284" s="42"/>
+      <c r="B284" s="7" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="285" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A285" s="42"/>
+      <c r="B285" s="11" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="286" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A286" s="42"/>
+      <c r="B286" s="35" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="287" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A287" s="42"/>
+      <c r="B287" s="34" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="288" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A288" s="42"/>
+      <c r="B288" s="7" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="289" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A289" s="42"/>
+      <c r="B289" s="34" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="290" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A290" s="42"/>
+      <c r="B290" s="7" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="291" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A291" s="42"/>
+      <c r="B291" s="11"/>
+    </row>
+    <row r="292" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A292" s="42"/>
+      <c r="B292" s="11" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="293" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A293" s="42"/>
+      <c r="B293" s="11" t="s">
+        <v>245</v>
+      </c>
+      <c r="C293" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="D293" s="2" t="s">
+        <v>247</v>
+      </c>
+      <c r="E293" s="2" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="294" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A294" s="42"/>
+      <c r="B294" s="39" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="295" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A295" s="43"/>
+      <c r="B295" s="33"/>
+      <c r="C295" s="2" t="s">
+        <v>249</v>
+      </c>
+      <c r="D295" s="2" t="s">
+        <v>250</v>
+      </c>
+      <c r="E295" s="2" t="s">
+        <v>251</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="26">
-    <mergeCell ref="A2:A6"/>
-    <mergeCell ref="A37:A46"/>
-    <mergeCell ref="A29:A35"/>
-    <mergeCell ref="A16:A27"/>
-    <mergeCell ref="A8:A14"/>
-    <mergeCell ref="A64:A78"/>
-    <mergeCell ref="A56:A62"/>
-    <mergeCell ref="A48:A54"/>
-    <mergeCell ref="A97:A102"/>
-    <mergeCell ref="A88:A95"/>
-    <mergeCell ref="A81:A86"/>
+  <mergeCells count="27">
+    <mergeCell ref="A276:A295"/>
     <mergeCell ref="A118:A124"/>
     <mergeCell ref="A111:A116"/>
     <mergeCell ref="A104:A109"/>
@@ -13156,6 +13896,17 @@
     <mergeCell ref="A159:A172"/>
     <mergeCell ref="A146:A156"/>
     <mergeCell ref="A134:A144"/>
+    <mergeCell ref="A64:A78"/>
+    <mergeCell ref="A56:A62"/>
+    <mergeCell ref="A48:A54"/>
+    <mergeCell ref="A97:A102"/>
+    <mergeCell ref="A88:A95"/>
+    <mergeCell ref="A81:A86"/>
+    <mergeCell ref="A2:A6"/>
+    <mergeCell ref="A37:A46"/>
+    <mergeCell ref="A29:A35"/>
+    <mergeCell ref="A16:A27"/>
+    <mergeCell ref="A8:A14"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Atualização do ex029 e planilha
</commit_message>
<xml_diff>
--- a/detalhesPython.xlsx
+++ b/detalhesPython.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\thiag\Documents\EstudosT\python\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1CE66AC9-C27E-4DF0-8BD3-822512DF9B48}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54704750-83A0-4D3C-9B7C-D21341F50E3E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{ECBDB9F7-0FAD-476C-A4A4-7948F29B869E}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="270" uniqueCount="252">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="281" uniqueCount="262">
   <si>
     <t>Descrição</t>
   </si>
@@ -11235,6 +11235,456 @@
   </si>
   <si>
     <t>sleep</t>
+  </si>
+  <si>
+    <t>ex029</t>
+  </si>
+  <si>
+    <t>Escreva um programa que leia a velocidade de um carro. Se ele ultrapassar 80Km/h, mostre uma mensagem dizendo que ele foi multado. A multa vai custar R$7,00 por cada Km acima do limite.</t>
+  </si>
+  <si>
+    <r>
+      <t>print</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>(</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE7DE79"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>'-'</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>*</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF78D1E1"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>40</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>print</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>(</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE7DE79"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>'Qual a velocidade atual do automóvel? '</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">velocidade </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>=</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color rgb="FF988BC7"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>int</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>(</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF988BC7"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>input</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>(</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE7DE79"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>'km/h:  '</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>))</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>if</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> velocidade </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF78D1E1"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>80</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>:</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">    </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF988BC7"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>print</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>(</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE7DE79"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>'MULTADO! Você excedeu o limite de velocidade de 80 km/h.'</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">    </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF988BC7"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>print</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>(</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE7DE79"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>'Você deve pagar uma multa de R$</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF78D1E1"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>{}</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE7DE79"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>,00'</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF67E480"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>format</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">((velocidade </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>-</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF78D1E1"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>80</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">) </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>*</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF78D1E1"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>7</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>))</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>print</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>(</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE7DE79"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>'Tenha uma ótima viagem e digija com segurança!'</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>)</t>
+    </r>
+  </si>
+  <si>
+    <t>Obs.: Exemplo de extrutura de condição simples. Usando somente o if. Último print sem identação pra sair nos 2 casos</t>
   </si>
 </sst>
 </file>
@@ -12116,10 +12566,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{73331524-72FC-41A3-82E6-4326A0999772}">
-  <dimension ref="A1:E295"/>
+  <dimension ref="A1:E309"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A274" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B276" sqref="B276"/>
+    <sheetView tabSelected="1" topLeftCell="A289" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B309" sqref="B309"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -13878,8 +14328,95 @@
         <v>251</v>
       </c>
     </row>
+    <row r="296" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="297" spans="1:5" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A297" s="41" t="s">
+        <v>252</v>
+      </c>
+      <c r="B297" s="31" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="298" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A298" s="42"/>
+      <c r="B298" s="40"/>
+    </row>
+    <row r="299" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A299" s="42"/>
+      <c r="B299" s="11" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="300" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A300" s="42"/>
+      <c r="B300" s="11" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="301" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A301" s="42"/>
+      <c r="B301" s="11" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="302" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A302" s="42"/>
+      <c r="B302" s="7" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="303" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A303" s="42"/>
+      <c r="B303" s="34" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="304" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A304" s="42"/>
+      <c r="B304" s="7" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="305" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A305" s="42"/>
+      <c r="B305" s="7" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="306" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A306" s="42"/>
+      <c r="B306" s="11" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="307" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A307" s="42"/>
+      <c r="B307" s="23"/>
+    </row>
+    <row r="308" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A308" s="42"/>
+      <c r="B308" s="26" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="309" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A309" s="43"/>
+      <c r="B309" s="18"/>
+    </row>
   </sheetData>
-  <mergeCells count="27">
+  <mergeCells count="28">
+    <mergeCell ref="A297:A309"/>
+    <mergeCell ref="A2:A6"/>
+    <mergeCell ref="A37:A46"/>
+    <mergeCell ref="A29:A35"/>
+    <mergeCell ref="A16:A27"/>
+    <mergeCell ref="A8:A14"/>
+    <mergeCell ref="A64:A78"/>
+    <mergeCell ref="A56:A62"/>
+    <mergeCell ref="A48:A54"/>
+    <mergeCell ref="A97:A102"/>
+    <mergeCell ref="A88:A95"/>
+    <mergeCell ref="A81:A86"/>
     <mergeCell ref="A276:A295"/>
     <mergeCell ref="A118:A124"/>
     <mergeCell ref="A111:A116"/>
@@ -13896,17 +14433,6 @@
     <mergeCell ref="A159:A172"/>
     <mergeCell ref="A146:A156"/>
     <mergeCell ref="A134:A144"/>
-    <mergeCell ref="A64:A78"/>
-    <mergeCell ref="A56:A62"/>
-    <mergeCell ref="A48:A54"/>
-    <mergeCell ref="A97:A102"/>
-    <mergeCell ref="A88:A95"/>
-    <mergeCell ref="A81:A86"/>
-    <mergeCell ref="A2:A6"/>
-    <mergeCell ref="A37:A46"/>
-    <mergeCell ref="A29:A35"/>
-    <mergeCell ref="A16:A27"/>
-    <mergeCell ref="A8:A14"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Atualizei o ex030 e planilha
</commit_message>
<xml_diff>
--- a/detalhesPython.xlsx
+++ b/detalhesPython.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\thiag\Documents\EstudosT\python\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54704750-83A0-4D3C-9B7C-D21341F50E3E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD553F8A-24DD-4E11-84CA-447119F6FCC4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{ECBDB9F7-0FAD-476C-A4A4-7948F29B869E}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="281" uniqueCount="262">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="288" uniqueCount="268">
   <si>
     <t>Descrição</t>
   </si>
@@ -11685,6 +11685,330 @@
   </si>
   <si>
     <t>Obs.: Exemplo de extrutura de condição simples. Usando somente o if. Último print sem identação pra sair nos 2 casos</t>
+  </si>
+  <si>
+    <t>ex030</t>
+  </si>
+  <si>
+    <t>Crie um programa que leia um número inteiro e mostre na tela se ele é PAR ou ÍMPAR.</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">num </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>=</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color rgb="FF988BC7"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>int</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>(</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF988BC7"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>input</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>(</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE7DE79"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>'Digite um número: '</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>))</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>if</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> num </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>%</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF78D1E1"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>2</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>==</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF78D1E1"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>0</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>:</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">    </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF988BC7"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>print</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>(</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE7DE79"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>'</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF78D1E1"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>{}</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE7DE79"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> é Par!'</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF67E480"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>format</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>(num))</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">    </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF988BC7"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>print</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>(</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE7DE79"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>'</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF78D1E1"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>{}</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE7DE79"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> é Ímpar!'</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF67E480"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>format</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>(num))</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -11805,7 +12129,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="25">
+  <borders count="26">
     <border>
       <left/>
       <right/>
@@ -12121,11 +12445,24 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color theme="0"/>
+      </left>
+      <right style="medium">
+        <color theme="0"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="44">
+  <cellXfs count="45">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -12251,6 +12588,9 @@
     </xf>
     <xf numFmtId="0" fontId="11" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -12566,10 +12906,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{73331524-72FC-41A3-82E6-4326A0999772}">
-  <dimension ref="A1:E309"/>
+  <dimension ref="A1:E318"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A289" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B309" sqref="B309"/>
+    <sheetView tabSelected="1" topLeftCell="A301" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="A311" sqref="A311:A318"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -14403,8 +14743,68 @@
       <c r="A309" s="43"/>
       <c r="B309" s="18"/>
     </row>
+    <row r="310" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="311" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A311" s="41" t="s">
+        <v>262</v>
+      </c>
+      <c r="B311" s="29" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="312" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A312" s="42"/>
+      <c r="B312" s="7"/>
+    </row>
+    <row r="313" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A313" s="42"/>
+      <c r="B313" s="7" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="314" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A314" s="42"/>
+      <c r="B314" s="34" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="315" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A315" s="42"/>
+      <c r="B315" s="7" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="316" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A316" s="42"/>
+      <c r="B316" s="34" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="317" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A317" s="42"/>
+      <c r="B317" s="44" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="318" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A318" s="43"/>
+      <c r="B318" s="16"/>
+    </row>
   </sheetData>
-  <mergeCells count="28">
+  <mergeCells count="29">
+    <mergeCell ref="A311:A318"/>
+    <mergeCell ref="A126:A132"/>
+    <mergeCell ref="A189:A196"/>
+    <mergeCell ref="A174:A187"/>
+    <mergeCell ref="A159:A172"/>
+    <mergeCell ref="A146:A156"/>
+    <mergeCell ref="A134:A144"/>
+    <mergeCell ref="A262:A274"/>
+    <mergeCell ref="A230:A237"/>
+    <mergeCell ref="A239:A246"/>
+    <mergeCell ref="A198:A215"/>
+    <mergeCell ref="A217:A228"/>
+    <mergeCell ref="A248:A260"/>
     <mergeCell ref="A297:A309"/>
     <mergeCell ref="A2:A6"/>
     <mergeCell ref="A37:A46"/>
@@ -14421,18 +14821,6 @@
     <mergeCell ref="A118:A124"/>
     <mergeCell ref="A111:A116"/>
     <mergeCell ref="A104:A109"/>
-    <mergeCell ref="A262:A274"/>
-    <mergeCell ref="A230:A237"/>
-    <mergeCell ref="A239:A246"/>
-    <mergeCell ref="A198:A215"/>
-    <mergeCell ref="A217:A228"/>
-    <mergeCell ref="A248:A260"/>
-    <mergeCell ref="A126:A132"/>
-    <mergeCell ref="A189:A196"/>
-    <mergeCell ref="A174:A187"/>
-    <mergeCell ref="A159:A172"/>
-    <mergeCell ref="A146:A156"/>
-    <mergeCell ref="A134:A144"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Atualizado o ex031 e planilha
</commit_message>
<xml_diff>
--- a/detalhesPython.xlsx
+++ b/detalhesPython.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\thiag\Documents\EstudosT\python\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD553F8A-24DD-4E11-84CA-447119F6FCC4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F44431C5-D141-4B5D-AB1E-1BF56F4F030D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{ECBDB9F7-0FAD-476C-A4A4-7948F29B869E}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="288" uniqueCount="268">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="296" uniqueCount="275">
   <si>
     <t>Descrição</t>
   </si>
@@ -12008,6 +12008,327 @@
         <family val="3"/>
       </rPr>
       <t>(num))</t>
+    </r>
+  </si>
+  <si>
+    <t>ex031</t>
+  </si>
+  <si>
+    <t>Desenvolva um programa que pergunte a distância de uma viagem em Km. Calcule o preço da passagem, 
+cobrando R$0,50 por Km para viagens de até 200Km e R$0,45 parta viagens mais longas.</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">distancia </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>=</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color rgb="FF988BC7"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>float</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>(</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF988BC7"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>input</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>(</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE7DE79"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>'Quantos km é a distância da sua viagem: '</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>))</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>if</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> distancia </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>&lt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF78D1E1"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>201</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>:</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">    preço </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>=</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> distancia </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>*</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF78D1E1"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>0.50</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">    preço </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>=</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> distancia </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>*</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF78D1E1"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>0.45</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>print</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>(</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE7DE79"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>'Sua passagem terá o valor de R$</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF78D1E1"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>{</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>:.2f</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF78D1E1"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>}</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE7DE79"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>'</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF67E480"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>format</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>(preço))</t>
     </r>
   </si>
 </sst>
@@ -12462,7 +12783,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="45">
+  <cellXfs count="46">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -12580,6 +12901,9 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="11" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -12589,9 +12913,7 @@
     <xf numFmtId="0" fontId="11" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="15" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -12906,10 +13228,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{73331524-72FC-41A3-82E6-4326A0999772}">
-  <dimension ref="A1:E318"/>
+  <dimension ref="A1:E328"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A301" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A311" sqref="A311:A318"/>
+    <sheetView tabSelected="1" topLeftCell="A313" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B328" sqref="B328"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -12928,7 +13250,7 @@
       </c>
     </row>
     <row r="2" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="41" t="s">
+      <c r="A2" s="42" t="s">
         <v>227</v>
       </c>
       <c r="B2" s="31" t="s">
@@ -12936,23 +13258,23 @@
       </c>
     </row>
     <row r="3" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="42"/>
+      <c r="A3" s="43"/>
       <c r="B3" s="7"/>
     </row>
     <row r="4" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="42"/>
+      <c r="A4" s="43"/>
       <c r="B4" s="7" t="s">
         <v>229</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="42"/>
+      <c r="A5" s="43"/>
       <c r="B5" s="39" t="s">
         <v>230</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="43"/>
+      <c r="A6" s="44"/>
       <c r="B6" s="33"/>
     </row>
     <row r="7" spans="1:2" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -12960,7 +13282,7 @@
       <c r="B7" s="20"/>
     </row>
     <row r="8" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="41" t="s">
+      <c r="A8" s="42" t="s">
         <v>220</v>
       </c>
       <c r="B8" s="31" t="s">
@@ -12968,35 +13290,35 @@
       </c>
     </row>
     <row r="9" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="42"/>
+      <c r="A9" s="43"/>
       <c r="B9" s="7"/>
     </row>
     <row r="10" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="42"/>
+      <c r="A10" s="43"/>
       <c r="B10" s="7" t="s">
         <v>222</v>
       </c>
     </row>
     <row r="11" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="42"/>
+      <c r="A11" s="43"/>
       <c r="B11" s="7" t="s">
         <v>223</v>
       </c>
     </row>
     <row r="12" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="42"/>
+      <c r="A12" s="43"/>
       <c r="B12" s="7" t="s">
         <v>224</v>
       </c>
     </row>
     <row r="13" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="42"/>
+      <c r="A13" s="43"/>
       <c r="B13" s="39" t="s">
         <v>225</v>
       </c>
     </row>
     <row r="14" spans="1:2" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="43"/>
+      <c r="A14" s="44"/>
       <c r="B14" s="33"/>
     </row>
     <row r="15" spans="1:2" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -13004,7 +13326,7 @@
       <c r="B15" s="20"/>
     </row>
     <row r="16" spans="1:2" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="41" t="s">
+      <c r="A16" s="42" t="s">
         <v>210</v>
       </c>
       <c r="B16" s="31" t="s">
@@ -13012,65 +13334,65 @@
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A17" s="42"/>
+      <c r="A17" s="43"/>
       <c r="B17" s="7"/>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A18" s="42"/>
+      <c r="A18" s="43"/>
       <c r="B18" s="7" t="s">
         <v>211</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A19" s="42"/>
+      <c r="A19" s="43"/>
       <c r="B19" s="11" t="s">
         <v>212</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A20" s="42"/>
+      <c r="A20" s="43"/>
       <c r="B20" s="11" t="s">
         <v>213</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A21" s="42"/>
+      <c r="A21" s="43"/>
       <c r="B21" s="11" t="s">
         <v>214</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A22" s="42"/>
+      <c r="A22" s="43"/>
       <c r="B22" s="11" t="s">
         <v>215</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A23" s="42"/>
+      <c r="A23" s="43"/>
       <c r="B23" s="11" t="s">
         <v>216</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A24" s="42"/>
+      <c r="A24" s="43"/>
       <c r="B24" s="11" t="s">
         <v>217</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A25" s="42"/>
+      <c r="A25" s="43"/>
       <c r="B25" s="11" t="s">
         <v>218</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A26" s="42"/>
+      <c r="A26" s="43"/>
       <c r="B26" s="39" t="s">
         <v>219</v>
       </c>
     </row>
     <row r="27" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="43"/>
+      <c r="A27" s="44"/>
       <c r="B27" s="33"/>
     </row>
     <row r="28" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -13078,7 +13400,7 @@
       <c r="B28" s="20"/>
     </row>
     <row r="29" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="41" t="s">
+      <c r="A29" s="42" t="s">
         <v>204</v>
       </c>
       <c r="B29" s="31" t="s">
@@ -13086,35 +13408,35 @@
       </c>
     </row>
     <row r="30" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="42"/>
+      <c r="A30" s="43"/>
       <c r="B30" s="7"/>
     </row>
     <row r="31" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="42"/>
+      <c r="A31" s="43"/>
       <c r="B31" s="7" t="s">
         <v>206</v>
       </c>
     </row>
     <row r="32" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="42"/>
+      <c r="A32" s="43"/>
       <c r="B32" s="7" t="s">
         <v>207</v>
       </c>
     </row>
     <row r="33" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="42"/>
+      <c r="A33" s="43"/>
       <c r="B33" s="7" t="s">
         <v>208</v>
       </c>
     </row>
     <row r="34" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="42"/>
+      <c r="A34" s="43"/>
       <c r="B34" s="39" t="s">
         <v>209</v>
       </c>
     </row>
     <row r="35" spans="1:2" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="43"/>
+      <c r="A35" s="44"/>
       <c r="B35" s="33"/>
     </row>
     <row r="36" spans="1:2" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -13122,7 +13444,7 @@
       <c r="B36" s="20"/>
     </row>
     <row r="37" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A37" s="41" t="s">
+      <c r="A37" s="42" t="s">
         <v>195</v>
       </c>
       <c r="B37" s="31" t="s">
@@ -13130,53 +13452,53 @@
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A38" s="42"/>
+      <c r="A38" s="43"/>
       <c r="B38" s="7"/>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A39" s="42"/>
+      <c r="A39" s="43"/>
       <c r="B39" s="7" t="s">
         <v>197</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A40" s="42"/>
+      <c r="A40" s="43"/>
       <c r="B40" s="7" t="s">
         <v>198</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A41" s="42"/>
+      <c r="A41" s="43"/>
       <c r="B41" s="7" t="s">
         <v>199</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A42" s="42"/>
+      <c r="A42" s="43"/>
       <c r="B42" s="7" t="s">
         <v>200</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A43" s="42"/>
+      <c r="A43" s="43"/>
       <c r="B43" s="11" t="s">
         <v>201</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A44" s="42"/>
+      <c r="A44" s="43"/>
       <c r="B44" s="11" t="s">
         <v>202</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A45" s="42"/>
+      <c r="A45" s="43"/>
       <c r="B45" s="39" t="s">
         <v>203</v>
       </c>
     </row>
     <row r="46" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A46" s="43"/>
+      <c r="A46" s="44"/>
       <c r="B46" s="33"/>
     </row>
     <row r="47" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -13184,7 +13506,7 @@
       <c r="B47" s="20"/>
     </row>
     <row r="48" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A48" s="41" t="s">
+      <c r="A48" s="42" t="s">
         <v>189</v>
       </c>
       <c r="B48" s="31" t="s">
@@ -13192,35 +13514,35 @@
       </c>
     </row>
     <row r="49" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A49" s="42"/>
+      <c r="A49" s="43"/>
       <c r="B49" s="7"/>
     </row>
     <row r="50" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A50" s="42"/>
+      <c r="A50" s="43"/>
       <c r="B50" s="7" t="s">
         <v>191</v>
       </c>
     </row>
     <row r="51" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A51" s="42"/>
+      <c r="A51" s="43"/>
       <c r="B51" s="7" t="s">
         <v>192</v>
       </c>
     </row>
     <row r="52" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A52" s="42"/>
+      <c r="A52" s="43"/>
       <c r="B52" s="7" t="s">
         <v>193</v>
       </c>
     </row>
     <row r="53" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A53" s="42"/>
+      <c r="A53" s="43"/>
       <c r="B53" s="39" t="s">
         <v>194</v>
       </c>
     </row>
     <row r="54" spans="1:2" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A54" s="43"/>
+      <c r="A54" s="44"/>
       <c r="B54" s="33"/>
     </row>
     <row r="55" spans="1:2" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -13228,7 +13550,7 @@
       <c r="B55" s="20"/>
     </row>
     <row r="56" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A56" s="41" t="s">
+      <c r="A56" s="42" t="s">
         <v>183</v>
       </c>
       <c r="B56" s="31" t="s">
@@ -13236,35 +13558,35 @@
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A57" s="42"/>
+      <c r="A57" s="43"/>
       <c r="B57" s="7"/>
     </row>
     <row r="58" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A58" s="42"/>
+      <c r="A58" s="43"/>
       <c r="B58" s="7" t="s">
         <v>185</v>
       </c>
     </row>
     <row r="59" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A59" s="42"/>
+      <c r="A59" s="43"/>
       <c r="B59" s="7" t="s">
         <v>186</v>
       </c>
     </row>
     <row r="60" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A60" s="42"/>
+      <c r="A60" s="43"/>
       <c r="B60" s="7" t="s">
         <v>187</v>
       </c>
     </row>
     <row r="61" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A61" s="42"/>
+      <c r="A61" s="43"/>
       <c r="B61" s="39" t="s">
         <v>188</v>
       </c>
     </row>
     <row r="62" spans="1:2" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A62" s="43"/>
+      <c r="A62" s="44"/>
       <c r="B62" s="33"/>
     </row>
     <row r="63" spans="1:2" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -13272,7 +13594,7 @@
       <c r="B63" s="20"/>
     </row>
     <row r="64" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A64" s="41" t="s">
+      <c r="A64" s="42" t="s">
         <v>169</v>
       </c>
       <c r="B64" s="31" t="s">
@@ -13280,83 +13602,83 @@
       </c>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A65" s="42"/>
+      <c r="A65" s="43"/>
       <c r="B65" s="7"/>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A66" s="42"/>
+      <c r="A66" s="43"/>
       <c r="B66" s="7" t="s">
         <v>171</v>
       </c>
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A67" s="42"/>
+      <c r="A67" s="43"/>
       <c r="B67" s="11" t="s">
         <v>172</v>
       </c>
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A68" s="42"/>
+      <c r="A68" s="43"/>
       <c r="B68" s="11" t="s">
         <v>173</v>
       </c>
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A69" s="42"/>
+      <c r="A69" s="43"/>
       <c r="B69" s="11" t="s">
         <v>174</v>
       </c>
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A70" s="42"/>
+      <c r="A70" s="43"/>
       <c r="B70" s="11" t="s">
         <v>175</v>
       </c>
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A71" s="42"/>
+      <c r="A71" s="43"/>
       <c r="B71" s="11" t="s">
         <v>176</v>
       </c>
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A72" s="42"/>
+      <c r="A72" s="43"/>
       <c r="B72" s="11" t="s">
         <v>177</v>
       </c>
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A73" s="42"/>
+      <c r="A73" s="43"/>
       <c r="B73" s="11" t="s">
         <v>178</v>
       </c>
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A74" s="42"/>
+      <c r="A74" s="43"/>
       <c r="B74" s="11" t="s">
         <v>179</v>
       </c>
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A75" s="42"/>
+      <c r="A75" s="43"/>
       <c r="B75" s="11" t="s">
         <v>180</v>
       </c>
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A76" s="42"/>
+      <c r="A76" s="43"/>
       <c r="B76" s="11" t="s">
         <v>181</v>
       </c>
     </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A77" s="42"/>
+      <c r="A77" s="43"/>
       <c r="B77" s="39" t="s">
         <v>182</v>
       </c>
     </row>
     <row r="78" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A78" s="43"/>
+      <c r="A78" s="44"/>
       <c r="B78" s="33"/>
     </row>
     <row r="79" spans="1:2" x14ac:dyDescent="0.25">
@@ -13368,7 +13690,7 @@
       <c r="B80" s="20"/>
     </row>
     <row r="81" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A81" s="41" t="s">
+      <c r="A81" s="42" t="s">
         <v>164</v>
       </c>
       <c r="B81" s="31" t="s">
@@ -13376,29 +13698,29 @@
       </c>
     </row>
     <row r="82" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A82" s="42"/>
+      <c r="A82" s="43"/>
       <c r="B82" s="7"/>
     </row>
     <row r="83" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A83" s="42"/>
+      <c r="A83" s="43"/>
       <c r="B83" s="7" t="s">
         <v>166</v>
       </c>
     </row>
     <row r="84" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A84" s="42"/>
+      <c r="A84" s="43"/>
       <c r="B84" s="7" t="s">
         <v>167</v>
       </c>
     </row>
     <row r="85" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A85" s="42"/>
+      <c r="A85" s="43"/>
       <c r="B85" s="39" t="s">
         <v>168</v>
       </c>
     </row>
     <row r="86" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A86" s="43"/>
+      <c r="A86" s="44"/>
       <c r="B86" s="33"/>
     </row>
     <row r="87" spans="1:2" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -13406,7 +13728,7 @@
       <c r="B87" s="20"/>
     </row>
     <row r="88" spans="1:2" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A88" s="41" t="s">
+      <c r="A88" s="42" t="s">
         <v>157</v>
       </c>
       <c r="B88" s="31" t="s">
@@ -13414,41 +13736,41 @@
       </c>
     </row>
     <row r="89" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A89" s="42"/>
+      <c r="A89" s="43"/>
       <c r="B89" s="7"/>
     </row>
     <row r="90" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A90" s="42"/>
+      <c r="A90" s="43"/>
       <c r="B90" s="7" t="s">
         <v>159</v>
       </c>
     </row>
     <row r="91" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A91" s="42"/>
+      <c r="A91" s="43"/>
       <c r="B91" s="7" t="s">
         <v>160</v>
       </c>
     </row>
     <row r="92" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A92" s="42"/>
+      <c r="A92" s="43"/>
       <c r="B92" s="7" t="s">
         <v>161</v>
       </c>
     </row>
     <row r="93" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A93" s="42"/>
+      <c r="A93" s="43"/>
       <c r="B93" s="11" t="s">
         <v>162</v>
       </c>
     </row>
     <row r="94" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A94" s="42"/>
+      <c r="A94" s="43"/>
       <c r="B94" s="39" t="s">
         <v>163</v>
       </c>
     </row>
     <row r="95" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A95" s="43"/>
+      <c r="A95" s="44"/>
       <c r="B95" s="33"/>
     </row>
     <row r="96" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -13456,7 +13778,7 @@
       <c r="B96" s="20"/>
     </row>
     <row r="97" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A97" s="41" t="s">
+      <c r="A97" s="42" t="s">
         <v>152</v>
       </c>
       <c r="B97" s="31" t="s">
@@ -13464,29 +13786,29 @@
       </c>
     </row>
     <row r="98" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A98" s="42"/>
+      <c r="A98" s="43"/>
       <c r="B98" s="7"/>
     </row>
     <row r="99" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A99" s="42"/>
+      <c r="A99" s="43"/>
       <c r="B99" s="7" t="s">
         <v>154</v>
       </c>
     </row>
     <row r="100" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A100" s="42"/>
+      <c r="A100" s="43"/>
       <c r="B100" s="7" t="s">
         <v>155</v>
       </c>
     </row>
     <row r="101" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A101" s="42"/>
+      <c r="A101" s="43"/>
       <c r="B101" s="39" t="s">
         <v>156</v>
       </c>
     </row>
     <row r="102" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A102" s="43"/>
+      <c r="A102" s="44"/>
       <c r="B102" s="33"/>
     </row>
     <row r="103" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -13494,7 +13816,7 @@
       <c r="B103" s="20"/>
     </row>
     <row r="104" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A104" s="41" t="s">
+      <c r="A104" s="42" t="s">
         <v>147</v>
       </c>
       <c r="B104" s="31" t="s">
@@ -13502,29 +13824,29 @@
       </c>
     </row>
     <row r="105" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A105" s="42"/>
+      <c r="A105" s="43"/>
       <c r="B105" s="7"/>
     </row>
     <row r="106" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A106" s="42"/>
+      <c r="A106" s="43"/>
       <c r="B106" s="7" t="s">
         <v>149</v>
       </c>
     </row>
     <row r="107" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A107" s="42"/>
+      <c r="A107" s="43"/>
       <c r="B107" s="7" t="s">
         <v>150</v>
       </c>
     </row>
     <row r="108" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A108" s="42"/>
+      <c r="A108" s="43"/>
       <c r="B108" s="39" t="s">
         <v>151</v>
       </c>
     </row>
     <row r="109" spans="1:2" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A109" s="43"/>
+      <c r="A109" s="44"/>
       <c r="B109" s="33"/>
     </row>
     <row r="110" spans="1:2" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -13532,7 +13854,7 @@
       <c r="B110" s="20"/>
     </row>
     <row r="111" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A111" s="41" t="s">
+      <c r="A111" s="42" t="s">
         <v>142</v>
       </c>
       <c r="B111" s="31" t="s">
@@ -13540,29 +13862,29 @@
       </c>
     </row>
     <row r="112" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A112" s="42"/>
+      <c r="A112" s="43"/>
       <c r="B112" s="7"/>
     </row>
     <row r="113" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A113" s="42"/>
+      <c r="A113" s="43"/>
       <c r="B113" s="7" t="s">
         <v>144</v>
       </c>
     </row>
     <row r="114" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A114" s="42"/>
+      <c r="A114" s="43"/>
       <c r="B114" s="7" t="s">
         <v>145</v>
       </c>
     </row>
     <row r="115" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A115" s="42"/>
+      <c r="A115" s="43"/>
       <c r="B115" s="39" t="s">
         <v>146</v>
       </c>
     </row>
     <row r="116" spans="1:2" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A116" s="43"/>
+      <c r="A116" s="44"/>
       <c r="B116" s="33"/>
     </row>
     <row r="117" spans="1:2" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -13570,7 +13892,7 @@
       <c r="B117" s="20"/>
     </row>
     <row r="118" spans="1:2" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A118" s="41" t="s">
+      <c r="A118" s="42" t="s">
         <v>136</v>
       </c>
       <c r="B118" s="31" t="s">
@@ -13578,35 +13900,35 @@
       </c>
     </row>
     <row r="119" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A119" s="42"/>
+      <c r="A119" s="43"/>
       <c r="B119" s="7"/>
     </row>
     <row r="120" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A120" s="42"/>
+      <c r="A120" s="43"/>
       <c r="B120" s="7" t="s">
         <v>138</v>
       </c>
     </row>
     <row r="121" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A121" s="42"/>
+      <c r="A121" s="43"/>
       <c r="B121" s="7" t="s">
         <v>139</v>
       </c>
     </row>
     <row r="122" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A122" s="42"/>
+      <c r="A122" s="43"/>
       <c r="B122" s="7" t="s">
         <v>140</v>
       </c>
     </row>
     <row r="123" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A123" s="42"/>
+      <c r="A123" s="43"/>
       <c r="B123" s="39" t="s">
         <v>141</v>
       </c>
     </row>
     <row r="124" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A124" s="43"/>
+      <c r="A124" s="44"/>
       <c r="B124" s="33"/>
     </row>
     <row r="125" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -13614,7 +13936,7 @@
       <c r="B125" s="20"/>
     </row>
     <row r="126" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A126" s="41" t="s">
+      <c r="A126" s="42" t="s">
         <v>127</v>
       </c>
       <c r="B126" s="31" t="s">
@@ -13622,33 +13944,33 @@
       </c>
     </row>
     <row r="127" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A127" s="42"/>
+      <c r="A127" s="43"/>
       <c r="B127" s="7"/>
     </row>
     <row r="128" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A128" s="42"/>
+      <c r="A128" s="43"/>
       <c r="B128" s="7" t="s">
         <v>129</v>
       </c>
     </row>
     <row r="129" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A129" s="42"/>
+      <c r="A129" s="43"/>
       <c r="B129" s="11" t="s">
         <v>130</v>
       </c>
     </row>
     <row r="130" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A130" s="42"/>
+      <c r="A130" s="43"/>
       <c r="B130" s="7"/>
     </row>
     <row r="131" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A131" s="42"/>
+      <c r="A131" s="43"/>
       <c r="B131" s="38" t="s">
         <v>131</v>
       </c>
     </row>
     <row r="132" spans="1:2" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A132" s="43"/>
+      <c r="A132" s="44"/>
       <c r="B132" s="33"/>
     </row>
     <row r="133" spans="1:2" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -13656,7 +13978,7 @@
       <c r="B133" s="20"/>
     </row>
     <row r="134" spans="1:2" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A134" s="41" t="s">
+      <c r="A134" s="42" t="s">
         <v>119</v>
       </c>
       <c r="B134" s="31" t="s">
@@ -13664,57 +13986,57 @@
       </c>
     </row>
     <row r="135" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A135" s="42"/>
+      <c r="A135" s="43"/>
       <c r="B135" s="7"/>
     </row>
     <row r="136" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A136" s="42"/>
+      <c r="A136" s="43"/>
       <c r="B136" s="34" t="s">
         <v>121</v>
       </c>
     </row>
     <row r="137" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A137" s="42"/>
+      <c r="A137" s="43"/>
       <c r="B137" s="7" t="s">
         <v>122</v>
       </c>
     </row>
     <row r="138" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A138" s="42"/>
+      <c r="A138" s="43"/>
       <c r="B138" s="7" t="s">
         <v>123</v>
       </c>
     </row>
     <row r="139" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A139" s="42"/>
+      <c r="A139" s="43"/>
       <c r="B139" s="7" t="s">
         <v>124</v>
       </c>
     </row>
     <row r="140" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A140" s="42"/>
+      <c r="A140" s="43"/>
       <c r="B140" s="11" t="s">
         <v>125</v>
       </c>
     </row>
     <row r="141" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A141" s="42"/>
+      <c r="A141" s="43"/>
       <c r="B141" s="11"/>
     </row>
     <row r="142" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A142" s="42"/>
+      <c r="A142" s="43"/>
       <c r="B142" s="11" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="143" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A143" s="42"/>
+      <c r="A143" s="43"/>
       <c r="B143" s="39" t="s">
         <v>126</v>
       </c>
     </row>
     <row r="144" spans="1:2" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A144" s="43"/>
+      <c r="A144" s="44"/>
       <c r="B144" s="33"/>
     </row>
     <row r="145" spans="1:5" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -13722,7 +14044,7 @@
       <c r="B145" s="20"/>
     </row>
     <row r="146" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A146" s="41" t="s">
+      <c r="A146" s="42" t="s">
         <v>106</v>
       </c>
       <c r="B146" s="31" t="s">
@@ -13730,59 +14052,59 @@
       </c>
     </row>
     <row r="147" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A147" s="42"/>
+      <c r="A147" s="43"/>
       <c r="B147" s="7"/>
     </row>
     <row r="148" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A148" s="42"/>
+      <c r="A148" s="43"/>
       <c r="B148" s="34" t="s">
         <v>108</v>
       </c>
     </row>
     <row r="149" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A149" s="42"/>
+      <c r="A149" s="43"/>
       <c r="B149" s="7" t="s">
         <v>109</v>
       </c>
     </row>
     <row r="150" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A150" s="42"/>
+      <c r="A150" s="43"/>
       <c r="B150" s="7" t="s">
         <v>110</v>
       </c>
     </row>
     <row r="151" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A151" s="42"/>
+      <c r="A151" s="43"/>
       <c r="B151" s="7" t="s">
         <v>111</v>
       </c>
     </row>
     <row r="152" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A152" s="42"/>
+      <c r="A152" s="43"/>
       <c r="B152" s="7" t="s">
         <v>112</v>
       </c>
     </row>
     <row r="153" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A153" s="42"/>
+      <c r="A153" s="43"/>
       <c r="B153" s="11" t="s">
         <v>113</v>
       </c>
     </row>
     <row r="154" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A154" s="42"/>
+      <c r="A154" s="43"/>
       <c r="B154" s="11" t="s">
         <v>114</v>
       </c>
     </row>
     <row r="155" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A155" s="42"/>
+      <c r="A155" s="43"/>
       <c r="B155" s="39" t="s">
         <v>115</v>
       </c>
     </row>
     <row r="156" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A156" s="43"/>
+      <c r="A156" s="44"/>
       <c r="B156" s="33"/>
       <c r="C156" s="2" t="s">
         <v>116</v>
@@ -13803,7 +14125,7 @@
       <c r="B158" s="20"/>
     </row>
     <row r="159" spans="1:5" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A159" s="41" t="s">
+      <c r="A159" s="42" t="s">
         <v>85</v>
       </c>
       <c r="B159" s="31" t="s">
@@ -13811,75 +14133,75 @@
       </c>
     </row>
     <row r="160" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A160" s="42"/>
+      <c r="A160" s="43"/>
       <c r="B160" s="7"/>
     </row>
     <row r="161" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A161" s="42"/>
+      <c r="A161" s="43"/>
       <c r="B161" s="34" t="s">
         <v>87</v>
       </c>
     </row>
     <row r="162" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A162" s="42"/>
+      <c r="A162" s="43"/>
       <c r="B162" s="7" t="s">
         <v>88</v>
       </c>
     </row>
     <row r="163" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A163" s="42"/>
+      <c r="A163" s="43"/>
       <c r="B163" s="7" t="s">
         <v>89</v>
       </c>
     </row>
     <row r="164" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A164" s="42"/>
+      <c r="A164" s="43"/>
       <c r="B164" s="7" t="s">
         <v>90</v>
       </c>
     </row>
     <row r="165" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A165" s="42"/>
+      <c r="A165" s="43"/>
       <c r="B165" s="7" t="s">
         <v>91</v>
       </c>
     </row>
     <row r="166" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A166" s="42"/>
+      <c r="A166" s="43"/>
       <c r="B166" s="7" t="s">
         <v>92</v>
       </c>
     </row>
     <row r="167" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A167" s="42"/>
+      <c r="A167" s="43"/>
       <c r="B167" s="7" t="s">
         <v>93</v>
       </c>
     </row>
     <row r="168" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A168" s="42"/>
+      <c r="A168" s="43"/>
       <c r="B168" s="11" t="s">
         <v>94</v>
       </c>
     </row>
     <row r="169" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A169" s="42"/>
+      <c r="A169" s="43"/>
       <c r="B169" s="11"/>
     </row>
     <row r="170" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A170" s="42"/>
+      <c r="A170" s="43"/>
       <c r="B170" s="36" t="s">
         <v>83</v>
       </c>
     </row>
     <row r="171" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A171" s="42"/>
+      <c r="A171" s="43"/>
       <c r="B171" s="37" t="s">
         <v>95</v>
       </c>
     </row>
     <row r="172" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A172" s="43"/>
+      <c r="A172" s="44"/>
       <c r="B172" s="33" t="s">
         <v>96</v>
       </c>
@@ -13895,7 +14217,7 @@
       <c r="B173" s="20"/>
     </row>
     <row r="174" spans="1:4" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A174" s="41" t="s">
+      <c r="A174" s="42" t="s">
         <v>73</v>
       </c>
       <c r="B174" s="31" t="s">
@@ -13903,69 +14225,69 @@
       </c>
     </row>
     <row r="175" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A175" s="42"/>
+      <c r="A175" s="43"/>
       <c r="B175" s="7"/>
     </row>
     <row r="176" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A176" s="42"/>
+      <c r="A176" s="43"/>
       <c r="B176" s="34" t="s">
         <v>75</v>
       </c>
     </row>
     <row r="177" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A177" s="42"/>
+      <c r="A177" s="43"/>
       <c r="B177" s="7" t="s">
         <v>76</v>
       </c>
     </row>
     <row r="178" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A178" s="42"/>
+      <c r="A178" s="43"/>
       <c r="B178" s="7" t="s">
         <v>77</v>
       </c>
     </row>
     <row r="179" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A179" s="42"/>
+      <c r="A179" s="43"/>
       <c r="B179" s="7" t="s">
         <v>78</v>
       </c>
     </row>
     <row r="180" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A180" s="42"/>
+      <c r="A180" s="43"/>
       <c r="B180" s="7" t="s">
         <v>79</v>
       </c>
     </row>
     <row r="181" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A181" s="42"/>
+      <c r="A181" s="43"/>
       <c r="B181" s="7" t="s">
         <v>80</v>
       </c>
     </row>
     <row r="182" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A182" s="42"/>
+      <c r="A182" s="43"/>
       <c r="B182" s="35" t="s">
         <v>81</v>
       </c>
     </row>
     <row r="183" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A183" s="42"/>
+      <c r="A183" s="43"/>
       <c r="B183" s="11" t="s">
         <v>82</v>
       </c>
     </row>
     <row r="184" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A184" s="42"/>
+      <c r="A184" s="43"/>
       <c r="B184" s="11"/>
     </row>
     <row r="185" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A185" s="42"/>
+      <c r="A185" s="43"/>
       <c r="B185" s="36" t="s">
         <v>83</v>
       </c>
     </row>
     <row r="186" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A186" s="42"/>
+      <c r="A186" s="43"/>
       <c r="B186" s="37" t="s">
         <v>84</v>
       </c>
@@ -13977,7 +14299,7 @@
       </c>
     </row>
     <row r="187" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A187" s="43"/>
+      <c r="A187" s="44"/>
       <c r="B187" s="33" t="s">
         <v>97</v>
       </c>
@@ -13993,7 +14315,7 @@
       <c r="B188" s="20"/>
     </row>
     <row r="189" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A189" s="41" t="s">
+      <c r="A189" s="42" t="s">
         <v>66</v>
       </c>
       <c r="B189" s="29" t="s">
@@ -14001,41 +14323,41 @@
       </c>
     </row>
     <row r="190" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A190" s="42"/>
+      <c r="A190" s="43"/>
       <c r="B190" s="7"/>
     </row>
     <row r="191" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A191" s="42"/>
+      <c r="A191" s="43"/>
       <c r="B191" s="34" t="s">
         <v>68</v>
       </c>
     </row>
     <row r="192" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A192" s="42"/>
+      <c r="A192" s="43"/>
       <c r="B192" s="7" t="s">
         <v>69</v>
       </c>
     </row>
     <row r="193" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A193" s="42"/>
+      <c r="A193" s="43"/>
       <c r="B193" s="7" t="s">
         <v>70</v>
       </c>
     </row>
     <row r="194" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A194" s="42"/>
+      <c r="A194" s="43"/>
       <c r="B194" s="7" t="s">
         <v>71</v>
       </c>
     </row>
     <row r="195" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A195" s="42"/>
+      <c r="A195" s="43"/>
       <c r="B195" s="11" t="s">
         <v>72</v>
       </c>
     </row>
     <row r="196" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A196" s="43"/>
+      <c r="A196" s="44"/>
       <c r="B196" s="18"/>
       <c r="C196" s="2" t="s">
         <v>104</v>
@@ -14049,7 +14371,7 @@
       <c r="B197" s="20"/>
     </row>
     <row r="198" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A198" s="41" t="s">
+      <c r="A198" s="42" t="s">
         <v>47</v>
       </c>
       <c r="B198" s="29" t="s">
@@ -14057,23 +14379,23 @@
       </c>
     </row>
     <row r="199" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A199" s="42"/>
+      <c r="A199" s="43"/>
       <c r="B199" s="21"/>
     </row>
     <row r="200" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A200" s="42"/>
+      <c r="A200" s="43"/>
       <c r="B200" s="21" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="201" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A201" s="42"/>
+      <c r="A201" s="43"/>
       <c r="B201" s="22" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="202" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A202" s="42"/>
+      <c r="A202" s="43"/>
       <c r="B202" s="22" t="s">
         <v>27</v>
       </c>
@@ -14082,7 +14404,7 @@
       </c>
     </row>
     <row r="203" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A203" s="42"/>
+      <c r="A203" s="43"/>
       <c r="B203" s="22" t="s">
         <v>28</v>
       </c>
@@ -14091,7 +14413,7 @@
       </c>
     </row>
     <row r="204" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A204" s="42"/>
+      <c r="A204" s="43"/>
       <c r="B204" s="22" t="s">
         <v>29</v>
       </c>
@@ -14103,7 +14425,7 @@
       </c>
     </row>
     <row r="205" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A205" s="42"/>
+      <c r="A205" s="43"/>
       <c r="B205" s="21" t="s">
         <v>30</v>
       </c>
@@ -14112,7 +14434,7 @@
       </c>
     </row>
     <row r="206" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A206" s="42"/>
+      <c r="A206" s="43"/>
       <c r="B206" s="24" t="s">
         <v>31</v>
       </c>
@@ -14121,53 +14443,53 @@
       </c>
     </row>
     <row r="207" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A207" s="42"/>
+      <c r="A207" s="43"/>
       <c r="B207" s="22"/>
     </row>
     <row r="208" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A208" s="42"/>
+      <c r="A208" s="43"/>
       <c r="B208" s="25" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="209" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A209" s="42"/>
+      <c r="A209" s="43"/>
       <c r="B209" s="26" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="210" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A210" s="42"/>
+      <c r="A210" s="43"/>
       <c r="B210" s="23" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="211" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A211" s="42"/>
+      <c r="A211" s="43"/>
       <c r="B211" s="23" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="212" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A212" s="42"/>
+      <c r="A212" s="43"/>
       <c r="B212" s="23" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="213" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A213" s="42"/>
+      <c r="A213" s="43"/>
       <c r="B213" s="23" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="214" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A214" s="42"/>
+      <c r="A214" s="43"/>
       <c r="B214" s="23" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="215" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A215" s="43"/>
+      <c r="A215" s="44"/>
       <c r="B215" s="27"/>
     </row>
     <row r="216" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -14175,7 +14497,7 @@
       <c r="B216" s="20"/>
     </row>
     <row r="217" spans="1:3" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A217" s="41" t="s">
+      <c r="A217" s="42" t="s">
         <v>2</v>
       </c>
       <c r="B217" s="29" t="s">
@@ -14183,11 +14505,11 @@
       </c>
     </row>
     <row r="218" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A218" s="42"/>
+      <c r="A218" s="43"/>
       <c r="B218" s="7"/>
     </row>
     <row r="219" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A219" s="42"/>
+      <c r="A219" s="43"/>
       <c r="B219" s="8" t="s">
         <v>4</v>
       </c>
@@ -14196,13 +14518,13 @@
       </c>
     </row>
     <row r="220" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A220" s="42"/>
+      <c r="A220" s="43"/>
       <c r="B220" s="9" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="221" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A221" s="42"/>
+      <c r="A221" s="43"/>
       <c r="B221" s="7" t="s">
         <v>6</v>
       </c>
@@ -14211,43 +14533,43 @@
       </c>
     </row>
     <row r="222" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A222" s="42"/>
+      <c r="A222" s="43"/>
       <c r="B222" s="10" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="223" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A223" s="42"/>
+      <c r="A223" s="43"/>
       <c r="B223" s="9" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="224" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A224" s="42"/>
+      <c r="A224" s="43"/>
       <c r="B224" s="11" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="225" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A225" s="42"/>
+      <c r="A225" s="43"/>
       <c r="B225" s="12" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="226" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A226" s="42"/>
+      <c r="A226" s="43"/>
       <c r="B226" s="12" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="227" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A227" s="42"/>
+      <c r="A227" s="43"/>
       <c r="B227" s="12" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="228" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A228" s="43"/>
+      <c r="A228" s="44"/>
       <c r="B228" s="13" t="s">
         <v>13</v>
       </c>
@@ -14257,7 +14579,7 @@
       <c r="B229" s="1"/>
     </row>
     <row r="230" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A230" s="41" t="s">
+      <c r="A230" s="42" t="s">
         <v>14</v>
       </c>
       <c r="B230" s="29" t="s">
@@ -14265,11 +14587,11 @@
       </c>
     </row>
     <row r="231" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A231" s="42"/>
+      <c r="A231" s="43"/>
       <c r="B231" s="7"/>
     </row>
     <row r="232" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A232" s="42"/>
+      <c r="A232" s="43"/>
       <c r="B232" s="7" t="s">
         <v>16</v>
       </c>
@@ -14278,7 +14600,7 @@
       </c>
     </row>
     <row r="233" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A233" s="42"/>
+      <c r="A233" s="43"/>
       <c r="B233" s="11" t="s">
         <v>17</v>
       </c>
@@ -14287,18 +14609,18 @@
       </c>
     </row>
     <row r="234" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A234" s="42"/>
+      <c r="A234" s="43"/>
       <c r="B234" s="7"/>
       <c r="D234" s="3"/>
     </row>
     <row r="235" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A235" s="42"/>
+      <c r="A235" s="43"/>
       <c r="B235" s="15" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="236" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A236" s="42"/>
+      <c r="A236" s="43"/>
       <c r="B236" s="26" t="s">
         <v>48</v>
       </c>
@@ -14307,7 +14629,7 @@
       </c>
     </row>
     <row r="237" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A237" s="43"/>
+      <c r="A237" s="44"/>
       <c r="B237" s="18" t="s">
         <v>21</v>
       </c>
@@ -14320,7 +14642,7 @@
       <c r="B238" s="14"/>
     </row>
     <row r="239" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A239" s="41" t="s">
+      <c r="A239" s="42" t="s">
         <v>19</v>
       </c>
       <c r="B239" s="29" t="s">
@@ -14328,11 +14650,11 @@
       </c>
     </row>
     <row r="240" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A240" s="42"/>
+      <c r="A240" s="43"/>
       <c r="B240" s="7"/>
     </row>
     <row r="241" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A241" s="42"/>
+      <c r="A241" s="43"/>
       <c r="B241" s="7" t="s">
         <v>22</v>
       </c>
@@ -14341,7 +14663,7 @@
       </c>
     </row>
     <row r="242" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A242" s="42"/>
+      <c r="A242" s="43"/>
       <c r="B242" s="11" t="s">
         <v>23</v>
       </c>
@@ -14350,21 +14672,21 @@
       </c>
     </row>
     <row r="243" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A243" s="42"/>
+      <c r="A243" s="43"/>
       <c r="B243" s="7"/>
     </row>
     <row r="244" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A244" s="42"/>
+      <c r="A244" s="43"/>
       <c r="B244" s="9"/>
     </row>
     <row r="245" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A245" s="42"/>
+      <c r="A245" s="43"/>
       <c r="B245" s="15" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="246" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A246" s="43"/>
+      <c r="A246" s="44"/>
       <c r="B246" s="16" t="s">
         <v>24</v>
       </c>
@@ -14377,7 +14699,7 @@
       <c r="B247" s="4"/>
     </row>
     <row r="248" spans="1:4" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A248" s="41" t="s">
+      <c r="A248" s="42" t="s">
         <v>56</v>
       </c>
       <c r="B248" s="31" t="s">
@@ -14385,45 +14707,45 @@
       </c>
     </row>
     <row r="249" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A249" s="42"/>
+      <c r="A249" s="43"/>
       <c r="B249" s="7"/>
     </row>
     <row r="250" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A250" s="42"/>
+      <c r="A250" s="43"/>
       <c r="B250" s="7" t="s">
         <v>52</v>
       </c>
     </row>
     <row r="251" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A251" s="42"/>
+      <c r="A251" s="43"/>
       <c r="B251" s="11" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="252" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A252" s="42"/>
+      <c r="A252" s="43"/>
       <c r="B252" s="11" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="253" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A253" s="42"/>
+      <c r="A253" s="43"/>
       <c r="B253" s="11" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="254" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A254" s="42"/>
+      <c r="A254" s="43"/>
       <c r="B254" s="9"/>
     </row>
     <row r="255" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A255" s="42"/>
+      <c r="A255" s="43"/>
       <c r="B255" s="7" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="256" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A256" s="42"/>
+      <c r="A256" s="43"/>
       <c r="B256" s="15" t="s">
         <v>57</v>
       </c>
@@ -14435,32 +14757,32 @@
       </c>
     </row>
     <row r="257" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A257" s="42"/>
+      <c r="A257" s="43"/>
       <c r="B257" s="32" t="s">
         <v>61</v>
       </c>
     </row>
     <row r="258" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A258" s="42"/>
+      <c r="A258" s="43"/>
       <c r="B258" s="32" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="259" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A259" s="42"/>
+      <c r="A259" s="43"/>
       <c r="B259" s="26" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="260" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A260" s="43"/>
+      <c r="A260" s="44"/>
       <c r="B260" s="18" t="s">
         <v>60</v>
       </c>
     </row>
     <row r="261" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="262" spans="1:2" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A262" s="41" t="s">
+      <c r="A262" s="42" t="s">
         <v>63</v>
       </c>
       <c r="B262" s="31" t="s">
@@ -14468,74 +14790,74 @@
       </c>
     </row>
     <row r="263" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A263" s="42"/>
+      <c r="A263" s="43"/>
       <c r="B263" s="40"/>
     </row>
     <row r="264" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A264" s="42"/>
+      <c r="A264" s="43"/>
       <c r="B264" s="7" t="s">
         <v>132</v>
       </c>
     </row>
     <row r="265" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A265" s="42"/>
+      <c r="A265" s="43"/>
       <c r="B265" s="7" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="266" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A266" s="42"/>
+      <c r="A266" s="43"/>
       <c r="B266" s="11" t="s">
         <v>133</v>
       </c>
     </row>
     <row r="267" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A267" s="42"/>
+      <c r="A267" s="43"/>
       <c r="B267" s="11" t="s">
         <v>134</v>
       </c>
     </row>
     <row r="268" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A268" s="42"/>
+      <c r="A268" s="43"/>
       <c r="B268" s="11" t="s">
         <v>135</v>
       </c>
     </row>
     <row r="269" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A269" s="42"/>
+      <c r="A269" s="43"/>
       <c r="B269" s="7"/>
     </row>
     <row r="270" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A270" s="42"/>
+      <c r="A270" s="43"/>
       <c r="B270" s="7" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="271" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A271" s="42"/>
+      <c r="A271" s="43"/>
       <c r="B271" s="26" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="272" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A272" s="42"/>
+      <c r="A272" s="43"/>
       <c r="B272" s="23" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="273" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A273" s="42"/>
+      <c r="A273" s="43"/>
       <c r="B273" s="26" t="s">
         <v>65</v>
       </c>
     </row>
     <row r="274" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A274" s="43"/>
+      <c r="A274" s="44"/>
       <c r="B274" s="18"/>
     </row>
     <row r="275" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="276" spans="1:2" ht="30.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A276" s="41" t="s">
+      <c r="A276" s="42" t="s">
         <v>231</v>
       </c>
       <c r="B276" s="31" t="s">
@@ -14543,99 +14865,99 @@
       </c>
     </row>
     <row r="277" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A277" s="42"/>
+      <c r="A277" s="43"/>
       <c r="B277" s="7"/>
     </row>
     <row r="278" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A278" s="42"/>
+      <c r="A278" s="43"/>
       <c r="B278" s="34" t="s">
         <v>233</v>
       </c>
     </row>
     <row r="279" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A279" s="42"/>
+      <c r="A279" s="43"/>
       <c r="B279" s="34" t="s">
         <v>234</v>
       </c>
     </row>
     <row r="280" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A280" s="42"/>
+      <c r="A280" s="43"/>
       <c r="B280" s="7" t="s">
         <v>235</v>
       </c>
     </row>
     <row r="281" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A281" s="42"/>
+      <c r="A281" s="43"/>
       <c r="B281" s="11" t="s">
         <v>236</v>
       </c>
     </row>
     <row r="282" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A282" s="42"/>
+      <c r="A282" s="43"/>
       <c r="B282" s="11" t="s">
         <v>237</v>
       </c>
     </row>
     <row r="283" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A283" s="42"/>
+      <c r="A283" s="43"/>
       <c r="B283" s="11" t="s">
         <v>236</v>
       </c>
     </row>
     <row r="284" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A284" s="42"/>
+      <c r="A284" s="43"/>
       <c r="B284" s="7" t="s">
         <v>238</v>
       </c>
     </row>
     <row r="285" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A285" s="42"/>
+      <c r="A285" s="43"/>
       <c r="B285" s="11" t="s">
         <v>239</v>
       </c>
     </row>
     <row r="286" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A286" s="42"/>
+      <c r="A286" s="43"/>
       <c r="B286" s="35" t="s">
         <v>240</v>
       </c>
     </row>
     <row r="287" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A287" s="42"/>
+      <c r="A287" s="43"/>
       <c r="B287" s="34" t="s">
         <v>241</v>
       </c>
     </row>
     <row r="288" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A288" s="42"/>
+      <c r="A288" s="43"/>
       <c r="B288" s="7" t="s">
         <v>242</v>
       </c>
     </row>
     <row r="289" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A289" s="42"/>
+      <c r="A289" s="43"/>
       <c r="B289" s="34" t="s">
         <v>243</v>
       </c>
     </row>
     <row r="290" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A290" s="42"/>
+      <c r="A290" s="43"/>
       <c r="B290" s="7" t="s">
         <v>244</v>
       </c>
     </row>
     <row r="291" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A291" s="42"/>
+      <c r="A291" s="43"/>
       <c r="B291" s="11"/>
     </row>
     <row r="292" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A292" s="42"/>
+      <c r="A292" s="43"/>
       <c r="B292" s="11" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="293" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A293" s="42"/>
+      <c r="A293" s="43"/>
       <c r="B293" s="11" t="s">
         <v>245</v>
       </c>
@@ -14650,13 +14972,13 @@
       </c>
     </row>
     <row r="294" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A294" s="42"/>
+      <c r="A294" s="43"/>
       <c r="B294" s="39" t="s">
         <v>246</v>
       </c>
     </row>
     <row r="295" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A295" s="43"/>
+      <c r="A295" s="44"/>
       <c r="B295" s="33"/>
       <c r="C295" s="2" t="s">
         <v>249</v>
@@ -14670,7 +14992,7 @@
     </row>
     <row r="296" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="297" spans="1:5" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A297" s="41" t="s">
+      <c r="A297" s="42" t="s">
         <v>252</v>
       </c>
       <c r="B297" s="31" t="s">
@@ -14678,74 +15000,74 @@
       </c>
     </row>
     <row r="298" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A298" s="42"/>
+      <c r="A298" s="43"/>
       <c r="B298" s="40"/>
     </row>
     <row r="299" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A299" s="42"/>
+      <c r="A299" s="43"/>
       <c r="B299" s="11" t="s">
         <v>254</v>
       </c>
     </row>
     <row r="300" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A300" s="42"/>
+      <c r="A300" s="43"/>
       <c r="B300" s="11" t="s">
         <v>255</v>
       </c>
     </row>
     <row r="301" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A301" s="42"/>
+      <c r="A301" s="43"/>
       <c r="B301" s="11" t="s">
         <v>254</v>
       </c>
     </row>
     <row r="302" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A302" s="42"/>
+      <c r="A302" s="43"/>
       <c r="B302" s="7" t="s">
         <v>256</v>
       </c>
     </row>
     <row r="303" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A303" s="42"/>
+      <c r="A303" s="43"/>
       <c r="B303" s="34" t="s">
         <v>257</v>
       </c>
     </row>
     <row r="304" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A304" s="42"/>
+      <c r="A304" s="43"/>
       <c r="B304" s="7" t="s">
         <v>258</v>
       </c>
     </row>
     <row r="305" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A305" s="42"/>
+      <c r="A305" s="43"/>
       <c r="B305" s="7" t="s">
         <v>259</v>
       </c>
     </row>
     <row r="306" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A306" s="42"/>
+      <c r="A306" s="43"/>
       <c r="B306" s="11" t="s">
         <v>260</v>
       </c>
     </row>
     <row r="307" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A307" s="42"/>
+      <c r="A307" s="43"/>
       <c r="B307" s="23"/>
     </row>
     <row r="308" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A308" s="42"/>
+      <c r="A308" s="43"/>
       <c r="B308" s="26" t="s">
         <v>261</v>
       </c>
     </row>
     <row r="309" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A309" s="43"/>
+      <c r="A309" s="44"/>
       <c r="B309" s="18"/>
     </row>
     <row r="310" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="311" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A311" s="41" t="s">
+      <c r="A311" s="42" t="s">
         <v>262</v>
       </c>
       <c r="B311" s="29" t="s">
@@ -14753,45 +15075,113 @@
       </c>
     </row>
     <row r="312" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A312" s="42"/>
+      <c r="A312" s="43"/>
       <c r="B312" s="7"/>
     </row>
     <row r="313" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A313" s="42"/>
+      <c r="A313" s="43"/>
       <c r="B313" s="7" t="s">
         <v>264</v>
       </c>
     </row>
     <row r="314" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A314" s="42"/>
+      <c r="A314" s="43"/>
       <c r="B314" s="34" t="s">
         <v>265</v>
       </c>
     </row>
     <row r="315" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A315" s="42"/>
+      <c r="A315" s="43"/>
       <c r="B315" s="7" t="s">
         <v>266</v>
       </c>
     </row>
     <row r="316" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A316" s="42"/>
+      <c r="A316" s="43"/>
       <c r="B316" s="34" t="s">
         <v>243</v>
       </c>
     </row>
     <row r="317" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A317" s="42"/>
-      <c r="B317" s="44" t="s">
+      <c r="A317" s="43"/>
+      <c r="B317" s="41" t="s">
         <v>267</v>
       </c>
     </row>
     <row r="318" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A318" s="43"/>
+      <c r="A318" s="44"/>
       <c r="B318" s="16"/>
     </row>
+    <row r="319" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="320" spans="1:2" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A320" s="42" t="s">
+        <v>268</v>
+      </c>
+      <c r="B320" s="31" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="321" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A321" s="43"/>
+      <c r="B321" s="7"/>
+    </row>
+    <row r="322" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A322" s="43"/>
+      <c r="B322" s="7" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="323" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A323" s="43"/>
+      <c r="B323" s="34" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="324" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A324" s="43"/>
+      <c r="B324" s="7" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="325" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A325" s="43"/>
+      <c r="B325" s="34" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="326" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A326" s="43"/>
+      <c r="B326" s="7" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="327" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A327" s="43"/>
+      <c r="B327" s="11" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="328" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A328" s="44"/>
+      <c r="B328" s="45"/>
+    </row>
   </sheetData>
-  <mergeCells count="29">
+  <mergeCells count="30">
+    <mergeCell ref="A118:A124"/>
+    <mergeCell ref="A111:A116"/>
+    <mergeCell ref="A104:A109"/>
+    <mergeCell ref="A320:A328"/>
+    <mergeCell ref="A64:A78"/>
+    <mergeCell ref="A56:A62"/>
+    <mergeCell ref="A48:A54"/>
+    <mergeCell ref="A97:A102"/>
+    <mergeCell ref="A88:A95"/>
+    <mergeCell ref="A81:A86"/>
+    <mergeCell ref="A2:A6"/>
+    <mergeCell ref="A37:A46"/>
+    <mergeCell ref="A29:A35"/>
+    <mergeCell ref="A16:A27"/>
+    <mergeCell ref="A8:A14"/>
     <mergeCell ref="A311:A318"/>
     <mergeCell ref="A126:A132"/>
     <mergeCell ref="A189:A196"/>
@@ -14806,21 +15196,7 @@
     <mergeCell ref="A217:A228"/>
     <mergeCell ref="A248:A260"/>
     <mergeCell ref="A297:A309"/>
-    <mergeCell ref="A2:A6"/>
-    <mergeCell ref="A37:A46"/>
-    <mergeCell ref="A29:A35"/>
-    <mergeCell ref="A16:A27"/>
-    <mergeCell ref="A8:A14"/>
-    <mergeCell ref="A64:A78"/>
-    <mergeCell ref="A56:A62"/>
-    <mergeCell ref="A48:A54"/>
-    <mergeCell ref="A97:A102"/>
-    <mergeCell ref="A88:A95"/>
-    <mergeCell ref="A81:A86"/>
     <mergeCell ref="A276:A295"/>
-    <mergeCell ref="A118:A124"/>
-    <mergeCell ref="A111:A116"/>
-    <mergeCell ref="A104:A109"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Atualizando ex032 e planilha
</commit_message>
<xml_diff>
--- a/detalhesPython.xlsx
+++ b/detalhesPython.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\thiag\Documents\EstudosT\python\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF0EFD33-AA59-4B3A-8373-35C4BB7C27E5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF3C4BCC-1703-4DAE-844D-DA85D0D04BE6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{ECBDB9F7-0FAD-476C-A4A4-7948F29B869E}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="298" uniqueCount="277">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="311" uniqueCount="289">
   <si>
     <t>Descrição</t>
   </si>
@@ -12350,6 +12350,642 @@
   </si>
   <si>
     <t>diminuir</t>
+  </si>
+  <si>
+    <t>ex032</t>
+  </si>
+  <si>
+    <t>Faça um programa que leia um ano qualquer e mostre se ele é bissexto.</t>
+  </si>
+  <si>
+    <r>
+      <t>from</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> datetime </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>import</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> date</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">ano </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>=</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color rgb="FF988BC7"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>int</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>(</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF988BC7"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>input</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>(</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE7DE79"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>'Digite um ano, ou digite 0 para o ano atual: '</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>))</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>if</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> ano </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>==</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF78D1E1"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>0</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>:</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">    ano </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>=</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> date.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF67E480"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>today</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>().year</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>if</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> (ano </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>%</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF78D1E1"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>4</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>==</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF78D1E1"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>0</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>and</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> ano </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>%</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF78D1E1"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>100</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>!=</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF78D1E1"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>0</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">) </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>or</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> (ano </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>%</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF78D1E1"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>400</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>==</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF78D1E1"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>0</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>):</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">    </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF988BC7"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>print</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>(</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE7DE79"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">'O ano </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF78D1E1"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>{}</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE7DE79"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> é Bissexto'</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF67E480"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>format</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>(ano))</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">    </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF988BC7"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>print</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>(</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE7DE79"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">'O ano </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF78D1E1"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>{}</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE7DE79"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> não é bissexto'</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF67E480"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>format</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>(ano))</t>
+    </r>
+  </si>
+  <si>
+    <t>Obs.: date.today().year ---&gt; Serve para o python identificar o ano atual no computador.</t>
+  </si>
+  <si>
+    <t>ano atual</t>
+  </si>
+  <si>
+    <t>data atual</t>
   </si>
 </sst>
 </file>
@@ -13248,10 +13884,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{73331524-72FC-41A3-82E6-4326A0999772}">
-  <dimension ref="A1:E328"/>
+  <dimension ref="A1:E342"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A313" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C328" sqref="C328"/>
+    <sheetView tabSelected="1" topLeftCell="A322" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="E341" sqref="E341"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -15192,8 +15828,104 @@
       <c r="A328" s="45"/>
       <c r="B328" s="42"/>
     </row>
+    <row r="329" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="330" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A330" s="43" t="s">
+        <v>277</v>
+      </c>
+      <c r="B330" s="31" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="331" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A331" s="44"/>
+      <c r="B331" s="40"/>
+    </row>
+    <row r="332" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A332" s="44"/>
+      <c r="B332" s="34" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="333" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A333" s="44"/>
+      <c r="B333" s="7" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="334" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A334" s="44"/>
+      <c r="B334" s="34" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="335" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A335" s="44"/>
+      <c r="B335" s="7" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="336" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A336" s="44"/>
+      <c r="B336" s="34" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="337" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A337" s="44"/>
+      <c r="B337" s="7" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="338" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A338" s="44"/>
+      <c r="B338" s="34" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="339" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A339" s="44"/>
+      <c r="B339" s="7" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="340" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A340" s="44"/>
+      <c r="B340" s="7"/>
+    </row>
+    <row r="341" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A341" s="44"/>
+      <c r="B341" s="11" t="s">
+        <v>286</v>
+      </c>
+      <c r="C341" s="2" t="s">
+        <v>287</v>
+      </c>
+      <c r="D341" s="2" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="342" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A342" s="45"/>
+      <c r="B342" s="42"/>
+    </row>
   </sheetData>
-  <mergeCells count="30">
+  <mergeCells count="31">
+    <mergeCell ref="A330:A342"/>
+    <mergeCell ref="A104:A109"/>
+    <mergeCell ref="A320:A328"/>
+    <mergeCell ref="A64:A78"/>
+    <mergeCell ref="A311:A318"/>
+    <mergeCell ref="A126:A132"/>
+    <mergeCell ref="A189:A196"/>
+    <mergeCell ref="A174:A187"/>
+    <mergeCell ref="A159:A172"/>
+    <mergeCell ref="A146:A156"/>
+    <mergeCell ref="A134:A144"/>
+    <mergeCell ref="A262:A274"/>
+    <mergeCell ref="A230:A237"/>
+    <mergeCell ref="A239:A246"/>
+    <mergeCell ref="A198:A215"/>
     <mergeCell ref="A217:A228"/>
     <mergeCell ref="A248:A260"/>
     <mergeCell ref="A297:A309"/>
@@ -15210,20 +15942,6 @@
     <mergeCell ref="A81:A86"/>
     <mergeCell ref="A118:A124"/>
     <mergeCell ref="A111:A116"/>
-    <mergeCell ref="A104:A109"/>
-    <mergeCell ref="A320:A328"/>
-    <mergeCell ref="A64:A78"/>
-    <mergeCell ref="A311:A318"/>
-    <mergeCell ref="A126:A132"/>
-    <mergeCell ref="A189:A196"/>
-    <mergeCell ref="A174:A187"/>
-    <mergeCell ref="A159:A172"/>
-    <mergeCell ref="A146:A156"/>
-    <mergeCell ref="A134:A144"/>
-    <mergeCell ref="A262:A274"/>
-    <mergeCell ref="A230:A237"/>
-    <mergeCell ref="A239:A246"/>
-    <mergeCell ref="A198:A215"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Criei o ex034 e atualizei a planilha
</commit_message>
<xml_diff>
--- a/detalhesPython.xlsx
+++ b/detalhesPython.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\thiag\Documents\EstudosT\python\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D556C8F-6F0E-413F-8E67-81DCFDA8C279}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C30E44D2-DCFF-41DC-B4E5-C449628F0527}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{ECBDB9F7-0FAD-476C-A4A4-7948F29B869E}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="325" uniqueCount="303">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="333" uniqueCount="309">
   <si>
     <t>Descrição</t>
   </si>
@@ -13430,6 +13430,485 @@
   </si>
   <si>
     <t>math</t>
+  </si>
+  <si>
+    <t>Escreva um programa que pergunte o salário de um funcionário e calcule o valor do seu aumento. Para salários superiores a R$1250,00, calcule um aumento de 10%. Para os inferiores ou iguais, o aumento é de 15%.</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">salario </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>=</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color rgb="FF988BC7"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>float</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>(</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF988BC7"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>input</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>(</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE7DE79"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>'Qual é o salário do funcionário? R$'</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>))</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>if</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> salario </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>&lt;=</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF78D1E1"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>1250</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>:</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">    novo </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>=</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> salario </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> (salario </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>*</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF78D1E1"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>15</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>/</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF78D1E1"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>100</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">    novo </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>=</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> salario </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> (salario </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>*</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF78D1E1"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>10</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>/</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF78D1E1"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>100</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>print</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>(</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE7DE79"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>'Quem ganhava R$</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF78D1E1"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>{</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>:.2f</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF78D1E1"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>}</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE7DE79"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> passa a ganhar R$</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF78D1E1"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>{</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>:.2f</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF78D1E1"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>}</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE7DE79"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> agora'</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF67E480"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>format</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>(salario, novo))</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -14328,10 +14807,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{73331524-72FC-41A3-82E6-4326A0999772}">
-  <dimension ref="A1:G354"/>
+  <dimension ref="A1:G364"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A332" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B351" sqref="B351"/>
+    <sheetView tabSelected="1" topLeftCell="A350" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B364" sqref="B364"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -16431,8 +16910,78 @@
       <c r="A354" s="45"/>
       <c r="B354" s="42"/>
     </row>
+    <row r="355" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="356" spans="1:7" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A356" s="43" t="s">
+        <v>289</v>
+      </c>
+      <c r="B356" s="31" t="s">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="357" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A357" s="44"/>
+      <c r="B357" s="40"/>
+    </row>
+    <row r="358" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A358" s="44"/>
+      <c r="B358" s="7" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="359" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A359" s="44"/>
+      <c r="B359" s="34" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="360" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A360" s="44"/>
+      <c r="B360" s="7" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="361" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A361" s="44"/>
+      <c r="B361" s="34" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="362" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A362" s="44"/>
+      <c r="B362" s="7" t="s">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="363" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A363" s="44"/>
+      <c r="B363" s="11" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="364" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A364" s="45"/>
+      <c r="B364" s="42"/>
+    </row>
   </sheetData>
-  <mergeCells count="32">
+  <mergeCells count="33">
+    <mergeCell ref="A356:A364"/>
+    <mergeCell ref="A330:A342"/>
+    <mergeCell ref="A104:A109"/>
+    <mergeCell ref="A320:A328"/>
+    <mergeCell ref="A64:A78"/>
+    <mergeCell ref="A311:A318"/>
+    <mergeCell ref="A126:A132"/>
+    <mergeCell ref="A189:A196"/>
+    <mergeCell ref="A174:A187"/>
+    <mergeCell ref="A159:A172"/>
+    <mergeCell ref="A146:A156"/>
+    <mergeCell ref="A134:A144"/>
+    <mergeCell ref="A262:A274"/>
+    <mergeCell ref="A230:A237"/>
+    <mergeCell ref="A239:A246"/>
+    <mergeCell ref="A198:A215"/>
+    <mergeCell ref="A217:A228"/>
     <mergeCell ref="A344:A354"/>
     <mergeCell ref="A248:A260"/>
     <mergeCell ref="A297:A309"/>
@@ -16449,22 +16998,6 @@
     <mergeCell ref="A81:A86"/>
     <mergeCell ref="A118:A124"/>
     <mergeCell ref="A111:A116"/>
-    <mergeCell ref="A330:A342"/>
-    <mergeCell ref="A104:A109"/>
-    <mergeCell ref="A320:A328"/>
-    <mergeCell ref="A64:A78"/>
-    <mergeCell ref="A311:A318"/>
-    <mergeCell ref="A126:A132"/>
-    <mergeCell ref="A189:A196"/>
-    <mergeCell ref="A174:A187"/>
-    <mergeCell ref="A159:A172"/>
-    <mergeCell ref="A146:A156"/>
-    <mergeCell ref="A134:A144"/>
-    <mergeCell ref="A262:A274"/>
-    <mergeCell ref="A230:A237"/>
-    <mergeCell ref="A239:A246"/>
-    <mergeCell ref="A198:A215"/>
-    <mergeCell ref="A217:A228"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Criei o ex035 e atualizei a planilha
</commit_message>
<xml_diff>
--- a/detalhesPython.xlsx
+++ b/detalhesPython.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\thiag\Documents\EstudosT\python\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C30E44D2-DCFF-41DC-B4E5-C449628F0527}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B6224F3-C28D-4FEB-93B6-638C064DF623}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{ECBDB9F7-0FAD-476C-A4A4-7948F29B869E}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="333" uniqueCount="309">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="345" uniqueCount="319">
   <si>
     <t>Descrição</t>
   </si>
@@ -13908,6 +13908,586 @@
         <family val="3"/>
       </rPr>
       <t>(salario, novo))</t>
+    </r>
+  </si>
+  <si>
+    <t>ex034</t>
+  </si>
+  <si>
+    <t>Desenvolva um programa que leia o comprimento de três retas e diga ao usuário se elas podem ou não formar um triângulo.</t>
+  </si>
+  <si>
+    <r>
+      <t>print</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>(</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE7DE79"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>'-='</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>*</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF78D1E1"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>15</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>print</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>(</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE7DE79"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>'Analisador de Triângulos'</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">r1 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>=</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color rgb="FF988BC7"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>float</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>(</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF988BC7"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>input</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>(</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE7DE79"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>'Primeiro segmento: '</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>))</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">r2 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>=</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color rgb="FF988BC7"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>float</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>(</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF988BC7"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>input</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>(</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE7DE79"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>'Segundo segmento: '</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>))</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">r3 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>=</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color rgb="FF988BC7"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>float</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>(</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF988BC7"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>input</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>(</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE7DE79"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>'Terceiro segmento: '</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>))</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>if</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> r1 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>&lt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> r2 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> r3 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>and</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> r2 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>&lt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> r1 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> r3 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>and</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> r3 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>&lt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> r1 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> r2:</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">    </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF988BC7"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>print</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>(</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE7DE79"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>'Os segmentos acima PODEM FORMAR triângulo!'</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">    </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF988BC7"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>print</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>(</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE7DE79"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>'Os segmentos acima NÃO podem formar triângulo!'</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>)</t>
     </r>
   </si>
 </sst>
@@ -14807,10 +15387,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{73331524-72FC-41A3-82E6-4326A0999772}">
-  <dimension ref="A1:G364"/>
+  <dimension ref="A1:G378"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A350" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B364" sqref="B364"/>
+    <sheetView tabSelected="1" topLeftCell="A356" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B375" sqref="B375"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -16963,8 +17543,103 @@
       <c r="A364" s="45"/>
       <c r="B364" s="42"/>
     </row>
+    <row r="365" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="366" spans="1:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A366" s="43" t="s">
+        <v>309</v>
+      </c>
+      <c r="B366" s="31" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="367" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A367" s="44"/>
+      <c r="B367" s="40"/>
+    </row>
+    <row r="368" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A368" s="44"/>
+      <c r="B368" s="11" t="s">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="369" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A369" s="44"/>
+      <c r="B369" s="11" t="s">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="370" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A370" s="44"/>
+      <c r="B370" s="11" t="s">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="371" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A371" s="44"/>
+      <c r="B371" s="7" t="s">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="372" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A372" s="44"/>
+      <c r="B372" s="7" t="s">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="373" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A373" s="44"/>
+      <c r="B373" s="7" t="s">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="374" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A374" s="44"/>
+      <c r="B374" s="34" t="s">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="375" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A375" s="44"/>
+      <c r="B375" s="7" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="376" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A376" s="44"/>
+      <c r="B376" s="34" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="377" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A377" s="44"/>
+      <c r="B377" s="7" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="378" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A378" s="45"/>
+      <c r="B378" s="42"/>
+    </row>
   </sheetData>
-  <mergeCells count="33">
+  <mergeCells count="34">
+    <mergeCell ref="A118:A124"/>
+    <mergeCell ref="A111:A116"/>
+    <mergeCell ref="A366:A378"/>
+    <mergeCell ref="A56:A62"/>
+    <mergeCell ref="A48:A54"/>
+    <mergeCell ref="A97:A102"/>
+    <mergeCell ref="A88:A95"/>
+    <mergeCell ref="A81:A86"/>
+    <mergeCell ref="A2:A6"/>
+    <mergeCell ref="A37:A46"/>
+    <mergeCell ref="A29:A35"/>
+    <mergeCell ref="A16:A27"/>
+    <mergeCell ref="A8:A14"/>
+    <mergeCell ref="A217:A228"/>
+    <mergeCell ref="A344:A354"/>
+    <mergeCell ref="A248:A260"/>
+    <mergeCell ref="A297:A309"/>
+    <mergeCell ref="A276:A295"/>
     <mergeCell ref="A356:A364"/>
     <mergeCell ref="A330:A342"/>
     <mergeCell ref="A104:A109"/>
@@ -16981,23 +17656,6 @@
     <mergeCell ref="A230:A237"/>
     <mergeCell ref="A239:A246"/>
     <mergeCell ref="A198:A215"/>
-    <mergeCell ref="A217:A228"/>
-    <mergeCell ref="A344:A354"/>
-    <mergeCell ref="A248:A260"/>
-    <mergeCell ref="A297:A309"/>
-    <mergeCell ref="A276:A295"/>
-    <mergeCell ref="A2:A6"/>
-    <mergeCell ref="A37:A46"/>
-    <mergeCell ref="A29:A35"/>
-    <mergeCell ref="A16:A27"/>
-    <mergeCell ref="A8:A14"/>
-    <mergeCell ref="A56:A62"/>
-    <mergeCell ref="A48:A54"/>
-    <mergeCell ref="A97:A102"/>
-    <mergeCell ref="A88:A95"/>
-    <mergeCell ref="A81:A86"/>
-    <mergeCell ref="A118:A124"/>
-    <mergeCell ref="A111:A116"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Atualizei a planilha prints sobre cores
</commit_message>
<xml_diff>
--- a/detalhesPython.xlsx
+++ b/detalhesPython.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\thiag\Documents\EstudosT\python\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B6224F3-C28D-4FEB-93B6-638C064DF623}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3905E9EB-2C51-4EC5-97FC-5B5D2ED75278}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{ECBDB9F7-0FAD-476C-A4A4-7948F29B869E}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="345" uniqueCount="319">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="349" uniqueCount="321">
   <si>
     <t>Descrição</t>
   </si>
@@ -14489,6 +14489,12 @@
       </rPr>
       <t>)</t>
     </r>
+  </si>
+  <si>
+    <t>cores</t>
+  </si>
+  <si>
+    <t>cor</t>
   </si>
 </sst>
 </file>
@@ -15090,6 +15096,319 @@
 </styleSheet>
 </file>
 
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>11206</xdr:colOff>
+      <xdr:row>379</xdr:row>
+      <xdr:rowOff>11206</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>7283824</xdr:colOff>
+      <xdr:row>392</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Imagem 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A2299AAA-718D-FFAD-4635-DE93F610D187}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="672353" y="75169059"/>
+          <a:ext cx="7272618" cy="2487706"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>11206</xdr:colOff>
+      <xdr:row>393</xdr:row>
+      <xdr:rowOff>11207</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>7272617</xdr:colOff>
+      <xdr:row>405</xdr:row>
+      <xdr:rowOff>168090</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="Imagem 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C56A61F9-D29B-8314-9B0B-2C4BC6EB2363}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="672353" y="77869678"/>
+          <a:ext cx="7261411" cy="2454088"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>33618</xdr:colOff>
+      <xdr:row>378</xdr:row>
+      <xdr:rowOff>190500</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>235324</xdr:colOff>
+      <xdr:row>392</xdr:row>
+      <xdr:rowOff>27461</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="6" name="Imagem 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A663E42B-9069-6D63-C12E-ED63AF9B94E9}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7989794" y="75146647"/>
+          <a:ext cx="4437530" cy="2537579"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>268941</xdr:colOff>
+      <xdr:row>379</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>456170</xdr:colOff>
+      <xdr:row>392</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="7" name="Imagem 6">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3FC418A6-1DFD-6E0D-87E8-F8F410B759C1}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="12460941" y="75157853"/>
+          <a:ext cx="4423053" cy="2498912"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>31486</xdr:colOff>
+      <xdr:row>392</xdr:row>
+      <xdr:rowOff>190500</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>313763</xdr:colOff>
+      <xdr:row>406</xdr:row>
+      <xdr:rowOff>33618</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="8" name="Imagem 7">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C35B106C-5403-13E2-E5C0-8BD1772A640E}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7987662" y="77847265"/>
+          <a:ext cx="5123219" cy="2543735"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>392204</xdr:colOff>
+      <xdr:row>392</xdr:row>
+      <xdr:rowOff>190501</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>343238</xdr:colOff>
+      <xdr:row>406</xdr:row>
+      <xdr:rowOff>33618</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="9" name="Imagem 8">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E18E3E5E-614C-21B0-6487-A5FC6E0F233E}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId6"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="13189322" y="77847266"/>
+          <a:ext cx="6002210" cy="2543734"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>493059</xdr:colOff>
+      <xdr:row>379</xdr:row>
+      <xdr:rowOff>1777</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>28</xdr:col>
+      <xdr:colOff>496148</xdr:colOff>
+      <xdr:row>392</xdr:row>
+      <xdr:rowOff>34122</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="10" name="Imagem 9">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A1CB6E25-602F-F327-FD3F-930A2F97DAF1}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId7"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="16920883" y="75159630"/>
+          <a:ext cx="7264500" cy="2531257"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema do Office">
   <a:themeElements>
@@ -15387,10 +15706,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{73331524-72FC-41A3-82E6-4326A0999772}">
-  <dimension ref="A1:G378"/>
+  <dimension ref="A1:G406"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A356" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B375" sqref="B375"/>
+    <sheetView tabSelected="1" topLeftCell="A393" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="A394" sqref="A394:A406"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -17620,29 +17939,126 @@
       <c r="A378" s="45"/>
       <c r="B378" s="42"/>
     </row>
+    <row r="379" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="380" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A380" s="43" t="s">
+        <v>319</v>
+      </c>
+      <c r="B380" s="31"/>
+    </row>
+    <row r="381" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A381" s="44"/>
+      <c r="B381" s="40"/>
+    </row>
+    <row r="382" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A382" s="44"/>
+      <c r="B382" s="11"/>
+    </row>
+    <row r="383" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A383" s="44"/>
+      <c r="B383" s="11"/>
+    </row>
+    <row r="384" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A384" s="44"/>
+      <c r="B384" s="11"/>
+    </row>
+    <row r="385" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A385" s="44"/>
+      <c r="B385" s="7"/>
+    </row>
+    <row r="386" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A386" s="44"/>
+      <c r="B386" s="7"/>
+    </row>
+    <row r="387" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A387" s="44"/>
+      <c r="B387" s="7"/>
+    </row>
+    <row r="388" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A388" s="44"/>
+      <c r="B388" s="34"/>
+    </row>
+    <row r="389" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A389" s="44"/>
+      <c r="B389" s="7"/>
+    </row>
+    <row r="390" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A390" s="44"/>
+      <c r="B390" s="34"/>
+    </row>
+    <row r="391" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A391" s="44"/>
+      <c r="B391" s="7"/>
+    </row>
+    <row r="392" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A392" s="45"/>
+      <c r="B392" s="42"/>
+      <c r="C392" s="2" t="s">
+        <v>320</v>
+      </c>
+      <c r="D392" s="2" t="s">
+        <v>319</v>
+      </c>
+    </row>
+    <row r="393" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="394" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A394" s="43" t="s">
+        <v>319</v>
+      </c>
+      <c r="B394" s="31"/>
+    </row>
+    <row r="395" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A395" s="44"/>
+      <c r="B395" s="40"/>
+    </row>
+    <row r="396" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A396" s="44"/>
+      <c r="B396" s="11"/>
+    </row>
+    <row r="397" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A397" s="44"/>
+      <c r="B397" s="11"/>
+    </row>
+    <row r="398" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A398" s="44"/>
+      <c r="B398" s="11"/>
+    </row>
+    <row r="399" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A399" s="44"/>
+      <c r="B399" s="7"/>
+    </row>
+    <row r="400" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A400" s="44"/>
+      <c r="B400" s="7"/>
+    </row>
+    <row r="401" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A401" s="44"/>
+      <c r="B401" s="7"/>
+    </row>
+    <row r="402" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A402" s="44"/>
+      <c r="B402" s="34"/>
+    </row>
+    <row r="403" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A403" s="44"/>
+      <c r="B403" s="7"/>
+    </row>
+    <row r="404" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A404" s="44"/>
+      <c r="B404" s="34"/>
+    </row>
+    <row r="405" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A405" s="44"/>
+      <c r="B405" s="7"/>
+    </row>
+    <row r="406" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A406" s="45"/>
+      <c r="B406" s="42"/>
+    </row>
   </sheetData>
-  <mergeCells count="34">
-    <mergeCell ref="A118:A124"/>
-    <mergeCell ref="A111:A116"/>
-    <mergeCell ref="A366:A378"/>
-    <mergeCell ref="A56:A62"/>
-    <mergeCell ref="A48:A54"/>
-    <mergeCell ref="A97:A102"/>
-    <mergeCell ref="A88:A95"/>
-    <mergeCell ref="A81:A86"/>
-    <mergeCell ref="A2:A6"/>
-    <mergeCell ref="A37:A46"/>
-    <mergeCell ref="A29:A35"/>
-    <mergeCell ref="A16:A27"/>
-    <mergeCell ref="A8:A14"/>
-    <mergeCell ref="A217:A228"/>
-    <mergeCell ref="A344:A354"/>
-    <mergeCell ref="A248:A260"/>
-    <mergeCell ref="A297:A309"/>
-    <mergeCell ref="A276:A295"/>
-    <mergeCell ref="A356:A364"/>
-    <mergeCell ref="A330:A342"/>
-    <mergeCell ref="A104:A109"/>
+  <mergeCells count="36">
+    <mergeCell ref="A380:A392"/>
+    <mergeCell ref="A394:A406"/>
     <mergeCell ref="A320:A328"/>
     <mergeCell ref="A64:A78"/>
     <mergeCell ref="A311:A318"/>
@@ -17656,8 +18072,30 @@
     <mergeCell ref="A230:A237"/>
     <mergeCell ref="A239:A246"/>
     <mergeCell ref="A198:A215"/>
+    <mergeCell ref="A2:A6"/>
+    <mergeCell ref="A37:A46"/>
+    <mergeCell ref="A29:A35"/>
+    <mergeCell ref="A16:A27"/>
+    <mergeCell ref="A8:A14"/>
+    <mergeCell ref="A118:A124"/>
+    <mergeCell ref="A111:A116"/>
+    <mergeCell ref="A366:A378"/>
+    <mergeCell ref="A56:A62"/>
+    <mergeCell ref="A48:A54"/>
+    <mergeCell ref="A97:A102"/>
+    <mergeCell ref="A88:A95"/>
+    <mergeCell ref="A81:A86"/>
+    <mergeCell ref="A217:A228"/>
+    <mergeCell ref="A344:A354"/>
+    <mergeCell ref="A248:A260"/>
+    <mergeCell ref="A297:A309"/>
+    <mergeCell ref="A276:A295"/>
+    <mergeCell ref="A356:A364"/>
+    <mergeCell ref="A330:A342"/>
+    <mergeCell ref="A104:A109"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Atualizei o ex036 e ex037
</commit_message>
<xml_diff>
--- a/detalhesPython.xlsx
+++ b/detalhesPython.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\thiag\Documents\EstudosT\python\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2ABCAFEC-17BB-4DB9-B8D7-E5819D2D243C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86025BF9-7BC6-4660-85F7-A3CE96F5A5EB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{ECBDB9F7-0FAD-476C-A4A4-7948F29B869E}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="349" uniqueCount="321">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="387" uniqueCount="353">
   <si>
     <t>Descrição</t>
   </si>
@@ -14495,6 +14495,2160 @@
   </si>
   <si>
     <t>cor</t>
+  </si>
+  <si>
+    <t>ex035</t>
+  </si>
+  <si>
+    <t>ex036</t>
+  </si>
+  <si>
+    <r>
+      <t>print</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>(</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE7DE79"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>'</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>\033</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE7DE79"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>[34m-</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>\033</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE7DE79"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>[m'</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>*</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF78D1E1"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>38</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>print</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>(</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE7DE79"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>'</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>\033</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE7DE79"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>[1;33m SIMULAÇÃO DE FINANCIAMENTO DE IMÓVEL</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>\033</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE7DE79"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>[m'</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">casa </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>=</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color rgb="FF988BC7"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>float</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>(</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF988BC7"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>input</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>(</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE7DE79"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>'Valor do imóvel? R$'</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>))</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">salario </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>=</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color rgb="FF988BC7"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>float</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>(</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF988BC7"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>input</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>(</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE7DE79"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>'Qual o valor do seu salário? R$'</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>))</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">anos </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>=</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color rgb="FF988BC7"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>int</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>(</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF988BC7"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>input</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>(</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE7DE79"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>'Parcelado em quantos anos? '</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>))</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">quantParcelas </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>=</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> anos </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>*</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF78D1E1"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>12</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">valorParcelas </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>=</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> casa </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>/</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> quantParcelas</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>print</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>(</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE7DE79"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>'</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>\033</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE7DE79"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>[1;33mVERIFICANDO...</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>\033</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE7DE79"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>[m'</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>if</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> valorParcelas </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>&gt;=</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> salario </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>*</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF78D1E1"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>30</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>/</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF78D1E1"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>100</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>:</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">    </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF988BC7"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>print</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>(</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE7DE79"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>'</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>\033</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE7DE79"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>[4;31mO valor da parcela excedeu o limite de 30</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF78D1E1"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>% d</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE7DE79"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>o seu salário.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>\n</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE7DE79"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>Empréstimo NÃO LIBERADO!</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>\033</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE7DE79"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>[m'</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">    </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF988BC7"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>print</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>(</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE7DE79"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>'</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>\033</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE7DE79"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">[4;32mOk, o empréstimo poderá ser liberado com </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF78D1E1"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>{</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>:.0f</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF78D1E1"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>}</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE7DE79"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> x R$</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF78D1E1"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>{</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>:.2f</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF78D1E1"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>}</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>\033</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE7DE79"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>[m'</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF67E480"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>format</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>(quantParcelas, valorParcelas))</t>
+    </r>
+  </si>
+  <si>
+    <t>ex037</t>
+  </si>
+  <si>
+    <t>Escreva um programa em Python que leia um número inteiro qualquer e peça para o usuário escolher qual será a base de conversão: 1 para binário, 2 para octal e 3 para hexadecimal.</t>
+  </si>
+  <si>
+    <r>
+      <t>print</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>(</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE7DE79"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>'</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>\033</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE7DE79"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>[35m-=</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>\033</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE7DE79"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>[m'</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>*</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF78D1E1"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>20</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">num </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>=</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color rgb="FF988BC7"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>int</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>(</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF988BC7"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>input</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>(</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE7DE79"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>'</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>\033</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE7DE79"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">[33mDigite um número inteiro: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>\033</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE7DE79"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>[m'</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>))</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>print</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>(</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE7DE79"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>'''</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>\033</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE7DE79"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>[1;30;45mEscolha uma das bases para conversão:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>\033</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE7DE79"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">[m </t>
+    </r>
+  </si>
+  <si>
+    <t>[ 1 ] Converter para BINÁRIO.</t>
+  </si>
+  <si>
+    <t>[ 2 ] Converter para OCTAL</t>
+  </si>
+  <si>
+    <r>
+      <t>[ 3 ] Converter para HEXADECIMAL'''</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">opção </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>=</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color rgb="FF988BC7"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>int</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>(</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF988BC7"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>input</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>(</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE7DE79"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>'</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>\033</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE7DE79"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">[33mSua opção: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>\033</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE7DE79"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>[m'</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>))</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>if</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> opção </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>==</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF78D1E1"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>1</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>:</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">    </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF988BC7"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>print</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>(</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE7DE79"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>'</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>\033</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE7DE79"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>[4;34m</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF78D1E1"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>{}</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>\033</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE7DE79"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">[m convertido para BINÁRIO é igual a </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>\033</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE7DE79"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>[33m</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF78D1E1"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>{}</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>\033</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE7DE79"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>[m'</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF67E480"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>format</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">(num, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF988BC7"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>bin</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>(num) [</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF78D1E1"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>2</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>:]))</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>elif</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> opção </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>==</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF78D1E1"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>2</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>:</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">    </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF988BC7"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>print</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>(</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE7DE79"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>'</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>\033</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE7DE79"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>[4;34m</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF78D1E1"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>{}</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>\033</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE7DE79"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">[m convertido para OCTAL é igual a </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>\033</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE7DE79"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>[33m</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF78D1E1"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>{}</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>\033</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE7DE79"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>[m'</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF67E480"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>format</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">(num, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF988BC7"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>oct</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>(num) [</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF78D1E1"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>2</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>:]))</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>elif</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> opção </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>==</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF78D1E1"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>3</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>:</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">    </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF988BC7"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>print</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>(</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE7DE79"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>'</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>\033</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE7DE79"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>[4;34m</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF78D1E1"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>{}</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>\033</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE7DE79"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">[m convertido para HEXADECIMAL é igual a </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>\033</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE7DE79"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>[33m</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF78D1E1"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>{}</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>\033</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE7DE79"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>[m'</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF67E480"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>format</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">(num, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF988BC7"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>hex</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>(num) [</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF78D1E1"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>2</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>:]))</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">    </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF988BC7"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>print</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>(</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE7DE79"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>'</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>\033</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE7DE79"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>[4;30;41mOpção inválida!</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>\033</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE7DE79"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>[m Tente novamente.'</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>)</t>
+    </r>
+  </si>
+  <si>
+    <t>Escreva um programa para aprovar o empréstimo bancário para a compra de uma casa. Pergunte o valor da casa, o salário do comprador e em quantos anos ele vai pagar. A prestação mensal não pode exceder 30% do salário ou então o empréstimo será negado.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> '''   ''' ---&gt; Aspas triplas para escrever em mais linhas sem precisar usar o "\n"</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> bin ---&gt; Binário, oct ---&gt; Octal e hex ---&gt; Hexadecimal</t>
   </si>
 </sst>
 </file>
@@ -14948,7 +17102,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="46">
+  <cellXfs count="52">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -15079,6 +17233,24 @@
     <xf numFmtId="0" fontId="11" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="3" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="21" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -15195,7 +17367,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>235324</xdr:colOff>
+      <xdr:colOff>235325</xdr:colOff>
       <xdr:row>392</xdr:row>
       <xdr:rowOff>27461</xdr:rowOff>
     </xdr:to>
@@ -15283,7 +17455,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>313763</xdr:colOff>
+      <xdr:colOff>313764</xdr:colOff>
       <xdr:row>406</xdr:row>
       <xdr:rowOff>33618</xdr:rowOff>
     </xdr:to>
@@ -15371,7 +17543,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>28</xdr:col>
-      <xdr:colOff>496148</xdr:colOff>
+      <xdr:colOff>496147</xdr:colOff>
       <xdr:row>392</xdr:row>
       <xdr:rowOff>34122</xdr:rowOff>
     </xdr:to>
@@ -15706,16 +17878,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{73331524-72FC-41A3-82E6-4326A0999772}">
-  <dimension ref="A1:G406"/>
+  <dimension ref="A1:G452"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A395" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A394" sqref="A394:A406"/>
+    <sheetView tabSelected="1" topLeftCell="A431" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B451" sqref="B451"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9.85546875" style="2" customWidth="1"/>
-    <col min="2" max="2" width="109.42578125" style="2" customWidth="1"/>
+    <col min="2" max="2" width="147.5703125" style="2" customWidth="1"/>
     <col min="3" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
@@ -17430,13 +19602,13 @@
     </row>
     <row r="292" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A292" s="44"/>
-      <c r="B292" s="11" t="s">
+      <c r="B292" s="36" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="293" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A293" s="44"/>
-      <c r="B293" s="11" t="s">
+      <c r="B293" s="36" t="s">
         <v>245</v>
       </c>
       <c r="C293" s="2" t="s">
@@ -17451,7 +19623,7 @@
     </row>
     <row r="294" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A294" s="44"/>
-      <c r="B294" s="39" t="s">
+      <c r="B294" s="50" t="s">
         <v>246</v>
       </c>
     </row>
@@ -17633,7 +19805,7 @@
     </row>
     <row r="327" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A327" s="44"/>
-      <c r="B327" s="11" t="s">
+      <c r="B327" s="36" t="s">
         <v>273</v>
       </c>
       <c r="C327" s="2" t="s">
@@ -17717,7 +19889,7 @@
     </row>
     <row r="341" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A341" s="44"/>
-      <c r="B341" s="11" t="s">
+      <c r="B341" s="36" t="s">
         <v>286</v>
       </c>
       <c r="C341" s="2" t="s">
@@ -17812,7 +19984,7 @@
     <row r="355" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="356" spans="1:7" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A356" s="43" t="s">
-        <v>289</v>
+        <v>309</v>
       </c>
       <c r="B356" s="31" t="s">
         <v>303</v>
@@ -17865,7 +20037,7 @@
     <row r="365" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="366" spans="1:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A366" s="43" t="s">
-        <v>309</v>
+        <v>321</v>
       </c>
       <c r="B366" s="31" t="s">
         <v>310</v>
@@ -18055,28 +20227,264 @@
       <c r="A406" s="45"/>
       <c r="B406" s="42"/>
     </row>
+    <row r="407" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="408" spans="1:2" ht="30.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A408" s="43" t="s">
+        <v>322</v>
+      </c>
+      <c r="B408" s="31" t="s">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="409" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A409" s="44"/>
+      <c r="B409" s="40"/>
+    </row>
+    <row r="410" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A410" s="44"/>
+      <c r="B410" s="34" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="411" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A411" s="44"/>
+      <c r="B411" s="46"/>
+    </row>
+    <row r="412" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A412" s="44"/>
+      <c r="B412" s="11" t="s">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="413" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A413" s="44"/>
+      <c r="B413" s="11" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="414" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A414" s="44"/>
+      <c r="B414" s="11" t="s">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="415" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A415" s="44"/>
+      <c r="B415" s="46"/>
+    </row>
+    <row r="416" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A416" s="44"/>
+      <c r="B416" s="7" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="417" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A417" s="44"/>
+      <c r="B417" s="7" t="s">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="418" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A418" s="44"/>
+      <c r="B418" s="7" t="s">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="419" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A419" s="44"/>
+      <c r="B419" s="7" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="420" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A420" s="44"/>
+      <c r="B420" s="7" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="421" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A421" s="44"/>
+      <c r="B421" s="46"/>
+    </row>
+    <row r="422" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A422" s="44"/>
+      <c r="B422" s="11" t="s">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="423" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A423" s="44"/>
+      <c r="B423" s="35" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="424" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A424" s="44"/>
+      <c r="B424" s="46"/>
+    </row>
+    <row r="425" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A425" s="44"/>
+      <c r="B425" s="34" t="s">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="426" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A426" s="44"/>
+      <c r="B426" s="47" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="427" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A427" s="44"/>
+      <c r="B427" s="34" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="428" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A428" s="44"/>
+      <c r="B428" s="47" t="s">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="429" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A429" s="45"/>
+      <c r="B429" s="49" t="s">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="430" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="431" spans="1:2" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A431" s="43" t="s">
+        <v>334</v>
+      </c>
+      <c r="B431" s="31" t="s">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="432" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A432" s="44"/>
+      <c r="B432" s="40"/>
+    </row>
+    <row r="433" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A433" s="44"/>
+      <c r="B433" s="11" t="s">
+        <v>336</v>
+      </c>
+    </row>
+    <row r="434" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A434" s="44"/>
+      <c r="B434" s="7" t="s">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="435" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A435" s="44"/>
+      <c r="B435" s="11" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="436" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A436" s="44"/>
+      <c r="B436" s="48" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="437" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A437" s="44"/>
+      <c r="B437" s="48" t="s">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="438" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A438" s="44"/>
+      <c r="B438" s="48" t="s">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="439" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A439" s="44"/>
+      <c r="B439" s="7" t="s">
+        <v>342</v>
+      </c>
+    </row>
+    <row r="440" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A440" s="44"/>
+      <c r="B440" s="34" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="441" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A441" s="44"/>
+      <c r="B441" s="7" t="s">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="442" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A442" s="44"/>
+      <c r="B442" s="34" t="s">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="443" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A443" s="44"/>
+      <c r="B443" s="7" t="s">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="444" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A444" s="44"/>
+      <c r="B444" s="34" t="s">
+        <v>347</v>
+      </c>
+    </row>
+    <row r="445" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A445" s="44"/>
+      <c r="B445" s="7" t="s">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="446" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A446" s="44"/>
+      <c r="B446" s="34" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="447" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A447" s="44"/>
+      <c r="B447" s="7" t="s">
+        <v>349</v>
+      </c>
+    </row>
+    <row r="448" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A448" s="44"/>
+      <c r="B448" s="34"/>
+    </row>
+    <row r="449" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A449" s="44"/>
+      <c r="B449" s="7" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="450" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A450" s="44"/>
+      <c r="B450" s="51" t="s">
+        <v>351</v>
+      </c>
+    </row>
+    <row r="451" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A451" s="44"/>
+      <c r="B451" s="47" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="452" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A452" s="45"/>
+      <c r="B452" s="42"/>
+    </row>
   </sheetData>
-  <mergeCells count="36">
-    <mergeCell ref="A111:A116"/>
-    <mergeCell ref="A366:A378"/>
-    <mergeCell ref="A56:A62"/>
-    <mergeCell ref="A48:A54"/>
-    <mergeCell ref="A97:A102"/>
-    <mergeCell ref="A88:A95"/>
-    <mergeCell ref="A81:A86"/>
-    <mergeCell ref="A217:A228"/>
-    <mergeCell ref="A344:A354"/>
-    <mergeCell ref="A248:A260"/>
-    <mergeCell ref="A297:A309"/>
-    <mergeCell ref="A276:A295"/>
-    <mergeCell ref="A356:A364"/>
-    <mergeCell ref="A330:A342"/>
-    <mergeCell ref="A104:A109"/>
-    <mergeCell ref="A2:A6"/>
-    <mergeCell ref="A37:A46"/>
-    <mergeCell ref="A29:A35"/>
-    <mergeCell ref="A16:A27"/>
-    <mergeCell ref="A8:A14"/>
+  <mergeCells count="38">
+    <mergeCell ref="A408:A429"/>
+    <mergeCell ref="A431:A452"/>
     <mergeCell ref="A380:A392"/>
     <mergeCell ref="A394:A406"/>
     <mergeCell ref="A320:A328"/>
@@ -18093,6 +20501,26 @@
     <mergeCell ref="A239:A246"/>
     <mergeCell ref="A198:A215"/>
     <mergeCell ref="A118:A124"/>
+    <mergeCell ref="A2:A6"/>
+    <mergeCell ref="A37:A46"/>
+    <mergeCell ref="A29:A35"/>
+    <mergeCell ref="A16:A27"/>
+    <mergeCell ref="A8:A14"/>
+    <mergeCell ref="A111:A116"/>
+    <mergeCell ref="A366:A378"/>
+    <mergeCell ref="A56:A62"/>
+    <mergeCell ref="A48:A54"/>
+    <mergeCell ref="A97:A102"/>
+    <mergeCell ref="A88:A95"/>
+    <mergeCell ref="A81:A86"/>
+    <mergeCell ref="A217:A228"/>
+    <mergeCell ref="A344:A354"/>
+    <mergeCell ref="A248:A260"/>
+    <mergeCell ref="A297:A309"/>
+    <mergeCell ref="A276:A295"/>
+    <mergeCell ref="A356:A364"/>
+    <mergeCell ref="A330:A342"/>
+    <mergeCell ref="A104:A109"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Atualizado o ex039 e planilha
</commit_message>
<xml_diff>
--- a/detalhesPython.xlsx
+++ b/detalhesPython.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\thiag\Documents\EstudosT\python\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86025BF9-7BC6-4660-85F7-A3CE96F5A5EB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82BF68F2-6094-4807-AA10-EC343DAAC969}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{ECBDB9F7-0FAD-476C-A4A4-7948F29B869E}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="387" uniqueCount="353">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="418" uniqueCount="377">
   <si>
     <t>Descrição</t>
   </si>
@@ -16649,6 +16649,1486 @@
   </si>
   <si>
     <t xml:space="preserve"> bin ---&gt; Binário, oct ---&gt; Octal e hex ---&gt; Hexadecimal</t>
+  </si>
+  <si>
+    <t>ex038</t>
+  </si>
+  <si>
+    <t>Escreva um programa que leia dois números inteiros e compare-os. mostrando na tela uma mensagem:</t>
+  </si>
+  <si>
+    <r>
+      <t>print</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>(</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE7DE79"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>'*'</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>*</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF78D1E1"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>20</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>if</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> n1 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> n2:</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">    </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF988BC7"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>print</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>(</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE7DE79"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>'</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>\033</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE7DE79"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>[4;30;45mO 1º número é maior</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>\033</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE7DE79"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>[m'</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>elif</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> n1 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>&lt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> n2:</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">    </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF988BC7"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>print</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>(</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE7DE79"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>'O 2º número é maior'</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">    </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF988BC7"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>print</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>(</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE7DE79"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>'Os números são iguais!'</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>)</t>
+    </r>
+  </si>
+  <si>
+    <t>Faça um programa que leia o ano de nascimento de um jovem e informe, de acordo com a sua idade, se ele ainda vai se alistar ao serviço militar, se é a hora exata de se alistar ou se já passou do tempo do alistamento. Seu programa também deverá mostrar o tempo que falta ou que passou do prazo.</t>
+  </si>
+  <si>
+    <t>ex039</t>
+  </si>
+  <si>
+    <r>
+      <t>print</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>(</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE7DE79"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>'</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>\033</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE7DE79"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">[32m* </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>\033</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE7DE79"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>[m'</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>*</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF78D1E1"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>15</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>print</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>(</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE7DE79"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>'</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>\033</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE7DE79"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>[34mAlistamento Militar</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>\033</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE7DE79"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>[m'</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF67E480"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>center</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>(</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF78D1E1"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>36</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>))</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">sexo </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>=</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color rgb="FF988BC7"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>str</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>(</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF988BC7"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>input</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>(</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE7DE79"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>'Sexo: Masculino ou Feminino: '</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>)).</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF67E480"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>strip</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>().</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF67E480"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>upper</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>()</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>if</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> sexo </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>==</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE7DE79"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>'FEMININO'</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>:</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>     </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF988BC7"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>print</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>(</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE7DE79"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>'</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>\n\033</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE7DE79"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>[4;31mAviso:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>\033</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE7DE79"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>[m Você não é obrigada a fazer o alistamento Militar!'</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">anoNascimento </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>=</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color rgb="FF988BC7"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>int</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>(</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF988BC7"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>input</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>(</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE7DE79"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>'</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>\n</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE7DE79"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>Digite o ano de nascimento: '</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>))</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">anoAtual </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>=</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> date.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF67E480"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>today</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>().year</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">idade </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>=</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> anoAtual </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>-</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> anoNascimento</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>if</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> idade </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>&lt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF78D1E1"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>18</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>:</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">    </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF988BC7"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>print</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>(</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE7DE79"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>'</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>\n</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE7DE79"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">Em </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF78D1E1"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>{}</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE7DE79"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">, você completa </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF78D1E1"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>{}</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE7DE79"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> anos de idade! Ainda faltam </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF78D1E1"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>{}</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE7DE79"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> anos para seu alistamento Militar.'</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF67E480"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>format</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">(anoAtual, idade, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF78D1E1"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>18</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>-</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> idade))</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>elif</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> idade </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>==</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF78D1E1"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>18</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>:</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">    </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF988BC7"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>print</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>(</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE7DE79"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>'</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>\n</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE7DE79"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">Em </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF78D1E1"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>{}</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE7DE79"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">, você completa </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF78D1E1"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>{}</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE7DE79"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> anos de idade! Deve se alistar para o Serviço Militar obrigatório!'</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF67E480"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>format</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>(anoAtual, idade))</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">    </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF988BC7"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>print</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>(</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE7DE79"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>'</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>\n</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE7DE79"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">Em </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF78D1E1"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>{}</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE7DE79"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">, você completa </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF78D1E1"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>{}</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE7DE79"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> anos de idade! Você deveria ter se alistado à </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF78D1E1"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>{}</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE7DE79"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> anos atrás!'</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF67E480"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>format</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">(anoAtual, idade, idade </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>-</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF78D1E1"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>18</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>))</t>
+    </r>
+  </si>
+  <si>
+    <t>.center(36) ---&gt; Serve para centralizar a string dentro de no caso 36 espaços de caracteres, podendo fazer também: .center(36, =) para preencher os outros espaços vazios....pesquisar</t>
   </si>
 </sst>
 </file>
@@ -17224,15 +18704,6 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="15" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -17250,6 +18721,15 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="21" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -17878,16 +19358,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{73331524-72FC-41A3-82E6-4326A0999772}">
-  <dimension ref="A1:G452"/>
+  <dimension ref="A1:G488"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A431" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B451" sqref="B451"/>
+    <sheetView tabSelected="1" topLeftCell="A460" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="A467" sqref="A467:A488"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9.85546875" style="2" customWidth="1"/>
-    <col min="2" max="2" width="147.5703125" style="2" customWidth="1"/>
+    <col min="2" max="2" width="166" style="2" customWidth="1"/>
     <col min="3" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
@@ -17900,7 +19380,7 @@
       </c>
     </row>
     <row r="2" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="43" t="s">
+      <c r="A2" s="49" t="s">
         <v>227</v>
       </c>
       <c r="B2" s="31" t="s">
@@ -17908,23 +19388,23 @@
       </c>
     </row>
     <row r="3" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="44"/>
+      <c r="A3" s="50"/>
       <c r="B3" s="7"/>
     </row>
     <row r="4" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="44"/>
+      <c r="A4" s="50"/>
       <c r="B4" s="7" t="s">
         <v>229</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="44"/>
+      <c r="A5" s="50"/>
       <c r="B5" s="39" t="s">
         <v>230</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="45"/>
+      <c r="A6" s="51"/>
       <c r="B6" s="33"/>
     </row>
     <row r="7" spans="1:2" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -17932,7 +19412,7 @@
       <c r="B7" s="20"/>
     </row>
     <row r="8" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="43" t="s">
+      <c r="A8" s="49" t="s">
         <v>220</v>
       </c>
       <c r="B8" s="31" t="s">
@@ -17940,35 +19420,35 @@
       </c>
     </row>
     <row r="9" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="44"/>
+      <c r="A9" s="50"/>
       <c r="B9" s="7"/>
     </row>
     <row r="10" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="44"/>
+      <c r="A10" s="50"/>
       <c r="B10" s="7" t="s">
         <v>222</v>
       </c>
     </row>
     <row r="11" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="44"/>
+      <c r="A11" s="50"/>
       <c r="B11" s="7" t="s">
         <v>223</v>
       </c>
     </row>
     <row r="12" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="44"/>
+      <c r="A12" s="50"/>
       <c r="B12" s="7" t="s">
         <v>224</v>
       </c>
     </row>
     <row r="13" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="44"/>
+      <c r="A13" s="50"/>
       <c r="B13" s="39" t="s">
         <v>225</v>
       </c>
     </row>
     <row r="14" spans="1:2" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="45"/>
+      <c r="A14" s="51"/>
       <c r="B14" s="33"/>
     </row>
     <row r="15" spans="1:2" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -17976,7 +19456,7 @@
       <c r="B15" s="20"/>
     </row>
     <row r="16" spans="1:2" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="43" t="s">
+      <c r="A16" s="49" t="s">
         <v>210</v>
       </c>
       <c r="B16" s="31" t="s">
@@ -17984,65 +19464,65 @@
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A17" s="44"/>
+      <c r="A17" s="50"/>
       <c r="B17" s="7"/>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A18" s="44"/>
+      <c r="A18" s="50"/>
       <c r="B18" s="7" t="s">
         <v>211</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A19" s="44"/>
+      <c r="A19" s="50"/>
       <c r="B19" s="11" t="s">
         <v>212</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A20" s="44"/>
+      <c r="A20" s="50"/>
       <c r="B20" s="11" t="s">
         <v>213</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A21" s="44"/>
+      <c r="A21" s="50"/>
       <c r="B21" s="11" t="s">
         <v>214</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A22" s="44"/>
+      <c r="A22" s="50"/>
       <c r="B22" s="11" t="s">
         <v>215</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A23" s="44"/>
+      <c r="A23" s="50"/>
       <c r="B23" s="11" t="s">
         <v>216</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A24" s="44"/>
+      <c r="A24" s="50"/>
       <c r="B24" s="11" t="s">
         <v>217</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A25" s="44"/>
+      <c r="A25" s="50"/>
       <c r="B25" s="11" t="s">
         <v>218</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A26" s="44"/>
+      <c r="A26" s="50"/>
       <c r="B26" s="39" t="s">
         <v>219</v>
       </c>
     </row>
     <row r="27" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="45"/>
+      <c r="A27" s="51"/>
       <c r="B27" s="33"/>
     </row>
     <row r="28" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -18050,7 +19530,7 @@
       <c r="B28" s="20"/>
     </row>
     <row r="29" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="43" t="s">
+      <c r="A29" s="49" t="s">
         <v>204</v>
       </c>
       <c r="B29" s="31" t="s">
@@ -18058,35 +19538,35 @@
       </c>
     </row>
     <row r="30" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="44"/>
+      <c r="A30" s="50"/>
       <c r="B30" s="7"/>
     </row>
     <row r="31" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="44"/>
+      <c r="A31" s="50"/>
       <c r="B31" s="7" t="s">
         <v>206</v>
       </c>
     </row>
     <row r="32" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="44"/>
+      <c r="A32" s="50"/>
       <c r="B32" s="7" t="s">
         <v>207</v>
       </c>
     </row>
     <row r="33" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="44"/>
+      <c r="A33" s="50"/>
       <c r="B33" s="7" t="s">
         <v>208</v>
       </c>
     </row>
     <row r="34" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="44"/>
+      <c r="A34" s="50"/>
       <c r="B34" s="39" t="s">
         <v>209</v>
       </c>
     </row>
     <row r="35" spans="1:2" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="45"/>
+      <c r="A35" s="51"/>
       <c r="B35" s="33"/>
     </row>
     <row r="36" spans="1:2" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -18094,7 +19574,7 @@
       <c r="B36" s="20"/>
     </row>
     <row r="37" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A37" s="43" t="s">
+      <c r="A37" s="49" t="s">
         <v>195</v>
       </c>
       <c r="B37" s="31" t="s">
@@ -18102,53 +19582,53 @@
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A38" s="44"/>
+      <c r="A38" s="50"/>
       <c r="B38" s="7"/>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A39" s="44"/>
+      <c r="A39" s="50"/>
       <c r="B39" s="7" t="s">
         <v>197</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A40" s="44"/>
+      <c r="A40" s="50"/>
       <c r="B40" s="7" t="s">
         <v>198</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A41" s="44"/>
+      <c r="A41" s="50"/>
       <c r="B41" s="7" t="s">
         <v>199</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A42" s="44"/>
+      <c r="A42" s="50"/>
       <c r="B42" s="7" t="s">
         <v>200</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A43" s="44"/>
+      <c r="A43" s="50"/>
       <c r="B43" s="11" t="s">
         <v>201</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A44" s="44"/>
+      <c r="A44" s="50"/>
       <c r="B44" s="11" t="s">
         <v>202</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A45" s="44"/>
+      <c r="A45" s="50"/>
       <c r="B45" s="39" t="s">
         <v>203</v>
       </c>
     </row>
     <row r="46" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A46" s="45"/>
+      <c r="A46" s="51"/>
       <c r="B46" s="33"/>
     </row>
     <row r="47" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -18156,7 +19636,7 @@
       <c r="B47" s="20"/>
     </row>
     <row r="48" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A48" s="43" t="s">
+      <c r="A48" s="49" t="s">
         <v>189</v>
       </c>
       <c r="B48" s="31" t="s">
@@ -18164,35 +19644,35 @@
       </c>
     </row>
     <row r="49" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A49" s="44"/>
+      <c r="A49" s="50"/>
       <c r="B49" s="7"/>
     </row>
     <row r="50" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A50" s="44"/>
+      <c r="A50" s="50"/>
       <c r="B50" s="7" t="s">
         <v>191</v>
       </c>
     </row>
     <row r="51" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A51" s="44"/>
+      <c r="A51" s="50"/>
       <c r="B51" s="7" t="s">
         <v>192</v>
       </c>
     </row>
     <row r="52" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A52" s="44"/>
+      <c r="A52" s="50"/>
       <c r="B52" s="7" t="s">
         <v>193</v>
       </c>
     </row>
     <row r="53" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A53" s="44"/>
+      <c r="A53" s="50"/>
       <c r="B53" s="39" t="s">
         <v>194</v>
       </c>
     </row>
     <row r="54" spans="1:2" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A54" s="45"/>
+      <c r="A54" s="51"/>
       <c r="B54" s="33"/>
     </row>
     <row r="55" spans="1:2" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -18200,7 +19680,7 @@
       <c r="B55" s="20"/>
     </row>
     <row r="56" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A56" s="43" t="s">
+      <c r="A56" s="49" t="s">
         <v>183</v>
       </c>
       <c r="B56" s="31" t="s">
@@ -18208,35 +19688,35 @@
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A57" s="44"/>
+      <c r="A57" s="50"/>
       <c r="B57" s="7"/>
     </row>
     <row r="58" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A58" s="44"/>
+      <c r="A58" s="50"/>
       <c r="B58" s="7" t="s">
         <v>185</v>
       </c>
     </row>
     <row r="59" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A59" s="44"/>
+      <c r="A59" s="50"/>
       <c r="B59" s="7" t="s">
         <v>186</v>
       </c>
     </row>
     <row r="60" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A60" s="44"/>
+      <c r="A60" s="50"/>
       <c r="B60" s="7" t="s">
         <v>187</v>
       </c>
     </row>
     <row r="61" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A61" s="44"/>
+      <c r="A61" s="50"/>
       <c r="B61" s="39" t="s">
         <v>188</v>
       </c>
     </row>
     <row r="62" spans="1:2" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A62" s="45"/>
+      <c r="A62" s="51"/>
       <c r="B62" s="33"/>
     </row>
     <row r="63" spans="1:2" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -18244,7 +19724,7 @@
       <c r="B63" s="20"/>
     </row>
     <row r="64" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A64" s="43" t="s">
+      <c r="A64" s="49" t="s">
         <v>169</v>
       </c>
       <c r="B64" s="31" t="s">
@@ -18252,83 +19732,83 @@
       </c>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A65" s="44"/>
+      <c r="A65" s="50"/>
       <c r="B65" s="7"/>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A66" s="44"/>
+      <c r="A66" s="50"/>
       <c r="B66" s="7" t="s">
         <v>171</v>
       </c>
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A67" s="44"/>
+      <c r="A67" s="50"/>
       <c r="B67" s="11" t="s">
         <v>172</v>
       </c>
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A68" s="44"/>
+      <c r="A68" s="50"/>
       <c r="B68" s="11" t="s">
         <v>173</v>
       </c>
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A69" s="44"/>
+      <c r="A69" s="50"/>
       <c r="B69" s="11" t="s">
         <v>174</v>
       </c>
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A70" s="44"/>
+      <c r="A70" s="50"/>
       <c r="B70" s="11" t="s">
         <v>175</v>
       </c>
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A71" s="44"/>
+      <c r="A71" s="50"/>
       <c r="B71" s="11" t="s">
         <v>176</v>
       </c>
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A72" s="44"/>
+      <c r="A72" s="50"/>
       <c r="B72" s="11" t="s">
         <v>177</v>
       </c>
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A73" s="44"/>
+      <c r="A73" s="50"/>
       <c r="B73" s="11" t="s">
         <v>178</v>
       </c>
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A74" s="44"/>
+      <c r="A74" s="50"/>
       <c r="B74" s="11" t="s">
         <v>179</v>
       </c>
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A75" s="44"/>
+      <c r="A75" s="50"/>
       <c r="B75" s="11" t="s">
         <v>180</v>
       </c>
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A76" s="44"/>
+      <c r="A76" s="50"/>
       <c r="B76" s="11" t="s">
         <v>181</v>
       </c>
     </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A77" s="44"/>
+      <c r="A77" s="50"/>
       <c r="B77" s="39" t="s">
         <v>182</v>
       </c>
     </row>
     <row r="78" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A78" s="45"/>
+      <c r="A78" s="51"/>
       <c r="B78" s="33"/>
     </row>
     <row r="79" spans="1:2" x14ac:dyDescent="0.25">
@@ -18340,7 +19820,7 @@
       <c r="B80" s="20"/>
     </row>
     <row r="81" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A81" s="43" t="s">
+      <c r="A81" s="49" t="s">
         <v>164</v>
       </c>
       <c r="B81" s="31" t="s">
@@ -18348,29 +19828,29 @@
       </c>
     </row>
     <row r="82" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A82" s="44"/>
+      <c r="A82" s="50"/>
       <c r="B82" s="7"/>
     </row>
     <row r="83" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A83" s="44"/>
+      <c r="A83" s="50"/>
       <c r="B83" s="7" t="s">
         <v>166</v>
       </c>
     </row>
     <row r="84" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A84" s="44"/>
+      <c r="A84" s="50"/>
       <c r="B84" s="7" t="s">
         <v>167</v>
       </c>
     </row>
     <row r="85" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A85" s="44"/>
+      <c r="A85" s="50"/>
       <c r="B85" s="39" t="s">
         <v>168</v>
       </c>
     </row>
     <row r="86" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A86" s="45"/>
+      <c r="A86" s="51"/>
       <c r="B86" s="33"/>
     </row>
     <row r="87" spans="1:2" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -18378,7 +19858,7 @@
       <c r="B87" s="20"/>
     </row>
     <row r="88" spans="1:2" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A88" s="43" t="s">
+      <c r="A88" s="49" t="s">
         <v>157</v>
       </c>
       <c r="B88" s="31" t="s">
@@ -18386,41 +19866,41 @@
       </c>
     </row>
     <row r="89" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A89" s="44"/>
+      <c r="A89" s="50"/>
       <c r="B89" s="7"/>
     </row>
     <row r="90" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A90" s="44"/>
+      <c r="A90" s="50"/>
       <c r="B90" s="7" t="s">
         <v>159</v>
       </c>
     </row>
     <row r="91" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A91" s="44"/>
+      <c r="A91" s="50"/>
       <c r="B91" s="7" t="s">
         <v>160</v>
       </c>
     </row>
     <row r="92" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A92" s="44"/>
+      <c r="A92" s="50"/>
       <c r="B92" s="7" t="s">
         <v>161</v>
       </c>
     </row>
     <row r="93" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A93" s="44"/>
+      <c r="A93" s="50"/>
       <c r="B93" s="11" t="s">
         <v>162</v>
       </c>
     </row>
     <row r="94" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A94" s="44"/>
+      <c r="A94" s="50"/>
       <c r="B94" s="39" t="s">
         <v>163</v>
       </c>
     </row>
     <row r="95" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A95" s="45"/>
+      <c r="A95" s="51"/>
       <c r="B95" s="33"/>
     </row>
     <row r="96" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -18428,7 +19908,7 @@
       <c r="B96" s="20"/>
     </row>
     <row r="97" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A97" s="43" t="s">
+      <c r="A97" s="49" t="s">
         <v>152</v>
       </c>
       <c r="B97" s="31" t="s">
@@ -18436,29 +19916,29 @@
       </c>
     </row>
     <row r="98" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A98" s="44"/>
+      <c r="A98" s="50"/>
       <c r="B98" s="7"/>
     </row>
     <row r="99" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A99" s="44"/>
+      <c r="A99" s="50"/>
       <c r="B99" s="7" t="s">
         <v>154</v>
       </c>
     </row>
     <row r="100" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A100" s="44"/>
+      <c r="A100" s="50"/>
       <c r="B100" s="7" t="s">
         <v>155</v>
       </c>
     </row>
     <row r="101" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A101" s="44"/>
+      <c r="A101" s="50"/>
       <c r="B101" s="39" t="s">
         <v>156</v>
       </c>
     </row>
     <row r="102" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A102" s="45"/>
+      <c r="A102" s="51"/>
       <c r="B102" s="33"/>
     </row>
     <row r="103" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -18466,7 +19946,7 @@
       <c r="B103" s="20"/>
     </row>
     <row r="104" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A104" s="43" t="s">
+      <c r="A104" s="49" t="s">
         <v>147</v>
       </c>
       <c r="B104" s="31" t="s">
@@ -18474,29 +19954,29 @@
       </c>
     </row>
     <row r="105" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A105" s="44"/>
+      <c r="A105" s="50"/>
       <c r="B105" s="7"/>
     </row>
     <row r="106" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A106" s="44"/>
+      <c r="A106" s="50"/>
       <c r="B106" s="7" t="s">
         <v>149</v>
       </c>
     </row>
     <row r="107" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A107" s="44"/>
+      <c r="A107" s="50"/>
       <c r="B107" s="7" t="s">
         <v>150</v>
       </c>
     </row>
     <row r="108" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A108" s="44"/>
+      <c r="A108" s="50"/>
       <c r="B108" s="39" t="s">
         <v>151</v>
       </c>
     </row>
     <row r="109" spans="1:2" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A109" s="45"/>
+      <c r="A109" s="51"/>
       <c r="B109" s="33"/>
     </row>
     <row r="110" spans="1:2" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -18504,7 +19984,7 @@
       <c r="B110" s="20"/>
     </row>
     <row r="111" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A111" s="43" t="s">
+      <c r="A111" s="49" t="s">
         <v>142</v>
       </c>
       <c r="B111" s="31" t="s">
@@ -18512,29 +19992,29 @@
       </c>
     </row>
     <row r="112" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A112" s="44"/>
+      <c r="A112" s="50"/>
       <c r="B112" s="7"/>
     </row>
     <row r="113" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A113" s="44"/>
+      <c r="A113" s="50"/>
       <c r="B113" s="7" t="s">
         <v>144</v>
       </c>
     </row>
     <row r="114" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A114" s="44"/>
+      <c r="A114" s="50"/>
       <c r="B114" s="7" t="s">
         <v>145</v>
       </c>
     </row>
     <row r="115" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A115" s="44"/>
+      <c r="A115" s="50"/>
       <c r="B115" s="39" t="s">
         <v>146</v>
       </c>
     </row>
     <row r="116" spans="1:2" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A116" s="45"/>
+      <c r="A116" s="51"/>
       <c r="B116" s="33"/>
     </row>
     <row r="117" spans="1:2" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -18542,7 +20022,7 @@
       <c r="B117" s="20"/>
     </row>
     <row r="118" spans="1:2" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A118" s="43" t="s">
+      <c r="A118" s="49" t="s">
         <v>136</v>
       </c>
       <c r="B118" s="31" t="s">
@@ -18550,35 +20030,35 @@
       </c>
     </row>
     <row r="119" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A119" s="44"/>
+      <c r="A119" s="50"/>
       <c r="B119" s="7"/>
     </row>
     <row r="120" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A120" s="44"/>
+      <c r="A120" s="50"/>
       <c r="B120" s="7" t="s">
         <v>138</v>
       </c>
     </row>
     <row r="121" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A121" s="44"/>
+      <c r="A121" s="50"/>
       <c r="B121" s="7" t="s">
         <v>139</v>
       </c>
     </row>
     <row r="122" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A122" s="44"/>
+      <c r="A122" s="50"/>
       <c r="B122" s="7" t="s">
         <v>140</v>
       </c>
     </row>
     <row r="123" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A123" s="44"/>
+      <c r="A123" s="50"/>
       <c r="B123" s="39" t="s">
         <v>141</v>
       </c>
     </row>
     <row r="124" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A124" s="45"/>
+      <c r="A124" s="51"/>
       <c r="B124" s="33"/>
     </row>
     <row r="125" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -18586,7 +20066,7 @@
       <c r="B125" s="20"/>
     </row>
     <row r="126" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A126" s="43" t="s">
+      <c r="A126" s="49" t="s">
         <v>127</v>
       </c>
       <c r="B126" s="31" t="s">
@@ -18594,33 +20074,33 @@
       </c>
     </row>
     <row r="127" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A127" s="44"/>
+      <c r="A127" s="50"/>
       <c r="B127" s="7"/>
     </row>
     <row r="128" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A128" s="44"/>
+      <c r="A128" s="50"/>
       <c r="B128" s="7" t="s">
         <v>129</v>
       </c>
     </row>
     <row r="129" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A129" s="44"/>
+      <c r="A129" s="50"/>
       <c r="B129" s="11" t="s">
         <v>130</v>
       </c>
     </row>
     <row r="130" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A130" s="44"/>
+      <c r="A130" s="50"/>
       <c r="B130" s="7"/>
     </row>
     <row r="131" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A131" s="44"/>
+      <c r="A131" s="50"/>
       <c r="B131" s="38" t="s">
         <v>131</v>
       </c>
     </row>
     <row r="132" spans="1:2" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A132" s="45"/>
+      <c r="A132" s="51"/>
       <c r="B132" s="33"/>
     </row>
     <row r="133" spans="1:2" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -18628,7 +20108,7 @@
       <c r="B133" s="20"/>
     </row>
     <row r="134" spans="1:2" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A134" s="43" t="s">
+      <c r="A134" s="49" t="s">
         <v>119</v>
       </c>
       <c r="B134" s="31" t="s">
@@ -18636,57 +20116,57 @@
       </c>
     </row>
     <row r="135" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A135" s="44"/>
+      <c r="A135" s="50"/>
       <c r="B135" s="7"/>
     </row>
     <row r="136" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A136" s="44"/>
+      <c r="A136" s="50"/>
       <c r="B136" s="34" t="s">
         <v>121</v>
       </c>
     </row>
     <row r="137" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A137" s="44"/>
+      <c r="A137" s="50"/>
       <c r="B137" s="7" t="s">
         <v>122</v>
       </c>
     </row>
     <row r="138" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A138" s="44"/>
+      <c r="A138" s="50"/>
       <c r="B138" s="7" t="s">
         <v>123</v>
       </c>
     </row>
     <row r="139" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A139" s="44"/>
+      <c r="A139" s="50"/>
       <c r="B139" s="7" t="s">
         <v>124</v>
       </c>
     </row>
     <row r="140" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A140" s="44"/>
+      <c r="A140" s="50"/>
       <c r="B140" s="11" t="s">
         <v>125</v>
       </c>
     </row>
     <row r="141" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A141" s="44"/>
+      <c r="A141" s="50"/>
       <c r="B141" s="11"/>
     </row>
     <row r="142" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A142" s="44"/>
+      <c r="A142" s="50"/>
       <c r="B142" s="11" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="143" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A143" s="44"/>
+      <c r="A143" s="50"/>
       <c r="B143" s="39" t="s">
         <v>126</v>
       </c>
     </row>
     <row r="144" spans="1:2" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A144" s="45"/>
+      <c r="A144" s="51"/>
       <c r="B144" s="33"/>
     </row>
     <row r="145" spans="1:5" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -18694,7 +20174,7 @@
       <c r="B145" s="20"/>
     </row>
     <row r="146" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A146" s="43" t="s">
+      <c r="A146" s="49" t="s">
         <v>106</v>
       </c>
       <c r="B146" s="31" t="s">
@@ -18702,59 +20182,59 @@
       </c>
     </row>
     <row r="147" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A147" s="44"/>
+      <c r="A147" s="50"/>
       <c r="B147" s="7"/>
     </row>
     <row r="148" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A148" s="44"/>
+      <c r="A148" s="50"/>
       <c r="B148" s="34" t="s">
         <v>108</v>
       </c>
     </row>
     <row r="149" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A149" s="44"/>
+      <c r="A149" s="50"/>
       <c r="B149" s="7" t="s">
         <v>109</v>
       </c>
     </row>
     <row r="150" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A150" s="44"/>
+      <c r="A150" s="50"/>
       <c r="B150" s="7" t="s">
         <v>110</v>
       </c>
     </row>
     <row r="151" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A151" s="44"/>
+      <c r="A151" s="50"/>
       <c r="B151" s="7" t="s">
         <v>111</v>
       </c>
     </row>
     <row r="152" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A152" s="44"/>
+      <c r="A152" s="50"/>
       <c r="B152" s="7" t="s">
         <v>112</v>
       </c>
     </row>
     <row r="153" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A153" s="44"/>
+      <c r="A153" s="50"/>
       <c r="B153" s="11" t="s">
         <v>113</v>
       </c>
     </row>
     <row r="154" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A154" s="44"/>
+      <c r="A154" s="50"/>
       <c r="B154" s="11" t="s">
         <v>114</v>
       </c>
     </row>
     <row r="155" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A155" s="44"/>
+      <c r="A155" s="50"/>
       <c r="B155" s="39" t="s">
         <v>115</v>
       </c>
     </row>
     <row r="156" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A156" s="45"/>
+      <c r="A156" s="51"/>
       <c r="B156" s="33"/>
       <c r="C156" s="2" t="s">
         <v>116</v>
@@ -18775,7 +20255,7 @@
       <c r="B158" s="20"/>
     </row>
     <row r="159" spans="1:5" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A159" s="43" t="s">
+      <c r="A159" s="49" t="s">
         <v>85</v>
       </c>
       <c r="B159" s="31" t="s">
@@ -18783,75 +20263,75 @@
       </c>
     </row>
     <row r="160" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A160" s="44"/>
+      <c r="A160" s="50"/>
       <c r="B160" s="7"/>
     </row>
     <row r="161" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A161" s="44"/>
+      <c r="A161" s="50"/>
       <c r="B161" s="34" t="s">
         <v>87</v>
       </c>
     </row>
     <row r="162" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A162" s="44"/>
+      <c r="A162" s="50"/>
       <c r="B162" s="7" t="s">
         <v>88</v>
       </c>
     </row>
     <row r="163" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A163" s="44"/>
+      <c r="A163" s="50"/>
       <c r="B163" s="7" t="s">
         <v>89</v>
       </c>
     </row>
     <row r="164" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A164" s="44"/>
+      <c r="A164" s="50"/>
       <c r="B164" s="7" t="s">
         <v>90</v>
       </c>
     </row>
     <row r="165" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A165" s="44"/>
+      <c r="A165" s="50"/>
       <c r="B165" s="7" t="s">
         <v>91</v>
       </c>
     </row>
     <row r="166" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A166" s="44"/>
+      <c r="A166" s="50"/>
       <c r="B166" s="7" t="s">
         <v>92</v>
       </c>
     </row>
     <row r="167" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A167" s="44"/>
+      <c r="A167" s="50"/>
       <c r="B167" s="7" t="s">
         <v>93</v>
       </c>
     </row>
     <row r="168" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A168" s="44"/>
+      <c r="A168" s="50"/>
       <c r="B168" s="11" t="s">
         <v>94</v>
       </c>
     </row>
     <row r="169" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A169" s="44"/>
+      <c r="A169" s="50"/>
       <c r="B169" s="11"/>
     </row>
     <row r="170" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A170" s="44"/>
+      <c r="A170" s="50"/>
       <c r="B170" s="36" t="s">
         <v>83</v>
       </c>
     </row>
     <row r="171" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A171" s="44"/>
+      <c r="A171" s="50"/>
       <c r="B171" s="37" t="s">
         <v>95</v>
       </c>
     </row>
     <row r="172" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A172" s="45"/>
+      <c r="A172" s="51"/>
       <c r="B172" s="33" t="s">
         <v>96</v>
       </c>
@@ -18867,7 +20347,7 @@
       <c r="B173" s="20"/>
     </row>
     <row r="174" spans="1:4" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A174" s="43" t="s">
+      <c r="A174" s="49" t="s">
         <v>73</v>
       </c>
       <c r="B174" s="31" t="s">
@@ -18875,69 +20355,69 @@
       </c>
     </row>
     <row r="175" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A175" s="44"/>
+      <c r="A175" s="50"/>
       <c r="B175" s="7"/>
     </row>
     <row r="176" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A176" s="44"/>
+      <c r="A176" s="50"/>
       <c r="B176" s="34" t="s">
         <v>75</v>
       </c>
     </row>
     <row r="177" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A177" s="44"/>
+      <c r="A177" s="50"/>
       <c r="B177" s="7" t="s">
         <v>76</v>
       </c>
     </row>
     <row r="178" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A178" s="44"/>
+      <c r="A178" s="50"/>
       <c r="B178" s="7" t="s">
         <v>77</v>
       </c>
     </row>
     <row r="179" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A179" s="44"/>
+      <c r="A179" s="50"/>
       <c r="B179" s="7" t="s">
         <v>78</v>
       </c>
     </row>
     <row r="180" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A180" s="44"/>
+      <c r="A180" s="50"/>
       <c r="B180" s="7" t="s">
         <v>79</v>
       </c>
     </row>
     <row r="181" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A181" s="44"/>
+      <c r="A181" s="50"/>
       <c r="B181" s="7" t="s">
         <v>80</v>
       </c>
     </row>
     <row r="182" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A182" s="44"/>
+      <c r="A182" s="50"/>
       <c r="B182" s="35" t="s">
         <v>81</v>
       </c>
     </row>
     <row r="183" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A183" s="44"/>
+      <c r="A183" s="50"/>
       <c r="B183" s="11" t="s">
         <v>82</v>
       </c>
     </row>
     <row r="184" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A184" s="44"/>
+      <c r="A184" s="50"/>
       <c r="B184" s="11"/>
     </row>
     <row r="185" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A185" s="44"/>
+      <c r="A185" s="50"/>
       <c r="B185" s="36" t="s">
         <v>83</v>
       </c>
     </row>
     <row r="186" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A186" s="44"/>
+      <c r="A186" s="50"/>
       <c r="B186" s="37" t="s">
         <v>84</v>
       </c>
@@ -18949,7 +20429,7 @@
       </c>
     </row>
     <row r="187" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A187" s="45"/>
+      <c r="A187" s="51"/>
       <c r="B187" s="33" t="s">
         <v>97</v>
       </c>
@@ -18965,7 +20445,7 @@
       <c r="B188" s="20"/>
     </row>
     <row r="189" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A189" s="43" t="s">
+      <c r="A189" s="49" t="s">
         <v>66</v>
       </c>
       <c r="B189" s="29" t="s">
@@ -18973,41 +20453,41 @@
       </c>
     </row>
     <row r="190" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A190" s="44"/>
+      <c r="A190" s="50"/>
       <c r="B190" s="7"/>
     </row>
     <row r="191" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A191" s="44"/>
+      <c r="A191" s="50"/>
       <c r="B191" s="34" t="s">
         <v>68</v>
       </c>
     </row>
     <row r="192" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A192" s="44"/>
+      <c r="A192" s="50"/>
       <c r="B192" s="7" t="s">
         <v>69</v>
       </c>
     </row>
     <row r="193" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A193" s="44"/>
+      <c r="A193" s="50"/>
       <c r="B193" s="7" t="s">
         <v>70</v>
       </c>
     </row>
     <row r="194" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A194" s="44"/>
+      <c r="A194" s="50"/>
       <c r="B194" s="7" t="s">
         <v>71</v>
       </c>
     </row>
     <row r="195" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A195" s="44"/>
+      <c r="A195" s="50"/>
       <c r="B195" s="11" t="s">
         <v>72</v>
       </c>
     </row>
     <row r="196" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A196" s="45"/>
+      <c r="A196" s="51"/>
       <c r="B196" s="18"/>
       <c r="C196" s="2" t="s">
         <v>104</v>
@@ -19021,7 +20501,7 @@
       <c r="B197" s="20"/>
     </row>
     <row r="198" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A198" s="43" t="s">
+      <c r="A198" s="49" t="s">
         <v>47</v>
       </c>
       <c r="B198" s="29" t="s">
@@ -19029,23 +20509,23 @@
       </c>
     </row>
     <row r="199" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A199" s="44"/>
+      <c r="A199" s="50"/>
       <c r="B199" s="21"/>
     </row>
     <row r="200" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A200" s="44"/>
+      <c r="A200" s="50"/>
       <c r="B200" s="21" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="201" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A201" s="44"/>
+      <c r="A201" s="50"/>
       <c r="B201" s="22" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="202" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A202" s="44"/>
+      <c r="A202" s="50"/>
       <c r="B202" s="22" t="s">
         <v>27</v>
       </c>
@@ -19054,7 +20534,7 @@
       </c>
     </row>
     <row r="203" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A203" s="44"/>
+      <c r="A203" s="50"/>
       <c r="B203" s="22" t="s">
         <v>28</v>
       </c>
@@ -19063,7 +20543,7 @@
       </c>
     </row>
     <row r="204" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A204" s="44"/>
+      <c r="A204" s="50"/>
       <c r="B204" s="22" t="s">
         <v>29</v>
       </c>
@@ -19075,7 +20555,7 @@
       </c>
     </row>
     <row r="205" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A205" s="44"/>
+      <c r="A205" s="50"/>
       <c r="B205" s="21" t="s">
         <v>30</v>
       </c>
@@ -19084,7 +20564,7 @@
       </c>
     </row>
     <row r="206" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A206" s="44"/>
+      <c r="A206" s="50"/>
       <c r="B206" s="24" t="s">
         <v>31</v>
       </c>
@@ -19093,53 +20573,53 @@
       </c>
     </row>
     <row r="207" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A207" s="44"/>
+      <c r="A207" s="50"/>
       <c r="B207" s="22"/>
     </row>
     <row r="208" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A208" s="44"/>
+      <c r="A208" s="50"/>
       <c r="B208" s="25" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="209" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A209" s="44"/>
+      <c r="A209" s="50"/>
       <c r="B209" s="26" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="210" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A210" s="44"/>
+      <c r="A210" s="50"/>
       <c r="B210" s="23" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="211" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A211" s="44"/>
+      <c r="A211" s="50"/>
       <c r="B211" s="23" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="212" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A212" s="44"/>
+      <c r="A212" s="50"/>
       <c r="B212" s="23" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="213" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A213" s="44"/>
+      <c r="A213" s="50"/>
       <c r="B213" s="23" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="214" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A214" s="44"/>
+      <c r="A214" s="50"/>
       <c r="B214" s="23" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="215" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A215" s="45"/>
+      <c r="A215" s="51"/>
       <c r="B215" s="27"/>
     </row>
     <row r="216" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -19147,7 +20627,7 @@
       <c r="B216" s="20"/>
     </row>
     <row r="217" spans="1:3" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A217" s="43" t="s">
+      <c r="A217" s="49" t="s">
         <v>2</v>
       </c>
       <c r="B217" s="29" t="s">
@@ -19155,11 +20635,11 @@
       </c>
     </row>
     <row r="218" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A218" s="44"/>
+      <c r="A218" s="50"/>
       <c r="B218" s="7"/>
     </row>
     <row r="219" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A219" s="44"/>
+      <c r="A219" s="50"/>
       <c r="B219" s="8" t="s">
         <v>4</v>
       </c>
@@ -19168,13 +20648,13 @@
       </c>
     </row>
     <row r="220" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A220" s="44"/>
+      <c r="A220" s="50"/>
       <c r="B220" s="9" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="221" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A221" s="44"/>
+      <c r="A221" s="50"/>
       <c r="B221" s="7" t="s">
         <v>6</v>
       </c>
@@ -19183,43 +20663,43 @@
       </c>
     </row>
     <row r="222" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A222" s="44"/>
+      <c r="A222" s="50"/>
       <c r="B222" s="10" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="223" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A223" s="44"/>
+      <c r="A223" s="50"/>
       <c r="B223" s="9" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="224" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A224" s="44"/>
+      <c r="A224" s="50"/>
       <c r="B224" s="11" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="225" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A225" s="44"/>
+      <c r="A225" s="50"/>
       <c r="B225" s="12" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="226" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A226" s="44"/>
+      <c r="A226" s="50"/>
       <c r="B226" s="12" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="227" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A227" s="44"/>
+      <c r="A227" s="50"/>
       <c r="B227" s="12" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="228" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A228" s="45"/>
+      <c r="A228" s="51"/>
       <c r="B228" s="13" t="s">
         <v>13</v>
       </c>
@@ -19229,7 +20709,7 @@
       <c r="B229" s="1"/>
     </row>
     <row r="230" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A230" s="43" t="s">
+      <c r="A230" s="49" t="s">
         <v>14</v>
       </c>
       <c r="B230" s="29" t="s">
@@ -19237,11 +20717,11 @@
       </c>
     </row>
     <row r="231" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A231" s="44"/>
+      <c r="A231" s="50"/>
       <c r="B231" s="7"/>
     </row>
     <row r="232" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A232" s="44"/>
+      <c r="A232" s="50"/>
       <c r="B232" s="7" t="s">
         <v>16</v>
       </c>
@@ -19250,7 +20730,7 @@
       </c>
     </row>
     <row r="233" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A233" s="44"/>
+      <c r="A233" s="50"/>
       <c r="B233" s="11" t="s">
         <v>17</v>
       </c>
@@ -19259,18 +20739,18 @@
       </c>
     </row>
     <row r="234" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A234" s="44"/>
+      <c r="A234" s="50"/>
       <c r="B234" s="7"/>
       <c r="D234" s="3"/>
     </row>
     <row r="235" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A235" s="44"/>
+      <c r="A235" s="50"/>
       <c r="B235" s="15" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="236" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A236" s="44"/>
+      <c r="A236" s="50"/>
       <c r="B236" s="26" t="s">
         <v>48</v>
       </c>
@@ -19279,7 +20759,7 @@
       </c>
     </row>
     <row r="237" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A237" s="45"/>
+      <c r="A237" s="51"/>
       <c r="B237" s="18" t="s">
         <v>21</v>
       </c>
@@ -19292,7 +20772,7 @@
       <c r="B238" s="14"/>
     </row>
     <row r="239" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A239" s="43" t="s">
+      <c r="A239" s="49" t="s">
         <v>19</v>
       </c>
       <c r="B239" s="29" t="s">
@@ -19300,11 +20780,11 @@
       </c>
     </row>
     <row r="240" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A240" s="44"/>
+      <c r="A240" s="50"/>
       <c r="B240" s="7"/>
     </row>
     <row r="241" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A241" s="44"/>
+      <c r="A241" s="50"/>
       <c r="B241" s="7" t="s">
         <v>22</v>
       </c>
@@ -19313,7 +20793,7 @@
       </c>
     </row>
     <row r="242" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A242" s="44"/>
+      <c r="A242" s="50"/>
       <c r="B242" s="11" t="s">
         <v>23</v>
       </c>
@@ -19322,21 +20802,21 @@
       </c>
     </row>
     <row r="243" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A243" s="44"/>
+      <c r="A243" s="50"/>
       <c r="B243" s="7"/>
     </row>
     <row r="244" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A244" s="44"/>
+      <c r="A244" s="50"/>
       <c r="B244" s="9"/>
     </row>
     <row r="245" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A245" s="44"/>
+      <c r="A245" s="50"/>
       <c r="B245" s="15" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="246" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A246" s="45"/>
+      <c r="A246" s="51"/>
       <c r="B246" s="16" t="s">
         <v>24</v>
       </c>
@@ -19349,7 +20829,7 @@
       <c r="B247" s="4"/>
     </row>
     <row r="248" spans="1:4" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A248" s="43" t="s">
+      <c r="A248" s="49" t="s">
         <v>56</v>
       </c>
       <c r="B248" s="31" t="s">
@@ -19357,45 +20837,45 @@
       </c>
     </row>
     <row r="249" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A249" s="44"/>
+      <c r="A249" s="50"/>
       <c r="B249" s="7"/>
     </row>
     <row r="250" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A250" s="44"/>
+      <c r="A250" s="50"/>
       <c r="B250" s="7" t="s">
         <v>52</v>
       </c>
     </row>
     <row r="251" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A251" s="44"/>
+      <c r="A251" s="50"/>
       <c r="B251" s="11" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="252" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A252" s="44"/>
+      <c r="A252" s="50"/>
       <c r="B252" s="11" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="253" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A253" s="44"/>
+      <c r="A253" s="50"/>
       <c r="B253" s="11" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="254" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A254" s="44"/>
+      <c r="A254" s="50"/>
       <c r="B254" s="9"/>
     </row>
     <row r="255" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A255" s="44"/>
+      <c r="A255" s="50"/>
       <c r="B255" s="7" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="256" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A256" s="44"/>
+      <c r="A256" s="50"/>
       <c r="B256" s="15" t="s">
         <v>57</v>
       </c>
@@ -19407,32 +20887,32 @@
       </c>
     </row>
     <row r="257" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A257" s="44"/>
+      <c r="A257" s="50"/>
       <c r="B257" s="32" t="s">
         <v>61</v>
       </c>
     </row>
     <row r="258" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A258" s="44"/>
+      <c r="A258" s="50"/>
       <c r="B258" s="32" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="259" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A259" s="44"/>
+      <c r="A259" s="50"/>
       <c r="B259" s="26" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="260" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A260" s="45"/>
+      <c r="A260" s="51"/>
       <c r="B260" s="18" t="s">
         <v>60</v>
       </c>
     </row>
     <row r="261" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="262" spans="1:2" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A262" s="43" t="s">
+      <c r="A262" s="49" t="s">
         <v>63</v>
       </c>
       <c r="B262" s="31" t="s">
@@ -19440,74 +20920,74 @@
       </c>
     </row>
     <row r="263" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A263" s="44"/>
+      <c r="A263" s="50"/>
       <c r="B263" s="40"/>
     </row>
     <row r="264" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A264" s="44"/>
+      <c r="A264" s="50"/>
       <c r="B264" s="7" t="s">
         <v>132</v>
       </c>
     </row>
     <row r="265" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A265" s="44"/>
+      <c r="A265" s="50"/>
       <c r="B265" s="7" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="266" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A266" s="44"/>
+      <c r="A266" s="50"/>
       <c r="B266" s="11" t="s">
         <v>133</v>
       </c>
     </row>
     <row r="267" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A267" s="44"/>
+      <c r="A267" s="50"/>
       <c r="B267" s="11" t="s">
         <v>134</v>
       </c>
     </row>
     <row r="268" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A268" s="44"/>
+      <c r="A268" s="50"/>
       <c r="B268" s="11" t="s">
         <v>135</v>
       </c>
     </row>
     <row r="269" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A269" s="44"/>
+      <c r="A269" s="50"/>
       <c r="B269" s="7"/>
     </row>
     <row r="270" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A270" s="44"/>
+      <c r="A270" s="50"/>
       <c r="B270" s="7" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="271" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A271" s="44"/>
+      <c r="A271" s="50"/>
       <c r="B271" s="26" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="272" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A272" s="44"/>
+      <c r="A272" s="50"/>
       <c r="B272" s="23" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="273" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A273" s="44"/>
+      <c r="A273" s="50"/>
       <c r="B273" s="26" t="s">
         <v>65</v>
       </c>
     </row>
     <row r="274" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A274" s="45"/>
+      <c r="A274" s="51"/>
       <c r="B274" s="18"/>
     </row>
     <row r="275" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="276" spans="1:2" ht="30.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A276" s="43" t="s">
+      <c r="A276" s="49" t="s">
         <v>231</v>
       </c>
       <c r="B276" s="31" t="s">
@@ -19515,99 +20995,99 @@
       </c>
     </row>
     <row r="277" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A277" s="44"/>
+      <c r="A277" s="50"/>
       <c r="B277" s="7"/>
     </row>
     <row r="278" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A278" s="44"/>
+      <c r="A278" s="50"/>
       <c r="B278" s="34" t="s">
         <v>233</v>
       </c>
     </row>
     <row r="279" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A279" s="44"/>
+      <c r="A279" s="50"/>
       <c r="B279" s="34" t="s">
         <v>234</v>
       </c>
     </row>
     <row r="280" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A280" s="44"/>
+      <c r="A280" s="50"/>
       <c r="B280" s="7" t="s">
         <v>235</v>
       </c>
     </row>
     <row r="281" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A281" s="44"/>
+      <c r="A281" s="50"/>
       <c r="B281" s="11" t="s">
         <v>236</v>
       </c>
     </row>
     <row r="282" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A282" s="44"/>
+      <c r="A282" s="50"/>
       <c r="B282" s="11" t="s">
         <v>237</v>
       </c>
     </row>
     <row r="283" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A283" s="44"/>
+      <c r="A283" s="50"/>
       <c r="B283" s="11" t="s">
         <v>236</v>
       </c>
     </row>
     <row r="284" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A284" s="44"/>
+      <c r="A284" s="50"/>
       <c r="B284" s="7" t="s">
         <v>238</v>
       </c>
     </row>
     <row r="285" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A285" s="44"/>
+      <c r="A285" s="50"/>
       <c r="B285" s="11" t="s">
         <v>239</v>
       </c>
     </row>
     <row r="286" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A286" s="44"/>
+      <c r="A286" s="50"/>
       <c r="B286" s="35" t="s">
         <v>240</v>
       </c>
     </row>
     <row r="287" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A287" s="44"/>
+      <c r="A287" s="50"/>
       <c r="B287" s="34" t="s">
         <v>241</v>
       </c>
     </row>
     <row r="288" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A288" s="44"/>
+      <c r="A288" s="50"/>
       <c r="B288" s="7" t="s">
         <v>242</v>
       </c>
     </row>
     <row r="289" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A289" s="44"/>
+      <c r="A289" s="50"/>
       <c r="B289" s="34" t="s">
         <v>243</v>
       </c>
     </row>
     <row r="290" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A290" s="44"/>
+      <c r="A290" s="50"/>
       <c r="B290" s="7" t="s">
         <v>244</v>
       </c>
     </row>
     <row r="291" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A291" s="44"/>
+      <c r="A291" s="50"/>
       <c r="B291" s="11"/>
     </row>
     <row r="292" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A292" s="44"/>
+      <c r="A292" s="50"/>
       <c r="B292" s="36" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="293" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A293" s="44"/>
+      <c r="A293" s="50"/>
       <c r="B293" s="36" t="s">
         <v>245</v>
       </c>
@@ -19622,13 +21102,13 @@
       </c>
     </row>
     <row r="294" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A294" s="44"/>
-      <c r="B294" s="50" t="s">
+      <c r="A294" s="50"/>
+      <c r="B294" s="47" t="s">
         <v>246</v>
       </c>
     </row>
     <row r="295" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A295" s="45"/>
+      <c r="A295" s="51"/>
       <c r="B295" s="33"/>
       <c r="C295" s="2" t="s">
         <v>249</v>
@@ -19642,7 +21122,7 @@
     </row>
     <row r="296" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="297" spans="1:5" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A297" s="43" t="s">
+      <c r="A297" s="49" t="s">
         <v>252</v>
       </c>
       <c r="B297" s="31" t="s">
@@ -19650,74 +21130,74 @@
       </c>
     </row>
     <row r="298" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A298" s="44"/>
+      <c r="A298" s="50"/>
       <c r="B298" s="40"/>
     </row>
     <row r="299" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A299" s="44"/>
+      <c r="A299" s="50"/>
       <c r="B299" s="11" t="s">
         <v>254</v>
       </c>
     </row>
     <row r="300" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A300" s="44"/>
+      <c r="A300" s="50"/>
       <c r="B300" s="11" t="s">
         <v>255</v>
       </c>
     </row>
     <row r="301" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A301" s="44"/>
+      <c r="A301" s="50"/>
       <c r="B301" s="11" t="s">
         <v>254</v>
       </c>
     </row>
     <row r="302" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A302" s="44"/>
+      <c r="A302" s="50"/>
       <c r="B302" s="7" t="s">
         <v>256</v>
       </c>
     </row>
     <row r="303" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A303" s="44"/>
+      <c r="A303" s="50"/>
       <c r="B303" s="34" t="s">
         <v>257</v>
       </c>
     </row>
     <row r="304" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A304" s="44"/>
+      <c r="A304" s="50"/>
       <c r="B304" s="7" t="s">
         <v>258</v>
       </c>
     </row>
     <row r="305" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A305" s="44"/>
+      <c r="A305" s="50"/>
       <c r="B305" s="7" t="s">
         <v>259</v>
       </c>
     </row>
     <row r="306" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A306" s="44"/>
+      <c r="A306" s="50"/>
       <c r="B306" s="11" t="s">
         <v>260</v>
       </c>
     </row>
     <row r="307" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A307" s="44"/>
+      <c r="A307" s="50"/>
       <c r="B307" s="23"/>
     </row>
     <row r="308" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A308" s="44"/>
+      <c r="A308" s="50"/>
       <c r="B308" s="26" t="s">
         <v>261</v>
       </c>
     </row>
     <row r="309" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A309" s="45"/>
+      <c r="A309" s="51"/>
       <c r="B309" s="18"/>
     </row>
     <row r="310" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="311" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A311" s="43" t="s">
+      <c r="A311" s="49" t="s">
         <v>262</v>
       </c>
       <c r="B311" s="29" t="s">
@@ -19725,46 +21205,46 @@
       </c>
     </row>
     <row r="312" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A312" s="44"/>
+      <c r="A312" s="50"/>
       <c r="B312" s="7"/>
     </row>
     <row r="313" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A313" s="44"/>
+      <c r="A313" s="50"/>
       <c r="B313" s="7" t="s">
         <v>264</v>
       </c>
     </row>
     <row r="314" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A314" s="44"/>
+      <c r="A314" s="50"/>
       <c r="B314" s="34" t="s">
         <v>265</v>
       </c>
     </row>
     <row r="315" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A315" s="44"/>
+      <c r="A315" s="50"/>
       <c r="B315" s="7" t="s">
         <v>266</v>
       </c>
     </row>
     <row r="316" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A316" s="44"/>
+      <c r="A316" s="50"/>
       <c r="B316" s="34" t="s">
         <v>243</v>
       </c>
     </row>
     <row r="317" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A317" s="44"/>
+      <c r="A317" s="50"/>
       <c r="B317" s="41" t="s">
         <v>267</v>
       </c>
     </row>
     <row r="318" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A318" s="45"/>
+      <c r="A318" s="51"/>
       <c r="B318" s="16"/>
     </row>
     <row r="319" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="320" spans="1:2" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A320" s="43" t="s">
+      <c r="A320" s="49" t="s">
         <v>268</v>
       </c>
       <c r="B320" s="31" t="s">
@@ -19772,39 +21252,39 @@
       </c>
     </row>
     <row r="321" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A321" s="44"/>
+      <c r="A321" s="50"/>
       <c r="B321" s="7"/>
     </row>
     <row r="322" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A322" s="44"/>
+      <c r="A322" s="50"/>
       <c r="B322" s="7" t="s">
         <v>270</v>
       </c>
     </row>
     <row r="323" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A323" s="44"/>
+      <c r="A323" s="50"/>
       <c r="B323" s="7" t="s">
         <v>272</v>
       </c>
     </row>
     <row r="324" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A324" s="44"/>
+      <c r="A324" s="50"/>
       <c r="B324" s="11" t="s">
         <v>271</v>
       </c>
     </row>
     <row r="325" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A325" s="44"/>
+      <c r="A325" s="50"/>
       <c r="B325" s="34"/>
     </row>
     <row r="326" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A326" s="44"/>
+      <c r="A326" s="50"/>
       <c r="B326" s="7" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="327" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A327" s="44"/>
+      <c r="A327" s="50"/>
       <c r="B327" s="36" t="s">
         <v>273</v>
       </c>
@@ -19819,12 +21299,12 @@
       </c>
     </row>
     <row r="328" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A328" s="45"/>
+      <c r="A328" s="51"/>
       <c r="B328" s="42"/>
     </row>
     <row r="329" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="330" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A330" s="43" t="s">
+      <c r="A330" s="49" t="s">
         <v>277</v>
       </c>
       <c r="B330" s="31" t="s">
@@ -19832,63 +21312,63 @@
       </c>
     </row>
     <row r="331" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A331" s="44"/>
+      <c r="A331" s="50"/>
       <c r="B331" s="40"/>
     </row>
     <row r="332" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A332" s="44"/>
+      <c r="A332" s="50"/>
       <c r="B332" s="34" t="s">
         <v>279</v>
       </c>
     </row>
     <row r="333" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A333" s="44"/>
+      <c r="A333" s="50"/>
       <c r="B333" s="7" t="s">
         <v>280</v>
       </c>
     </row>
     <row r="334" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A334" s="44"/>
+      <c r="A334" s="50"/>
       <c r="B334" s="34" t="s">
         <v>281</v>
       </c>
     </row>
     <row r="335" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A335" s="44"/>
+      <c r="A335" s="50"/>
       <c r="B335" s="7" t="s">
         <v>282</v>
       </c>
     </row>
     <row r="336" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A336" s="44"/>
+      <c r="A336" s="50"/>
       <c r="B336" s="34" t="s">
         <v>283</v>
       </c>
     </row>
     <row r="337" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A337" s="44"/>
+      <c r="A337" s="50"/>
       <c r="B337" s="7" t="s">
         <v>284</v>
       </c>
     </row>
     <row r="338" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A338" s="44"/>
+      <c r="A338" s="50"/>
       <c r="B338" s="34" t="s">
         <v>243</v>
       </c>
     </row>
     <row r="339" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A339" s="44"/>
+      <c r="A339" s="50"/>
       <c r="B339" s="7" t="s">
         <v>285</v>
       </c>
     </row>
     <row r="340" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A340" s="44"/>
+      <c r="A340" s="50"/>
       <c r="B340" s="7"/>
     </row>
     <row r="341" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A341" s="44"/>
+      <c r="A341" s="50"/>
       <c r="B341" s="36" t="s">
         <v>286</v>
       </c>
@@ -19900,12 +21380,12 @@
       </c>
     </row>
     <row r="342" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A342" s="45"/>
+      <c r="A342" s="51"/>
       <c r="B342" s="42"/>
     </row>
     <row r="343" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="344" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A344" s="43" t="s">
+      <c r="A344" s="49" t="s">
         <v>289</v>
       </c>
       <c r="B344" s="31" t="s">
@@ -19913,51 +21393,51 @@
       </c>
     </row>
     <row r="345" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A345" s="44"/>
+      <c r="A345" s="50"/>
       <c r="B345" s="40"/>
     </row>
     <row r="346" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A346" s="44"/>
+      <c r="A346" s="50"/>
       <c r="B346" s="34" t="s">
         <v>291</v>
       </c>
     </row>
     <row r="347" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A347" s="44"/>
+      <c r="A347" s="50"/>
       <c r="B347" s="7" t="s">
         <v>292</v>
       </c>
     </row>
     <row r="348" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A348" s="44"/>
+      <c r="A348" s="50"/>
       <c r="B348" s="7" t="s">
         <v>293</v>
       </c>
     </row>
     <row r="349" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A349" s="44"/>
+      <c r="A349" s="50"/>
       <c r="B349" s="7" t="s">
         <v>294</v>
       </c>
     </row>
     <row r="350" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A350" s="44"/>
+      <c r="A350" s="50"/>
       <c r="B350" s="11" t="s">
         <v>295</v>
       </c>
     </row>
     <row r="351" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A351" s="44"/>
+      <c r="A351" s="50"/>
       <c r="B351" s="11" t="s">
         <v>296</v>
       </c>
     </row>
     <row r="352" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A352" s="44"/>
+      <c r="A352" s="50"/>
       <c r="B352" s="34"/>
     </row>
     <row r="353" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A353" s="44"/>
+      <c r="A353" s="50"/>
       <c r="B353" s="7" t="s">
         <v>297</v>
       </c>
@@ -19978,12 +21458,12 @@
       </c>
     </row>
     <row r="354" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A354" s="45"/>
+      <c r="A354" s="51"/>
       <c r="B354" s="42"/>
     </row>
     <row r="355" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="356" spans="1:7" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A356" s="43" t="s">
+      <c r="A356" s="49" t="s">
         <v>309</v>
       </c>
       <c r="B356" s="31" t="s">
@@ -19991,52 +21471,52 @@
       </c>
     </row>
     <row r="357" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A357" s="44"/>
+      <c r="A357" s="50"/>
       <c r="B357" s="40"/>
     </row>
     <row r="358" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A358" s="44"/>
+      <c r="A358" s="50"/>
       <c r="B358" s="7" t="s">
         <v>304</v>
       </c>
     </row>
     <row r="359" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A359" s="44"/>
+      <c r="A359" s="50"/>
       <c r="B359" s="34" t="s">
         <v>305</v>
       </c>
     </row>
     <row r="360" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A360" s="44"/>
+      <c r="A360" s="50"/>
       <c r="B360" s="7" t="s">
         <v>306</v>
       </c>
     </row>
     <row r="361" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A361" s="44"/>
+      <c r="A361" s="50"/>
       <c r="B361" s="34" t="s">
         <v>243</v>
       </c>
     </row>
     <row r="362" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A362" s="44"/>
+      <c r="A362" s="50"/>
       <c r="B362" s="7" t="s">
         <v>307</v>
       </c>
     </row>
     <row r="363" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A363" s="44"/>
+      <c r="A363" s="50"/>
       <c r="B363" s="11" t="s">
         <v>308</v>
       </c>
     </row>
     <row r="364" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A364" s="45"/>
+      <c r="A364" s="51"/>
       <c r="B364" s="42"/>
     </row>
     <row r="365" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="366" spans="1:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A366" s="43" t="s">
+      <c r="A366" s="49" t="s">
         <v>321</v>
       </c>
       <c r="B366" s="31" t="s">
@@ -20044,126 +21524,126 @@
       </c>
     </row>
     <row r="367" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A367" s="44"/>
+      <c r="A367" s="50"/>
       <c r="B367" s="40"/>
     </row>
     <row r="368" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A368" s="44"/>
+      <c r="A368" s="50"/>
       <c r="B368" s="11" t="s">
         <v>311</v>
       </c>
     </row>
     <row r="369" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A369" s="44"/>
+      <c r="A369" s="50"/>
       <c r="B369" s="11" t="s">
         <v>312</v>
       </c>
     </row>
     <row r="370" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A370" s="44"/>
+      <c r="A370" s="50"/>
       <c r="B370" s="11" t="s">
         <v>311</v>
       </c>
     </row>
     <row r="371" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A371" s="44"/>
+      <c r="A371" s="50"/>
       <c r="B371" s="7" t="s">
         <v>313</v>
       </c>
     </row>
     <row r="372" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A372" s="44"/>
+      <c r="A372" s="50"/>
       <c r="B372" s="7" t="s">
         <v>314</v>
       </c>
     </row>
     <row r="373" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A373" s="44"/>
+      <c r="A373" s="50"/>
       <c r="B373" s="7" t="s">
         <v>315</v>
       </c>
     </row>
     <row r="374" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A374" s="44"/>
+      <c r="A374" s="50"/>
       <c r="B374" s="34" t="s">
         <v>316</v>
       </c>
     </row>
     <row r="375" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A375" s="44"/>
+      <c r="A375" s="50"/>
       <c r="B375" s="7" t="s">
         <v>317</v>
       </c>
     </row>
     <row r="376" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A376" s="44"/>
+      <c r="A376" s="50"/>
       <c r="B376" s="34" t="s">
         <v>243</v>
       </c>
     </row>
     <row r="377" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A377" s="44"/>
+      <c r="A377" s="50"/>
       <c r="B377" s="7" t="s">
         <v>318</v>
       </c>
     </row>
     <row r="378" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A378" s="45"/>
+      <c r="A378" s="51"/>
       <c r="B378" s="42"/>
     </row>
     <row r="379" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="380" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A380" s="43" t="s">
+      <c r="A380" s="49" t="s">
         <v>319</v>
       </c>
       <c r="B380" s="31"/>
     </row>
     <row r="381" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A381" s="44"/>
+      <c r="A381" s="50"/>
       <c r="B381" s="40"/>
     </row>
     <row r="382" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A382" s="44"/>
+      <c r="A382" s="50"/>
       <c r="B382" s="11"/>
     </row>
     <row r="383" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A383" s="44"/>
+      <c r="A383" s="50"/>
       <c r="B383" s="11"/>
     </row>
     <row r="384" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A384" s="44"/>
+      <c r="A384" s="50"/>
       <c r="B384" s="11"/>
     </row>
     <row r="385" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A385" s="44"/>
+      <c r="A385" s="50"/>
       <c r="B385" s="7"/>
     </row>
     <row r="386" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A386" s="44"/>
+      <c r="A386" s="50"/>
       <c r="B386" s="7"/>
     </row>
     <row r="387" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A387" s="44"/>
+      <c r="A387" s="50"/>
       <c r="B387" s="7"/>
     </row>
     <row r="388" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A388" s="44"/>
+      <c r="A388" s="50"/>
       <c r="B388" s="34"/>
     </row>
     <row r="389" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A389" s="44"/>
+      <c r="A389" s="50"/>
       <c r="B389" s="7"/>
     </row>
     <row r="390" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A390" s="44"/>
+      <c r="A390" s="50"/>
       <c r="B390" s="34"/>
     </row>
     <row r="391" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A391" s="44"/>
+      <c r="A391" s="50"/>
       <c r="B391" s="7"/>
     </row>
     <row r="392" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A392" s="45"/>
+      <c r="A392" s="51"/>
       <c r="B392" s="42"/>
       <c r="C392" s="2" t="s">
         <v>320</v>
@@ -20174,62 +21654,62 @@
     </row>
     <row r="393" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="394" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A394" s="43" t="s">
+      <c r="A394" s="49" t="s">
         <v>319</v>
       </c>
       <c r="B394" s="31"/>
     </row>
     <row r="395" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A395" s="44"/>
+      <c r="A395" s="50"/>
       <c r="B395" s="40"/>
     </row>
     <row r="396" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A396" s="44"/>
+      <c r="A396" s="50"/>
       <c r="B396" s="11"/>
     </row>
     <row r="397" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A397" s="44"/>
+      <c r="A397" s="50"/>
       <c r="B397" s="11"/>
     </row>
     <row r="398" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A398" s="44"/>
+      <c r="A398" s="50"/>
       <c r="B398" s="11"/>
     </row>
     <row r="399" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A399" s="44"/>
+      <c r="A399" s="50"/>
       <c r="B399" s="7"/>
     </row>
     <row r="400" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A400" s="44"/>
+      <c r="A400" s="50"/>
       <c r="B400" s="7"/>
     </row>
     <row r="401" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A401" s="44"/>
+      <c r="A401" s="50"/>
       <c r="B401" s="7"/>
     </row>
     <row r="402" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A402" s="44"/>
+      <c r="A402" s="50"/>
       <c r="B402" s="34"/>
     </row>
     <row r="403" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A403" s="44"/>
+      <c r="A403" s="50"/>
       <c r="B403" s="7"/>
     </row>
     <row r="404" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A404" s="44"/>
+      <c r="A404" s="50"/>
       <c r="B404" s="34"/>
     </row>
     <row r="405" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A405" s="44"/>
+      <c r="A405" s="50"/>
       <c r="B405" s="7"/>
     </row>
     <row r="406" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A406" s="45"/>
+      <c r="A406" s="51"/>
       <c r="B406" s="42"/>
     </row>
     <row r="407" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="408" spans="1:2" ht="30.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A408" s="43" t="s">
+      <c r="A408" s="49" t="s">
         <v>322</v>
       </c>
       <c r="B408" s="31" t="s">
@@ -20237,124 +21717,124 @@
       </c>
     </row>
     <row r="409" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A409" s="44"/>
+      <c r="A409" s="50"/>
       <c r="B409" s="40"/>
     </row>
     <row r="410" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A410" s="44"/>
+      <c r="A410" s="50"/>
       <c r="B410" s="34" t="s">
         <v>234</v>
       </c>
     </row>
     <row r="411" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A411" s="44"/>
-      <c r="B411" s="46"/>
+      <c r="A411" s="50"/>
+      <c r="B411" s="43"/>
     </row>
     <row r="412" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A412" s="44"/>
+      <c r="A412" s="50"/>
       <c r="B412" s="11" t="s">
         <v>323</v>
       </c>
     </row>
     <row r="413" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A413" s="44"/>
+      <c r="A413" s="50"/>
       <c r="B413" s="11" t="s">
         <v>324</v>
       </c>
     </row>
     <row r="414" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A414" s="44"/>
+      <c r="A414" s="50"/>
       <c r="B414" s="11" t="s">
         <v>323</v>
       </c>
     </row>
     <row r="415" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A415" s="44"/>
-      <c r="B415" s="46"/>
+      <c r="A415" s="50"/>
+      <c r="B415" s="43"/>
     </row>
     <row r="416" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A416" s="44"/>
+      <c r="A416" s="50"/>
       <c r="B416" s="7" t="s">
         <v>325</v>
       </c>
     </row>
     <row r="417" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A417" s="44"/>
+      <c r="A417" s="50"/>
       <c r="B417" s="7" t="s">
         <v>326</v>
       </c>
     </row>
     <row r="418" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A418" s="44"/>
+      <c r="A418" s="50"/>
       <c r="B418" s="7" t="s">
         <v>327</v>
       </c>
     </row>
     <row r="419" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A419" s="44"/>
+      <c r="A419" s="50"/>
       <c r="B419" s="7" t="s">
         <v>328</v>
       </c>
     </row>
     <row r="420" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A420" s="44"/>
+      <c r="A420" s="50"/>
       <c r="B420" s="7" t="s">
         <v>329</v>
       </c>
     </row>
     <row r="421" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A421" s="44"/>
-      <c r="B421" s="46"/>
+      <c r="A421" s="50"/>
+      <c r="B421" s="43"/>
     </row>
     <row r="422" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A422" s="44"/>
+      <c r="A422" s="50"/>
       <c r="B422" s="11" t="s">
         <v>330</v>
       </c>
     </row>
     <row r="423" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A423" s="44"/>
+      <c r="A423" s="50"/>
       <c r="B423" s="35" t="s">
         <v>240</v>
       </c>
     </row>
     <row r="424" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A424" s="44"/>
-      <c r="B424" s="46"/>
+      <c r="A424" s="50"/>
+      <c r="B424" s="43"/>
     </row>
     <row r="425" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A425" s="44"/>
+      <c r="A425" s="50"/>
       <c r="B425" s="34" t="s">
         <v>331</v>
       </c>
     </row>
-    <row r="426" spans="1:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="A426" s="44"/>
-      <c r="B426" s="47" t="s">
+    <row r="426" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A426" s="50"/>
+      <c r="B426" s="44" t="s">
         <v>332</v>
       </c>
     </row>
     <row r="427" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A427" s="44"/>
+      <c r="A427" s="50"/>
       <c r="B427" s="34" t="s">
         <v>243</v>
       </c>
     </row>
-    <row r="428" spans="1:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="A428" s="44"/>
-      <c r="B428" s="47" t="s">
+    <row r="428" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A428" s="50"/>
+      <c r="B428" s="44" t="s">
         <v>333</v>
       </c>
     </row>
     <row r="429" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A429" s="45"/>
-      <c r="B429" s="49" t="s">
+      <c r="A429" s="51"/>
+      <c r="B429" s="46" t="s">
         <v>297</v>
       </c>
     </row>
     <row r="430" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="431" spans="1:2" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A431" s="43" t="s">
+      <c r="A431" s="49" t="s">
         <v>334</v>
       </c>
       <c r="B431" s="31" t="s">
@@ -20362,132 +21842,344 @@
       </c>
     </row>
     <row r="432" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A432" s="44"/>
+      <c r="A432" s="50"/>
       <c r="B432" s="40"/>
     </row>
     <row r="433" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A433" s="44"/>
+      <c r="A433" s="50"/>
       <c r="B433" s="11" t="s">
         <v>336</v>
       </c>
     </row>
     <row r="434" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A434" s="44"/>
+      <c r="A434" s="50"/>
       <c r="B434" s="7" t="s">
         <v>337</v>
       </c>
     </row>
     <row r="435" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A435" s="44"/>
+      <c r="A435" s="50"/>
       <c r="B435" s="11" t="s">
         <v>338</v>
       </c>
     </row>
     <row r="436" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A436" s="44"/>
-      <c r="B436" s="48" t="s">
+      <c r="A436" s="50"/>
+      <c r="B436" s="45" t="s">
         <v>339</v>
       </c>
     </row>
     <row r="437" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A437" s="44"/>
-      <c r="B437" s="48" t="s">
+      <c r="A437" s="50"/>
+      <c r="B437" s="45" t="s">
         <v>340</v>
       </c>
     </row>
     <row r="438" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A438" s="44"/>
-      <c r="B438" s="48" t="s">
+      <c r="A438" s="50"/>
+      <c r="B438" s="45" t="s">
         <v>341</v>
       </c>
     </row>
     <row r="439" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A439" s="44"/>
+      <c r="A439" s="50"/>
       <c r="B439" s="7" t="s">
         <v>342</v>
       </c>
     </row>
     <row r="440" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A440" s="44"/>
+      <c r="A440" s="50"/>
       <c r="B440" s="34" t="s">
         <v>343</v>
       </c>
     </row>
     <row r="441" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A441" s="44"/>
+      <c r="A441" s="50"/>
       <c r="B441" s="7" t="s">
         <v>344</v>
       </c>
     </row>
     <row r="442" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A442" s="44"/>
+      <c r="A442" s="50"/>
       <c r="B442" s="34" t="s">
         <v>345</v>
       </c>
     </row>
     <row r="443" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A443" s="44"/>
+      <c r="A443" s="50"/>
       <c r="B443" s="7" t="s">
         <v>346</v>
       </c>
     </row>
     <row r="444" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A444" s="44"/>
+      <c r="A444" s="50"/>
       <c r="B444" s="34" t="s">
         <v>347</v>
       </c>
     </row>
     <row r="445" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A445" s="44"/>
+      <c r="A445" s="50"/>
       <c r="B445" s="7" t="s">
         <v>348</v>
       </c>
     </row>
     <row r="446" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A446" s="44"/>
+      <c r="A446" s="50"/>
       <c r="B446" s="34" t="s">
         <v>243</v>
       </c>
     </row>
     <row r="447" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A447" s="44"/>
+      <c r="A447" s="50"/>
       <c r="B447" s="7" t="s">
         <v>349</v>
       </c>
     </row>
     <row r="448" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A448" s="44"/>
+      <c r="A448" s="50"/>
       <c r="B448" s="34"/>
     </row>
     <row r="449" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A449" s="44"/>
+      <c r="A449" s="50"/>
       <c r="B449" s="7" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="450" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A450" s="44"/>
-      <c r="B450" s="51" t="s">
+      <c r="A450" s="50"/>
+      <c r="B450" s="48" t="s">
         <v>351</v>
       </c>
     </row>
     <row r="451" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A451" s="44"/>
-      <c r="B451" s="47" t="s">
+      <c r="A451" s="50"/>
+      <c r="B451" s="44" t="s">
         <v>352</v>
       </c>
     </row>
     <row r="452" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A452" s="45"/>
+      <c r="A452" s="51"/>
       <c r="B452" s="42"/>
     </row>
+    <row r="453" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="454" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A454" s="49" t="s">
+        <v>353</v>
+      </c>
+      <c r="B454" s="31" t="s">
+        <v>354</v>
+      </c>
+    </row>
+    <row r="455" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A455" s="50"/>
+      <c r="B455" s="40"/>
+    </row>
+    <row r="456" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A456" s="50"/>
+      <c r="B456" s="11" t="s">
+        <v>355</v>
+      </c>
+    </row>
+    <row r="457" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A457" s="50"/>
+      <c r="B457" s="7" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="458" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A458" s="50"/>
+      <c r="B458" s="7" t="s">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="459" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A459" s="50"/>
+      <c r="B459" s="34" t="s">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="460" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A460" s="50"/>
+      <c r="B460" s="7" t="s">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="461" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A461" s="50"/>
+      <c r="B461" s="34" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="462" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A462" s="50"/>
+      <c r="B462" s="7" t="s">
+        <v>359</v>
+      </c>
+    </row>
+    <row r="463" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A463" s="50"/>
+      <c r="B463" s="34" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="464" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A464" s="50"/>
+      <c r="B464" s="7" t="s">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="465" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A465" s="51"/>
+      <c r="B465" s="42"/>
+    </row>
+    <row r="466" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="467" spans="1:2" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A467" s="49" t="s">
+        <v>362</v>
+      </c>
+      <c r="B467" s="31" t="s">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="468" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A468" s="50"/>
+      <c r="B468" s="40"/>
+    </row>
+    <row r="469" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A469" s="50"/>
+      <c r="B469" s="34" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="470" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A470" s="50"/>
+      <c r="B470" s="11" t="s">
+        <v>363</v>
+      </c>
+    </row>
+    <row r="471" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A471" s="50"/>
+      <c r="B471" s="11" t="s">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="472" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A472" s="50"/>
+      <c r="B472" s="11" t="s">
+        <v>363</v>
+      </c>
+    </row>
+    <row r="473" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A473" s="50"/>
+      <c r="B473" s="7" t="s">
+        <v>365</v>
+      </c>
+    </row>
+    <row r="474" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A474" s="50"/>
+      <c r="B474" s="34" t="s">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="475" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A475" s="50"/>
+      <c r="B475" s="7" t="s">
+        <v>367</v>
+      </c>
+    </row>
+    <row r="476" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A476" s="50"/>
+      <c r="B476" s="7" t="s">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="477" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A477" s="50"/>
+      <c r="B477" s="7" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="478" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A478" s="50"/>
+      <c r="B478" s="7" t="s">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="479" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A479" s="50"/>
+      <c r="B479" s="34" t="s">
+        <v>371</v>
+      </c>
+    </row>
+    <row r="480" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A480" s="50"/>
+      <c r="B480" s="7" t="s">
+        <v>372</v>
+      </c>
+    </row>
+    <row r="481" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A481" s="50"/>
+      <c r="B481" s="34" t="s">
+        <v>373</v>
+      </c>
+    </row>
+    <row r="482" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A482" s="50"/>
+      <c r="B482" s="7" t="s">
+        <v>374</v>
+      </c>
+    </row>
+    <row r="483" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A483" s="50"/>
+      <c r="B483" s="34" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="484" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A484" s="50"/>
+      <c r="B484" s="7" t="s">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="485" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A485" s="50"/>
+      <c r="B485" s="11"/>
+    </row>
+    <row r="486" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A486" s="50"/>
+      <c r="B486" s="7" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="487" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A487" s="50"/>
+      <c r="B487" s="48" t="s">
+        <v>376</v>
+      </c>
+    </row>
+    <row r="488" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A488" s="51"/>
+      <c r="B488" s="42"/>
+    </row>
   </sheetData>
-  <mergeCells count="38">
-    <mergeCell ref="A408:A429"/>
-    <mergeCell ref="A431:A452"/>
-    <mergeCell ref="A380:A392"/>
-    <mergeCell ref="A394:A406"/>
-    <mergeCell ref="A320:A328"/>
+  <mergeCells count="40">
+    <mergeCell ref="A454:A465"/>
+    <mergeCell ref="A467:A488"/>
+    <mergeCell ref="A297:A309"/>
+    <mergeCell ref="A276:A295"/>
+    <mergeCell ref="A356:A364"/>
+    <mergeCell ref="A330:A342"/>
+    <mergeCell ref="A104:A109"/>
+    <mergeCell ref="A56:A62"/>
+    <mergeCell ref="A48:A54"/>
+    <mergeCell ref="A97:A102"/>
+    <mergeCell ref="A88:A95"/>
+    <mergeCell ref="A81:A86"/>
+    <mergeCell ref="A2:A6"/>
+    <mergeCell ref="A37:A46"/>
+    <mergeCell ref="A29:A35"/>
+    <mergeCell ref="A16:A27"/>
+    <mergeCell ref="A8:A14"/>
     <mergeCell ref="A64:A78"/>
     <mergeCell ref="A311:A318"/>
     <mergeCell ref="A126:A132"/>
@@ -20501,26 +22193,16 @@
     <mergeCell ref="A239:A246"/>
     <mergeCell ref="A198:A215"/>
     <mergeCell ref="A118:A124"/>
-    <mergeCell ref="A2:A6"/>
-    <mergeCell ref="A37:A46"/>
-    <mergeCell ref="A29:A35"/>
-    <mergeCell ref="A16:A27"/>
-    <mergeCell ref="A8:A14"/>
     <mergeCell ref="A111:A116"/>
+    <mergeCell ref="A217:A228"/>
+    <mergeCell ref="A248:A260"/>
+    <mergeCell ref="A408:A429"/>
+    <mergeCell ref="A431:A452"/>
+    <mergeCell ref="A380:A392"/>
+    <mergeCell ref="A394:A406"/>
+    <mergeCell ref="A320:A328"/>
     <mergeCell ref="A366:A378"/>
-    <mergeCell ref="A56:A62"/>
-    <mergeCell ref="A48:A54"/>
-    <mergeCell ref="A97:A102"/>
-    <mergeCell ref="A88:A95"/>
-    <mergeCell ref="A81:A86"/>
-    <mergeCell ref="A217:A228"/>
     <mergeCell ref="A344:A354"/>
-    <mergeCell ref="A248:A260"/>
-    <mergeCell ref="A297:A309"/>
-    <mergeCell ref="A276:A295"/>
-    <mergeCell ref="A356:A364"/>
-    <mergeCell ref="A330:A342"/>
-    <mergeCell ref="A104:A109"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Atualizado o ex040 e planilha
</commit_message>
<xml_diff>
--- a/detalhesPython.xlsx
+++ b/detalhesPython.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\thiag\Documents\EstudosT\python\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82BF68F2-6094-4807-AA10-EC343DAAC969}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E886344-1C6C-49FC-B6A8-2482E2348FE5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{ECBDB9F7-0FAD-476C-A4A4-7948F29B869E}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="418" uniqueCount="377">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="429" uniqueCount="387">
   <si>
     <t>Descrição</t>
   </si>
@@ -18129,6 +18129,729 @@
   </si>
   <si>
     <t>.center(36) ---&gt; Serve para centralizar a string dentro de no caso 36 espaços de caracteres, podendo fazer também: .center(36, =) para preencher os outros espaços vazios....pesquisar</t>
+  </si>
+  <si>
+    <t>ex040</t>
+  </si>
+  <si>
+    <t>Crie um programa que leia duas notas de um aluno e calcule sua média, mostrando uma mensagem no final, de acordo com a média atingida:</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">n1 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>=</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color rgb="FF988BC7"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>float</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>(</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF988BC7"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>input</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>(</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE7DE79"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>'Digite a primeira nota: '</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>))</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">n2 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>=</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color rgb="FF988BC7"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>float</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>(</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF988BC7"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>input</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>(</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE7DE79"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>'Digite a segunda nota: '</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>))</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">media </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>=</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> (n1 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> n2) </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>/</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF78D1E1"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>2</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>if</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> media </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>&lt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF78D1E1"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>5</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>:</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">    </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF988BC7"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>print</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>(</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE7DE79"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>'</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>\033</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE7DE79"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>[31mALUNO REPROVADO!</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>\033</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE7DE79"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">[m Média </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF78D1E1"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>{}</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE7DE79"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>'</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF67E480"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>format</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>(media))</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>elif</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> media </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF78D1E1"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>5</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>and</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> media </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>&lt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF78D1E1"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>6.9</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>:</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">    </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF988BC7"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>print</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>(</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE7DE79"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>'</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>\033</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE7DE79"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>[33mRECUPERAÇÃO!</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>\033</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE7DE79"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">[m Média </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF78D1E1"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>{}</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE7DE79"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>'</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF67E480"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>format</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>(media))</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">    </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF988BC7"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>print</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>(</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE7DE79"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>'</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>\033</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE7DE79"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>[32mAPROVADO!</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>\033</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE7DE79"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">[m Média </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF78D1E1"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>{}</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE7DE79"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>'</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF67E480"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>format</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>(media))</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -19358,10 +20081,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{73331524-72FC-41A3-82E6-4326A0999772}">
-  <dimension ref="A1:G488"/>
+  <dimension ref="A1:G501"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A460" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A467" sqref="A467:A488"/>
+    <sheetView tabSelected="1" topLeftCell="A488" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B490" sqref="B490"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -21833,7 +22556,7 @@
       </c>
     </row>
     <row r="430" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="431" spans="1:2" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="431" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A431" s="49" t="s">
         <v>334</v>
       </c>
@@ -22161,38 +22884,80 @@
       <c r="A488" s="51"/>
       <c r="B488" s="42"/>
     </row>
+    <row r="489" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="490" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A490" s="49" t="s">
+        <v>377</v>
+      </c>
+      <c r="B490" s="31" t="s">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="491" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A491" s="50"/>
+      <c r="B491" s="40"/>
+    </row>
+    <row r="492" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A492" s="50"/>
+      <c r="B492" s="7" t="s">
+        <v>379</v>
+      </c>
+    </row>
+    <row r="493" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A493" s="50"/>
+      <c r="B493" s="7" t="s">
+        <v>380</v>
+      </c>
+    </row>
+    <row r="494" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A494" s="50"/>
+      <c r="B494" s="7" t="s">
+        <v>381</v>
+      </c>
+    </row>
+    <row r="495" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A495" s="50"/>
+      <c r="B495" s="34" t="s">
+        <v>382</v>
+      </c>
+    </row>
+    <row r="496" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A496" s="50"/>
+      <c r="B496" s="7" t="s">
+        <v>383</v>
+      </c>
+    </row>
+    <row r="497" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A497" s="50"/>
+      <c r="B497" s="34" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="498" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A498" s="50"/>
+      <c r="B498" s="7" t="s">
+        <v>385</v>
+      </c>
+    </row>
+    <row r="499" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A499" s="50"/>
+      <c r="B499" s="34" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="500" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A500" s="50"/>
+      <c r="B500" s="7" t="s">
+        <v>386</v>
+      </c>
+    </row>
+    <row r="501" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A501" s="51"/>
+      <c r="B501" s="42"/>
+    </row>
   </sheetData>
-  <mergeCells count="40">
-    <mergeCell ref="A454:A465"/>
-    <mergeCell ref="A467:A488"/>
-    <mergeCell ref="A297:A309"/>
-    <mergeCell ref="A276:A295"/>
-    <mergeCell ref="A356:A364"/>
-    <mergeCell ref="A330:A342"/>
-    <mergeCell ref="A104:A109"/>
-    <mergeCell ref="A56:A62"/>
-    <mergeCell ref="A48:A54"/>
-    <mergeCell ref="A97:A102"/>
-    <mergeCell ref="A88:A95"/>
-    <mergeCell ref="A81:A86"/>
-    <mergeCell ref="A2:A6"/>
-    <mergeCell ref="A37:A46"/>
-    <mergeCell ref="A29:A35"/>
-    <mergeCell ref="A16:A27"/>
-    <mergeCell ref="A8:A14"/>
-    <mergeCell ref="A64:A78"/>
-    <mergeCell ref="A311:A318"/>
-    <mergeCell ref="A126:A132"/>
-    <mergeCell ref="A189:A196"/>
-    <mergeCell ref="A174:A187"/>
-    <mergeCell ref="A159:A172"/>
-    <mergeCell ref="A146:A156"/>
-    <mergeCell ref="A134:A144"/>
-    <mergeCell ref="A262:A274"/>
-    <mergeCell ref="A230:A237"/>
-    <mergeCell ref="A239:A246"/>
-    <mergeCell ref="A198:A215"/>
-    <mergeCell ref="A118:A124"/>
+  <mergeCells count="41">
+    <mergeCell ref="A490:A501"/>
     <mergeCell ref="A111:A116"/>
     <mergeCell ref="A217:A228"/>
     <mergeCell ref="A248:A260"/>
@@ -22203,6 +22968,36 @@
     <mergeCell ref="A320:A328"/>
     <mergeCell ref="A366:A378"/>
     <mergeCell ref="A344:A354"/>
+    <mergeCell ref="A262:A274"/>
+    <mergeCell ref="A230:A237"/>
+    <mergeCell ref="A239:A246"/>
+    <mergeCell ref="A198:A215"/>
+    <mergeCell ref="A118:A124"/>
+    <mergeCell ref="A126:A132"/>
+    <mergeCell ref="A189:A196"/>
+    <mergeCell ref="A174:A187"/>
+    <mergeCell ref="A159:A172"/>
+    <mergeCell ref="A146:A156"/>
+    <mergeCell ref="A134:A144"/>
+    <mergeCell ref="A2:A6"/>
+    <mergeCell ref="A37:A46"/>
+    <mergeCell ref="A29:A35"/>
+    <mergeCell ref="A16:A27"/>
+    <mergeCell ref="A8:A14"/>
+    <mergeCell ref="A104:A109"/>
+    <mergeCell ref="A56:A62"/>
+    <mergeCell ref="A48:A54"/>
+    <mergeCell ref="A97:A102"/>
+    <mergeCell ref="A88:A95"/>
+    <mergeCell ref="A81:A86"/>
+    <mergeCell ref="A64:A78"/>
+    <mergeCell ref="A454:A465"/>
+    <mergeCell ref="A467:A488"/>
+    <mergeCell ref="A297:A309"/>
+    <mergeCell ref="A276:A295"/>
+    <mergeCell ref="A356:A364"/>
+    <mergeCell ref="A330:A342"/>
+    <mergeCell ref="A311:A318"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Atualizado o ex041 e planilha
</commit_message>
<xml_diff>
--- a/detalhesPython.xlsx
+++ b/detalhesPython.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\thiag\Documents\EstudosT\python\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E886344-1C6C-49FC-B6A8-2482E2348FE5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF1C2B1C-86B4-4F4A-A8F8-CABA0FB3A9F9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{ECBDB9F7-0FAD-476C-A4A4-7948F29B869E}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="429" uniqueCount="387">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="447" uniqueCount="402">
   <si>
     <t>Descrição</t>
   </si>
@@ -18851,6 +18851,1086 @@
         <family val="3"/>
       </rPr>
       <t>(media))</t>
+    </r>
+  </si>
+  <si>
+    <t>ex041</t>
+  </si>
+  <si>
+    <t>A Confederação Nacional de Natação precisa de um programa que leia o ano de nascimento de um atleta e mostre sua categoria, de acordo com a idade:</t>
+  </si>
+  <si>
+    <r>
+      <t>print</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>(</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE7DE79"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>'</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>\033</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE7DE79"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>[34m-=</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>\033</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE7DE79"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>[m'</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>*</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF78D1E1"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>16</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>print</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>(</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE7DE79"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>'</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>\033</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE7DE79"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>[4;33mConfederação Nacional de Natação</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>\033</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE7DE79"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>[m'</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">nascimento </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>=</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color rgb="FF988BC7"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>int</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>(</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF988BC7"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>input</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>(</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE7DE79"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>'Ano de nascimento: '</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>))</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">idade </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>=</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> date.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF67E480"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>today</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">().year </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>-</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> nascimento</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>if</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> idade </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>&lt;=</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF78D1E1"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>9</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>:</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">    </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF988BC7"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>print</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>(</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE7DE79"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>'</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF78D1E1"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>{}</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE7DE79"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> Anos - Categoria: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>\033</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE7DE79"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>[35mMIRIM</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>\033</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE7DE79"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>[m'</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF67E480"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>format</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>(idade))</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>elif</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> idade </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>&lt;=</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF78D1E1"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>14</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>:</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">    </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF988BC7"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>print</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>(</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE7DE79"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>'</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF78D1E1"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>{}</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE7DE79"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> Anos - Categoria: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>\033</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE7DE79"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>[36mINFANTIL</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>\033</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE7DE79"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>[m'</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF67E480"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>format</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>(idade))</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>elif</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> idade </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>&lt;=</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF78D1E1"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>19</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>:</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">    </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF988BC7"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>print</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>(</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE7DE79"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>'</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF78D1E1"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>{}</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE7DE79"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> Anos - Categoria: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>\033</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE7DE79"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>[32mJUNIOR</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>\033</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE7DE79"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>[m'</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF67E480"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>format</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>(idade))</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>elif</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> idade </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>&lt;=</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF78D1E1"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>25</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>:</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">    </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF988BC7"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>print</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>(</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE7DE79"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>'</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF78D1E1"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>{}</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE7DE79"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> Anos - Categoria: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>\033</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE7DE79"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>[34mSENIOR</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>\033</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE7DE79"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>[m'</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF67E480"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>format</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>(idade))</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">    </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF988BC7"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>print</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>(</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE7DE79"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>'</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF78D1E1"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>{}</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE7DE79"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> Anos - Categoria: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>\033</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE7DE79"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>[31mMASTER</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>\033</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE7DE79"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>[m'</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF67E480"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>format</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>(idade))</t>
     </r>
   </si>
 </sst>
@@ -20081,10 +21161,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{73331524-72FC-41A3-82E6-4326A0999772}">
-  <dimension ref="A1:G501"/>
+  <dimension ref="A1:G521"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A488" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B490" sqref="B490"/>
+    <sheetView tabSelected="1" topLeftCell="A501" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B503" sqref="B503"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -22955,8 +24035,147 @@
       <c r="A501" s="51"/>
       <c r="B501" s="42"/>
     </row>
+    <row r="502" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="503" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A503" s="49" t="s">
+        <v>387</v>
+      </c>
+      <c r="B503" s="31" t="s">
+        <v>388</v>
+      </c>
+    </row>
+    <row r="504" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A504" s="50"/>
+      <c r="B504" s="40"/>
+    </row>
+    <row r="505" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A505" s="50"/>
+      <c r="B505" s="34" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="506" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A506" s="50"/>
+      <c r="B506" s="11" t="s">
+        <v>389</v>
+      </c>
+    </row>
+    <row r="507" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A507" s="50"/>
+      <c r="B507" s="11" t="s">
+        <v>390</v>
+      </c>
+    </row>
+    <row r="508" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A508" s="50"/>
+      <c r="B508" s="11" t="s">
+        <v>389</v>
+      </c>
+    </row>
+    <row r="509" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A509" s="50"/>
+      <c r="B509" s="7" t="s">
+        <v>391</v>
+      </c>
+    </row>
+    <row r="510" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A510" s="50"/>
+      <c r="B510" s="7" t="s">
+        <v>392</v>
+      </c>
+    </row>
+    <row r="511" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A511" s="50"/>
+      <c r="B511" s="34" t="s">
+        <v>393</v>
+      </c>
+    </row>
+    <row r="512" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A512" s="50"/>
+      <c r="B512" s="7" t="s">
+        <v>394</v>
+      </c>
+    </row>
+    <row r="513" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A513" s="50"/>
+      <c r="B513" s="34" t="s">
+        <v>395</v>
+      </c>
+    </row>
+    <row r="514" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A514" s="50"/>
+      <c r="B514" s="7" t="s">
+        <v>396</v>
+      </c>
+    </row>
+    <row r="515" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A515" s="50"/>
+      <c r="B515" s="34" t="s">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="516" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A516" s="50"/>
+      <c r="B516" s="7" t="s">
+        <v>398</v>
+      </c>
+    </row>
+    <row r="517" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A517" s="50"/>
+      <c r="B517" s="34" t="s">
+        <v>399</v>
+      </c>
+    </row>
+    <row r="518" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A518" s="50"/>
+      <c r="B518" s="7" t="s">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="519" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A519" s="50"/>
+      <c r="B519" s="34" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="520" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A520" s="50"/>
+      <c r="B520" s="7" t="s">
+        <v>401</v>
+      </c>
+    </row>
+    <row r="521" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A521" s="51"/>
+      <c r="B521" s="42"/>
+    </row>
   </sheetData>
-  <mergeCells count="41">
+  <mergeCells count="42">
+    <mergeCell ref="A503:A521"/>
+    <mergeCell ref="A454:A465"/>
+    <mergeCell ref="A467:A488"/>
+    <mergeCell ref="A297:A309"/>
+    <mergeCell ref="A276:A295"/>
+    <mergeCell ref="A356:A364"/>
+    <mergeCell ref="A330:A342"/>
+    <mergeCell ref="A311:A318"/>
+    <mergeCell ref="A104:A109"/>
+    <mergeCell ref="A56:A62"/>
+    <mergeCell ref="A48:A54"/>
+    <mergeCell ref="A97:A102"/>
+    <mergeCell ref="A88:A95"/>
+    <mergeCell ref="A81:A86"/>
+    <mergeCell ref="A64:A78"/>
+    <mergeCell ref="A2:A6"/>
+    <mergeCell ref="A37:A46"/>
+    <mergeCell ref="A29:A35"/>
+    <mergeCell ref="A16:A27"/>
+    <mergeCell ref="A8:A14"/>
+    <mergeCell ref="A126:A132"/>
+    <mergeCell ref="A189:A196"/>
+    <mergeCell ref="A174:A187"/>
+    <mergeCell ref="A159:A172"/>
+    <mergeCell ref="A146:A156"/>
+    <mergeCell ref="A134:A144"/>
     <mergeCell ref="A490:A501"/>
     <mergeCell ref="A111:A116"/>
     <mergeCell ref="A217:A228"/>
@@ -22973,31 +24192,6 @@
     <mergeCell ref="A239:A246"/>
     <mergeCell ref="A198:A215"/>
     <mergeCell ref="A118:A124"/>
-    <mergeCell ref="A126:A132"/>
-    <mergeCell ref="A189:A196"/>
-    <mergeCell ref="A174:A187"/>
-    <mergeCell ref="A159:A172"/>
-    <mergeCell ref="A146:A156"/>
-    <mergeCell ref="A134:A144"/>
-    <mergeCell ref="A2:A6"/>
-    <mergeCell ref="A37:A46"/>
-    <mergeCell ref="A29:A35"/>
-    <mergeCell ref="A16:A27"/>
-    <mergeCell ref="A8:A14"/>
-    <mergeCell ref="A104:A109"/>
-    <mergeCell ref="A56:A62"/>
-    <mergeCell ref="A48:A54"/>
-    <mergeCell ref="A97:A102"/>
-    <mergeCell ref="A88:A95"/>
-    <mergeCell ref="A81:A86"/>
-    <mergeCell ref="A64:A78"/>
-    <mergeCell ref="A454:A465"/>
-    <mergeCell ref="A467:A488"/>
-    <mergeCell ref="A297:A309"/>
-    <mergeCell ref="A276:A295"/>
-    <mergeCell ref="A356:A364"/>
-    <mergeCell ref="A330:A342"/>
-    <mergeCell ref="A311:A318"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Atualizado o ex043 e planilha
</commit_message>
<xml_diff>
--- a/detalhesPython.xlsx
+++ b/detalhesPython.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\thiag\Documents\EstudosT\python\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97DFCC82-78E8-4C9E-A963-8A2EBB7DBD99}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1B05D34-726C-4EFF-89A0-F5CE9A8220AA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{ECBDB9F7-0FAD-476C-A4A4-7948F29B869E}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="467" uniqueCount="415">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="482" uniqueCount="428">
   <si>
     <t>Descrição</t>
   </si>
@@ -20460,6 +20460,917 @@
   </si>
   <si>
     <t>Refaça o DESAFIO 35 dos triângulos, acrescentando o recurso de mostrar que tipo de triângulo será formado:</t>
+  </si>
+  <si>
+    <t>Desenvolva uma lógica que leia o peso e a altura de uma pessoa, calcule seu Índice de Massa Corporal (IMC) e mostre seu status, de acordo com a tabela abaixo:</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">altura </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>=</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color rgb="FF988BC7"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>float</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>(</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF988BC7"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>input</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>(</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE7DE79"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>'Digite sua altura: '</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>))</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">peso </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>=</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color rgb="FF988BC7"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>float</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>(</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF988BC7"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>input</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>(</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE7DE79"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>'Digite seu peso: '</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>))</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">imc </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>=</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> peso </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>/</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> (altura </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>**</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF78D1E1"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>2</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>if</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> imc </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>&lt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF78D1E1"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>18.5</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>:</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">    </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF988BC7"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>print</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>(</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE7DE79"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">'IMC: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF78D1E1"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>{</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>:.1f</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF78D1E1"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>}</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE7DE79"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> - Abaixo do peso.'</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF67E480"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>format</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>(imc))</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>elif</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> imc </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>&lt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF78D1E1"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>25</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>:</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">    </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF988BC7"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>print</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>(</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE7DE79"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">'IMC: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF78D1E1"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>{</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>:.1f</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF78D1E1"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>}</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE7DE79"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> - Peso ideal, PARABÉNS!.'</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF67E480"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>format</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>(imc))</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>elif</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> imc </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>&lt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF78D1E1"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>30</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>:</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">    </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF988BC7"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>print</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>(</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE7DE79"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">'IMC: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF78D1E1"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>{</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>:.1f</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF78D1E1"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>}</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE7DE79"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> - Sobrepeso.'</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF67E480"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>format</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>(imc))</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>elif</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> imc </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>&lt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF78D1E1"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>40</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>:</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">    </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF988BC7"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>print</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>(</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE7DE79"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">'IMC: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF78D1E1"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>{</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>:.1f</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF78D1E1"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>}</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE7DE79"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> - Obesidade.'</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF67E480"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>format</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>(imc))</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">    </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF988BC7"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>print</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>(</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE7DE79"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">'IMC: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF78D1E1"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>{</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>:.1f</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF78D1E1"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>}</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE7DE79"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> - Obesidade Mórbida! CUIDADO!'</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF67E480"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>format</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>(imc))</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -21696,10 +22607,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{73331524-72FC-41A3-82E6-4326A0999772}">
-  <dimension ref="A1:G544"/>
+  <dimension ref="A1:G561"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A518" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A523" sqref="A523:A544"/>
+    <sheetView tabSelected="1" topLeftCell="A542" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="A546" sqref="A546:A561"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -24812,8 +25723,131 @@
       <c r="A544" s="51"/>
       <c r="B544" s="42"/>
     </row>
+    <row r="545" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="546" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A546" s="49" t="s">
+        <v>402</v>
+      </c>
+      <c r="B546" s="31" t="s">
+        <v>415</v>
+      </c>
+    </row>
+    <row r="547" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A547" s="50"/>
+      <c r="B547" s="40"/>
+    </row>
+    <row r="548" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A548" s="50"/>
+      <c r="B548" s="7" t="s">
+        <v>416</v>
+      </c>
+    </row>
+    <row r="549" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A549" s="50"/>
+      <c r="B549" s="7" t="s">
+        <v>417</v>
+      </c>
+    </row>
+    <row r="550" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A550" s="50"/>
+      <c r="B550" s="7" t="s">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="551" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A551" s="50"/>
+      <c r="B551" s="34" t="s">
+        <v>419</v>
+      </c>
+    </row>
+    <row r="552" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A552" s="50"/>
+      <c r="B552" s="7" t="s">
+        <v>420</v>
+      </c>
+    </row>
+    <row r="553" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A553" s="50"/>
+      <c r="B553" s="34" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="554" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A554" s="50"/>
+      <c r="B554" s="7" t="s">
+        <v>422</v>
+      </c>
+    </row>
+    <row r="555" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A555" s="50"/>
+      <c r="B555" s="34" t="s">
+        <v>423</v>
+      </c>
+    </row>
+    <row r="556" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A556" s="50"/>
+      <c r="B556" s="7" t="s">
+        <v>424</v>
+      </c>
+    </row>
+    <row r="557" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A557" s="50"/>
+      <c r="B557" s="34" t="s">
+        <v>425</v>
+      </c>
+    </row>
+    <row r="558" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A558" s="50"/>
+      <c r="B558" s="7" t="s">
+        <v>426</v>
+      </c>
+    </row>
+    <row r="559" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A559" s="50"/>
+      <c r="B559" s="34" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="560" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A560" s="50"/>
+      <c r="B560" s="7" t="s">
+        <v>427</v>
+      </c>
+    </row>
+    <row r="561" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A561" s="51"/>
+      <c r="B561" s="42"/>
+    </row>
   </sheetData>
-  <mergeCells count="43">
+  <mergeCells count="44">
+    <mergeCell ref="A546:A561"/>
+    <mergeCell ref="A503:A521"/>
+    <mergeCell ref="A454:A465"/>
+    <mergeCell ref="A467:A488"/>
+    <mergeCell ref="A297:A309"/>
+    <mergeCell ref="A276:A295"/>
+    <mergeCell ref="A356:A364"/>
+    <mergeCell ref="A330:A342"/>
+    <mergeCell ref="A311:A318"/>
+    <mergeCell ref="A490:A501"/>
+    <mergeCell ref="A104:A109"/>
+    <mergeCell ref="A56:A62"/>
+    <mergeCell ref="A48:A54"/>
+    <mergeCell ref="A97:A102"/>
+    <mergeCell ref="A88:A95"/>
+    <mergeCell ref="A81:A86"/>
+    <mergeCell ref="A64:A78"/>
+    <mergeCell ref="A2:A6"/>
+    <mergeCell ref="A37:A46"/>
+    <mergeCell ref="A29:A35"/>
+    <mergeCell ref="A16:A27"/>
+    <mergeCell ref="A8:A14"/>
+    <mergeCell ref="A126:A132"/>
+    <mergeCell ref="A189:A196"/>
+    <mergeCell ref="A174:A187"/>
+    <mergeCell ref="A159:A172"/>
+    <mergeCell ref="A146:A156"/>
+    <mergeCell ref="A134:A144"/>
     <mergeCell ref="A523:A544"/>
     <mergeCell ref="A111:A116"/>
     <mergeCell ref="A217:A228"/>
@@ -24830,33 +25864,6 @@
     <mergeCell ref="A239:A246"/>
     <mergeCell ref="A198:A215"/>
     <mergeCell ref="A118:A124"/>
-    <mergeCell ref="A126:A132"/>
-    <mergeCell ref="A189:A196"/>
-    <mergeCell ref="A174:A187"/>
-    <mergeCell ref="A159:A172"/>
-    <mergeCell ref="A146:A156"/>
-    <mergeCell ref="A134:A144"/>
-    <mergeCell ref="A2:A6"/>
-    <mergeCell ref="A37:A46"/>
-    <mergeCell ref="A29:A35"/>
-    <mergeCell ref="A16:A27"/>
-    <mergeCell ref="A8:A14"/>
-    <mergeCell ref="A104:A109"/>
-    <mergeCell ref="A56:A62"/>
-    <mergeCell ref="A48:A54"/>
-    <mergeCell ref="A97:A102"/>
-    <mergeCell ref="A88:A95"/>
-    <mergeCell ref="A81:A86"/>
-    <mergeCell ref="A64:A78"/>
-    <mergeCell ref="A503:A521"/>
-    <mergeCell ref="A454:A465"/>
-    <mergeCell ref="A467:A488"/>
-    <mergeCell ref="A297:A309"/>
-    <mergeCell ref="A276:A295"/>
-    <mergeCell ref="A356:A364"/>
-    <mergeCell ref="A330:A342"/>
-    <mergeCell ref="A311:A318"/>
-    <mergeCell ref="A490:A501"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Atualizado ex044 e planilha
</commit_message>
<xml_diff>
--- a/detalhesPython.xlsx
+++ b/detalhesPython.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\thiag\Documents\EstudosT\python\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Thiago Henrique\Documents\EstudosT\python\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1B05D34-726C-4EFF-89A0-F5CE9A8220AA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A641DB1-D3A2-4FE9-B15D-C7E07D05B4F5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{ECBDB9F7-0FAD-476C-A4A4-7948F29B869E}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="15750" xr2:uid="{ECBDB9F7-0FAD-476C-A4A4-7948F29B869E}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="482" uniqueCount="428">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="503" uniqueCount="449">
   <si>
     <t>Descrição</t>
   </si>
@@ -21370,6 +21370,2147 @@
         <family val="3"/>
       </rPr>
       <t>(imc))</t>
+    </r>
+  </si>
+  <si>
+    <t>ex043</t>
+  </si>
+  <si>
+    <t>Elabore um programa que calcule o valor a ser pago por um produto, considerando o seu preço normal e condição de pagamento:</t>
+  </si>
+  <si>
+    <r>
+      <t>print</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>(</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE7DE79"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>' LOJAS CAMPONÊZ '</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF67E480"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>center</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>(</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF78D1E1"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>30</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE7DE79"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>'='</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>))</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">preçoNormal </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>=</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color rgb="FF988BC7"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>float</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>(</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF988BC7"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>input</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>(</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE7DE79"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>'Valor dos produtos: '</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>))</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>print</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>(</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE7DE79"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>'</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>\n</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE7DE79"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>Valor do produto: R$</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF78D1E1"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>{</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>:.2f</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF78D1E1"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>}</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE7DE79"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>'</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF67E480"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>format</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">(preçoNormal), </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color rgb="FFE89E64"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>end</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>=</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE7DE79"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>' '</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>if</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> condPagamento </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>==</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF78D1E1"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>1</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>:</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">    </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF988BC7"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>print</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>(</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE7DE79"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>', Valor com 10</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF78D1E1"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>% d</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE7DE79"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>e desconto: R$</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF78D1E1"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>{</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>:.2f</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF78D1E1"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>}</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>\n</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE7DE79"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>'</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF67E480"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>format</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">(preçoNormal </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>-</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> (preçoNormal </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>*</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF78D1E1"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>10</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>/</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF78D1E1"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>100</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>)))</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>elif</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> condPagamento </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>==</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF78D1E1"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>2</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>:</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">    </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF988BC7"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>print</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>(</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE7DE79"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>', Valor com 5</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF78D1E1"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>% d</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE7DE79"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>e desconto: R$</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF78D1E1"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>{</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>:.2f</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF78D1E1"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>}</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>\n</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE7DE79"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>'</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF67E480"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>format</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">(preçoNormal </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>-</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> (preçoNormal </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>*</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF78D1E1"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>5</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>/</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF78D1E1"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>100</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>)))</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>elif</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> condPagamento </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>==</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF78D1E1"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>3</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>:</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">    parcelas </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>=</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color rgb="FF988BC7"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>int</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>(</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF988BC7"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>input</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>(</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE7DE79"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>', Quantas vezes: '</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>))</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">    </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>if</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> parcelas </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>==</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF78D1E1"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>1</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>:</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">        </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF988BC7"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>print</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>(</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE7DE79"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>'</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>\n</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE7DE79"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>Valor normal: R$</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF78D1E1"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>{</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>:.2f</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF78D1E1"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>}</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE7DE79"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>'</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF67E480"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>format</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>(preçoNormal))</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">    </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>elif</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> parcelas </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>==</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF78D1E1"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>2</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>:</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">        </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF988BC7"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>print</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>(</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE7DE79"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>'</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>\n</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE7DE79"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>Então ficará 2x de R$</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF78D1E1"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>{</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>:.2f</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF78D1E1"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>}</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE7DE79"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>'</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF67E480"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>format</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">(preçoNormal </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>/</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF78D1E1"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>2</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>))</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>elif</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> condPagamento </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>==</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF78D1E1"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>4</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>:</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">    pcJuros </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>=</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> preçoNormal </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> (preçoNormal </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>*</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF78D1E1"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>20</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>/</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF78D1E1"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>100</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">    </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF988BC7"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>print</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>(</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE7DE79"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>', Valor com 20</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF78D1E1"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>% d</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE7DE79"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>e juros ficará: R$</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF78D1E1"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>{</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>:.2f</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF78D1E1"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>}</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE7DE79"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>'</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF67E480"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>format</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>(pcJuros))</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">    parcelas </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>=</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color rgb="FF988BC7"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>int</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>(</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF988BC7"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>input</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>(</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE7DE79"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>'</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>\n</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE7DE79"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>Quantas parcelas: '</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>))</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">    </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF988BC7"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>print</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>(</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE7DE79"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>'</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>\n</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE7DE79"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">Então ficará </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF78D1E1"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>{}</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE7DE79"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> parcelas de R$</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF78D1E1"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>{</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>:.2f</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF78D1E1"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>}</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE7DE79"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>, Total de R$</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF78D1E1"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>{</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>:.2f</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF78D1E1"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>}</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE7DE79"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>'</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF67E480"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>format</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">(parcelas, pcJuros </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>/</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> parcelas, pcJuros))</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">condPagamento </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>=</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color rgb="FF988BC7"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>int</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>(</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF988BC7"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>input</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>(</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE7DE79"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>'</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>\n</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE7DE79"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>[1] À Vista dinheiro/cheque - 10</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF78D1E1"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>% d</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE7DE79"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>e desconto</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>\n</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE7DE79"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>[2] À Vista no cartão de débito - 5</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF78D1E1"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>% d</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE7DE79"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>e desconto</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">\n
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE7DE79"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>[3] Em até 2x no cartão de crédito - Valor normal</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>\n</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE7DE79"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>[4] 3x ou mais no cartão de crédito - 20</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF78D1E1"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>% d</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE7DE79"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>e Juros</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>\n\n</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE7DE79"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>Informe a condição de pagamento: '</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>))</t>
     </r>
   </si>
 </sst>
@@ -22096,7 +24237,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>235325</xdr:colOff>
+      <xdr:colOff>235324</xdr:colOff>
       <xdr:row>392</xdr:row>
       <xdr:rowOff>27461</xdr:rowOff>
     </xdr:to>
@@ -22140,7 +24281,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>16</xdr:col>
-      <xdr:colOff>456170</xdr:colOff>
+      <xdr:colOff>456171</xdr:colOff>
       <xdr:row>392</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
@@ -22184,7 +24325,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>313764</xdr:colOff>
+      <xdr:colOff>313763</xdr:colOff>
       <xdr:row>406</xdr:row>
       <xdr:rowOff>33618</xdr:rowOff>
     </xdr:to>
@@ -22607,16 +24748,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{73331524-72FC-41A3-82E6-4326A0999772}">
-  <dimension ref="A1:G561"/>
+  <dimension ref="A1:G584"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A542" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A546" sqref="A546:A561"/>
+    <sheetView tabSelected="1" topLeftCell="A548" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="D565" sqref="D565"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9.85546875" style="2" customWidth="1"/>
-    <col min="2" max="2" width="166" style="2" customWidth="1"/>
+    <col min="2" max="2" width="168.140625" style="2" customWidth="1"/>
     <col min="3" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
@@ -25818,37 +27959,140 @@
       <c r="A561" s="51"/>
       <c r="B561" s="42"/>
     </row>
+    <row r="562" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="563" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A563" s="49" t="s">
+        <v>428</v>
+      </c>
+      <c r="B563" s="31" t="s">
+        <v>429</v>
+      </c>
+    </row>
+    <row r="564" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A564" s="50"/>
+      <c r="B564" s="40"/>
+    </row>
+    <row r="565" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A565" s="50"/>
+      <c r="B565" s="11" t="s">
+        <v>430</v>
+      </c>
+    </row>
+    <row r="566" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A566" s="50"/>
+      <c r="B566" s="7" t="s">
+        <v>431</v>
+      </c>
+    </row>
+    <row r="567" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+      <c r="A567" s="50"/>
+      <c r="B567" s="44" t="s">
+        <v>448</v>
+      </c>
+    </row>
+    <row r="568" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A568" s="50"/>
+      <c r="B568" s="11" t="s">
+        <v>432</v>
+      </c>
+    </row>
+    <row r="569" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A569" s="50"/>
+      <c r="B569" s="34" t="s">
+        <v>433</v>
+      </c>
+    </row>
+    <row r="570" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A570" s="50"/>
+      <c r="B570" s="7" t="s">
+        <v>434</v>
+      </c>
+    </row>
+    <row r="571" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A571" s="50"/>
+      <c r="B571" s="34" t="s">
+        <v>435</v>
+      </c>
+    </row>
+    <row r="572" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A572" s="50"/>
+      <c r="B572" s="7" t="s">
+        <v>436</v>
+      </c>
+    </row>
+    <row r="573" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A573" s="50"/>
+      <c r="B573" s="34" t="s">
+        <v>437</v>
+      </c>
+    </row>
+    <row r="574" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A574" s="50"/>
+      <c r="B574" s="7" t="s">
+        <v>438</v>
+      </c>
+    </row>
+    <row r="575" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A575" s="50"/>
+      <c r="B575" s="7" t="s">
+        <v>439</v>
+      </c>
+    </row>
+    <row r="576" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A576" s="50"/>
+      <c r="B576" s="7" t="s">
+        <v>440</v>
+      </c>
+    </row>
+    <row r="577" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A577" s="50"/>
+      <c r="B577" s="7" t="s">
+        <v>441</v>
+      </c>
+    </row>
+    <row r="578" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A578" s="50"/>
+      <c r="B578" s="7" t="s">
+        <v>442</v>
+      </c>
+    </row>
+    <row r="579" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A579" s="50"/>
+      <c r="B579" s="34" t="s">
+        <v>443</v>
+      </c>
+    </row>
+    <row r="580" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A580" s="50"/>
+      <c r="B580" s="7" t="s">
+        <v>444</v>
+      </c>
+    </row>
+    <row r="581" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A581" s="50"/>
+      <c r="B581" s="7" t="s">
+        <v>445</v>
+      </c>
+    </row>
+    <row r="582" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A582" s="50"/>
+      <c r="B582" s="7" t="s">
+        <v>446</v>
+      </c>
+    </row>
+    <row r="583" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A583" s="50"/>
+      <c r="B583" s="7" t="s">
+        <v>447</v>
+      </c>
+    </row>
+    <row r="584" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A584" s="51"/>
+      <c r="B584" s="42"/>
+    </row>
   </sheetData>
-  <mergeCells count="44">
-    <mergeCell ref="A546:A561"/>
-    <mergeCell ref="A503:A521"/>
-    <mergeCell ref="A454:A465"/>
-    <mergeCell ref="A467:A488"/>
-    <mergeCell ref="A297:A309"/>
-    <mergeCell ref="A276:A295"/>
-    <mergeCell ref="A356:A364"/>
-    <mergeCell ref="A330:A342"/>
-    <mergeCell ref="A311:A318"/>
-    <mergeCell ref="A490:A501"/>
-    <mergeCell ref="A104:A109"/>
-    <mergeCell ref="A56:A62"/>
-    <mergeCell ref="A48:A54"/>
-    <mergeCell ref="A97:A102"/>
-    <mergeCell ref="A88:A95"/>
-    <mergeCell ref="A81:A86"/>
-    <mergeCell ref="A64:A78"/>
-    <mergeCell ref="A2:A6"/>
-    <mergeCell ref="A37:A46"/>
-    <mergeCell ref="A29:A35"/>
-    <mergeCell ref="A16:A27"/>
-    <mergeCell ref="A8:A14"/>
-    <mergeCell ref="A126:A132"/>
-    <mergeCell ref="A189:A196"/>
-    <mergeCell ref="A174:A187"/>
-    <mergeCell ref="A159:A172"/>
-    <mergeCell ref="A146:A156"/>
-    <mergeCell ref="A134:A144"/>
-    <mergeCell ref="A523:A544"/>
+  <mergeCells count="45">
+    <mergeCell ref="A563:A584"/>
     <mergeCell ref="A111:A116"/>
     <mergeCell ref="A217:A228"/>
     <mergeCell ref="A248:A260"/>
@@ -25864,6 +28108,35 @@
     <mergeCell ref="A239:A246"/>
     <mergeCell ref="A198:A215"/>
     <mergeCell ref="A118:A124"/>
+    <mergeCell ref="A126:A132"/>
+    <mergeCell ref="A189:A196"/>
+    <mergeCell ref="A174:A187"/>
+    <mergeCell ref="A159:A172"/>
+    <mergeCell ref="A146:A156"/>
+    <mergeCell ref="A134:A144"/>
+    <mergeCell ref="A2:A6"/>
+    <mergeCell ref="A37:A46"/>
+    <mergeCell ref="A29:A35"/>
+    <mergeCell ref="A16:A27"/>
+    <mergeCell ref="A8:A14"/>
+    <mergeCell ref="A104:A109"/>
+    <mergeCell ref="A56:A62"/>
+    <mergeCell ref="A48:A54"/>
+    <mergeCell ref="A97:A102"/>
+    <mergeCell ref="A88:A95"/>
+    <mergeCell ref="A81:A86"/>
+    <mergeCell ref="A64:A78"/>
+    <mergeCell ref="A276:A295"/>
+    <mergeCell ref="A356:A364"/>
+    <mergeCell ref="A330:A342"/>
+    <mergeCell ref="A311:A318"/>
+    <mergeCell ref="A490:A501"/>
+    <mergeCell ref="A546:A561"/>
+    <mergeCell ref="A503:A521"/>
+    <mergeCell ref="A454:A465"/>
+    <mergeCell ref="A467:A488"/>
+    <mergeCell ref="A297:A309"/>
+    <mergeCell ref="A523:A544"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Atualizado o ex045 e planilha
</commit_message>
<xml_diff>
--- a/detalhesPython.xlsx
+++ b/detalhesPython.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Thiago Henrique\Documents\EstudosT\python\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A641DB1-D3A2-4FE9-B15D-C7E07D05B4F5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44B16CF9-4D56-4700-BC7F-AAB7FA88A7B6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="15750" xr2:uid="{ECBDB9F7-0FAD-476C-A4A4-7948F29B869E}"/>
+    <workbookView xWindow="-28920" yWindow="15" windowWidth="29040" windowHeight="15990" xr2:uid="{ECBDB9F7-0FAD-476C-A4A4-7948F29B869E}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="503" uniqueCount="449">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="552" uniqueCount="481">
   <si>
     <t>Descrição</t>
   </si>
@@ -23511,6 +23511,1300 @@
         <family val="3"/>
       </rPr>
       <t>))</t>
+    </r>
+  </si>
+  <si>
+    <t>ex045</t>
+  </si>
+  <si>
+    <t>ex044</t>
+  </si>
+  <si>
+    <t>Crie um programa que faça o computador jogar Jokenpô com você.</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">itens </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>=</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> (</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE7DE79"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>'Pedra'</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE7DE79"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>'Papel'</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE7DE79"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>'Tesoura'</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">computador </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>=</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF67E480"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>randint</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>(</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF78D1E1"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>0</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF78D1E1"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>2</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>print</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>(</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE7DE79"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>'''Suas opções:</t>
+    </r>
+  </si>
+  <si>
+    <t>[ 0 ] PEDRA</t>
+  </si>
+  <si>
+    <t>[ 1 ] PAPEL</t>
+  </si>
+  <si>
+    <r>
+      <t>[ 2 ] TESOURA'''</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">jogador </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>=</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color rgb="FF988BC7"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>int</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>(</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF988BC7"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>input</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>(</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE7DE79"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>'Qual é a sua jogada? '</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>))</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>print</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>(</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE7DE79"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>'JO'</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>sleep</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>(</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF78D1E1"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>1</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>print</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>(</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE7DE79"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>'KEN'</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>print</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>(</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE7DE79"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>'PO!!!'</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>print</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>(</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE7DE79"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>'-='</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>*</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF78D1E1"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>11</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>print</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>(</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE7DE79"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">'Jogador    --&gt; </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF78D1E1"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>{}</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE7DE79"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>'</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF67E480"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>format</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>(itens[jogador]))</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>print</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>(</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE7DE79"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">'Computador --&gt; </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF78D1E1"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>{}</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE7DE79"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>'</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF67E480"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>format</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>(itens[computador]))</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>if</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> computador </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>==</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF78D1E1"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>0</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>:</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">    </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>if</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> jogador </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>==</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF78D1E1"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>0</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>:</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">        </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF988BC7"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>print</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>(</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE7DE79"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>'EMPATE!'</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">    </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>elif</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> jogador </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>==</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF78D1E1"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>1</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>:</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">        </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF988BC7"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>print</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>(</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE7DE79"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>'Jogador VENCEU!'</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>)    </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">    </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>elif</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> jogador </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>==</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF78D1E1"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>2</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>:</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">        </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF988BC7"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>print</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>(</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE7DE79"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>'Computador VENCEU!'</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">    </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>else</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>:</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">        </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF988BC7"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>print</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>(</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE7DE79"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>'JOGADA INVÁLIDA'</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>elif</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> computador </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>==</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF78D1E1"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>1</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>:</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">        </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF988BC7"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>print</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>(</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE7DE79"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>'EMPATE!'</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>)    </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">        </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF988BC7"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>print</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>(</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE7DE79"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>'Jogador VENCEU!'</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">        </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF988BC7"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>print</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>(</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE7DE79"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>'JOGADA INVÁLIDA'</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">)       </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>elif</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> computador </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>==</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF78D1E1"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>2</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>:</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">        </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF988BC7"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>print</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>(</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE7DE79"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>'Computador VENCEU!'</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>)    </t>
     </r>
   </si>
 </sst>
@@ -24748,10 +26042,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{73331524-72FC-41A3-82E6-4326A0999772}">
-  <dimension ref="A1:G584"/>
+  <dimension ref="A1:G635"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A548" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D565" sqref="D565"/>
+    <sheetView tabSelected="1" topLeftCell="A579" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B635" sqref="A635:XFD635"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -27867,7 +29161,7 @@
     <row r="545" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="546" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A546" s="49" t="s">
-        <v>402</v>
+        <v>428</v>
       </c>
       <c r="B546" s="31" t="s">
         <v>415</v>
@@ -27962,7 +29256,7 @@
     <row r="562" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="563" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A563" s="49" t="s">
-        <v>428</v>
+        <v>450</v>
       </c>
       <c r="B563" s="31" t="s">
         <v>429</v>
@@ -27984,7 +29278,7 @@
         <v>431</v>
       </c>
     </row>
-    <row r="567" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+    <row r="567" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A567" s="50"/>
       <c r="B567" s="44" t="s">
         <v>448</v>
@@ -28090,8 +29384,337 @@
       <c r="A584" s="51"/>
       <c r="B584" s="42"/>
     </row>
+    <row r="585" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="586" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A586" s="49" t="s">
+        <v>449</v>
+      </c>
+      <c r="B586" s="31" t="s">
+        <v>451</v>
+      </c>
+    </row>
+    <row r="587" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A587" s="50"/>
+      <c r="B587" s="40"/>
+    </row>
+    <row r="588" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A588" s="50"/>
+      <c r="B588" s="34" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="589" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A589" s="50"/>
+      <c r="B589" s="34" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="590" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A590" s="50"/>
+      <c r="B590" s="7" t="s">
+        <v>452</v>
+      </c>
+    </row>
+    <row r="591" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A591" s="50"/>
+      <c r="B591" s="7" t="s">
+        <v>453</v>
+      </c>
+    </row>
+    <row r="592" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A592" s="50"/>
+      <c r="B592" s="11" t="s">
+        <v>454</v>
+      </c>
+    </row>
+    <row r="593" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A593" s="50"/>
+      <c r="B593" s="45" t="s">
+        <v>455</v>
+      </c>
+    </row>
+    <row r="594" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A594" s="50"/>
+      <c r="B594" s="45" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="595" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A595" s="50"/>
+      <c r="B595" s="45" t="s">
+        <v>457</v>
+      </c>
+    </row>
+    <row r="596" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A596" s="50"/>
+      <c r="B596" s="7" t="s">
+        <v>458</v>
+      </c>
+    </row>
+    <row r="597" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A597" s="50"/>
+      <c r="B597" s="11" t="s">
+        <v>459</v>
+      </c>
+    </row>
+    <row r="598" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A598" s="50"/>
+      <c r="B598" s="35" t="s">
+        <v>460</v>
+      </c>
+    </row>
+    <row r="599" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A599" s="50"/>
+      <c r="B599" s="11" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="600" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A600" s="50"/>
+      <c r="B600" s="35" t="s">
+        <v>460</v>
+      </c>
+    </row>
+    <row r="601" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A601" s="50"/>
+      <c r="B601" s="11" t="s">
+        <v>462</v>
+      </c>
+    </row>
+    <row r="602" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A602" s="50"/>
+      <c r="B602" s="35" t="s">
+        <v>460</v>
+      </c>
+    </row>
+    <row r="603" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A603" s="50"/>
+      <c r="B603" s="11" t="s">
+        <v>463</v>
+      </c>
+    </row>
+    <row r="604" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A604" s="50"/>
+      <c r="B604" s="11" t="s">
+        <v>464</v>
+      </c>
+    </row>
+    <row r="605" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A605" s="50"/>
+      <c r="B605" s="11" t="s">
+        <v>465</v>
+      </c>
+    </row>
+    <row r="606" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A606" s="50"/>
+      <c r="B606" s="11" t="s">
+        <v>463</v>
+      </c>
+    </row>
+    <row r="607" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A607" s="50"/>
+      <c r="B607" s="35" t="s">
+        <v>460</v>
+      </c>
+    </row>
+    <row r="608" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A608" s="50"/>
+      <c r="B608" s="34" t="s">
+        <v>466</v>
+      </c>
+    </row>
+    <row r="609" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A609" s="50"/>
+      <c r="B609" s="7" t="s">
+        <v>467</v>
+      </c>
+    </row>
+    <row r="610" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A610" s="50"/>
+      <c r="B610" s="7" t="s">
+        <v>468</v>
+      </c>
+    </row>
+    <row r="611" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A611" s="50"/>
+      <c r="B611" s="7" t="s">
+        <v>469</v>
+      </c>
+    </row>
+    <row r="612" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A612" s="50"/>
+      <c r="B612" s="7" t="s">
+        <v>470</v>
+      </c>
+    </row>
+    <row r="613" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A613" s="50"/>
+      <c r="B613" s="7" t="s">
+        <v>471</v>
+      </c>
+    </row>
+    <row r="614" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A614" s="50"/>
+      <c r="B614" s="7" t="s">
+        <v>472</v>
+      </c>
+    </row>
+    <row r="615" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A615" s="50"/>
+      <c r="B615" s="7" t="s">
+        <v>473</v>
+      </c>
+    </row>
+    <row r="616" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A616" s="50"/>
+      <c r="B616" s="7" t="s">
+        <v>474</v>
+      </c>
+    </row>
+    <row r="617" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A617" s="50"/>
+      <c r="B617" s="34" t="s">
+        <v>475</v>
+      </c>
+    </row>
+    <row r="618" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A618" s="50"/>
+      <c r="B618" s="7" t="s">
+        <v>467</v>
+      </c>
+    </row>
+    <row r="619" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A619" s="50"/>
+      <c r="B619" s="7" t="s">
+        <v>472</v>
+      </c>
+    </row>
+    <row r="620" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A620" s="50"/>
+      <c r="B620" s="7" t="s">
+        <v>469</v>
+      </c>
+    </row>
+    <row r="621" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A621" s="50"/>
+      <c r="B621" s="7" t="s">
+        <v>476</v>
+      </c>
+    </row>
+    <row r="622" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A622" s="50"/>
+      <c r="B622" s="7" t="s">
+        <v>471</v>
+      </c>
+    </row>
+    <row r="623" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A623" s="50"/>
+      <c r="B623" s="7" t="s">
+        <v>477</v>
+      </c>
+    </row>
+    <row r="624" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A624" s="50"/>
+      <c r="B624" s="7" t="s">
+        <v>473</v>
+      </c>
+    </row>
+    <row r="625" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A625" s="50"/>
+      <c r="B625" s="7" t="s">
+        <v>478</v>
+      </c>
+    </row>
+    <row r="626" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A626" s="50"/>
+      <c r="B626" s="34" t="s">
+        <v>479</v>
+      </c>
+    </row>
+    <row r="627" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A627" s="50"/>
+      <c r="B627" s="7" t="s">
+        <v>467</v>
+      </c>
+    </row>
+    <row r="628" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A628" s="50"/>
+      <c r="B628" s="7" t="s">
+        <v>477</v>
+      </c>
+    </row>
+    <row r="629" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A629" s="50"/>
+      <c r="B629" s="7" t="s">
+        <v>469</v>
+      </c>
+    </row>
+    <row r="630" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A630" s="50"/>
+      <c r="B630" s="7" t="s">
+        <v>480</v>
+      </c>
+    </row>
+    <row r="631" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A631" s="50"/>
+      <c r="B631" s="7" t="s">
+        <v>471</v>
+      </c>
+    </row>
+    <row r="632" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A632" s="50"/>
+      <c r="B632" s="7" t="s">
+        <v>468</v>
+      </c>
+    </row>
+    <row r="633" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A633" s="50"/>
+      <c r="B633" s="7" t="s">
+        <v>473</v>
+      </c>
+    </row>
+    <row r="634" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A634" s="50"/>
+      <c r="B634" s="7" t="s">
+        <v>474</v>
+      </c>
+    </row>
+    <row r="635" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A635" s="51"/>
+      <c r="B635" s="42"/>
+    </row>
   </sheetData>
-  <mergeCells count="45">
+  <mergeCells count="46">
+    <mergeCell ref="A586:A635"/>
+    <mergeCell ref="A546:A561"/>
+    <mergeCell ref="A503:A521"/>
+    <mergeCell ref="A454:A465"/>
+    <mergeCell ref="A467:A488"/>
+    <mergeCell ref="A297:A309"/>
+    <mergeCell ref="A523:A544"/>
+    <mergeCell ref="A276:A295"/>
+    <mergeCell ref="A356:A364"/>
+    <mergeCell ref="A330:A342"/>
+    <mergeCell ref="A311:A318"/>
+    <mergeCell ref="A490:A501"/>
+    <mergeCell ref="A104:A109"/>
+    <mergeCell ref="A56:A62"/>
+    <mergeCell ref="A48:A54"/>
+    <mergeCell ref="A97:A102"/>
+    <mergeCell ref="A88:A95"/>
+    <mergeCell ref="A81:A86"/>
+    <mergeCell ref="A64:A78"/>
+    <mergeCell ref="A2:A6"/>
+    <mergeCell ref="A37:A46"/>
+    <mergeCell ref="A29:A35"/>
+    <mergeCell ref="A16:A27"/>
+    <mergeCell ref="A8:A14"/>
+    <mergeCell ref="A126:A132"/>
+    <mergeCell ref="A189:A196"/>
+    <mergeCell ref="A174:A187"/>
+    <mergeCell ref="A159:A172"/>
+    <mergeCell ref="A146:A156"/>
+    <mergeCell ref="A134:A144"/>
     <mergeCell ref="A563:A584"/>
     <mergeCell ref="A111:A116"/>
     <mergeCell ref="A217:A228"/>
@@ -28108,35 +29731,6 @@
     <mergeCell ref="A239:A246"/>
     <mergeCell ref="A198:A215"/>
     <mergeCell ref="A118:A124"/>
-    <mergeCell ref="A126:A132"/>
-    <mergeCell ref="A189:A196"/>
-    <mergeCell ref="A174:A187"/>
-    <mergeCell ref="A159:A172"/>
-    <mergeCell ref="A146:A156"/>
-    <mergeCell ref="A134:A144"/>
-    <mergeCell ref="A2:A6"/>
-    <mergeCell ref="A37:A46"/>
-    <mergeCell ref="A29:A35"/>
-    <mergeCell ref="A16:A27"/>
-    <mergeCell ref="A8:A14"/>
-    <mergeCell ref="A104:A109"/>
-    <mergeCell ref="A56:A62"/>
-    <mergeCell ref="A48:A54"/>
-    <mergeCell ref="A97:A102"/>
-    <mergeCell ref="A88:A95"/>
-    <mergeCell ref="A81:A86"/>
-    <mergeCell ref="A64:A78"/>
-    <mergeCell ref="A276:A295"/>
-    <mergeCell ref="A356:A364"/>
-    <mergeCell ref="A330:A342"/>
-    <mergeCell ref="A311:A318"/>
-    <mergeCell ref="A490:A501"/>
-    <mergeCell ref="A546:A561"/>
-    <mergeCell ref="A503:A521"/>
-    <mergeCell ref="A454:A465"/>
-    <mergeCell ref="A467:A488"/>
-    <mergeCell ref="A297:A309"/>
-    <mergeCell ref="A523:A544"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Atualizado o ex046 e planilha
</commit_message>
<xml_diff>
--- a/detalhesPython.xlsx
+++ b/detalhesPython.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Thiago Henrique\Documents\EstudosT\python\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\thiag\Documents\EstudosT\python\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44B16CF9-4D56-4700-BC7F-AAB7FA88A7B6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A0808A8-1D38-44CA-999C-7F0288B4CED0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="15" windowWidth="29040" windowHeight="15990" xr2:uid="{ECBDB9F7-0FAD-476C-A4A4-7948F29B869E}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{ECBDB9F7-0FAD-476C-A4A4-7948F29B869E}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="552" uniqueCount="481">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="559" uniqueCount="487">
   <si>
     <t>Descrição</t>
   </si>
@@ -24805,6 +24805,266 @@
         <family val="3"/>
       </rPr>
       <t>)    </t>
+    </r>
+  </si>
+  <si>
+    <t>ex046</t>
+  </si>
+  <si>
+    <t>Faça um programa que mostre na tela uma contagem regressiva para o estouro de fogos de artifício, indo de 10 até 0, com uma pausa de 1 segundo entre eles.</t>
+  </si>
+  <si>
+    <r>
+      <t>for</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> c </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>in</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF988BC7"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>range</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>(</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF78D1E1"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>10</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>-</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF78D1E1"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>1</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>-</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF78D1E1"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>1</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>):</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">    </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF988BC7"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>print</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>(c)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">    </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF67E480"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>sleep</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>(</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF78D1E1"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>0.5</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>print</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>(</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE7DE79"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>'Parabéns!</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>\U0001F3C6</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE7DE79"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>\U0001F389</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE7DE79"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>'</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>)</t>
     </r>
   </si>
 </sst>
@@ -26042,10 +26302,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{73331524-72FC-41A3-82E6-4326A0999772}">
-  <dimension ref="A1:G635"/>
+  <dimension ref="A1:G644"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A579" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B635" sqref="A635:XFD635"/>
+    <sheetView tabSelected="1" topLeftCell="A633" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B640" sqref="B640"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -29683,39 +29943,56 @@
       <c r="A635" s="51"/>
       <c r="B635" s="42"/>
     </row>
+    <row r="636" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="637" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A637" s="49" t="s">
+        <v>481</v>
+      </c>
+      <c r="B637" s="31" t="s">
+        <v>482</v>
+      </c>
+    </row>
+    <row r="638" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A638" s="50"/>
+      <c r="B638" s="40"/>
+    </row>
+    <row r="639" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A639" s="50"/>
+      <c r="B639" s="34" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="640" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A640" s="50"/>
+      <c r="B640" s="34" t="s">
+        <v>483</v>
+      </c>
+    </row>
+    <row r="641" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A641" s="50"/>
+      <c r="B641" s="7" t="s">
+        <v>484</v>
+      </c>
+    </row>
+    <row r="642" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A642" s="50"/>
+      <c r="B642" s="7" t="s">
+        <v>485</v>
+      </c>
+    </row>
+    <row r="643" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A643" s="50"/>
+      <c r="B643" s="11" t="s">
+        <v>486</v>
+      </c>
+    </row>
+    <row r="644" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A644" s="51"/>
+      <c r="B644" s="42"/>
+    </row>
   </sheetData>
-  <mergeCells count="46">
-    <mergeCell ref="A586:A635"/>
-    <mergeCell ref="A546:A561"/>
-    <mergeCell ref="A503:A521"/>
-    <mergeCell ref="A454:A465"/>
-    <mergeCell ref="A467:A488"/>
-    <mergeCell ref="A297:A309"/>
-    <mergeCell ref="A523:A544"/>
-    <mergeCell ref="A276:A295"/>
-    <mergeCell ref="A356:A364"/>
-    <mergeCell ref="A330:A342"/>
-    <mergeCell ref="A311:A318"/>
-    <mergeCell ref="A490:A501"/>
-    <mergeCell ref="A104:A109"/>
-    <mergeCell ref="A56:A62"/>
-    <mergeCell ref="A48:A54"/>
-    <mergeCell ref="A97:A102"/>
-    <mergeCell ref="A88:A95"/>
-    <mergeCell ref="A81:A86"/>
-    <mergeCell ref="A64:A78"/>
-    <mergeCell ref="A2:A6"/>
-    <mergeCell ref="A37:A46"/>
-    <mergeCell ref="A29:A35"/>
-    <mergeCell ref="A16:A27"/>
-    <mergeCell ref="A8:A14"/>
-    <mergeCell ref="A126:A132"/>
-    <mergeCell ref="A189:A196"/>
-    <mergeCell ref="A174:A187"/>
-    <mergeCell ref="A159:A172"/>
-    <mergeCell ref="A146:A156"/>
-    <mergeCell ref="A134:A144"/>
-    <mergeCell ref="A563:A584"/>
+  <mergeCells count="47">
+    <mergeCell ref="A637:A644"/>
     <mergeCell ref="A111:A116"/>
     <mergeCell ref="A217:A228"/>
     <mergeCell ref="A248:A260"/>
@@ -29731,6 +30008,37 @@
     <mergeCell ref="A239:A246"/>
     <mergeCell ref="A198:A215"/>
     <mergeCell ref="A118:A124"/>
+    <mergeCell ref="A126:A132"/>
+    <mergeCell ref="A189:A196"/>
+    <mergeCell ref="A174:A187"/>
+    <mergeCell ref="A159:A172"/>
+    <mergeCell ref="A146:A156"/>
+    <mergeCell ref="A134:A144"/>
+    <mergeCell ref="A2:A6"/>
+    <mergeCell ref="A37:A46"/>
+    <mergeCell ref="A29:A35"/>
+    <mergeCell ref="A16:A27"/>
+    <mergeCell ref="A8:A14"/>
+    <mergeCell ref="A104:A109"/>
+    <mergeCell ref="A56:A62"/>
+    <mergeCell ref="A48:A54"/>
+    <mergeCell ref="A97:A102"/>
+    <mergeCell ref="A88:A95"/>
+    <mergeCell ref="A81:A86"/>
+    <mergeCell ref="A64:A78"/>
+    <mergeCell ref="A297:A309"/>
+    <mergeCell ref="A523:A544"/>
+    <mergeCell ref="A276:A295"/>
+    <mergeCell ref="A356:A364"/>
+    <mergeCell ref="A330:A342"/>
+    <mergeCell ref="A311:A318"/>
+    <mergeCell ref="A490:A501"/>
+    <mergeCell ref="A586:A635"/>
+    <mergeCell ref="A546:A561"/>
+    <mergeCell ref="A503:A521"/>
+    <mergeCell ref="A454:A465"/>
+    <mergeCell ref="A467:A488"/>
+    <mergeCell ref="A563:A584"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Alterado o ex047 e planilha
</commit_message>
<xml_diff>
--- a/detalhesPython.xlsx
+++ b/detalhesPython.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\thiag\Documents\EstudosT\python\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A0808A8-1D38-44CA-999C-7F0288B4CED0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EBAABC53-7376-434E-8C3C-73F63DEA1816}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{ECBDB9F7-0FAD-476C-A4A4-7948F29B869E}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="559" uniqueCount="487">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="563" uniqueCount="491">
   <si>
     <t>Descrição</t>
   </si>
@@ -25056,6 +25056,194 @@
         <family val="3"/>
       </rPr>
       <t>'</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>)</t>
+    </r>
+  </si>
+  <si>
+    <t>ex047</t>
+  </si>
+  <si>
+    <t>Crie um programa que mostre na tela todos os números pares que estão no intervalo entre 1 e 50.</t>
+  </si>
+  <si>
+    <r>
+      <t>for</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> c </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>in</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF988BC7"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>range</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>(</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF78D1E1"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>2</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF78D1E1"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>51</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF78D1E1"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>2</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>):</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">    </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF988BC7"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>print</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">(c, </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color rgb="FFE89E64"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>end</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>=</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE7DE79"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>', '</t>
     </r>
     <r>
       <rPr>
@@ -26302,10 +26490,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{73331524-72FC-41A3-82E6-4326A0999772}">
-  <dimension ref="A1:G644"/>
+  <dimension ref="A1:G650"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A633" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B640" sqref="B640"/>
+      <selection activeCell="B648" sqref="B648"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -29990,8 +30178,69 @@
       <c r="A644" s="51"/>
       <c r="B644" s="42"/>
     </row>
+    <row r="645" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="646" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A646" s="49" t="s">
+        <v>487</v>
+      </c>
+      <c r="B646" s="31" t="s">
+        <v>488</v>
+      </c>
+    </row>
+    <row r="647" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A647" s="50"/>
+      <c r="B647" s="40"/>
+    </row>
+    <row r="648" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A648" s="50"/>
+      <c r="B648" s="34" t="s">
+        <v>489</v>
+      </c>
+    </row>
+    <row r="649" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A649" s="50"/>
+      <c r="B649" s="7" t="s">
+        <v>490</v>
+      </c>
+    </row>
+    <row r="650" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A650" s="51"/>
+      <c r="B650" s="42"/>
+    </row>
   </sheetData>
-  <mergeCells count="47">
+  <mergeCells count="48">
+    <mergeCell ref="A646:A650"/>
+    <mergeCell ref="A586:A635"/>
+    <mergeCell ref="A546:A561"/>
+    <mergeCell ref="A503:A521"/>
+    <mergeCell ref="A454:A465"/>
+    <mergeCell ref="A467:A488"/>
+    <mergeCell ref="A563:A584"/>
+    <mergeCell ref="A297:A309"/>
+    <mergeCell ref="A523:A544"/>
+    <mergeCell ref="A276:A295"/>
+    <mergeCell ref="A356:A364"/>
+    <mergeCell ref="A330:A342"/>
+    <mergeCell ref="A311:A318"/>
+    <mergeCell ref="A490:A501"/>
+    <mergeCell ref="A104:A109"/>
+    <mergeCell ref="A56:A62"/>
+    <mergeCell ref="A48:A54"/>
+    <mergeCell ref="A97:A102"/>
+    <mergeCell ref="A88:A95"/>
+    <mergeCell ref="A81:A86"/>
+    <mergeCell ref="A64:A78"/>
+    <mergeCell ref="A2:A6"/>
+    <mergeCell ref="A37:A46"/>
+    <mergeCell ref="A29:A35"/>
+    <mergeCell ref="A16:A27"/>
+    <mergeCell ref="A8:A14"/>
+    <mergeCell ref="A126:A132"/>
+    <mergeCell ref="A189:A196"/>
+    <mergeCell ref="A174:A187"/>
+    <mergeCell ref="A159:A172"/>
+    <mergeCell ref="A146:A156"/>
+    <mergeCell ref="A134:A144"/>
     <mergeCell ref="A637:A644"/>
     <mergeCell ref="A111:A116"/>
     <mergeCell ref="A217:A228"/>
@@ -30008,37 +30257,6 @@
     <mergeCell ref="A239:A246"/>
     <mergeCell ref="A198:A215"/>
     <mergeCell ref="A118:A124"/>
-    <mergeCell ref="A126:A132"/>
-    <mergeCell ref="A189:A196"/>
-    <mergeCell ref="A174:A187"/>
-    <mergeCell ref="A159:A172"/>
-    <mergeCell ref="A146:A156"/>
-    <mergeCell ref="A134:A144"/>
-    <mergeCell ref="A2:A6"/>
-    <mergeCell ref="A37:A46"/>
-    <mergeCell ref="A29:A35"/>
-    <mergeCell ref="A16:A27"/>
-    <mergeCell ref="A8:A14"/>
-    <mergeCell ref="A104:A109"/>
-    <mergeCell ref="A56:A62"/>
-    <mergeCell ref="A48:A54"/>
-    <mergeCell ref="A97:A102"/>
-    <mergeCell ref="A88:A95"/>
-    <mergeCell ref="A81:A86"/>
-    <mergeCell ref="A64:A78"/>
-    <mergeCell ref="A297:A309"/>
-    <mergeCell ref="A523:A544"/>
-    <mergeCell ref="A276:A295"/>
-    <mergeCell ref="A356:A364"/>
-    <mergeCell ref="A330:A342"/>
-    <mergeCell ref="A311:A318"/>
-    <mergeCell ref="A490:A501"/>
-    <mergeCell ref="A586:A635"/>
-    <mergeCell ref="A546:A561"/>
-    <mergeCell ref="A503:A521"/>
-    <mergeCell ref="A454:A465"/>
-    <mergeCell ref="A467:A488"/>
-    <mergeCell ref="A563:A584"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Atualizado o ex08 e Planilha
</commit_message>
<xml_diff>
--- a/detalhesPython.xlsx
+++ b/detalhesPython.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\thiag\Documents\EstudosT\python\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EBAABC53-7376-434E-8C3C-73F63DEA1816}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B496A115-AE84-43D3-8C99-DA461EDCA4E6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{ECBDB9F7-0FAD-476C-A4A4-7948F29B869E}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="563" uniqueCount="491">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="575" uniqueCount="502">
   <si>
     <t>Descrição</t>
   </si>
@@ -25254,6 +25254,422 @@
       </rPr>
       <t>)</t>
     </r>
+  </si>
+  <si>
+    <t>ex048</t>
+  </si>
+  <si>
+    <t>Faça um programa que calcule a soma entre todos os números que são múltiplos de três e que se encontram no intervalo de 1 até 500.</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">soma </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>=</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF78D1E1"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>0</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">cont </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>=</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF78D1E1"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>0</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>for</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> c </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>in</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF988BC7"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>range</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>(</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF78D1E1"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>1</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF78D1E1"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>501</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF78D1E1"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>2</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>):</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">    </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>if</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> c </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>%</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF78D1E1"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>3</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>==</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF78D1E1"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>0</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>:</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">        soma </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>+=</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> c</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">        cont </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>+=</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF78D1E1"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>1</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>print</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>(</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE7DE79"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">'A soma de todos os </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF78D1E1"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>{}</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE7DE79"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> valores solicitados é </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF78D1E1"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>{}</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE7DE79"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>'</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF67E480"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>format</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>(cont, soma))</t>
+    </r>
+  </si>
+  <si>
+    <t>soma é um acumulador, para ir acumulando (no caso somando) os valores True do if</t>
+  </si>
+  <si>
+    <t>cont é um contador, para ir contando (no caso somando) a quantidade de True do if. ( cont += 1 substitui o cont = cont + 1 )</t>
   </si>
 </sst>
 </file>
@@ -26490,10 +26906,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{73331524-72FC-41A3-82E6-4326A0999772}">
-  <dimension ref="A1:G650"/>
+  <dimension ref="A1:G665"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A633" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B648" sqref="B648"/>
+    <sheetView tabSelected="1" topLeftCell="A642" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="A652" sqref="A652:A665"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -30207,41 +30623,90 @@
       <c r="A650" s="51"/>
       <c r="B650" s="42"/>
     </row>
+    <row r="651" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="652" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A652" s="49" t="s">
+        <v>491</v>
+      </c>
+      <c r="B652" s="31" t="s">
+        <v>492</v>
+      </c>
+    </row>
+    <row r="653" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A653" s="50"/>
+      <c r="B653" s="40"/>
+    </row>
+    <row r="654" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A654" s="50"/>
+      <c r="B654" s="7" t="s">
+        <v>493</v>
+      </c>
+    </row>
+    <row r="655" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A655" s="50"/>
+      <c r="B655" s="7" t="s">
+        <v>494</v>
+      </c>
+    </row>
+    <row r="656" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A656" s="50"/>
+      <c r="B656" s="34" t="s">
+        <v>495</v>
+      </c>
+    </row>
+    <row r="657" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A657" s="50"/>
+      <c r="B657" s="7" t="s">
+        <v>496</v>
+      </c>
+    </row>
+    <row r="658" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A658" s="50"/>
+      <c r="B658" s="7" t="s">
+        <v>497</v>
+      </c>
+    </row>
+    <row r="659" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A659" s="50"/>
+      <c r="B659" s="7" t="s">
+        <v>498</v>
+      </c>
+    </row>
+    <row r="660" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A660" s="50"/>
+      <c r="B660" s="11" t="s">
+        <v>499</v>
+      </c>
+    </row>
+    <row r="661" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A661" s="50"/>
+      <c r="B661" s="11"/>
+    </row>
+    <row r="662" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A662" s="50"/>
+      <c r="B662" s="11" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="663" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A663" s="50"/>
+      <c r="B663" s="7" t="s">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="664" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A664" s="50"/>
+      <c r="B664" s="36" t="s">
+        <v>501</v>
+      </c>
+    </row>
+    <row r="665" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A665" s="51"/>
+      <c r="B665" s="42"/>
+    </row>
   </sheetData>
-  <mergeCells count="48">
-    <mergeCell ref="A646:A650"/>
-    <mergeCell ref="A586:A635"/>
-    <mergeCell ref="A546:A561"/>
-    <mergeCell ref="A503:A521"/>
-    <mergeCell ref="A454:A465"/>
-    <mergeCell ref="A467:A488"/>
-    <mergeCell ref="A563:A584"/>
-    <mergeCell ref="A297:A309"/>
-    <mergeCell ref="A523:A544"/>
-    <mergeCell ref="A276:A295"/>
-    <mergeCell ref="A356:A364"/>
-    <mergeCell ref="A330:A342"/>
-    <mergeCell ref="A311:A318"/>
-    <mergeCell ref="A490:A501"/>
-    <mergeCell ref="A104:A109"/>
-    <mergeCell ref="A56:A62"/>
-    <mergeCell ref="A48:A54"/>
-    <mergeCell ref="A97:A102"/>
-    <mergeCell ref="A88:A95"/>
-    <mergeCell ref="A81:A86"/>
-    <mergeCell ref="A64:A78"/>
-    <mergeCell ref="A2:A6"/>
-    <mergeCell ref="A37:A46"/>
-    <mergeCell ref="A29:A35"/>
-    <mergeCell ref="A16:A27"/>
-    <mergeCell ref="A8:A14"/>
-    <mergeCell ref="A126:A132"/>
-    <mergeCell ref="A189:A196"/>
-    <mergeCell ref="A174:A187"/>
-    <mergeCell ref="A159:A172"/>
-    <mergeCell ref="A146:A156"/>
-    <mergeCell ref="A134:A144"/>
-    <mergeCell ref="A637:A644"/>
+  <mergeCells count="49">
+    <mergeCell ref="A652:A665"/>
     <mergeCell ref="A111:A116"/>
     <mergeCell ref="A217:A228"/>
     <mergeCell ref="A248:A260"/>
@@ -30257,6 +30722,39 @@
     <mergeCell ref="A239:A246"/>
     <mergeCell ref="A198:A215"/>
     <mergeCell ref="A118:A124"/>
+    <mergeCell ref="A126:A132"/>
+    <mergeCell ref="A189:A196"/>
+    <mergeCell ref="A174:A187"/>
+    <mergeCell ref="A159:A172"/>
+    <mergeCell ref="A146:A156"/>
+    <mergeCell ref="A134:A144"/>
+    <mergeCell ref="A2:A6"/>
+    <mergeCell ref="A37:A46"/>
+    <mergeCell ref="A29:A35"/>
+    <mergeCell ref="A16:A27"/>
+    <mergeCell ref="A8:A14"/>
+    <mergeCell ref="A104:A109"/>
+    <mergeCell ref="A56:A62"/>
+    <mergeCell ref="A48:A54"/>
+    <mergeCell ref="A97:A102"/>
+    <mergeCell ref="A88:A95"/>
+    <mergeCell ref="A81:A86"/>
+    <mergeCell ref="A64:A78"/>
+    <mergeCell ref="A297:A309"/>
+    <mergeCell ref="A523:A544"/>
+    <mergeCell ref="A276:A295"/>
+    <mergeCell ref="A356:A364"/>
+    <mergeCell ref="A330:A342"/>
+    <mergeCell ref="A311:A318"/>
+    <mergeCell ref="A490:A501"/>
+    <mergeCell ref="A646:A650"/>
+    <mergeCell ref="A586:A635"/>
+    <mergeCell ref="A546:A561"/>
+    <mergeCell ref="A503:A521"/>
+    <mergeCell ref="A454:A465"/>
+    <mergeCell ref="A467:A488"/>
+    <mergeCell ref="A563:A584"/>
+    <mergeCell ref="A637:A644"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Atualizado o ex049 e Planilha
</commit_message>
<xml_diff>
--- a/detalhesPython.xlsx
+++ b/detalhesPython.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\thiag\Documents\EstudosT\python\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B496A115-AE84-43D3-8C99-DA461EDCA4E6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2EBB3B21-08B4-4808-9097-27FAD0B9ECE3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{ECBDB9F7-0FAD-476C-A4A4-7948F29B869E}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="575" uniqueCount="502">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="580" uniqueCount="505">
   <si>
     <t>Descrição</t>
   </si>
@@ -25670,6 +25670,226 @@
   </si>
   <si>
     <t>cont é um contador, para ir contando (no caso somando) a quantidade de True do if. ( cont += 1 substitui o cont = cont + 1 )</t>
+  </si>
+  <si>
+    <t>Refaça o DESAFIO 9, mostrando a tabuada de um número que o usuário escolher, só que agora utilizando um laço for.</t>
+  </si>
+  <si>
+    <r>
+      <t>for</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> c </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>in</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF988BC7"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>range</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>(</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF78D1E1"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>1</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF78D1E1"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>11</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>):</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">    </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF988BC7"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>print</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>(</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE7DE79"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>'</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF78D1E1"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>{}</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE7DE79"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> x </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF78D1E1"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>{}</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE7DE79"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> = </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF78D1E1"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>{}</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE7DE79"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>'</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF67E480"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>format</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">(num, c, num </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>*</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> c))</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -26906,10 +27126,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{73331524-72FC-41A3-82E6-4326A0999772}">
-  <dimension ref="A1:G665"/>
+  <dimension ref="A1:G672"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A642" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A652" sqref="A652:A665"/>
+    <sheetView tabSelected="1" topLeftCell="A654" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="A667" sqref="A667:A672"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -30704,8 +30924,77 @@
       <c r="A665" s="51"/>
       <c r="B665" s="42"/>
     </row>
+    <row r="666" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="667" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A667" s="49" t="s">
+        <v>491</v>
+      </c>
+      <c r="B667" s="31" t="s">
+        <v>502</v>
+      </c>
+    </row>
+    <row r="668" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A668" s="50"/>
+      <c r="B668" s="40"/>
+    </row>
+    <row r="669" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A669" s="50"/>
+      <c r="B669" s="7" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="670" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A670" s="50"/>
+      <c r="B670" s="34" t="s">
+        <v>503</v>
+      </c>
+    </row>
+    <row r="671" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A671" s="50"/>
+      <c r="B671" s="7" t="s">
+        <v>504</v>
+      </c>
+    </row>
+    <row r="672" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A672" s="51"/>
+      <c r="B672" s="42"/>
+    </row>
   </sheetData>
-  <mergeCells count="49">
+  <mergeCells count="50">
+    <mergeCell ref="A667:A672"/>
+    <mergeCell ref="A646:A650"/>
+    <mergeCell ref="A586:A635"/>
+    <mergeCell ref="A546:A561"/>
+    <mergeCell ref="A503:A521"/>
+    <mergeCell ref="A454:A465"/>
+    <mergeCell ref="A467:A488"/>
+    <mergeCell ref="A563:A584"/>
+    <mergeCell ref="A637:A644"/>
+    <mergeCell ref="A297:A309"/>
+    <mergeCell ref="A523:A544"/>
+    <mergeCell ref="A276:A295"/>
+    <mergeCell ref="A356:A364"/>
+    <mergeCell ref="A330:A342"/>
+    <mergeCell ref="A311:A318"/>
+    <mergeCell ref="A490:A501"/>
+    <mergeCell ref="A104:A109"/>
+    <mergeCell ref="A56:A62"/>
+    <mergeCell ref="A48:A54"/>
+    <mergeCell ref="A97:A102"/>
+    <mergeCell ref="A88:A95"/>
+    <mergeCell ref="A81:A86"/>
+    <mergeCell ref="A64:A78"/>
+    <mergeCell ref="A2:A6"/>
+    <mergeCell ref="A37:A46"/>
+    <mergeCell ref="A29:A35"/>
+    <mergeCell ref="A16:A27"/>
+    <mergeCell ref="A8:A14"/>
+    <mergeCell ref="A126:A132"/>
+    <mergeCell ref="A189:A196"/>
+    <mergeCell ref="A174:A187"/>
+    <mergeCell ref="A159:A172"/>
+    <mergeCell ref="A146:A156"/>
+    <mergeCell ref="A134:A144"/>
     <mergeCell ref="A652:A665"/>
     <mergeCell ref="A111:A116"/>
     <mergeCell ref="A217:A228"/>
@@ -30722,39 +31011,6 @@
     <mergeCell ref="A239:A246"/>
     <mergeCell ref="A198:A215"/>
     <mergeCell ref="A118:A124"/>
-    <mergeCell ref="A126:A132"/>
-    <mergeCell ref="A189:A196"/>
-    <mergeCell ref="A174:A187"/>
-    <mergeCell ref="A159:A172"/>
-    <mergeCell ref="A146:A156"/>
-    <mergeCell ref="A134:A144"/>
-    <mergeCell ref="A2:A6"/>
-    <mergeCell ref="A37:A46"/>
-    <mergeCell ref="A29:A35"/>
-    <mergeCell ref="A16:A27"/>
-    <mergeCell ref="A8:A14"/>
-    <mergeCell ref="A104:A109"/>
-    <mergeCell ref="A56:A62"/>
-    <mergeCell ref="A48:A54"/>
-    <mergeCell ref="A97:A102"/>
-    <mergeCell ref="A88:A95"/>
-    <mergeCell ref="A81:A86"/>
-    <mergeCell ref="A64:A78"/>
-    <mergeCell ref="A297:A309"/>
-    <mergeCell ref="A523:A544"/>
-    <mergeCell ref="A276:A295"/>
-    <mergeCell ref="A356:A364"/>
-    <mergeCell ref="A330:A342"/>
-    <mergeCell ref="A311:A318"/>
-    <mergeCell ref="A490:A501"/>
-    <mergeCell ref="A646:A650"/>
-    <mergeCell ref="A586:A635"/>
-    <mergeCell ref="A546:A561"/>
-    <mergeCell ref="A503:A521"/>
-    <mergeCell ref="A454:A465"/>
-    <mergeCell ref="A467:A488"/>
-    <mergeCell ref="A563:A584"/>
-    <mergeCell ref="A637:A644"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Alterado o ex050 e Planilha
</commit_message>
<xml_diff>
--- a/detalhesPython.xlsx
+++ b/detalhesPython.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\thiag\Documents\EstudosT\python\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2EBB3B21-08B4-4808-9097-27FAD0B9ECE3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE80D8C4-4D95-4168-8367-6BE0FC2DAA46}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{ECBDB9F7-0FAD-476C-A4A4-7948F29B869E}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="580" uniqueCount="505">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="590" uniqueCount="513">
   <si>
     <t>Descrição</t>
   </si>
@@ -25889,6 +25889,383 @@
         <family val="3"/>
       </rPr>
       <t xml:space="preserve"> c))</t>
+    </r>
+  </si>
+  <si>
+    <t>ex049</t>
+  </si>
+  <si>
+    <t>ex050</t>
+  </si>
+  <si>
+    <t>Desenvolva um programa que leia seis números inteiros e mostre a soma apenas daqueles que forem pares. Se o valor digitado for ímpar, desconsidere-o.</t>
+  </si>
+  <si>
+    <r>
+      <t>for</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> c </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>in</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF988BC7"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>range</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>(</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF78D1E1"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>1</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF78D1E1"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>7</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>):</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">    num </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>=</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color rgb="FF988BC7"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>int</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>(</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF988BC7"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>input</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>(</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE7DE79"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>'Digite um número: '</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>))</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">    </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>if</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> num </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>%</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF78D1E1"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>2</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>==</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF78D1E1"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>0</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>:</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">        soma </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>+=</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> num</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>print</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>(</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE7DE79"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">'Foi informado </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF78D1E1"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>{}</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE7DE79"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> números PARES e a soma dos números pares é: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF78D1E1"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>{}</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE7DE79"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>'</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF67E480"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>format</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">(cont, soma)) </t>
     </r>
   </si>
 </sst>
@@ -27126,10 +27503,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{73331524-72FC-41A3-82E6-4326A0999772}">
-  <dimension ref="A1:G672"/>
+  <dimension ref="A1:G684"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A654" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A667" sqref="A667:A672"/>
+    <sheetView tabSelected="1" topLeftCell="A651" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B674" sqref="B674"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -30927,7 +31304,7 @@
     <row r="666" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="667" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A667" s="49" t="s">
-        <v>491</v>
+        <v>505</v>
       </c>
       <c r="B667" s="31" t="s">
         <v>502</v>
@@ -30959,43 +31336,74 @@
       <c r="A672" s="51"/>
       <c r="B672" s="42"/>
     </row>
+    <row r="673" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="674" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A674" s="49" t="s">
+        <v>506</v>
+      </c>
+      <c r="B674" s="31" t="s">
+        <v>507</v>
+      </c>
+    </row>
+    <row r="675" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A675" s="50"/>
+      <c r="B675" s="40"/>
+    </row>
+    <row r="676" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A676" s="50"/>
+      <c r="B676" s="7" t="s">
+        <v>493</v>
+      </c>
+    </row>
+    <row r="677" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A677" s="50"/>
+      <c r="B677" s="7" t="s">
+        <v>494</v>
+      </c>
+    </row>
+    <row r="678" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A678" s="50"/>
+      <c r="B678" s="34" t="s">
+        <v>508</v>
+      </c>
+    </row>
+    <row r="679" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A679" s="50"/>
+      <c r="B679" s="7" t="s">
+        <v>509</v>
+      </c>
+    </row>
+    <row r="680" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A680" s="50"/>
+      <c r="B680" s="7" t="s">
+        <v>510</v>
+      </c>
+    </row>
+    <row r="681" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A681" s="50"/>
+      <c r="B681" s="7" t="s">
+        <v>511</v>
+      </c>
+    </row>
+    <row r="682" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A682" s="50"/>
+      <c r="B682" s="7" t="s">
+        <v>498</v>
+      </c>
+    </row>
+    <row r="683" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A683" s="50"/>
+      <c r="B683" s="11" t="s">
+        <v>512</v>
+      </c>
+    </row>
+    <row r="684" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A684" s="51"/>
+      <c r="B684" s="42"/>
+    </row>
   </sheetData>
-  <mergeCells count="50">
-    <mergeCell ref="A667:A672"/>
-    <mergeCell ref="A646:A650"/>
-    <mergeCell ref="A586:A635"/>
-    <mergeCell ref="A546:A561"/>
-    <mergeCell ref="A503:A521"/>
-    <mergeCell ref="A454:A465"/>
-    <mergeCell ref="A467:A488"/>
-    <mergeCell ref="A563:A584"/>
-    <mergeCell ref="A637:A644"/>
-    <mergeCell ref="A297:A309"/>
-    <mergeCell ref="A523:A544"/>
-    <mergeCell ref="A276:A295"/>
-    <mergeCell ref="A356:A364"/>
-    <mergeCell ref="A330:A342"/>
-    <mergeCell ref="A311:A318"/>
-    <mergeCell ref="A490:A501"/>
-    <mergeCell ref="A104:A109"/>
-    <mergeCell ref="A56:A62"/>
-    <mergeCell ref="A48:A54"/>
-    <mergeCell ref="A97:A102"/>
-    <mergeCell ref="A88:A95"/>
-    <mergeCell ref="A81:A86"/>
-    <mergeCell ref="A64:A78"/>
-    <mergeCell ref="A2:A6"/>
-    <mergeCell ref="A37:A46"/>
-    <mergeCell ref="A29:A35"/>
-    <mergeCell ref="A16:A27"/>
-    <mergeCell ref="A8:A14"/>
-    <mergeCell ref="A126:A132"/>
-    <mergeCell ref="A189:A196"/>
-    <mergeCell ref="A174:A187"/>
-    <mergeCell ref="A159:A172"/>
-    <mergeCell ref="A146:A156"/>
-    <mergeCell ref="A134:A144"/>
-    <mergeCell ref="A652:A665"/>
+  <mergeCells count="51">
+    <mergeCell ref="A674:A684"/>
     <mergeCell ref="A111:A116"/>
     <mergeCell ref="A217:A228"/>
     <mergeCell ref="A248:A260"/>
@@ -31011,6 +31419,41 @@
     <mergeCell ref="A239:A246"/>
     <mergeCell ref="A198:A215"/>
     <mergeCell ref="A118:A124"/>
+    <mergeCell ref="A126:A132"/>
+    <mergeCell ref="A189:A196"/>
+    <mergeCell ref="A174:A187"/>
+    <mergeCell ref="A159:A172"/>
+    <mergeCell ref="A146:A156"/>
+    <mergeCell ref="A134:A144"/>
+    <mergeCell ref="A2:A6"/>
+    <mergeCell ref="A37:A46"/>
+    <mergeCell ref="A29:A35"/>
+    <mergeCell ref="A16:A27"/>
+    <mergeCell ref="A8:A14"/>
+    <mergeCell ref="A104:A109"/>
+    <mergeCell ref="A56:A62"/>
+    <mergeCell ref="A48:A54"/>
+    <mergeCell ref="A97:A102"/>
+    <mergeCell ref="A88:A95"/>
+    <mergeCell ref="A81:A86"/>
+    <mergeCell ref="A64:A78"/>
+    <mergeCell ref="A276:A295"/>
+    <mergeCell ref="A356:A364"/>
+    <mergeCell ref="A330:A342"/>
+    <mergeCell ref="A311:A318"/>
+    <mergeCell ref="A490:A501"/>
+    <mergeCell ref="A454:A465"/>
+    <mergeCell ref="A467:A488"/>
+    <mergeCell ref="A563:A584"/>
+    <mergeCell ref="A637:A644"/>
+    <mergeCell ref="A297:A309"/>
+    <mergeCell ref="A523:A544"/>
+    <mergeCell ref="A667:A672"/>
+    <mergeCell ref="A646:A650"/>
+    <mergeCell ref="A586:A635"/>
+    <mergeCell ref="A546:A561"/>
+    <mergeCell ref="A503:A521"/>
+    <mergeCell ref="A652:A665"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Atualizado o ex051 e Planilha
</commit_message>
<xml_diff>
--- a/detalhesPython.xlsx
+++ b/detalhesPython.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\thiag\Documents\EstudosT\python\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE80D8C4-4D95-4168-8367-6BE0FC2DAA46}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A9BE41F-5B5D-449C-90DB-07B8C28D31DB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{ECBDB9F7-0FAD-476C-A4A4-7948F29B869E}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="590" uniqueCount="513">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="603" uniqueCount="524">
   <si>
     <t>Descrição</t>
   </si>
@@ -26267,6 +26267,598 @@
       </rPr>
       <t xml:space="preserve">(cont, soma)) </t>
     </r>
+  </si>
+  <si>
+    <t>ex051</t>
+  </si>
+  <si>
+    <t>Desenvolva um programa que leia o primeiro termo e a razão de uma PA. No final, mostre os 10 primeiros termos dessa progressão.</t>
+  </si>
+  <si>
+    <r>
+      <t>print</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>(</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE7DE79"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>'='</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>*</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF78D1E1"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>30</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>print</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>(</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE7DE79"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>'10 TERMOS DE UMA P. A.'</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF67E480"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>center</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>(</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF78D1E1"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>30</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>))</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">t1 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>=</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color rgb="FF988BC7"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>int</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>(</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF988BC7"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>input</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>(</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE7DE79"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>'Digite o primeiro termo: '</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>))</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">razao </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>=</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color rgb="FF988BC7"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>int</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>(</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF988BC7"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>input</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>(</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE7DE79"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>'Digite a razão: '</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>))</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">decimo </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>=</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> t1 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> (</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF78D1E1"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>10</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>-</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF78D1E1"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>1</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">) </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>*</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> razao</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>for</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> c </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>in</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF988BC7"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>range</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">(t1, decimo </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> razao, razao):</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">    </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF988BC7"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>print</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">(c, </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color rgb="FFE89E64"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>end</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>=</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE7DE79"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>' → '</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>print</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>(</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE7DE79"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>'ACABOU!'</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>)</t>
+    </r>
+  </si>
+  <si>
+    <t>decimo = t1 + (10 - 1) * razao   ---&gt; É uma expressão matemática para chegar no 10° termo de uma projeção aritimética</t>
   </si>
 </sst>
 </file>
@@ -27503,10 +28095,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{73331524-72FC-41A3-82E6-4326A0999772}">
-  <dimension ref="A1:G684"/>
+  <dimension ref="A1:G700"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A651" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B674" sqref="B674"/>
+    <sheetView tabSelected="1" topLeftCell="A684" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B699" sqref="B699"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -31281,7 +31873,7 @@
     </row>
     <row r="662" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A662" s="50"/>
-      <c r="B662" s="11" t="s">
+      <c r="B662" s="36" t="s">
         <v>18</v>
       </c>
     </row>
@@ -31401,8 +31993,131 @@
       <c r="A684" s="51"/>
       <c r="B684" s="42"/>
     </row>
+    <row r="685" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="686" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A686" s="49" t="s">
+        <v>513</v>
+      </c>
+      <c r="B686" s="31" t="s">
+        <v>514</v>
+      </c>
+    </row>
+    <row r="687" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A687" s="50"/>
+      <c r="B687" s="40"/>
+    </row>
+    <row r="688" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A688" s="50"/>
+      <c r="B688" s="11" t="s">
+        <v>515</v>
+      </c>
+    </row>
+    <row r="689" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A689" s="50"/>
+      <c r="B689" s="11" t="s">
+        <v>516</v>
+      </c>
+    </row>
+    <row r="690" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A690" s="50"/>
+      <c r="B690" s="11" t="s">
+        <v>515</v>
+      </c>
+    </row>
+    <row r="691" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A691" s="50"/>
+      <c r="B691" s="7" t="s">
+        <v>517</v>
+      </c>
+    </row>
+    <row r="692" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A692" s="50"/>
+      <c r="B692" s="7" t="s">
+        <v>518</v>
+      </c>
+    </row>
+    <row r="693" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A693" s="50"/>
+      <c r="B693" s="7" t="s">
+        <v>519</v>
+      </c>
+    </row>
+    <row r="694" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A694" s="50"/>
+      <c r="B694" s="34" t="s">
+        <v>520</v>
+      </c>
+    </row>
+    <row r="695" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A695" s="50"/>
+      <c r="B695" s="7" t="s">
+        <v>521</v>
+      </c>
+    </row>
+    <row r="696" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A696" s="50"/>
+      <c r="B696" s="11" t="s">
+        <v>522</v>
+      </c>
+    </row>
+    <row r="697" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A697" s="50"/>
+      <c r="B697" s="7"/>
+    </row>
+    <row r="698" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A698" s="50"/>
+      <c r="B698" s="36" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="699" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A699" s="50"/>
+      <c r="B699" s="7" t="s">
+        <v>523</v>
+      </c>
+    </row>
+    <row r="700" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A700" s="51"/>
+      <c r="B700" s="42"/>
+    </row>
   </sheetData>
-  <mergeCells count="51">
+  <mergeCells count="52">
+    <mergeCell ref="A686:A700"/>
+    <mergeCell ref="A563:A584"/>
+    <mergeCell ref="A637:A644"/>
+    <mergeCell ref="A297:A309"/>
+    <mergeCell ref="A523:A544"/>
+    <mergeCell ref="A667:A672"/>
+    <mergeCell ref="A646:A650"/>
+    <mergeCell ref="A586:A635"/>
+    <mergeCell ref="A546:A561"/>
+    <mergeCell ref="A503:A521"/>
+    <mergeCell ref="A652:A665"/>
+    <mergeCell ref="A276:A295"/>
+    <mergeCell ref="A356:A364"/>
+    <mergeCell ref="A330:A342"/>
+    <mergeCell ref="A311:A318"/>
+    <mergeCell ref="A490:A501"/>
+    <mergeCell ref="A454:A465"/>
+    <mergeCell ref="A467:A488"/>
+    <mergeCell ref="A104:A109"/>
+    <mergeCell ref="A56:A62"/>
+    <mergeCell ref="A48:A54"/>
+    <mergeCell ref="A97:A102"/>
+    <mergeCell ref="A88:A95"/>
+    <mergeCell ref="A81:A86"/>
+    <mergeCell ref="A64:A78"/>
+    <mergeCell ref="A2:A6"/>
+    <mergeCell ref="A37:A46"/>
+    <mergeCell ref="A29:A35"/>
+    <mergeCell ref="A16:A27"/>
+    <mergeCell ref="A8:A14"/>
+    <mergeCell ref="A126:A132"/>
+    <mergeCell ref="A189:A196"/>
+    <mergeCell ref="A174:A187"/>
+    <mergeCell ref="A159:A172"/>
+    <mergeCell ref="A146:A156"/>
+    <mergeCell ref="A134:A144"/>
     <mergeCell ref="A674:A684"/>
     <mergeCell ref="A111:A116"/>
     <mergeCell ref="A217:A228"/>
@@ -31419,41 +32134,6 @@
     <mergeCell ref="A239:A246"/>
     <mergeCell ref="A198:A215"/>
     <mergeCell ref="A118:A124"/>
-    <mergeCell ref="A126:A132"/>
-    <mergeCell ref="A189:A196"/>
-    <mergeCell ref="A174:A187"/>
-    <mergeCell ref="A159:A172"/>
-    <mergeCell ref="A146:A156"/>
-    <mergeCell ref="A134:A144"/>
-    <mergeCell ref="A2:A6"/>
-    <mergeCell ref="A37:A46"/>
-    <mergeCell ref="A29:A35"/>
-    <mergeCell ref="A16:A27"/>
-    <mergeCell ref="A8:A14"/>
-    <mergeCell ref="A104:A109"/>
-    <mergeCell ref="A56:A62"/>
-    <mergeCell ref="A48:A54"/>
-    <mergeCell ref="A97:A102"/>
-    <mergeCell ref="A88:A95"/>
-    <mergeCell ref="A81:A86"/>
-    <mergeCell ref="A64:A78"/>
-    <mergeCell ref="A276:A295"/>
-    <mergeCell ref="A356:A364"/>
-    <mergeCell ref="A330:A342"/>
-    <mergeCell ref="A311:A318"/>
-    <mergeCell ref="A490:A501"/>
-    <mergeCell ref="A454:A465"/>
-    <mergeCell ref="A467:A488"/>
-    <mergeCell ref="A563:A584"/>
-    <mergeCell ref="A637:A644"/>
-    <mergeCell ref="A297:A309"/>
-    <mergeCell ref="A523:A544"/>
-    <mergeCell ref="A667:A672"/>
-    <mergeCell ref="A646:A650"/>
-    <mergeCell ref="A586:A635"/>
-    <mergeCell ref="A546:A561"/>
-    <mergeCell ref="A503:A521"/>
-    <mergeCell ref="A652:A665"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Criei o ex052 e atualizado planilha
</commit_message>
<xml_diff>
--- a/detalhesPython.xlsx
+++ b/detalhesPython.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\thiag\Documents\EstudosT\python\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A9BE41F-5B5D-449C-90DB-07B8C28D31DB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3D0BC93-EC88-4C06-B13F-280C8BDB343F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{ECBDB9F7-0FAD-476C-A4A4-7948F29B869E}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="603" uniqueCount="524">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="619" uniqueCount="537">
   <si>
     <t>Descrição</t>
   </si>
@@ -26859,6 +26859,817 @@
   </si>
   <si>
     <t>decimo = t1 + (10 - 1) * razao   ---&gt; É uma expressão matemática para chegar no 10° termo de uma projeção aritimética</t>
+  </si>
+  <si>
+    <t>ex052</t>
+  </si>
+  <si>
+    <t>Faça um programa que leia um número inteiro e diga se ele é ou não um número primo.</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">tot </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>=</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF78D1E1"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>0</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>for</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> c </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>in</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF988BC7"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>range</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>(</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF78D1E1"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>1</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">, num </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF78D1E1"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>1</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>):</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">    </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>if</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> num </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>%</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> c </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>==</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF78D1E1"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>0</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>:</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">        </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF988BC7"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>print</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>(</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE7DE79"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>'</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>\033</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE7DE79"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>[32m'</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">, </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color rgb="FFE89E64"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>end</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>=</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE7DE79"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>''</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">        tot </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>+=</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF78D1E1"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>1</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">        </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF988BC7"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>print</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>(</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE7DE79"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>'</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>\033</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE7DE79"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>[31m'</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">, </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color rgb="FFE89E64"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>end</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>=</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE7DE79"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>''</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">    </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF988BC7"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>print</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>(</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE7DE79"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>'</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF78D1E1"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>{}</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE7DE79"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> '</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF67E480"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>format</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">(c), </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color rgb="FFE89E64"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>end</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>=</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE7DE79"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>''</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>print</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>(</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE7DE79"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>'</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>\n\033</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE7DE79"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">[mO </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF78D1E1"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>{}</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE7DE79"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> foi divisível </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF78D1E1"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>{}</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE7DE79"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> vezes'</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF67E480"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>format</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>(num, tot))</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>if</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> tot </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>==</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF78D1E1"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>2</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>:</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">    </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF988BC7"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>print</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>(</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE7DE79"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>'E por isso ele É PRIMO!'</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">    </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF988BC7"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>print</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>(</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE7DE79"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>'E por isso ele NÃO É PRIMO!'</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>)</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -28095,10 +28906,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{73331524-72FC-41A3-82E6-4326A0999772}">
-  <dimension ref="A1:G700"/>
+  <dimension ref="A1:G718"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A684" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B699" sqref="B699"/>
+    <sheetView tabSelected="1" topLeftCell="A693" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C715" sqref="C715"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -32080,45 +32891,110 @@
       <c r="A700" s="51"/>
       <c r="B700" s="42"/>
     </row>
+    <row r="701" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="702" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A702" s="49" t="s">
+        <v>524</v>
+      </c>
+      <c r="B702" s="31" t="s">
+        <v>525</v>
+      </c>
+    </row>
+    <row r="703" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A703" s="50"/>
+      <c r="B703" s="40"/>
+    </row>
+    <row r="704" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A704" s="50"/>
+      <c r="B704" s="7" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="705" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A705" s="50"/>
+      <c r="B705" s="7" t="s">
+        <v>526</v>
+      </c>
+    </row>
+    <row r="706" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A706" s="50"/>
+      <c r="B706" s="34" t="s">
+        <v>527</v>
+      </c>
+    </row>
+    <row r="707" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A707" s="50"/>
+      <c r="B707" s="7" t="s">
+        <v>528</v>
+      </c>
+    </row>
+    <row r="708" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A708" s="50"/>
+      <c r="B708" s="7" t="s">
+        <v>529</v>
+      </c>
+    </row>
+    <row r="709" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A709" s="50"/>
+      <c r="B709" s="7" t="s">
+        <v>530</v>
+      </c>
+    </row>
+    <row r="710" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A710" s="50"/>
+      <c r="B710" s="7" t="s">
+        <v>473</v>
+      </c>
+    </row>
+    <row r="711" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A711" s="50"/>
+      <c r="B711" s="7" t="s">
+        <v>531</v>
+      </c>
+    </row>
+    <row r="712" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A712" s="50"/>
+      <c r="B712" s="7" t="s">
+        <v>532</v>
+      </c>
+    </row>
+    <row r="713" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A713" s="50"/>
+      <c r="B713" s="11" t="s">
+        <v>533</v>
+      </c>
+    </row>
+    <row r="714" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A714" s="50"/>
+      <c r="B714" s="34" t="s">
+        <v>534</v>
+      </c>
+    </row>
+    <row r="715" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A715" s="50"/>
+      <c r="B715" s="7" t="s">
+        <v>535</v>
+      </c>
+    </row>
+    <row r="716" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A716" s="50"/>
+      <c r="B716" s="34" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="717" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A717" s="50"/>
+      <c r="B717" s="7" t="s">
+        <v>536</v>
+      </c>
+    </row>
+    <row r="718" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A718" s="51"/>
+      <c r="B718" s="42"/>
+    </row>
   </sheetData>
-  <mergeCells count="52">
-    <mergeCell ref="A686:A700"/>
-    <mergeCell ref="A563:A584"/>
-    <mergeCell ref="A637:A644"/>
-    <mergeCell ref="A297:A309"/>
-    <mergeCell ref="A523:A544"/>
-    <mergeCell ref="A667:A672"/>
-    <mergeCell ref="A646:A650"/>
-    <mergeCell ref="A586:A635"/>
-    <mergeCell ref="A546:A561"/>
-    <mergeCell ref="A503:A521"/>
-    <mergeCell ref="A652:A665"/>
-    <mergeCell ref="A276:A295"/>
-    <mergeCell ref="A356:A364"/>
-    <mergeCell ref="A330:A342"/>
-    <mergeCell ref="A311:A318"/>
-    <mergeCell ref="A490:A501"/>
-    <mergeCell ref="A454:A465"/>
-    <mergeCell ref="A467:A488"/>
-    <mergeCell ref="A104:A109"/>
-    <mergeCell ref="A56:A62"/>
-    <mergeCell ref="A48:A54"/>
-    <mergeCell ref="A97:A102"/>
-    <mergeCell ref="A88:A95"/>
-    <mergeCell ref="A81:A86"/>
-    <mergeCell ref="A64:A78"/>
-    <mergeCell ref="A2:A6"/>
-    <mergeCell ref="A37:A46"/>
-    <mergeCell ref="A29:A35"/>
-    <mergeCell ref="A16:A27"/>
-    <mergeCell ref="A8:A14"/>
-    <mergeCell ref="A126:A132"/>
-    <mergeCell ref="A189:A196"/>
-    <mergeCell ref="A174:A187"/>
-    <mergeCell ref="A159:A172"/>
-    <mergeCell ref="A146:A156"/>
-    <mergeCell ref="A134:A144"/>
-    <mergeCell ref="A674:A684"/>
+  <mergeCells count="53">
+    <mergeCell ref="A702:A718"/>
     <mergeCell ref="A111:A116"/>
     <mergeCell ref="A217:A228"/>
     <mergeCell ref="A248:A260"/>
@@ -32134,6 +33010,43 @@
     <mergeCell ref="A239:A246"/>
     <mergeCell ref="A198:A215"/>
     <mergeCell ref="A118:A124"/>
+    <mergeCell ref="A126:A132"/>
+    <mergeCell ref="A189:A196"/>
+    <mergeCell ref="A174:A187"/>
+    <mergeCell ref="A159:A172"/>
+    <mergeCell ref="A146:A156"/>
+    <mergeCell ref="A134:A144"/>
+    <mergeCell ref="A2:A6"/>
+    <mergeCell ref="A37:A46"/>
+    <mergeCell ref="A29:A35"/>
+    <mergeCell ref="A16:A27"/>
+    <mergeCell ref="A8:A14"/>
+    <mergeCell ref="A104:A109"/>
+    <mergeCell ref="A56:A62"/>
+    <mergeCell ref="A48:A54"/>
+    <mergeCell ref="A97:A102"/>
+    <mergeCell ref="A88:A95"/>
+    <mergeCell ref="A81:A86"/>
+    <mergeCell ref="A64:A78"/>
+    <mergeCell ref="A276:A295"/>
+    <mergeCell ref="A356:A364"/>
+    <mergeCell ref="A330:A342"/>
+    <mergeCell ref="A311:A318"/>
+    <mergeCell ref="A490:A501"/>
+    <mergeCell ref="A454:A465"/>
+    <mergeCell ref="A467:A488"/>
+    <mergeCell ref="A686:A700"/>
+    <mergeCell ref="A563:A584"/>
+    <mergeCell ref="A637:A644"/>
+    <mergeCell ref="A297:A309"/>
+    <mergeCell ref="A523:A544"/>
+    <mergeCell ref="A667:A672"/>
+    <mergeCell ref="A646:A650"/>
+    <mergeCell ref="A586:A635"/>
+    <mergeCell ref="A546:A561"/>
+    <mergeCell ref="A503:A521"/>
+    <mergeCell ref="A652:A665"/>
+    <mergeCell ref="A674:A684"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Criei o ex053 com for e planilha
</commit_message>
<xml_diff>
--- a/detalhesPython.xlsx
+++ b/detalhesPython.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\thiag\Documents\EstudosT\python\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3D0BC93-EC88-4C06-B13F-280C8BDB343F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D5F5AEB-9835-4749-8B17-4FD8A69129A5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{ECBDB9F7-0FAD-476C-A4A4-7948F29B869E}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="619" uniqueCount="537">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="632" uniqueCount="548">
   <si>
     <t>Descrição</t>
   </si>
@@ -27660,6 +27660,627 @@
         <family val="3"/>
       </rPr>
       <t>'E por isso ele NÃO É PRIMO!'</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>)</t>
+    </r>
+  </si>
+  <si>
+    <t>ex053</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">frase </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>=</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color rgb="FF988BC7"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>str</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>(</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF988BC7"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>input</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>(</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE7DE79"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>'Digite uma frase: '</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>)).</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF67E480"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>strip</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>().</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF67E480"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>upper</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>()</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">palavras </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>=</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> frase.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF67E480"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>split</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>()</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">junto </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>=</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE7DE79"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>''</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF67E480"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>join</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>(palavras)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">inverso </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>=</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE7DE79"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>''</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>for</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> letra </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>in</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF988BC7"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>range</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>(</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF988BC7"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>len</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">(junto) </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>-</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF78D1E1"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>1</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>-</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF78D1E1"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>1</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>-</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF78D1E1"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>1</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>):</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">    inverso </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>+=</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> junto[letra]</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>print</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>(</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE7DE79"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">'O inverso de </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF78D1E1"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>{}</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE7DE79"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> é </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF78D1E1"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>{}</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE7DE79"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>'</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF67E480"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>format</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>(junto, inverso))</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>if</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> inverso </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>==</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> junto:</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">    </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF988BC7"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>print</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>(</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE7DE79"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>'Temos um palíndromo!'</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">    </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF988BC7"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>print</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>(</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE7DE79"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>'A frase digitada não é palíndromo!'</t>
     </r>
     <r>
       <rPr>
@@ -27777,7 +28398,7 @@
       <family val="3"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -27793,6 +28414,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="1"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -28130,7 +28757,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="52">
+  <cellXfs count="56">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -28278,6 +28905,18 @@
     </xf>
     <xf numFmtId="0" fontId="11" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -28906,10 +29545,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{73331524-72FC-41A3-82E6-4326A0999772}">
-  <dimension ref="A1:G718"/>
+  <dimension ref="A1:G752"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A693" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C715" sqref="C715"/>
+    <sheetView tabSelected="1" topLeftCell="A722" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B740" sqref="B740"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -32992,8 +33631,205 @@
       <c r="A718" s="51"/>
       <c r="B718" s="42"/>
     </row>
+    <row r="719" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="720" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A720" s="49" t="s">
+        <v>537</v>
+      </c>
+      <c r="B720" s="31" t="s">
+        <v>429</v>
+      </c>
+    </row>
+    <row r="721" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A721" s="50"/>
+      <c r="B721" s="40"/>
+    </row>
+    <row r="722" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A722" s="50"/>
+      <c r="B722" s="52" t="s">
+        <v>538</v>
+      </c>
+    </row>
+    <row r="723" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A723" s="50"/>
+      <c r="B723" s="52" t="s">
+        <v>539</v>
+      </c>
+    </row>
+    <row r="724" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A724" s="50"/>
+      <c r="B724" s="52" t="s">
+        <v>540</v>
+      </c>
+    </row>
+    <row r="725" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A725" s="50"/>
+      <c r="B725" s="52" t="s">
+        <v>541</v>
+      </c>
+    </row>
+    <row r="726" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A726" s="50"/>
+      <c r="B726" s="53" t="s">
+        <v>542</v>
+      </c>
+    </row>
+    <row r="727" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A727" s="50"/>
+      <c r="B727" s="52" t="s">
+        <v>543</v>
+      </c>
+    </row>
+    <row r="728" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A728" s="50"/>
+      <c r="B728" s="54" t="s">
+        <v>544</v>
+      </c>
+    </row>
+    <row r="729" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A729" s="50"/>
+      <c r="B729" s="53" t="s">
+        <v>545</v>
+      </c>
+    </row>
+    <row r="730" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A730" s="50"/>
+      <c r="B730" s="52" t="s">
+        <v>546</v>
+      </c>
+    </row>
+    <row r="731" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A731" s="50"/>
+      <c r="B731" s="53" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="732" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A732" s="50"/>
+      <c r="B732" s="52" t="s">
+        <v>547</v>
+      </c>
+    </row>
+    <row r="733" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A733" s="50"/>
+      <c r="B733" s="7"/>
+    </row>
+    <row r="734" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A734" s="50"/>
+      <c r="B734" s="55"/>
+    </row>
+    <row r="735" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A735" s="50"/>
+      <c r="B735" s="7"/>
+    </row>
+    <row r="736" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A736" s="50"/>
+      <c r="B736" s="7"/>
+    </row>
+    <row r="737" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A737" s="50"/>
+      <c r="B737" s="7"/>
+    </row>
+    <row r="738" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A738" s="50"/>
+      <c r="B738" s="7"/>
+    </row>
+    <row r="739" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A739" s="50"/>
+      <c r="B739" s="7"/>
+    </row>
+    <row r="740" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A740" s="50"/>
+      <c r="B740" s="7"/>
+    </row>
+    <row r="741" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A741" s="50"/>
+      <c r="B741" s="7"/>
+    </row>
+    <row r="742" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A742" s="50"/>
+      <c r="B742" s="7"/>
+    </row>
+    <row r="743" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A743" s="50"/>
+      <c r="B743" s="7"/>
+    </row>
+    <row r="744" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A744" s="50"/>
+      <c r="B744" s="7"/>
+    </row>
+    <row r="745" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A745" s="50"/>
+      <c r="B745" s="7"/>
+    </row>
+    <row r="746" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A746" s="50"/>
+      <c r="B746" s="7"/>
+    </row>
+    <row r="747" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A747" s="50"/>
+      <c r="B747" s="34"/>
+    </row>
+    <row r="748" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A748" s="50"/>
+      <c r="B748" s="7"/>
+    </row>
+    <row r="749" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A749" s="50"/>
+      <c r="B749" s="7"/>
+    </row>
+    <row r="750" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A750" s="50"/>
+      <c r="B750" s="7"/>
+    </row>
+    <row r="751" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A751" s="50"/>
+      <c r="B751" s="7"/>
+    </row>
+    <row r="752" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A752" s="51"/>
+      <c r="B752" s="42"/>
+    </row>
   </sheetData>
-  <mergeCells count="53">
+  <mergeCells count="54">
+    <mergeCell ref="A720:A752"/>
+    <mergeCell ref="A686:A700"/>
+    <mergeCell ref="A563:A584"/>
+    <mergeCell ref="A637:A644"/>
+    <mergeCell ref="A297:A309"/>
+    <mergeCell ref="A523:A544"/>
+    <mergeCell ref="A667:A672"/>
+    <mergeCell ref="A646:A650"/>
+    <mergeCell ref="A586:A635"/>
+    <mergeCell ref="A546:A561"/>
+    <mergeCell ref="A503:A521"/>
+    <mergeCell ref="A652:A665"/>
+    <mergeCell ref="A674:A684"/>
+    <mergeCell ref="A276:A295"/>
+    <mergeCell ref="A356:A364"/>
+    <mergeCell ref="A330:A342"/>
+    <mergeCell ref="A311:A318"/>
+    <mergeCell ref="A490:A501"/>
+    <mergeCell ref="A454:A465"/>
+    <mergeCell ref="A467:A488"/>
+    <mergeCell ref="A104:A109"/>
+    <mergeCell ref="A56:A62"/>
+    <mergeCell ref="A48:A54"/>
+    <mergeCell ref="A97:A102"/>
+    <mergeCell ref="A88:A95"/>
+    <mergeCell ref="A81:A86"/>
+    <mergeCell ref="A64:A78"/>
+    <mergeCell ref="A2:A6"/>
+    <mergeCell ref="A37:A46"/>
+    <mergeCell ref="A29:A35"/>
+    <mergeCell ref="A16:A27"/>
+    <mergeCell ref="A8:A14"/>
+    <mergeCell ref="A126:A132"/>
+    <mergeCell ref="A189:A196"/>
+    <mergeCell ref="A174:A187"/>
+    <mergeCell ref="A159:A172"/>
+    <mergeCell ref="A146:A156"/>
+    <mergeCell ref="A134:A144"/>
     <mergeCell ref="A702:A718"/>
     <mergeCell ref="A111:A116"/>
     <mergeCell ref="A217:A228"/>
@@ -33010,43 +33846,6 @@
     <mergeCell ref="A239:A246"/>
     <mergeCell ref="A198:A215"/>
     <mergeCell ref="A118:A124"/>
-    <mergeCell ref="A126:A132"/>
-    <mergeCell ref="A189:A196"/>
-    <mergeCell ref="A174:A187"/>
-    <mergeCell ref="A159:A172"/>
-    <mergeCell ref="A146:A156"/>
-    <mergeCell ref="A134:A144"/>
-    <mergeCell ref="A2:A6"/>
-    <mergeCell ref="A37:A46"/>
-    <mergeCell ref="A29:A35"/>
-    <mergeCell ref="A16:A27"/>
-    <mergeCell ref="A8:A14"/>
-    <mergeCell ref="A104:A109"/>
-    <mergeCell ref="A56:A62"/>
-    <mergeCell ref="A48:A54"/>
-    <mergeCell ref="A97:A102"/>
-    <mergeCell ref="A88:A95"/>
-    <mergeCell ref="A81:A86"/>
-    <mergeCell ref="A64:A78"/>
-    <mergeCell ref="A276:A295"/>
-    <mergeCell ref="A356:A364"/>
-    <mergeCell ref="A330:A342"/>
-    <mergeCell ref="A311:A318"/>
-    <mergeCell ref="A490:A501"/>
-    <mergeCell ref="A454:A465"/>
-    <mergeCell ref="A467:A488"/>
-    <mergeCell ref="A686:A700"/>
-    <mergeCell ref="A563:A584"/>
-    <mergeCell ref="A637:A644"/>
-    <mergeCell ref="A297:A309"/>
-    <mergeCell ref="A523:A544"/>
-    <mergeCell ref="A667:A672"/>
-    <mergeCell ref="A646:A650"/>
-    <mergeCell ref="A586:A635"/>
-    <mergeCell ref="A546:A561"/>
-    <mergeCell ref="A503:A521"/>
-    <mergeCell ref="A652:A665"/>
-    <mergeCell ref="A674:A684"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Atualizado o ex053 e planilha
</commit_message>
<xml_diff>
--- a/detalhesPython.xlsx
+++ b/detalhesPython.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\thiag\Documents\EstudosT\python\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D5F5AEB-9835-4749-8B17-4FD8A69129A5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2EA1E12F-FF07-4D00-BA3D-9E5D55383AA4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{ECBDB9F7-0FAD-476C-A4A4-7948F29B869E}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="632" uniqueCount="548">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="649" uniqueCount="556">
   <si>
     <t>Descrição</t>
   </si>
@@ -28291,6 +28291,77 @@
       </rPr>
       <t>)</t>
     </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">inverso </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>=</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> junto[</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>::-</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF78D1E1"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>1</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>]</t>
+    </r>
+  </si>
+  <si>
+    <t>1ª FORMA, USANDO FOR:</t>
+  </si>
+  <si>
+    <t>2º FORMA, USANDO FATIAMENTO:</t>
+  </si>
+  <si>
+    <t>Usado o .strip() para tirar os espaços do começo e do fim da frase</t>
+  </si>
+  <si>
+    <t>Usado o .upper() para deixar a frase toda com letras maiúsculas</t>
+  </si>
+  <si>
+    <t>Usado o frase.split() para pegar a frase e separar em uma lista</t>
+  </si>
+  <si>
+    <t>Usado o ''.join(palavras) para juntar todas as palavras da lista, o asterisco sem nada é para tirar os espaços! Se fosse '*' ficaria THIAGO*HENRIQUE</t>
+  </si>
+  <si>
+    <t>O for ficou muito confuso pra mim, se precisar é melhor assistir a aula novamente: https://www.youtube.com/watch?v=5VBWe6BXzRo&amp;t=657s</t>
   </si>
 </sst>
 </file>
@@ -28398,7 +28469,7 @@
       <family val="3"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -28414,12 +28485,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="1"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -28757,7 +28822,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="56">
+  <cellXfs count="53">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -28906,18 +28971,7 @@
     <xf numFmtId="0" fontId="11" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -29078,7 +29132,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>16</xdr:col>
-      <xdr:colOff>456171</xdr:colOff>
+      <xdr:colOff>456170</xdr:colOff>
       <xdr:row>392</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
@@ -29210,7 +29264,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>28</xdr:col>
-      <xdr:colOff>496147</xdr:colOff>
+      <xdr:colOff>496148</xdr:colOff>
       <xdr:row>392</xdr:row>
       <xdr:rowOff>34122</xdr:rowOff>
     </xdr:to>
@@ -29545,16 +29599,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{73331524-72FC-41A3-82E6-4326A0999772}">
-  <dimension ref="A1:G752"/>
+  <dimension ref="A1:G755"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A722" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B740" sqref="B740"/>
+    <sheetView tabSelected="1" topLeftCell="A717" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="A720" sqref="A720:A755"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9.85546875" style="2" customWidth="1"/>
-    <col min="2" max="2" width="168.140625" style="2" customWidth="1"/>
+    <col min="2" max="2" width="175.140625" style="2" customWidth="1"/>
     <col min="3" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
@@ -33646,89 +33700,93 @@
     </row>
     <row r="722" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A722" s="50"/>
-      <c r="B722" s="52" t="s">
-        <v>538</v>
+      <c r="B722" s="7" t="s">
+        <v>549</v>
       </c>
     </row>
     <row r="723" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A723" s="50"/>
-      <c r="B723" s="52" t="s">
-        <v>539</v>
-      </c>
+      <c r="B723" s="7"/>
     </row>
     <row r="724" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A724" s="50"/>
-      <c r="B724" s="52" t="s">
-        <v>540</v>
+      <c r="B724" s="7" t="s">
+        <v>538</v>
       </c>
     </row>
     <row r="725" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A725" s="50"/>
-      <c r="B725" s="52" t="s">
-        <v>541</v>
+      <c r="B725" s="7" t="s">
+        <v>539</v>
       </c>
     </row>
     <row r="726" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A726" s="50"/>
-      <c r="B726" s="53" t="s">
-        <v>542</v>
+      <c r="B726" s="7" t="s">
+        <v>540</v>
       </c>
     </row>
     <row r="727" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A727" s="50"/>
-      <c r="B727" s="52" t="s">
-        <v>543</v>
+      <c r="B727" s="7" t="s">
+        <v>541</v>
       </c>
     </row>
     <row r="728" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A728" s="50"/>
-      <c r="B728" s="54" t="s">
-        <v>544</v>
+      <c r="B728" s="34" t="s">
+        <v>542</v>
       </c>
     </row>
     <row r="729" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A729" s="50"/>
-      <c r="B729" s="53" t="s">
-        <v>545</v>
+      <c r="B729" s="7" t="s">
+        <v>543</v>
       </c>
     </row>
     <row r="730" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A730" s="50"/>
-      <c r="B730" s="52" t="s">
-        <v>546</v>
+      <c r="B730" s="11" t="s">
+        <v>544</v>
       </c>
     </row>
     <row r="731" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A731" s="50"/>
-      <c r="B731" s="53" t="s">
-        <v>243</v>
+      <c r="B731" s="34" t="s">
+        <v>545</v>
       </c>
     </row>
     <row r="732" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A732" s="50"/>
-      <c r="B732" s="52" t="s">
-        <v>547</v>
+      <c r="B732" s="7" t="s">
+        <v>546</v>
       </c>
     </row>
     <row r="733" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A733" s="50"/>
-      <c r="B733" s="7"/>
+      <c r="B733" s="34" t="s">
+        <v>243</v>
+      </c>
     </row>
     <row r="734" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A734" s="50"/>
-      <c r="B734" s="55"/>
-    </row>
-    <row r="735" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B734" s="7" t="s">
+        <v>547</v>
+      </c>
+    </row>
+    <row r="735" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A735" s="50"/>
       <c r="B735" s="7"/>
     </row>
     <row r="736" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A736" s="50"/>
-      <c r="B736" s="7"/>
+      <c r="B736" s="40"/>
     </row>
     <row r="737" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A737" s="50"/>
-      <c r="B737" s="7"/>
+      <c r="B737" s="7" t="s">
+        <v>550</v>
+      </c>
     </row>
     <row r="738" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A738" s="50"/>
@@ -33736,39 +33794,57 @@
     </row>
     <row r="739" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A739" s="50"/>
-      <c r="B739" s="7"/>
+      <c r="B739" s="7" t="s">
+        <v>538</v>
+      </c>
     </row>
     <row r="740" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A740" s="50"/>
-      <c r="B740" s="7"/>
+      <c r="B740" s="7" t="s">
+        <v>539</v>
+      </c>
     </row>
     <row r="741" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A741" s="50"/>
-      <c r="B741" s="7"/>
+      <c r="B741" s="7" t="s">
+        <v>540</v>
+      </c>
     </row>
     <row r="742" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A742" s="50"/>
-      <c r="B742" s="7"/>
+      <c r="B742" s="7" t="s">
+        <v>548</v>
+      </c>
     </row>
     <row r="743" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A743" s="50"/>
-      <c r="B743" s="7"/>
+      <c r="B743" s="11" t="s">
+        <v>544</v>
+      </c>
     </row>
     <row r="744" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A744" s="50"/>
-      <c r="B744" s="7"/>
+      <c r="B744" s="34" t="s">
+        <v>545</v>
+      </c>
     </row>
     <row r="745" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A745" s="50"/>
-      <c r="B745" s="7"/>
+      <c r="B745" s="7" t="s">
+        <v>546</v>
+      </c>
     </row>
     <row r="746" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A746" s="50"/>
-      <c r="B746" s="7"/>
+      <c r="B746" s="34" t="s">
+        <v>243</v>
+      </c>
     </row>
     <row r="747" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A747" s="50"/>
-      <c r="B747" s="34"/>
+      <c r="B747" s="7" t="s">
+        <v>547</v>
+      </c>
     </row>
     <row r="748" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A748" s="50"/>
@@ -33776,61 +33852,46 @@
     </row>
     <row r="749" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A749" s="50"/>
-      <c r="B749" s="7"/>
+      <c r="B749" s="36" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="750" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A750" s="50"/>
-      <c r="B750" s="7"/>
+      <c r="B750" s="36" t="s">
+        <v>551</v>
+      </c>
     </row>
     <row r="751" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A751" s="50"/>
-      <c r="B751" s="7"/>
-    </row>
-    <row r="752" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A752" s="51"/>
-      <c r="B752" s="42"/>
+      <c r="B751" s="36" t="s">
+        <v>552</v>
+      </c>
+    </row>
+    <row r="752" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A752" s="50"/>
+      <c r="B752" s="36" t="s">
+        <v>553</v>
+      </c>
+    </row>
+    <row r="753" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A753" s="50"/>
+      <c r="B753" s="36" t="s">
+        <v>554</v>
+      </c>
+    </row>
+    <row r="754" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A754" s="50"/>
+      <c r="B754" s="36" t="s">
+        <v>555</v>
+      </c>
+    </row>
+    <row r="755" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A755" s="51"/>
+      <c r="B755" s="52"/>
     </row>
   </sheetData>
   <mergeCells count="54">
-    <mergeCell ref="A720:A752"/>
-    <mergeCell ref="A686:A700"/>
-    <mergeCell ref="A563:A584"/>
-    <mergeCell ref="A637:A644"/>
-    <mergeCell ref="A297:A309"/>
-    <mergeCell ref="A523:A544"/>
-    <mergeCell ref="A667:A672"/>
-    <mergeCell ref="A646:A650"/>
-    <mergeCell ref="A586:A635"/>
-    <mergeCell ref="A546:A561"/>
-    <mergeCell ref="A503:A521"/>
-    <mergeCell ref="A652:A665"/>
-    <mergeCell ref="A674:A684"/>
-    <mergeCell ref="A276:A295"/>
-    <mergeCell ref="A356:A364"/>
-    <mergeCell ref="A330:A342"/>
-    <mergeCell ref="A311:A318"/>
-    <mergeCell ref="A490:A501"/>
-    <mergeCell ref="A454:A465"/>
-    <mergeCell ref="A467:A488"/>
-    <mergeCell ref="A104:A109"/>
-    <mergeCell ref="A56:A62"/>
-    <mergeCell ref="A48:A54"/>
-    <mergeCell ref="A97:A102"/>
-    <mergeCell ref="A88:A95"/>
-    <mergeCell ref="A81:A86"/>
-    <mergeCell ref="A64:A78"/>
-    <mergeCell ref="A2:A6"/>
-    <mergeCell ref="A37:A46"/>
-    <mergeCell ref="A29:A35"/>
-    <mergeCell ref="A16:A27"/>
-    <mergeCell ref="A8:A14"/>
-    <mergeCell ref="A126:A132"/>
-    <mergeCell ref="A189:A196"/>
-    <mergeCell ref="A174:A187"/>
-    <mergeCell ref="A159:A172"/>
-    <mergeCell ref="A146:A156"/>
-    <mergeCell ref="A134:A144"/>
-    <mergeCell ref="A702:A718"/>
     <mergeCell ref="A111:A116"/>
     <mergeCell ref="A217:A228"/>
     <mergeCell ref="A248:A260"/>
@@ -33846,6 +33907,45 @@
     <mergeCell ref="A239:A246"/>
     <mergeCell ref="A198:A215"/>
     <mergeCell ref="A118:A124"/>
+    <mergeCell ref="A126:A132"/>
+    <mergeCell ref="A189:A196"/>
+    <mergeCell ref="A174:A187"/>
+    <mergeCell ref="A159:A172"/>
+    <mergeCell ref="A146:A156"/>
+    <mergeCell ref="A134:A144"/>
+    <mergeCell ref="A2:A6"/>
+    <mergeCell ref="A37:A46"/>
+    <mergeCell ref="A29:A35"/>
+    <mergeCell ref="A16:A27"/>
+    <mergeCell ref="A8:A14"/>
+    <mergeCell ref="A104:A109"/>
+    <mergeCell ref="A56:A62"/>
+    <mergeCell ref="A48:A54"/>
+    <mergeCell ref="A97:A102"/>
+    <mergeCell ref="A88:A95"/>
+    <mergeCell ref="A81:A86"/>
+    <mergeCell ref="A64:A78"/>
+    <mergeCell ref="A276:A295"/>
+    <mergeCell ref="A356:A364"/>
+    <mergeCell ref="A330:A342"/>
+    <mergeCell ref="A311:A318"/>
+    <mergeCell ref="A490:A501"/>
+    <mergeCell ref="A454:A465"/>
+    <mergeCell ref="A467:A488"/>
+    <mergeCell ref="A720:A755"/>
+    <mergeCell ref="A686:A700"/>
+    <mergeCell ref="A563:A584"/>
+    <mergeCell ref="A637:A644"/>
+    <mergeCell ref="A297:A309"/>
+    <mergeCell ref="A523:A544"/>
+    <mergeCell ref="A667:A672"/>
+    <mergeCell ref="A646:A650"/>
+    <mergeCell ref="A586:A635"/>
+    <mergeCell ref="A546:A561"/>
+    <mergeCell ref="A503:A521"/>
+    <mergeCell ref="A652:A665"/>
+    <mergeCell ref="A674:A684"/>
+    <mergeCell ref="A702:A718"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Criei o ex055 e Planilha
</commit_message>
<xml_diff>
--- a/detalhesPython.xlsx
+++ b/detalhesPython.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\thiag\Documents\EstudosT\python\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{779A26D6-744F-44EF-ACC2-4777B643BD57}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D622811-3861-4DB1-B39C-2C7687F37E0C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{ECBDB9F7-0FAD-476C-A4A4-7948F29B869E}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="664" uniqueCount="569">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="680" uniqueCount="584">
   <si>
     <t>Descrição</t>
   </si>
@@ -28936,6 +28936,645 @@
         <family val="3"/>
       </rPr>
       <t>(totmenor))</t>
+    </r>
+  </si>
+  <si>
+    <t>ex055</t>
+  </si>
+  <si>
+    <t>Faça um programa que leia o peso de cinco pessoas. No final, mostre qual foi o maior e o menor peso lidos.</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">maiorpeso </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>=</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF78D1E1"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>0</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">menorpeso </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>=</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF78D1E1"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>0</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>for</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> c </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>in</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF988BC7"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>range</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>(</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF78D1E1"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>1</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF78D1E1"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>6</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>):</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">    peso </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>=</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color rgb="FF988BC7"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>float</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>(</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF988BC7"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>input</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>(</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE7DE79"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">'Peso da </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF78D1E1"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>{}</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE7DE79"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>ª pessoa: '</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF67E480"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>format</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>(c)))</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">    </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>if</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> c </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>==</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF78D1E1"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>1</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>:</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">        maiorpeso </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>=</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> peso</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">        menorpeso </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>=</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> peso</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">        </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>if</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> peso </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> maiorpeso:</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">            maiorpeso </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>=</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> peso</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">        </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>if</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> peso </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>&lt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> menorpeso:</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">            menorpeso </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>=</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> peso</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>print</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>(</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE7DE79"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">'O MAIOR peso informado foi: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF78D1E1"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>{}</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE7DE79"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>kg'</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF67E480"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>format</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>(maiorpeso))</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>print</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>(</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE7DE79"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">'O MENOR peso informado foi: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF78D1E1"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>{}</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE7DE79"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>kg'</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF67E480"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>format</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>(menorpeso))</t>
     </r>
   </si>
 </sst>
@@ -30174,10 +30813,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{73331524-72FC-41A3-82E6-4326A0999772}">
-  <dimension ref="A1:G772"/>
+  <dimension ref="A1:G790"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A751" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B774" sqref="B774"/>
+    <sheetView tabSelected="1" topLeftCell="A768" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B780" sqref="B780"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -34560,47 +35199,110 @@
       <c r="A772" s="52"/>
       <c r="B772" s="42"/>
     </row>
+    <row r="773" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="774" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A774" s="50" t="s">
+        <v>569</v>
+      </c>
+      <c r="B774" s="31" t="s">
+        <v>570</v>
+      </c>
+    </row>
+    <row r="775" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A775" s="51"/>
+      <c r="B775" s="40"/>
+    </row>
+    <row r="776" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A776" s="51"/>
+      <c r="B776" s="7" t="s">
+        <v>571</v>
+      </c>
+    </row>
+    <row r="777" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A777" s="51"/>
+      <c r="B777" s="7" t="s">
+        <v>572</v>
+      </c>
+    </row>
+    <row r="778" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A778" s="51"/>
+      <c r="B778" s="34" t="s">
+        <v>573</v>
+      </c>
+    </row>
+    <row r="779" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A779" s="51"/>
+      <c r="B779" s="7" t="s">
+        <v>574</v>
+      </c>
+    </row>
+    <row r="780" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A780" s="51"/>
+      <c r="B780" s="7" t="s">
+        <v>575</v>
+      </c>
+    </row>
+    <row r="781" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A781" s="51"/>
+      <c r="B781" s="7" t="s">
+        <v>576</v>
+      </c>
+    </row>
+    <row r="782" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A782" s="51"/>
+      <c r="B782" s="7" t="s">
+        <v>577</v>
+      </c>
+    </row>
+    <row r="783" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A783" s="51"/>
+      <c r="B783" s="7" t="s">
+        <v>473</v>
+      </c>
+    </row>
+    <row r="784" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A784" s="51"/>
+      <c r="B784" s="7" t="s">
+        <v>578</v>
+      </c>
+    </row>
+    <row r="785" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A785" s="51"/>
+      <c r="B785" s="7" t="s">
+        <v>579</v>
+      </c>
+    </row>
+    <row r="786" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A786" s="51"/>
+      <c r="B786" s="7" t="s">
+        <v>580</v>
+      </c>
+    </row>
+    <row r="787" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A787" s="51"/>
+      <c r="B787" s="7" t="s">
+        <v>581</v>
+      </c>
+    </row>
+    <row r="788" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A788" s="51"/>
+      <c r="B788" s="11" t="s">
+        <v>582</v>
+      </c>
+    </row>
+    <row r="789" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A789" s="51"/>
+      <c r="B789" s="11" t="s">
+        <v>583</v>
+      </c>
+    </row>
+    <row r="790" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A790" s="52"/>
+      <c r="B790" s="42"/>
+    </row>
   </sheetData>
-  <mergeCells count="55">
-    <mergeCell ref="A757:A772"/>
-    <mergeCell ref="A720:A755"/>
-    <mergeCell ref="A686:A700"/>
-    <mergeCell ref="A563:A584"/>
-    <mergeCell ref="A637:A644"/>
-    <mergeCell ref="A297:A309"/>
-    <mergeCell ref="A523:A544"/>
-    <mergeCell ref="A667:A672"/>
-    <mergeCell ref="A646:A650"/>
-    <mergeCell ref="A586:A635"/>
-    <mergeCell ref="A546:A561"/>
-    <mergeCell ref="A503:A521"/>
-    <mergeCell ref="A652:A665"/>
-    <mergeCell ref="A674:A684"/>
-    <mergeCell ref="A702:A718"/>
-    <mergeCell ref="A276:A295"/>
-    <mergeCell ref="A356:A364"/>
-    <mergeCell ref="A330:A342"/>
-    <mergeCell ref="A311:A318"/>
-    <mergeCell ref="A490:A501"/>
-    <mergeCell ref="A454:A465"/>
-    <mergeCell ref="A467:A488"/>
-    <mergeCell ref="A104:A109"/>
-    <mergeCell ref="A56:A62"/>
-    <mergeCell ref="A48:A54"/>
-    <mergeCell ref="A97:A102"/>
-    <mergeCell ref="A88:A95"/>
-    <mergeCell ref="A81:A86"/>
-    <mergeCell ref="A64:A78"/>
-    <mergeCell ref="A2:A6"/>
-    <mergeCell ref="A37:A46"/>
-    <mergeCell ref="A29:A35"/>
-    <mergeCell ref="A16:A27"/>
-    <mergeCell ref="A8:A14"/>
-    <mergeCell ref="A189:A196"/>
-    <mergeCell ref="A174:A187"/>
-    <mergeCell ref="A159:A172"/>
-    <mergeCell ref="A146:A156"/>
-    <mergeCell ref="A134:A144"/>
+  <mergeCells count="56">
+    <mergeCell ref="A774:A790"/>
     <mergeCell ref="A111:A116"/>
     <mergeCell ref="A217:A228"/>
     <mergeCell ref="A248:A260"/>
@@ -34617,6 +35319,45 @@
     <mergeCell ref="A198:A215"/>
     <mergeCell ref="A118:A124"/>
     <mergeCell ref="A126:A132"/>
+    <mergeCell ref="A189:A196"/>
+    <mergeCell ref="A174:A187"/>
+    <mergeCell ref="A159:A172"/>
+    <mergeCell ref="A146:A156"/>
+    <mergeCell ref="A134:A144"/>
+    <mergeCell ref="A2:A6"/>
+    <mergeCell ref="A37:A46"/>
+    <mergeCell ref="A29:A35"/>
+    <mergeCell ref="A16:A27"/>
+    <mergeCell ref="A8:A14"/>
+    <mergeCell ref="A104:A109"/>
+    <mergeCell ref="A56:A62"/>
+    <mergeCell ref="A48:A54"/>
+    <mergeCell ref="A97:A102"/>
+    <mergeCell ref="A88:A95"/>
+    <mergeCell ref="A81:A86"/>
+    <mergeCell ref="A64:A78"/>
+    <mergeCell ref="A276:A295"/>
+    <mergeCell ref="A356:A364"/>
+    <mergeCell ref="A330:A342"/>
+    <mergeCell ref="A311:A318"/>
+    <mergeCell ref="A490:A501"/>
+    <mergeCell ref="A454:A465"/>
+    <mergeCell ref="A467:A488"/>
+    <mergeCell ref="A297:A309"/>
+    <mergeCell ref="A523:A544"/>
+    <mergeCell ref="A667:A672"/>
+    <mergeCell ref="A646:A650"/>
+    <mergeCell ref="A586:A635"/>
+    <mergeCell ref="A546:A561"/>
+    <mergeCell ref="A503:A521"/>
+    <mergeCell ref="A652:A665"/>
+    <mergeCell ref="A757:A772"/>
+    <mergeCell ref="A720:A755"/>
+    <mergeCell ref="A686:A700"/>
+    <mergeCell ref="A563:A584"/>
+    <mergeCell ref="A637:A644"/>
+    <mergeCell ref="A674:A684"/>
+    <mergeCell ref="A702:A718"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Atualizado o ex057 e planilha
</commit_message>
<xml_diff>
--- a/detalhesPython.xlsx
+++ b/detalhesPython.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\thiag\Documents\EstudosT\python\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83D6E589-C88A-4DE2-8DC8-108D23D92763}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6BD93F4A-94F5-4DBF-97D9-F935579C5301}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{ECBDB9F7-0FAD-476C-A4A4-7948F29B869E}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="706" uniqueCount="607">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="714" uniqueCount="614">
   <si>
     <t>Descrição</t>
   </si>
@@ -30876,6 +30876,415 @@
   </si>
   <si>
     <t>nomevelho = ''  ---&gt; Para informar variável para string, usar o aspas em branco....</t>
+  </si>
+  <si>
+    <t>ex057</t>
+  </si>
+  <si>
+    <t>Faça um programa que leia o sexo de uma pessoa, mas só aceite os valores ‘M’ ou ‘F’. Caso esteja errado, peça a digitação novamente até ter um valor correto.</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">sexo </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>=</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color rgb="FF988BC7"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>str</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>(</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF988BC7"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>input</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>(</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE7DE79"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>'Digite seu sexo: [M/F] '</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>)).</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF67E480"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>strip</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>().</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF67E480"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>upper</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>()[</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF78D1E1"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>0</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>]</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>while</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> sexo </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>not</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>in</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE7DE79"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>'MmFf'</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>:</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">    sexo </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>=</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color rgb="FF988BC7"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>str</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>(</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF988BC7"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>input</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>(</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE7DE79"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>'Opção Inválida! Por favor, informe seu sexo: '</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>)).</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF67E480"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>strip</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>().</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF67E480"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>upper</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>()[</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF78D1E1"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>0</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>]</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>print</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>(</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE7DE79"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">'Sexo </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF78D1E1"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>{}</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE7DE79"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> registrado com sucesso!'</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF67E480"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>format</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>(sexo))</t>
+    </r>
+  </si>
+  <si>
+    <t>.upper()[0]  ---&gt; Serve para variável sexo coletar somente o caractere 0 de python, ou o primeiro.</t>
   </si>
 </sst>
 </file>
@@ -31336,7 +31745,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="56">
+  <cellXfs count="53">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -31485,15 +31894,6 @@
     </xf>
     <xf numFmtId="0" fontId="11" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -32122,10 +32522,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{73331524-72FC-41A3-82E6-4326A0999772}">
-  <dimension ref="A1:G819"/>
+  <dimension ref="A1:G830"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A789" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A792" sqref="A792:A819"/>
+    <sheetView tabSelected="1" topLeftCell="A799" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B828" sqref="B828"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -36624,133 +37024,133 @@
     </row>
     <row r="794" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A794" s="51"/>
-      <c r="B794" s="53" t="s">
+      <c r="B794" s="7" t="s">
         <v>586</v>
       </c>
     </row>
     <row r="795" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A795" s="51"/>
-      <c r="B795" s="53" t="s">
+      <c r="B795" s="7" t="s">
         <v>587</v>
       </c>
     </row>
     <row r="796" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A796" s="51"/>
-      <c r="B796" s="53" t="s">
+      <c r="B796" s="7" t="s">
         <v>588</v>
       </c>
     </row>
     <row r="797" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A797" s="51"/>
-      <c r="B797" s="53" t="s">
+      <c r="B797" s="7" t="s">
         <v>589</v>
       </c>
     </row>
     <row r="798" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A798" s="51"/>
-      <c r="B798" s="54" t="s">
+      <c r="B798" s="34" t="s">
         <v>590</v>
       </c>
     </row>
     <row r="799" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A799" s="51"/>
-      <c r="B799" s="53" t="s">
+      <c r="B799" s="7" t="s">
         <v>591</v>
       </c>
     </row>
     <row r="800" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A800" s="51"/>
-      <c r="B800" s="53" t="s">
+      <c r="B800" s="7" t="s">
         <v>592</v>
       </c>
     </row>
     <row r="801" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A801" s="51"/>
-      <c r="B801" s="53" t="s">
+      <c r="B801" s="7" t="s">
         <v>593</v>
       </c>
     </row>
     <row r="802" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A802" s="51"/>
-      <c r="B802" s="53" t="s">
+      <c r="B802" s="7" t="s">
         <v>594</v>
       </c>
     </row>
     <row r="803" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A803" s="51"/>
-      <c r="B803" s="53" t="s">
+      <c r="B803" s="7" t="s">
         <v>595</v>
       </c>
     </row>
     <row r="804" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A804" s="51"/>
-      <c r="B804" s="53" t="s">
+      <c r="B804" s="7" t="s">
         <v>596</v>
       </c>
     </row>
     <row r="805" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A805" s="51"/>
-      <c r="B805" s="53" t="s">
+      <c r="B805" s="7" t="s">
         <v>597</v>
       </c>
     </row>
     <row r="806" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A806" s="51"/>
-      <c r="B806" s="53" t="s">
+      <c r="B806" s="7" t="s">
         <v>598</v>
       </c>
     </row>
     <row r="807" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A807" s="51"/>
-      <c r="B807" s="53" t="s">
+      <c r="B807" s="7" t="s">
         <v>599</v>
       </c>
     </row>
     <row r="808" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A808" s="51"/>
-      <c r="B808" s="53" t="s">
+      <c r="B808" s="7" t="s">
         <v>597</v>
       </c>
     </row>
     <row r="809" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A809" s="51"/>
-      <c r="B809" s="53" t="s">
+      <c r="B809" s="7" t="s">
         <v>598</v>
       </c>
     </row>
     <row r="810" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A810" s="51"/>
-      <c r="B810" s="53" t="s">
+      <c r="B810" s="7" t="s">
         <v>600</v>
       </c>
     </row>
     <row r="811" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A811" s="51"/>
-      <c r="B811" s="53" t="s">
+      <c r="B811" s="7" t="s">
         <v>601</v>
       </c>
     </row>
     <row r="812" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A812" s="51"/>
-      <c r="B812" s="53" t="s">
+      <c r="B812" s="7" t="s">
         <v>602</v>
       </c>
     </row>
     <row r="813" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A813" s="51"/>
-      <c r="B813" s="55" t="s">
+      <c r="B813" s="11" t="s">
         <v>603</v>
       </c>
     </row>
     <row r="814" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A814" s="51"/>
-      <c r="B814" s="55" t="s">
+      <c r="B814" s="11" t="s">
         <v>604</v>
       </c>
     </row>
     <row r="815" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A815" s="51"/>
-      <c r="B815" s="55" t="s">
+      <c r="B815" s="11" t="s">
         <v>605</v>
       </c>
     </row>
@@ -36774,8 +37174,107 @@
       <c r="A819" s="52"/>
       <c r="B819" s="42"/>
     </row>
+    <row r="820" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="821" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A821" s="50" t="s">
+        <v>607</v>
+      </c>
+      <c r="B821" s="31" t="s">
+        <v>608</v>
+      </c>
+    </row>
+    <row r="822" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A822" s="51"/>
+      <c r="B822" s="40"/>
+    </row>
+    <row r="823" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A823" s="51"/>
+      <c r="B823" s="7" t="s">
+        <v>609</v>
+      </c>
+    </row>
+    <row r="824" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A824" s="51"/>
+      <c r="B824" s="34" t="s">
+        <v>610</v>
+      </c>
+    </row>
+    <row r="825" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A825" s="51"/>
+      <c r="B825" s="7" t="s">
+        <v>611</v>
+      </c>
+    </row>
+    <row r="826" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A826" s="51"/>
+      <c r="B826" s="11" t="s">
+        <v>612</v>
+      </c>
+    </row>
+    <row r="827" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A827" s="51"/>
+      <c r="B827" s="7"/>
+    </row>
+    <row r="828" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A828" s="51"/>
+      <c r="B828" s="36" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="829" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A829" s="51"/>
+      <c r="B829" s="36" t="s">
+        <v>613</v>
+      </c>
+    </row>
+    <row r="830" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A830" s="52"/>
+      <c r="B830" s="49"/>
+    </row>
   </sheetData>
-  <mergeCells count="57">
+  <mergeCells count="58">
+    <mergeCell ref="A821:A830"/>
+    <mergeCell ref="A111:A116"/>
+    <mergeCell ref="A217:A228"/>
+    <mergeCell ref="A248:A260"/>
+    <mergeCell ref="A408:A429"/>
+    <mergeCell ref="A431:A452"/>
+    <mergeCell ref="A380:A392"/>
+    <mergeCell ref="A394:A406"/>
+    <mergeCell ref="A320:A328"/>
+    <mergeCell ref="A366:A378"/>
+    <mergeCell ref="A344:A354"/>
+    <mergeCell ref="A262:A274"/>
+    <mergeCell ref="A230:A237"/>
+    <mergeCell ref="A239:A246"/>
+    <mergeCell ref="A198:A215"/>
+    <mergeCell ref="A118:A124"/>
+    <mergeCell ref="A126:A132"/>
+    <mergeCell ref="A189:A196"/>
+    <mergeCell ref="A174:A187"/>
+    <mergeCell ref="A159:A172"/>
+    <mergeCell ref="A146:A156"/>
+    <mergeCell ref="A134:A144"/>
+    <mergeCell ref="A2:A6"/>
+    <mergeCell ref="A37:A46"/>
+    <mergeCell ref="A29:A35"/>
+    <mergeCell ref="A16:A27"/>
+    <mergeCell ref="A8:A14"/>
+    <mergeCell ref="A104:A109"/>
+    <mergeCell ref="A56:A62"/>
+    <mergeCell ref="A48:A54"/>
+    <mergeCell ref="A97:A102"/>
+    <mergeCell ref="A88:A95"/>
+    <mergeCell ref="A81:A86"/>
+    <mergeCell ref="A64:A78"/>
+    <mergeCell ref="A276:A295"/>
+    <mergeCell ref="A356:A364"/>
+    <mergeCell ref="A330:A342"/>
+    <mergeCell ref="A311:A318"/>
+    <mergeCell ref="A490:A501"/>
+    <mergeCell ref="A454:A465"/>
+    <mergeCell ref="A467:A488"/>
+    <mergeCell ref="A297:A309"/>
     <mergeCell ref="A792:A819"/>
     <mergeCell ref="A503:A521"/>
     <mergeCell ref="A652:A665"/>
@@ -36791,48 +37290,7 @@
     <mergeCell ref="A646:A650"/>
     <mergeCell ref="A586:A635"/>
     <mergeCell ref="A546:A561"/>
-    <mergeCell ref="A276:A295"/>
-    <mergeCell ref="A356:A364"/>
-    <mergeCell ref="A330:A342"/>
-    <mergeCell ref="A311:A318"/>
-    <mergeCell ref="A490:A501"/>
-    <mergeCell ref="A454:A465"/>
-    <mergeCell ref="A467:A488"/>
-    <mergeCell ref="A297:A309"/>
-    <mergeCell ref="A104:A109"/>
-    <mergeCell ref="A56:A62"/>
-    <mergeCell ref="A48:A54"/>
-    <mergeCell ref="A97:A102"/>
-    <mergeCell ref="A88:A95"/>
-    <mergeCell ref="A81:A86"/>
-    <mergeCell ref="A64:A78"/>
-    <mergeCell ref="A2:A6"/>
-    <mergeCell ref="A37:A46"/>
-    <mergeCell ref="A29:A35"/>
-    <mergeCell ref="A16:A27"/>
-    <mergeCell ref="A8:A14"/>
-    <mergeCell ref="A126:A132"/>
-    <mergeCell ref="A189:A196"/>
-    <mergeCell ref="A174:A187"/>
-    <mergeCell ref="A159:A172"/>
-    <mergeCell ref="A146:A156"/>
-    <mergeCell ref="A134:A144"/>
     <mergeCell ref="A774:A790"/>
-    <mergeCell ref="A111:A116"/>
-    <mergeCell ref="A217:A228"/>
-    <mergeCell ref="A248:A260"/>
-    <mergeCell ref="A408:A429"/>
-    <mergeCell ref="A431:A452"/>
-    <mergeCell ref="A380:A392"/>
-    <mergeCell ref="A394:A406"/>
-    <mergeCell ref="A320:A328"/>
-    <mergeCell ref="A366:A378"/>
-    <mergeCell ref="A344:A354"/>
-    <mergeCell ref="A262:A274"/>
-    <mergeCell ref="A230:A237"/>
-    <mergeCell ref="A239:A246"/>
-    <mergeCell ref="A198:A215"/>
-    <mergeCell ref="A118:A124"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Criei o ex058 e planilha
</commit_message>
<xml_diff>
--- a/detalhesPython.xlsx
+++ b/detalhesPython.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\thiag\Documents\EstudosT\python\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6BD93F4A-94F5-4DBF-97D9-F935579C5301}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{347DCEA8-4E78-4FE3-B532-A46FA5C94936}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{ECBDB9F7-0FAD-476C-A4A4-7948F29B869E}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="714" uniqueCount="614">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="716" uniqueCount="616">
   <si>
     <t>Descrição</t>
   </si>
@@ -31285,6 +31285,12 @@
   </si>
   <si>
     <t>.upper()[0]  ---&gt; Serve para variável sexo coletar somente o caractere 0 de python, ou o primeiro.</t>
+  </si>
+  <si>
+    <t>ex058</t>
+  </si>
+  <si>
+    <t>Melhore o jogo do DESAFIO 28 onde o computador vai “pensar” em um número entre 0 e 10. Só que agora o jogador vai tentar adivinhar até acertar, mostrando no final quantos palpites foram necessários para vencer.</t>
   </si>
 </sst>
 </file>
@@ -32522,10 +32528,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{73331524-72FC-41A3-82E6-4326A0999772}">
-  <dimension ref="A1:G830"/>
+  <dimension ref="A1:G859"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A799" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B828" sqref="B828"/>
+    <sheetView tabSelected="1" topLeftCell="A463" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B475" sqref="B475"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -37231,8 +37237,168 @@
       <c r="A830" s="52"/>
       <c r="B830" s="49"/>
     </row>
+    <row r="831" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="832" spans="1:2" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A832" s="50" t="s">
+        <v>614</v>
+      </c>
+      <c r="B832" s="31" t="s">
+        <v>615</v>
+      </c>
+    </row>
+    <row r="833" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A833" s="51"/>
+      <c r="B833" s="40"/>
+    </row>
+    <row r="834" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A834" s="51"/>
+      <c r="B834" s="7"/>
+    </row>
+    <row r="835" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A835" s="51"/>
+      <c r="B835" s="7"/>
+    </row>
+    <row r="836" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A836" s="51"/>
+      <c r="B836" s="7"/>
+    </row>
+    <row r="837" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A837" s="51"/>
+      <c r="B837" s="7"/>
+    </row>
+    <row r="838" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A838" s="51"/>
+      <c r="B838" s="34"/>
+    </row>
+    <row r="839" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A839" s="51"/>
+      <c r="B839" s="7"/>
+    </row>
+    <row r="840" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A840" s="51"/>
+      <c r="B840" s="7"/>
+    </row>
+    <row r="841" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A841" s="51"/>
+      <c r="B841" s="7"/>
+    </row>
+    <row r="842" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A842" s="51"/>
+      <c r="B842" s="7"/>
+    </row>
+    <row r="843" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A843" s="51"/>
+      <c r="B843" s="7"/>
+    </row>
+    <row r="844" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A844" s="51"/>
+      <c r="B844" s="7"/>
+    </row>
+    <row r="845" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A845" s="51"/>
+      <c r="B845" s="7"/>
+    </row>
+    <row r="846" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A846" s="51"/>
+      <c r="B846" s="7"/>
+    </row>
+    <row r="847" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A847" s="51"/>
+      <c r="B847" s="7"/>
+    </row>
+    <row r="848" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A848" s="51"/>
+      <c r="B848" s="7"/>
+    </row>
+    <row r="849" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A849" s="51"/>
+      <c r="B849" s="7"/>
+    </row>
+    <row r="850" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A850" s="51"/>
+      <c r="B850" s="7"/>
+    </row>
+    <row r="851" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A851" s="51"/>
+      <c r="B851" s="7"/>
+    </row>
+    <row r="852" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A852" s="51"/>
+      <c r="B852" s="7"/>
+    </row>
+    <row r="853" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A853" s="51"/>
+      <c r="B853" s="11"/>
+    </row>
+    <row r="854" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A854" s="51"/>
+      <c r="B854" s="11"/>
+    </row>
+    <row r="855" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A855" s="51"/>
+      <c r="B855" s="11"/>
+    </row>
+    <row r="856" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A856" s="51"/>
+      <c r="B856" s="7"/>
+    </row>
+    <row r="857" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A857" s="51"/>
+      <c r="B857" s="36"/>
+    </row>
+    <row r="858" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A858" s="51"/>
+      <c r="B858" s="36"/>
+    </row>
+    <row r="859" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A859" s="52"/>
+      <c r="B859" s="42"/>
+    </row>
   </sheetData>
-  <mergeCells count="58">
+  <mergeCells count="59">
+    <mergeCell ref="A832:A859"/>
+    <mergeCell ref="A792:A819"/>
+    <mergeCell ref="A503:A521"/>
+    <mergeCell ref="A652:A665"/>
+    <mergeCell ref="A757:A772"/>
+    <mergeCell ref="A720:A755"/>
+    <mergeCell ref="A686:A700"/>
+    <mergeCell ref="A563:A584"/>
+    <mergeCell ref="A637:A644"/>
+    <mergeCell ref="A674:A684"/>
+    <mergeCell ref="A702:A718"/>
+    <mergeCell ref="A523:A544"/>
+    <mergeCell ref="A667:A672"/>
+    <mergeCell ref="A646:A650"/>
+    <mergeCell ref="A586:A635"/>
+    <mergeCell ref="A546:A561"/>
+    <mergeCell ref="A774:A790"/>
+    <mergeCell ref="A276:A295"/>
+    <mergeCell ref="A356:A364"/>
+    <mergeCell ref="A330:A342"/>
+    <mergeCell ref="A311:A318"/>
+    <mergeCell ref="A490:A501"/>
+    <mergeCell ref="A454:A465"/>
+    <mergeCell ref="A467:A488"/>
+    <mergeCell ref="A297:A309"/>
+    <mergeCell ref="A104:A109"/>
+    <mergeCell ref="A56:A62"/>
+    <mergeCell ref="A48:A54"/>
+    <mergeCell ref="A97:A102"/>
+    <mergeCell ref="A88:A95"/>
+    <mergeCell ref="A81:A86"/>
+    <mergeCell ref="A64:A78"/>
+    <mergeCell ref="A2:A6"/>
+    <mergeCell ref="A37:A46"/>
+    <mergeCell ref="A29:A35"/>
+    <mergeCell ref="A16:A27"/>
+    <mergeCell ref="A8:A14"/>
+    <mergeCell ref="A126:A132"/>
+    <mergeCell ref="A189:A196"/>
+    <mergeCell ref="A174:A187"/>
+    <mergeCell ref="A159:A172"/>
+    <mergeCell ref="A146:A156"/>
+    <mergeCell ref="A134:A144"/>
     <mergeCell ref="A821:A830"/>
     <mergeCell ref="A111:A116"/>
     <mergeCell ref="A217:A228"/>
@@ -37249,48 +37415,6 @@
     <mergeCell ref="A239:A246"/>
     <mergeCell ref="A198:A215"/>
     <mergeCell ref="A118:A124"/>
-    <mergeCell ref="A126:A132"/>
-    <mergeCell ref="A189:A196"/>
-    <mergeCell ref="A174:A187"/>
-    <mergeCell ref="A159:A172"/>
-    <mergeCell ref="A146:A156"/>
-    <mergeCell ref="A134:A144"/>
-    <mergeCell ref="A2:A6"/>
-    <mergeCell ref="A37:A46"/>
-    <mergeCell ref="A29:A35"/>
-    <mergeCell ref="A16:A27"/>
-    <mergeCell ref="A8:A14"/>
-    <mergeCell ref="A104:A109"/>
-    <mergeCell ref="A56:A62"/>
-    <mergeCell ref="A48:A54"/>
-    <mergeCell ref="A97:A102"/>
-    <mergeCell ref="A88:A95"/>
-    <mergeCell ref="A81:A86"/>
-    <mergeCell ref="A64:A78"/>
-    <mergeCell ref="A276:A295"/>
-    <mergeCell ref="A356:A364"/>
-    <mergeCell ref="A330:A342"/>
-    <mergeCell ref="A311:A318"/>
-    <mergeCell ref="A490:A501"/>
-    <mergeCell ref="A454:A465"/>
-    <mergeCell ref="A467:A488"/>
-    <mergeCell ref="A297:A309"/>
-    <mergeCell ref="A792:A819"/>
-    <mergeCell ref="A503:A521"/>
-    <mergeCell ref="A652:A665"/>
-    <mergeCell ref="A757:A772"/>
-    <mergeCell ref="A720:A755"/>
-    <mergeCell ref="A686:A700"/>
-    <mergeCell ref="A563:A584"/>
-    <mergeCell ref="A637:A644"/>
-    <mergeCell ref="A674:A684"/>
-    <mergeCell ref="A702:A718"/>
-    <mergeCell ref="A523:A544"/>
-    <mergeCell ref="A667:A672"/>
-    <mergeCell ref="A646:A650"/>
-    <mergeCell ref="A586:A635"/>
-    <mergeCell ref="A546:A561"/>
-    <mergeCell ref="A774:A790"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Atualizado o ex058.py e planilha
</commit_message>
<xml_diff>
--- a/detalhesPython.xlsx
+++ b/detalhesPython.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\thiag\Documents\EstudosT\python\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{347DCEA8-4E78-4FE3-B532-A46FA5C94936}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{121E337C-EEE0-4346-A900-5E0C6A551AF1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{ECBDB9F7-0FAD-476C-A4A4-7948F29B869E}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="716" uniqueCount="616">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="737" uniqueCount="633">
   <si>
     <t>Descrição</t>
   </si>
@@ -31291,6 +31291,747 @@
   </si>
   <si>
     <t>Melhore o jogo do DESAFIO 28 onde o computador vai “pensar” em um número entre 0 e 10. Só que agora o jogador vai tentar adivinhar até acertar, mostrando no final quantos palpites foram necessários para vencer.</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">tentativas </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>=</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF78D1E1"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>0</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">computador </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>=</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF67E480"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>randint</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>(</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF78D1E1"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>0</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF78D1E1"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>10</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>print</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>(</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE7DE79"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>'-'</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>*</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF78D1E1"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>70</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>print</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>(</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE7DE79"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>'Sou seu computador! Adivinhe o número que estou pensando entre 0 e 10.'</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">acertou </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>=</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF78D1E1"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>False</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">palpites </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>=</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF78D1E1"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>0</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>while</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>not</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> acertou:</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">    jogador </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>=</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color rgb="FF988BC7"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>int</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>(</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF988BC7"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>input</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>(</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE7DE79"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>'</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>\n</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE7DE79"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>Qual é o seu palpite? '</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>))</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">    palpites </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>+=</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF78D1E1"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>1</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">    </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>if</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> jogador </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>==</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> computador:</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">        acertou </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>=</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF78D1E1"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>True</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">        </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>if</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> jogador </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>&lt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> computador:</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">            </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF988BC7"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>print</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>(</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE7DE79"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>'Mais... Tente novamente!'</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">        </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>else</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>:</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">            </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF988BC7"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>print</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>(</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE7DE79"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>'Menos... Tente novamente!'</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>print</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>(</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE7DE79"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>'</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>\n</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE7DE79"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">Você acertou com </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF78D1E1"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>{}</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE7DE79"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> tentativas. Parabéns!'</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF67E480"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>format</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>(palpites))</t>
+    </r>
+  </si>
+  <si>
+    <t>o randint(0, 10)  ---&gt; Ele realmente escolhe de 0 à 10. E não de 0 à 9.</t>
   </si>
 </sst>
 </file>
@@ -32528,10 +33269,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{73331524-72FC-41A3-82E6-4326A0999772}">
-  <dimension ref="A1:G859"/>
+  <dimension ref="A1:G856"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A463" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B475" sqref="B475"/>
+    <sheetView tabSelected="1" topLeftCell="A831" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="A832" sqref="A832:A856"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -37252,79 +37993,117 @@
     </row>
     <row r="834" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A834" s="51"/>
-      <c r="B834" s="7"/>
+      <c r="B834" s="34" t="s">
+        <v>233</v>
+      </c>
     </row>
     <row r="835" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A835" s="51"/>
-      <c r="B835" s="7"/>
+      <c r="B835" s="7" t="s">
+        <v>616</v>
+      </c>
     </row>
     <row r="836" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A836" s="51"/>
-      <c r="B836" s="7"/>
+      <c r="B836" s="7" t="s">
+        <v>617</v>
+      </c>
     </row>
     <row r="837" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A837" s="51"/>
-      <c r="B837" s="7"/>
+      <c r="B837" s="11" t="s">
+        <v>618</v>
+      </c>
     </row>
     <row r="838" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A838" s="51"/>
-      <c r="B838" s="34"/>
+      <c r="B838" s="11" t="s">
+        <v>619</v>
+      </c>
     </row>
     <row r="839" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A839" s="51"/>
-      <c r="B839" s="7"/>
+      <c r="B839" s="11" t="s">
+        <v>618</v>
+      </c>
     </row>
     <row r="840" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A840" s="51"/>
-      <c r="B840" s="7"/>
+      <c r="B840" s="7" t="s">
+        <v>620</v>
+      </c>
     </row>
     <row r="841" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A841" s="51"/>
-      <c r="B841" s="7"/>
+      <c r="B841" s="7" t="s">
+        <v>621</v>
+      </c>
     </row>
     <row r="842" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A842" s="51"/>
-      <c r="B842" s="7"/>
+      <c r="B842" s="34" t="s">
+        <v>622</v>
+      </c>
     </row>
     <row r="843" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A843" s="51"/>
-      <c r="B843" s="7"/>
+      <c r="B843" s="7" t="s">
+        <v>623</v>
+      </c>
     </row>
     <row r="844" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A844" s="51"/>
-      <c r="B844" s="7"/>
+      <c r="B844" s="7" t="s">
+        <v>624</v>
+      </c>
     </row>
     <row r="845" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A845" s="51"/>
-      <c r="B845" s="7"/>
+      <c r="B845" s="7" t="s">
+        <v>625</v>
+      </c>
     </row>
     <row r="846" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A846" s="51"/>
-      <c r="B846" s="7"/>
+      <c r="B846" s="7" t="s">
+        <v>626</v>
+      </c>
     </row>
     <row r="847" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A847" s="51"/>
-      <c r="B847" s="7"/>
+      <c r="B847" s="7" t="s">
+        <v>473</v>
+      </c>
     </row>
     <row r="848" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A848" s="51"/>
-      <c r="B848" s="7"/>
+      <c r="B848" s="7" t="s">
+        <v>627</v>
+      </c>
     </row>
     <row r="849" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A849" s="51"/>
-      <c r="B849" s="7"/>
+      <c r="B849" s="7" t="s">
+        <v>628</v>
+      </c>
     </row>
     <row r="850" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A850" s="51"/>
-      <c r="B850" s="7"/>
+      <c r="B850" s="7" t="s">
+        <v>629</v>
+      </c>
     </row>
     <row r="851" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A851" s="51"/>
-      <c r="B851" s="7"/>
+      <c r="B851" s="7" t="s">
+        <v>630</v>
+      </c>
     </row>
     <row r="852" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A852" s="51"/>
-      <c r="B852" s="7"/>
+      <c r="B852" s="11" t="s">
+        <v>631</v>
+      </c>
     </row>
     <row r="853" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A853" s="51"/>
@@ -37332,73 +38111,22 @@
     </row>
     <row r="854" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A854" s="51"/>
-      <c r="B854" s="11"/>
+      <c r="B854" s="36" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="855" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A855" s="51"/>
-      <c r="B855" s="11"/>
-    </row>
-    <row r="856" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A856" s="51"/>
-      <c r="B856" s="7"/>
-    </row>
-    <row r="857" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A857" s="51"/>
-      <c r="B857" s="36"/>
-    </row>
-    <row r="858" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A858" s="51"/>
-      <c r="B858" s="36"/>
-    </row>
-    <row r="859" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A859" s="52"/>
-      <c r="B859" s="42"/>
+      <c r="B855" s="36" t="s">
+        <v>632</v>
+      </c>
+    </row>
+    <row r="856" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A856" s="52"/>
+      <c r="B856" s="42"/>
     </row>
   </sheetData>
   <mergeCells count="59">
-    <mergeCell ref="A832:A859"/>
-    <mergeCell ref="A792:A819"/>
-    <mergeCell ref="A503:A521"/>
-    <mergeCell ref="A652:A665"/>
-    <mergeCell ref="A757:A772"/>
-    <mergeCell ref="A720:A755"/>
-    <mergeCell ref="A686:A700"/>
-    <mergeCell ref="A563:A584"/>
-    <mergeCell ref="A637:A644"/>
-    <mergeCell ref="A674:A684"/>
-    <mergeCell ref="A702:A718"/>
-    <mergeCell ref="A523:A544"/>
-    <mergeCell ref="A667:A672"/>
-    <mergeCell ref="A646:A650"/>
-    <mergeCell ref="A586:A635"/>
-    <mergeCell ref="A546:A561"/>
-    <mergeCell ref="A774:A790"/>
-    <mergeCell ref="A276:A295"/>
-    <mergeCell ref="A356:A364"/>
-    <mergeCell ref="A330:A342"/>
-    <mergeCell ref="A311:A318"/>
-    <mergeCell ref="A490:A501"/>
-    <mergeCell ref="A454:A465"/>
-    <mergeCell ref="A467:A488"/>
-    <mergeCell ref="A297:A309"/>
-    <mergeCell ref="A104:A109"/>
-    <mergeCell ref="A56:A62"/>
-    <mergeCell ref="A48:A54"/>
-    <mergeCell ref="A97:A102"/>
-    <mergeCell ref="A88:A95"/>
-    <mergeCell ref="A81:A86"/>
-    <mergeCell ref="A64:A78"/>
-    <mergeCell ref="A2:A6"/>
-    <mergeCell ref="A37:A46"/>
-    <mergeCell ref="A29:A35"/>
-    <mergeCell ref="A16:A27"/>
-    <mergeCell ref="A8:A14"/>
-    <mergeCell ref="A126:A132"/>
-    <mergeCell ref="A189:A196"/>
-    <mergeCell ref="A174:A187"/>
-    <mergeCell ref="A159:A172"/>
-    <mergeCell ref="A146:A156"/>
-    <mergeCell ref="A134:A144"/>
     <mergeCell ref="A821:A830"/>
     <mergeCell ref="A111:A116"/>
     <mergeCell ref="A217:A228"/>
@@ -37415,6 +38143,49 @@
     <mergeCell ref="A239:A246"/>
     <mergeCell ref="A198:A215"/>
     <mergeCell ref="A118:A124"/>
+    <mergeCell ref="A126:A132"/>
+    <mergeCell ref="A189:A196"/>
+    <mergeCell ref="A174:A187"/>
+    <mergeCell ref="A159:A172"/>
+    <mergeCell ref="A146:A156"/>
+    <mergeCell ref="A134:A144"/>
+    <mergeCell ref="A2:A6"/>
+    <mergeCell ref="A37:A46"/>
+    <mergeCell ref="A29:A35"/>
+    <mergeCell ref="A16:A27"/>
+    <mergeCell ref="A8:A14"/>
+    <mergeCell ref="A104:A109"/>
+    <mergeCell ref="A56:A62"/>
+    <mergeCell ref="A48:A54"/>
+    <mergeCell ref="A97:A102"/>
+    <mergeCell ref="A88:A95"/>
+    <mergeCell ref="A81:A86"/>
+    <mergeCell ref="A64:A78"/>
+    <mergeCell ref="A774:A790"/>
+    <mergeCell ref="A276:A295"/>
+    <mergeCell ref="A356:A364"/>
+    <mergeCell ref="A330:A342"/>
+    <mergeCell ref="A311:A318"/>
+    <mergeCell ref="A490:A501"/>
+    <mergeCell ref="A454:A465"/>
+    <mergeCell ref="A467:A488"/>
+    <mergeCell ref="A297:A309"/>
+    <mergeCell ref="A832:A856"/>
+    <mergeCell ref="A792:A819"/>
+    <mergeCell ref="A503:A521"/>
+    <mergeCell ref="A652:A665"/>
+    <mergeCell ref="A757:A772"/>
+    <mergeCell ref="A720:A755"/>
+    <mergeCell ref="A686:A700"/>
+    <mergeCell ref="A563:A584"/>
+    <mergeCell ref="A637:A644"/>
+    <mergeCell ref="A674:A684"/>
+    <mergeCell ref="A702:A718"/>
+    <mergeCell ref="A523:A544"/>
+    <mergeCell ref="A667:A672"/>
+    <mergeCell ref="A646:A650"/>
+    <mergeCell ref="A586:A635"/>
+    <mergeCell ref="A546:A561"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Alterado o ex059 e planilha
</commit_message>
<xml_diff>
--- a/detalhesPython.xlsx
+++ b/detalhesPython.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\thiag\Documents\EstudosT\python\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Thiago Henrique\Documents\EstudosT\python\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{121E337C-EEE0-4346-A900-5E0C6A551AF1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{080B0975-0848-49D3-94D1-B1C9042BA918}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{ECBDB9F7-0FAD-476C-A4A4-7948F29B869E}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="15990" xr2:uid="{ECBDB9F7-0FAD-476C-A4A4-7948F29B869E}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="737" uniqueCount="633">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="780" uniqueCount="673">
   <si>
     <t>Descrição</t>
   </si>
@@ -32032,6 +32032,1963 @@
   </si>
   <si>
     <t>o randint(0, 10)  ---&gt; Ele realmente escolhe de 0 à 10. E não de 0 à 9.</t>
+  </si>
+  <si>
+    <t>ex059</t>
+  </si>
+  <si>
+    <t>Crie um programa que leia dois valores e mostre um menu na tela:</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">primeiro </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>=</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color rgb="FF988BC7"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>int</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>(</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF988BC7"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>input</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>(</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE7DE79"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>'Primeiro valor: '</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>))</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">segundo </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>=</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color rgb="FF988BC7"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>int</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>(</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF988BC7"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>input</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>(</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE7DE79"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>'Segundo valor: '</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>))</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">resultado </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>=</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF78D1E1"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>0</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">opção </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>=</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF78D1E1"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>0</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">sair </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>=</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF78D1E1"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>False</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>while</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> opção </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>!=</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF78D1E1"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>5</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>:</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">    </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF988BC7"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>print</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>(</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE7DE79"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>'''</t>
+    </r>
+  </si>
+  <si>
+    <t>    [ 1 ] Somar</t>
+  </si>
+  <si>
+    <t>    [ 2 ] Multiplicar</t>
+  </si>
+  <si>
+    <t>    [ 3 ] Maior</t>
+  </si>
+  <si>
+    <t>    [ 4 ] Novos números</t>
+  </si>
+  <si>
+    <r>
+      <t>    [ 5 ] Sair do programa'''</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">    opção </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>=</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color rgb="FF988BC7"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>int</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>(</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF988BC7"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>input</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>(</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE7DE79"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>'</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>\n</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE7DE79"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>&gt;&gt;&gt;&gt;&gt; Qual é a sua opção? '</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>))</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">    </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF67E480"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>sleep</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>(</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF78D1E1"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>1</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">    </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>if</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> opção </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>==</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF78D1E1"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>1</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>:</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">        resultado </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>=</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> primeiro </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> segundo</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">        </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF988BC7"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>print</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>(</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE7DE79"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>'</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>\n</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE7DE79"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">O resultado da soma de </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF78D1E1"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>{}</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE7DE79"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> + </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF78D1E1"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>{}</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE7DE79"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> = </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF78D1E1"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>{}</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE7DE79"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>'</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF67E480"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>format</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>(primeiro, segundo, resultado))</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">    </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>elif</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> opção </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>==</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF78D1E1"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>2</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>:</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">        resultado </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>=</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> primeiro </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>*</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> segundo</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">        </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF988BC7"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>print</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>(</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE7DE79"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>'</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>\n</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE7DE79"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">O resultado de </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF78D1E1"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>{}</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE7DE79"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> x </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF78D1E1"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>{}</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE7DE79"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> = </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF78D1E1"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>{}</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE7DE79"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>'</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF67E480"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>format</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>(primeiro, segundo, resultado))</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">    </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>elif</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> opção </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>==</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF78D1E1"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>3</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>:</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">        </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>if</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> primeiro </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> segundo:</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">            resultado </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>=</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> primeiro</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">        </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>elif</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> segundo </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> primeiro:</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">            resultado </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>=</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> segundo</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">            </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF988BC7"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>print</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>(</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE7DE79"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>'</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>\n</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE7DE79"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>São IGUAIS!'</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>)            </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">        </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF988BC7"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>print</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>(</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE7DE79"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">'Entre </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF78D1E1"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>{}</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE7DE79"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> e </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF78D1E1"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>{}</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE7DE79"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> o MAIOR é o </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF78D1E1"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>{}</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE7DE79"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>!'</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF67E480"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>format</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>(primeiro, segundo, resultado))</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">    </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>elif</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> opção </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>==</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF78D1E1"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>4</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>:</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">        </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF988BC7"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>print</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>(</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE7DE79"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>'</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>\n</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE7DE79"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>Informe os novos números novamente:'</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">        primeiro </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>=</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color rgb="FF988BC7"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>int</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>(</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF988BC7"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>input</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>(</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE7DE79"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>'Primeiro valor: '</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>))</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">        segundo </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>=</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color rgb="FF988BC7"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>int</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>(</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF988BC7"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>input</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>(</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE7DE79"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>'Segundo valor: '</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>))</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">    </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>elif</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> opção </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>==</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF78D1E1"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>5</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>:</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">        </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF988BC7"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>print</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>(</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE7DE79"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>'Finalizando..'</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">        </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF988BC7"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>print</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>(</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE7DE79"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>'Opção Inválida! Tente novamente!'</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">    </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF988BC7"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>print</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>(</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE7DE79"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>'=-='</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>*</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF78D1E1"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>11</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">    </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF67E480"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>sleep</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>(</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF78D1E1"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>2</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>print</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>(</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE7DE79"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>'Fim do programa! Volte sempre!'</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>print</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>(</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE7DE79"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>'=-='</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>*</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF78D1E1"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>11</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>)</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -33269,10 +35226,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{73331524-72FC-41A3-82E6-4326A0999772}">
-  <dimension ref="A1:G856"/>
+  <dimension ref="A1:G902"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A831" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A832" sqref="A832:A856"/>
+    <sheetView tabSelected="1" topLeftCell="A861" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="A858" sqref="A858:A902"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -38125,8 +40082,319 @@
       <c r="A856" s="52"/>
       <c r="B856" s="42"/>
     </row>
+    <row r="857" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="858" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A858" s="50" t="s">
+        <v>633</v>
+      </c>
+      <c r="B858" s="31" t="s">
+        <v>634</v>
+      </c>
+    </row>
+    <row r="859" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A859" s="51"/>
+      <c r="B859" s="40"/>
+    </row>
+    <row r="860" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A860" s="51"/>
+      <c r="B860" s="34" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="861" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A861" s="51"/>
+      <c r="B861" s="7" t="s">
+        <v>635</v>
+      </c>
+    </row>
+    <row r="862" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A862" s="51"/>
+      <c r="B862" s="7" t="s">
+        <v>636</v>
+      </c>
+    </row>
+    <row r="863" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A863" s="51"/>
+      <c r="B863" s="7" t="s">
+        <v>637</v>
+      </c>
+    </row>
+    <row r="864" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A864" s="51"/>
+      <c r="B864" s="7" t="s">
+        <v>638</v>
+      </c>
+    </row>
+    <row r="865" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A865" s="51"/>
+      <c r="B865" s="7" t="s">
+        <v>639</v>
+      </c>
+    </row>
+    <row r="866" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A866" s="51"/>
+      <c r="B866" s="34" t="s">
+        <v>640</v>
+      </c>
+    </row>
+    <row r="867" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A867" s="51"/>
+      <c r="B867" s="7" t="s">
+        <v>641</v>
+      </c>
+    </row>
+    <row r="868" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A868" s="51"/>
+      <c r="B868" s="45" t="s">
+        <v>642</v>
+      </c>
+    </row>
+    <row r="869" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A869" s="51"/>
+      <c r="B869" s="45" t="s">
+        <v>643</v>
+      </c>
+    </row>
+    <row r="870" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A870" s="51"/>
+      <c r="B870" s="45" t="s">
+        <v>644</v>
+      </c>
+    </row>
+    <row r="871" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A871" s="51"/>
+      <c r="B871" s="45" t="s">
+        <v>645</v>
+      </c>
+    </row>
+    <row r="872" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A872" s="51"/>
+      <c r="B872" s="45" t="s">
+        <v>646</v>
+      </c>
+    </row>
+    <row r="873" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A873" s="51"/>
+      <c r="B873" s="7" t="s">
+        <v>647</v>
+      </c>
+    </row>
+    <row r="874" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A874" s="51"/>
+      <c r="B874" s="7" t="s">
+        <v>648</v>
+      </c>
+    </row>
+    <row r="875" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A875" s="51"/>
+      <c r="B875" s="7" t="s">
+        <v>649</v>
+      </c>
+    </row>
+    <row r="876" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A876" s="51"/>
+      <c r="B876" s="7" t="s">
+        <v>650</v>
+      </c>
+    </row>
+    <row r="877" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A877" s="51"/>
+      <c r="B877" s="7" t="s">
+        <v>651</v>
+      </c>
+    </row>
+    <row r="878" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A878" s="51"/>
+      <c r="B878" s="7" t="s">
+        <v>652</v>
+      </c>
+    </row>
+    <row r="879" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A879" s="51"/>
+      <c r="B879" s="7" t="s">
+        <v>653</v>
+      </c>
+    </row>
+    <row r="880" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A880" s="51"/>
+      <c r="B880" s="7" t="s">
+        <v>654</v>
+      </c>
+    </row>
+    <row r="881" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A881" s="51"/>
+      <c r="B881" s="7" t="s">
+        <v>655</v>
+      </c>
+    </row>
+    <row r="882" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A882" s="51"/>
+      <c r="B882" s="7" t="s">
+        <v>656</v>
+      </c>
+    </row>
+    <row r="883" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A883" s="51"/>
+      <c r="B883" s="7" t="s">
+        <v>657</v>
+      </c>
+    </row>
+    <row r="884" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A884" s="51"/>
+      <c r="B884" s="7" t="s">
+        <v>658</v>
+      </c>
+    </row>
+    <row r="885" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A885" s="51"/>
+      <c r="B885" s="7" t="s">
+        <v>659</v>
+      </c>
+    </row>
+    <row r="886" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A886" s="51"/>
+      <c r="B886" s="7" t="s">
+        <v>629</v>
+      </c>
+    </row>
+    <row r="887" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A887" s="51"/>
+      <c r="B887" s="7" t="s">
+        <v>660</v>
+      </c>
+    </row>
+    <row r="888" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A888" s="51"/>
+      <c r="B888" s="7" t="s">
+        <v>661</v>
+      </c>
+    </row>
+    <row r="889" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A889" s="51"/>
+      <c r="B889" s="7" t="s">
+        <v>662</v>
+      </c>
+    </row>
+    <row r="890" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A890" s="51"/>
+      <c r="B890" s="7" t="s">
+        <v>663</v>
+      </c>
+    </row>
+    <row r="891" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A891" s="51"/>
+      <c r="B891" s="7" t="s">
+        <v>664</v>
+      </c>
+    </row>
+    <row r="892" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A892" s="51"/>
+      <c r="B892" s="7" t="s">
+        <v>665</v>
+      </c>
+    </row>
+    <row r="893" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A893" s="51"/>
+      <c r="B893" s="7" t="s">
+        <v>666</v>
+      </c>
+    </row>
+    <row r="894" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A894" s="51"/>
+      <c r="B894" s="7" t="s">
+        <v>667</v>
+      </c>
+    </row>
+    <row r="895" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A895" s="51"/>
+      <c r="B895" s="7" t="s">
+        <v>473</v>
+      </c>
+    </row>
+    <row r="896" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A896" s="51"/>
+      <c r="B896" s="7" t="s">
+        <v>668</v>
+      </c>
+    </row>
+    <row r="897" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A897" s="51"/>
+      <c r="B897" s="7" t="s">
+        <v>669</v>
+      </c>
+    </row>
+    <row r="898" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A898" s="51"/>
+      <c r="B898" s="7" t="s">
+        <v>670</v>
+      </c>
+    </row>
+    <row r="899" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A899" s="51"/>
+      <c r="B899" s="11" t="s">
+        <v>671</v>
+      </c>
+    </row>
+    <row r="900" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A900" s="51"/>
+      <c r="B900" s="11" t="s">
+        <v>672</v>
+      </c>
+    </row>
+    <row r="901" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A901" s="51"/>
+      <c r="B901" s="11"/>
+    </row>
+    <row r="902" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A902" s="52"/>
+      <c r="B902" s="42"/>
+    </row>
   </sheetData>
-  <mergeCells count="59">
+  <mergeCells count="60">
+    <mergeCell ref="A858:A902"/>
+    <mergeCell ref="A832:A856"/>
+    <mergeCell ref="A792:A819"/>
+    <mergeCell ref="A503:A521"/>
+    <mergeCell ref="A652:A665"/>
+    <mergeCell ref="A757:A772"/>
+    <mergeCell ref="A720:A755"/>
+    <mergeCell ref="A686:A700"/>
+    <mergeCell ref="A563:A584"/>
+    <mergeCell ref="A637:A644"/>
+    <mergeCell ref="A674:A684"/>
+    <mergeCell ref="A702:A718"/>
+    <mergeCell ref="A523:A544"/>
+    <mergeCell ref="A667:A672"/>
+    <mergeCell ref="A646:A650"/>
+    <mergeCell ref="A586:A635"/>
+    <mergeCell ref="A546:A561"/>
+    <mergeCell ref="A774:A790"/>
+    <mergeCell ref="A276:A295"/>
+    <mergeCell ref="A356:A364"/>
+    <mergeCell ref="A330:A342"/>
+    <mergeCell ref="A311:A318"/>
+    <mergeCell ref="A490:A501"/>
+    <mergeCell ref="A454:A465"/>
+    <mergeCell ref="A467:A488"/>
+    <mergeCell ref="A297:A309"/>
+    <mergeCell ref="A104:A109"/>
+    <mergeCell ref="A56:A62"/>
+    <mergeCell ref="A48:A54"/>
+    <mergeCell ref="A97:A102"/>
+    <mergeCell ref="A88:A95"/>
+    <mergeCell ref="A81:A86"/>
+    <mergeCell ref="A64:A78"/>
+    <mergeCell ref="A2:A6"/>
+    <mergeCell ref="A37:A46"/>
+    <mergeCell ref="A29:A35"/>
+    <mergeCell ref="A16:A27"/>
+    <mergeCell ref="A8:A14"/>
+    <mergeCell ref="A126:A132"/>
+    <mergeCell ref="A189:A196"/>
+    <mergeCell ref="A174:A187"/>
+    <mergeCell ref="A159:A172"/>
+    <mergeCell ref="A146:A156"/>
+    <mergeCell ref="A134:A144"/>
     <mergeCell ref="A821:A830"/>
     <mergeCell ref="A111:A116"/>
     <mergeCell ref="A217:A228"/>
@@ -38143,49 +40411,6 @@
     <mergeCell ref="A239:A246"/>
     <mergeCell ref="A198:A215"/>
     <mergeCell ref="A118:A124"/>
-    <mergeCell ref="A126:A132"/>
-    <mergeCell ref="A189:A196"/>
-    <mergeCell ref="A174:A187"/>
-    <mergeCell ref="A159:A172"/>
-    <mergeCell ref="A146:A156"/>
-    <mergeCell ref="A134:A144"/>
-    <mergeCell ref="A2:A6"/>
-    <mergeCell ref="A37:A46"/>
-    <mergeCell ref="A29:A35"/>
-    <mergeCell ref="A16:A27"/>
-    <mergeCell ref="A8:A14"/>
-    <mergeCell ref="A104:A109"/>
-    <mergeCell ref="A56:A62"/>
-    <mergeCell ref="A48:A54"/>
-    <mergeCell ref="A97:A102"/>
-    <mergeCell ref="A88:A95"/>
-    <mergeCell ref="A81:A86"/>
-    <mergeCell ref="A64:A78"/>
-    <mergeCell ref="A774:A790"/>
-    <mergeCell ref="A276:A295"/>
-    <mergeCell ref="A356:A364"/>
-    <mergeCell ref="A330:A342"/>
-    <mergeCell ref="A311:A318"/>
-    <mergeCell ref="A490:A501"/>
-    <mergeCell ref="A454:A465"/>
-    <mergeCell ref="A467:A488"/>
-    <mergeCell ref="A297:A309"/>
-    <mergeCell ref="A832:A856"/>
-    <mergeCell ref="A792:A819"/>
-    <mergeCell ref="A503:A521"/>
-    <mergeCell ref="A652:A665"/>
-    <mergeCell ref="A757:A772"/>
-    <mergeCell ref="A720:A755"/>
-    <mergeCell ref="A686:A700"/>
-    <mergeCell ref="A563:A584"/>
-    <mergeCell ref="A637:A644"/>
-    <mergeCell ref="A674:A684"/>
-    <mergeCell ref="A702:A718"/>
-    <mergeCell ref="A523:A544"/>
-    <mergeCell ref="A667:A672"/>
-    <mergeCell ref="A646:A650"/>
-    <mergeCell ref="A586:A635"/>
-    <mergeCell ref="A546:A561"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Atualizado ex060 calculado matematicamente utilizando o for
</commit_message>
<xml_diff>
--- a/detalhesPython.xlsx
+++ b/detalhesPython.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Thiago Henrique\Documents\EstudosT\python\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{080B0975-0848-49D3-94D1-B1C9042BA918}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AAD9CA10-EAC7-4774-8DC3-1A2D85615472}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="15990" xr2:uid="{ECBDB9F7-0FAD-476C-A4A4-7948F29B869E}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="780" uniqueCount="673">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="807" uniqueCount="694">
   <si>
     <t>Descrição</t>
   </si>
@@ -33989,13 +33989,1230 @@
       </rPr>
       <t>)</t>
     </r>
+  </si>
+  <si>
+    <t>ex060</t>
+  </si>
+  <si>
+    <t>Faça um programa que leia um número qualquer e mostre o seu fatorial.</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">num </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>=</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color rgb="FF988BC7"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>int</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>(</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF988BC7"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>input</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>(</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE7DE79"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>'Digite um número para calcular seu Fatorial: '</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>))</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>print</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>(</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE7DE79"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>'</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>\n</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE7DE79"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">Calculando o </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF78D1E1"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>{}</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE7DE79"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>! = '</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF67E480"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>format</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">(num), </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color rgb="FFE89E64"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>end</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>=</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE7DE79"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>''</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">f </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>=</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF78D1E1"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>1</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>for</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> c </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>in</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF988BC7"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>range</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">(num, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF78D1E1"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>0</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>-</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF78D1E1"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>1</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>):</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">    </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF988BC7"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>print</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>(</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE7DE79"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>'</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF78D1E1"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>{}</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE7DE79"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>'</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF67E480"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>format</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">(c), </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color rgb="FFE89E64"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>end</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>=</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE7DE79"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>''</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">    </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF988BC7"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>print</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>(</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE7DE79"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>' x '</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>if</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> c </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF78D1E1"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>1</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>else</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE7DE79"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>' = '</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">, </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color rgb="FFE89E64"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>end</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>=</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE7DE79"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>''</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">    f </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>*=</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> c</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>print</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>(</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE7DE79"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>'</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF78D1E1"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>{}</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>\n</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE7DE79"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>'</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF67E480"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>format</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>(f))</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>from</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> math </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>import</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> factorial</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">fatorial </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>=</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF67E480"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>factorial</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>(num)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>print</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>(</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE7DE79"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">'O fatorial de </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF78D1E1"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>{}</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE7DE79"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> é </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF78D1E1"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>{}</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE7DE79"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>.'</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF67E480"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>format</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>(num, fatorial))</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">num </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>=</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color rgb="FF988BC7"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>int</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>(</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF988BC7"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>input</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>(</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE7DE79"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>'</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>\n</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE7DE79"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>Digite um número para calcular seu Fatorial: '</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>))</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">c </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>=</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> num           </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF5A4B81"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>#c é o contador</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>print</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>(</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE7DE79"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>'</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>\n</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE7DE79"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">Calculando </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF78D1E1"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>{}</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE7DE79"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>! = '</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF67E480"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>format</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">(num), </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color rgb="FFE89E64"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>end</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>=</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE7DE79"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>''</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>while</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> c </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF78D1E1"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>0</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>:</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">    c </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>-=</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF78D1E1"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>1</t>
+    </r>
+  </si>
+  <si>
+    <t>Exemplo utilizando factorial da biblioteca math:</t>
+  </si>
+  <si>
+    <t>Exemplo calculado matemáticamente utilizando o laço de repetição while:</t>
+  </si>
+  <si>
+    <t>Exemplo calculado matemáticamente utilizando o laço de repetição for:</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="15" x14ac:knownFonts="1">
+  <fonts count="16" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -34092,6 +35309,14 @@
       <i/>
       <sz val="11"/>
       <color rgb="FFE89E64"/>
+      <name val="Consolas"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <i/>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF7030A0"/>
       <name val="Consolas"/>
       <family val="3"/>
     </font>
@@ -34449,7 +35674,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="53">
+  <cellXfs count="55">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -34598,6 +35823,12 @@
     </xf>
     <xf numFmtId="0" fontId="11" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -35226,10 +36457,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{73331524-72FC-41A3-82E6-4326A0999772}">
-  <dimension ref="A1:G902"/>
+  <dimension ref="A1:G938"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A861" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A858" sqref="A858:A902"/>
+    <sheetView tabSelected="1" topLeftCell="A901" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="A904" sqref="A904:A938"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -40349,8 +41580,248 @@
       <c r="A902" s="52"/>
       <c r="B902" s="42"/>
     </row>
+    <row r="903" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="904" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A904" s="50" t="s">
+        <v>673</v>
+      </c>
+      <c r="B904" s="31" t="s">
+        <v>674</v>
+      </c>
+    </row>
+    <row r="905" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A905" s="51"/>
+      <c r="B905" s="40"/>
+    </row>
+    <row r="906" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A906" s="51"/>
+      <c r="B906" s="54" t="s">
+        <v>691</v>
+      </c>
+    </row>
+    <row r="907" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A907" s="51"/>
+      <c r="B907" s="7"/>
+    </row>
+    <row r="908" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A908" s="51"/>
+      <c r="B908" s="34" t="s">
+        <v>683</v>
+      </c>
+    </row>
+    <row r="909" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A909" s="51"/>
+      <c r="B909" s="7" t="s">
+        <v>675</v>
+      </c>
+    </row>
+    <row r="910" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A910" s="51"/>
+      <c r="B910" s="7" t="s">
+        <v>684</v>
+      </c>
+    </row>
+    <row r="911" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A911" s="51"/>
+      <c r="B911" s="11" t="s">
+        <v>685</v>
+      </c>
+    </row>
+    <row r="912" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A912" s="51"/>
+      <c r="B912" s="11"/>
+    </row>
+    <row r="913" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A913" s="51"/>
+      <c r="B913" s="53"/>
+    </row>
+    <row r="914" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A914" s="51"/>
+      <c r="B914" s="54" t="s">
+        <v>692</v>
+      </c>
+    </row>
+    <row r="915" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A915" s="51"/>
+      <c r="B915" s="43"/>
+    </row>
+    <row r="916" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A916" s="51"/>
+      <c r="B916" s="7" t="s">
+        <v>686</v>
+      </c>
+    </row>
+    <row r="917" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A917" s="51"/>
+      <c r="B917" s="7" t="s">
+        <v>687</v>
+      </c>
+    </row>
+    <row r="918" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A918" s="51"/>
+      <c r="B918" s="7" t="s">
+        <v>677</v>
+      </c>
+    </row>
+    <row r="919" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A919" s="51"/>
+      <c r="B919" s="11" t="s">
+        <v>688</v>
+      </c>
+    </row>
+    <row r="920" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A920" s="51"/>
+      <c r="B920" s="34" t="s">
+        <v>689</v>
+      </c>
+    </row>
+    <row r="921" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A921" s="51"/>
+      <c r="B921" s="7" t="s">
+        <v>679</v>
+      </c>
+    </row>
+    <row r="922" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A922" s="51"/>
+      <c r="B922" s="7" t="s">
+        <v>680</v>
+      </c>
+    </row>
+    <row r="923" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A923" s="51"/>
+      <c r="B923" s="7" t="s">
+        <v>681</v>
+      </c>
+    </row>
+    <row r="924" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A924" s="51"/>
+      <c r="B924" s="7" t="s">
+        <v>690</v>
+      </c>
+    </row>
+    <row r="925" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A925" s="51"/>
+      <c r="B925" s="11" t="s">
+        <v>682</v>
+      </c>
+    </row>
+    <row r="926" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A926" s="51"/>
+      <c r="B926" s="11"/>
+    </row>
+    <row r="927" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A927" s="51"/>
+      <c r="B927" s="53"/>
+    </row>
+    <row r="928" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A928" s="51"/>
+      <c r="B928" s="54" t="s">
+        <v>693</v>
+      </c>
+    </row>
+    <row r="929" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A929" s="51"/>
+      <c r="B929" s="43"/>
+    </row>
+    <row r="930" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A930" s="51"/>
+      <c r="B930" s="7" t="s">
+        <v>675</v>
+      </c>
+    </row>
+    <row r="931" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A931" s="51"/>
+      <c r="B931" s="11" t="s">
+        <v>676</v>
+      </c>
+    </row>
+    <row r="932" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A932" s="51"/>
+      <c r="B932" s="7" t="s">
+        <v>677</v>
+      </c>
+    </row>
+    <row r="933" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A933" s="51"/>
+      <c r="B933" s="34" t="s">
+        <v>678</v>
+      </c>
+    </row>
+    <row r="934" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A934" s="51"/>
+      <c r="B934" s="7" t="s">
+        <v>679</v>
+      </c>
+    </row>
+    <row r="935" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A935" s="51"/>
+      <c r="B935" s="7" t="s">
+        <v>680</v>
+      </c>
+    </row>
+    <row r="936" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A936" s="51"/>
+      <c r="B936" s="7" t="s">
+        <v>681</v>
+      </c>
+    </row>
+    <row r="937" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A937" s="51"/>
+      <c r="B937" s="11" t="s">
+        <v>682</v>
+      </c>
+    </row>
+    <row r="938" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A938" s="52"/>
+      <c r="B938" s="42"/>
+    </row>
   </sheetData>
-  <mergeCells count="60">
+  <mergeCells count="61">
+    <mergeCell ref="A904:A938"/>
+    <mergeCell ref="A821:A830"/>
+    <mergeCell ref="A111:A116"/>
+    <mergeCell ref="A217:A228"/>
+    <mergeCell ref="A248:A260"/>
+    <mergeCell ref="A408:A429"/>
+    <mergeCell ref="A431:A452"/>
+    <mergeCell ref="A380:A392"/>
+    <mergeCell ref="A394:A406"/>
+    <mergeCell ref="A320:A328"/>
+    <mergeCell ref="A366:A378"/>
+    <mergeCell ref="A344:A354"/>
+    <mergeCell ref="A262:A274"/>
+    <mergeCell ref="A230:A237"/>
+    <mergeCell ref="A239:A246"/>
+    <mergeCell ref="A198:A215"/>
+    <mergeCell ref="A118:A124"/>
+    <mergeCell ref="A126:A132"/>
+    <mergeCell ref="A189:A196"/>
+    <mergeCell ref="A174:A187"/>
+    <mergeCell ref="A159:A172"/>
+    <mergeCell ref="A146:A156"/>
+    <mergeCell ref="A134:A144"/>
+    <mergeCell ref="A2:A6"/>
+    <mergeCell ref="A37:A46"/>
+    <mergeCell ref="A29:A35"/>
+    <mergeCell ref="A16:A27"/>
+    <mergeCell ref="A8:A14"/>
+    <mergeCell ref="A104:A109"/>
+    <mergeCell ref="A56:A62"/>
+    <mergeCell ref="A48:A54"/>
+    <mergeCell ref="A97:A102"/>
+    <mergeCell ref="A88:A95"/>
+    <mergeCell ref="A81:A86"/>
+    <mergeCell ref="A64:A78"/>
+    <mergeCell ref="A546:A561"/>
+    <mergeCell ref="A774:A790"/>
+    <mergeCell ref="A276:A295"/>
+    <mergeCell ref="A356:A364"/>
+    <mergeCell ref="A330:A342"/>
+    <mergeCell ref="A311:A318"/>
+    <mergeCell ref="A490:A501"/>
+    <mergeCell ref="A454:A465"/>
+    <mergeCell ref="A467:A488"/>
+    <mergeCell ref="A297:A309"/>
     <mergeCell ref="A858:A902"/>
     <mergeCell ref="A832:A856"/>
     <mergeCell ref="A792:A819"/>
@@ -40367,50 +41838,6 @@
     <mergeCell ref="A667:A672"/>
     <mergeCell ref="A646:A650"/>
     <mergeCell ref="A586:A635"/>
-    <mergeCell ref="A546:A561"/>
-    <mergeCell ref="A774:A790"/>
-    <mergeCell ref="A276:A295"/>
-    <mergeCell ref="A356:A364"/>
-    <mergeCell ref="A330:A342"/>
-    <mergeCell ref="A311:A318"/>
-    <mergeCell ref="A490:A501"/>
-    <mergeCell ref="A454:A465"/>
-    <mergeCell ref="A467:A488"/>
-    <mergeCell ref="A297:A309"/>
-    <mergeCell ref="A104:A109"/>
-    <mergeCell ref="A56:A62"/>
-    <mergeCell ref="A48:A54"/>
-    <mergeCell ref="A97:A102"/>
-    <mergeCell ref="A88:A95"/>
-    <mergeCell ref="A81:A86"/>
-    <mergeCell ref="A64:A78"/>
-    <mergeCell ref="A2:A6"/>
-    <mergeCell ref="A37:A46"/>
-    <mergeCell ref="A29:A35"/>
-    <mergeCell ref="A16:A27"/>
-    <mergeCell ref="A8:A14"/>
-    <mergeCell ref="A126:A132"/>
-    <mergeCell ref="A189:A196"/>
-    <mergeCell ref="A174:A187"/>
-    <mergeCell ref="A159:A172"/>
-    <mergeCell ref="A146:A156"/>
-    <mergeCell ref="A134:A144"/>
-    <mergeCell ref="A821:A830"/>
-    <mergeCell ref="A111:A116"/>
-    <mergeCell ref="A217:A228"/>
-    <mergeCell ref="A248:A260"/>
-    <mergeCell ref="A408:A429"/>
-    <mergeCell ref="A431:A452"/>
-    <mergeCell ref="A380:A392"/>
-    <mergeCell ref="A394:A406"/>
-    <mergeCell ref="A320:A328"/>
-    <mergeCell ref="A366:A378"/>
-    <mergeCell ref="A344:A354"/>
-    <mergeCell ref="A262:A274"/>
-    <mergeCell ref="A230:A237"/>
-    <mergeCell ref="A239:A246"/>
-    <mergeCell ref="A198:A215"/>
-    <mergeCell ref="A118:A124"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Criei o ex062 ainda não finalizado
</commit_message>
<xml_diff>
--- a/detalhesPython.xlsx
+++ b/detalhesPython.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Thiago Henrique\Documents\EstudosT\python\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F37BC589-5A82-4E8C-ABE9-94AA348F4EBC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83FA2002-87DB-4E69-9550-6AE137820B0C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="15" windowWidth="29040" windowHeight="15990" xr2:uid="{ECBDB9F7-0FAD-476C-A4A4-7948F29B869E}"/>
+    <workbookView xWindow="-14400" yWindow="135" windowWidth="14400" windowHeight="15750" xr2:uid="{ECBDB9F7-0FAD-476C-A4A4-7948F29B869E}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -37057,8 +37057,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{73331524-72FC-41A3-82E6-4326A0999772}">
   <dimension ref="A1:G957"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A915" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C950" sqref="C950"/>
+    <sheetView tabSelected="1" topLeftCell="A927" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B953" sqref="B953"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -42480,6 +42480,52 @@
     </row>
   </sheetData>
   <mergeCells count="62">
+    <mergeCell ref="A904:A938"/>
+    <mergeCell ref="A821:A830"/>
+    <mergeCell ref="A111:A116"/>
+    <mergeCell ref="A217:A228"/>
+    <mergeCell ref="A248:A260"/>
+    <mergeCell ref="A408:A429"/>
+    <mergeCell ref="A431:A452"/>
+    <mergeCell ref="A380:A392"/>
+    <mergeCell ref="A394:A406"/>
+    <mergeCell ref="A320:A328"/>
+    <mergeCell ref="A366:A378"/>
+    <mergeCell ref="A344:A354"/>
+    <mergeCell ref="A262:A274"/>
+    <mergeCell ref="A230:A237"/>
+    <mergeCell ref="A239:A246"/>
+    <mergeCell ref="A198:A215"/>
+    <mergeCell ref="A118:A124"/>
+    <mergeCell ref="A126:A132"/>
+    <mergeCell ref="A189:A196"/>
+    <mergeCell ref="A174:A187"/>
+    <mergeCell ref="A159:A172"/>
+    <mergeCell ref="A146:A156"/>
+    <mergeCell ref="A134:A144"/>
+    <mergeCell ref="A2:A6"/>
+    <mergeCell ref="A37:A46"/>
+    <mergeCell ref="A29:A35"/>
+    <mergeCell ref="A16:A27"/>
+    <mergeCell ref="A8:A14"/>
+    <mergeCell ref="A104:A109"/>
+    <mergeCell ref="A56:A62"/>
+    <mergeCell ref="A48:A54"/>
+    <mergeCell ref="A97:A102"/>
+    <mergeCell ref="A88:A95"/>
+    <mergeCell ref="A81:A86"/>
+    <mergeCell ref="A64:A78"/>
+    <mergeCell ref="A586:A635"/>
+    <mergeCell ref="A546:A561"/>
+    <mergeCell ref="A774:A790"/>
+    <mergeCell ref="A276:A295"/>
+    <mergeCell ref="A356:A364"/>
+    <mergeCell ref="A330:A342"/>
+    <mergeCell ref="A311:A318"/>
+    <mergeCell ref="A490:A501"/>
+    <mergeCell ref="A454:A465"/>
+    <mergeCell ref="A467:A488"/>
+    <mergeCell ref="A297:A309"/>
     <mergeCell ref="A940:A957"/>
     <mergeCell ref="A858:A902"/>
     <mergeCell ref="A832:A856"/>
@@ -42496,52 +42542,6 @@
     <mergeCell ref="A523:A544"/>
     <mergeCell ref="A667:A672"/>
     <mergeCell ref="A646:A650"/>
-    <mergeCell ref="A586:A635"/>
-    <mergeCell ref="A546:A561"/>
-    <mergeCell ref="A774:A790"/>
-    <mergeCell ref="A276:A295"/>
-    <mergeCell ref="A356:A364"/>
-    <mergeCell ref="A330:A342"/>
-    <mergeCell ref="A311:A318"/>
-    <mergeCell ref="A490:A501"/>
-    <mergeCell ref="A454:A465"/>
-    <mergeCell ref="A467:A488"/>
-    <mergeCell ref="A297:A309"/>
-    <mergeCell ref="A104:A109"/>
-    <mergeCell ref="A56:A62"/>
-    <mergeCell ref="A48:A54"/>
-    <mergeCell ref="A97:A102"/>
-    <mergeCell ref="A88:A95"/>
-    <mergeCell ref="A81:A86"/>
-    <mergeCell ref="A64:A78"/>
-    <mergeCell ref="A2:A6"/>
-    <mergeCell ref="A37:A46"/>
-    <mergeCell ref="A29:A35"/>
-    <mergeCell ref="A16:A27"/>
-    <mergeCell ref="A8:A14"/>
-    <mergeCell ref="A118:A124"/>
-    <mergeCell ref="A126:A132"/>
-    <mergeCell ref="A189:A196"/>
-    <mergeCell ref="A174:A187"/>
-    <mergeCell ref="A159:A172"/>
-    <mergeCell ref="A146:A156"/>
-    <mergeCell ref="A134:A144"/>
-    <mergeCell ref="A904:A938"/>
-    <mergeCell ref="A821:A830"/>
-    <mergeCell ref="A111:A116"/>
-    <mergeCell ref="A217:A228"/>
-    <mergeCell ref="A248:A260"/>
-    <mergeCell ref="A408:A429"/>
-    <mergeCell ref="A431:A452"/>
-    <mergeCell ref="A380:A392"/>
-    <mergeCell ref="A394:A406"/>
-    <mergeCell ref="A320:A328"/>
-    <mergeCell ref="A366:A378"/>
-    <mergeCell ref="A344:A354"/>
-    <mergeCell ref="A262:A274"/>
-    <mergeCell ref="A230:A237"/>
-    <mergeCell ref="A239:A246"/>
-    <mergeCell ref="A198:A215"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Atualizado ex062 e planilha
</commit_message>
<xml_diff>
--- a/detalhesPython.xlsx
+++ b/detalhesPython.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Thiago Henrique\Documents\EstudosT\python\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\thiag\Documents\EstudosT\python\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83FA2002-87DB-4E69-9550-6AE137820B0C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C64AF576-8AB9-40B0-81F1-3F96F500B62B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-14400" yWindow="135" windowWidth="14400" windowHeight="15750" xr2:uid="{ECBDB9F7-0FAD-476C-A4A4-7948F29B869E}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{ECBDB9F7-0FAD-476C-A4A4-7948F29B869E}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="823" uniqueCount="708">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="843" uniqueCount="720">
   <si>
     <t>Descrição</t>
   </si>
@@ -35804,6 +35804,568 @@
   </si>
   <si>
     <t>Utilizando o while não precisa da fórmula matemática.</t>
+  </si>
+  <si>
+    <t>ex062</t>
+  </si>
+  <si>
+    <t>Melhore o DESAFIO 61, perguntando para o usuário se ele quer mostrar mais alguns termos. O programa encerrará quando ele disser que quer mostrar 0 termos.</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">mais </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>=</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF78D1E1"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>10</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">total </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>=</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF78D1E1"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>0</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>while</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> mais </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>!=</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF78D1E1"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>0</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>:</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">    total </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>=</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> total </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> mais</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">    </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>while</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> cont </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>&lt;=</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> total:</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">        </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF988BC7"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>print</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>(</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE7DE79"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>'</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF78D1E1"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>{}</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE7DE79"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> → '</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF67E480"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>format</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">(termo), </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color rgb="FFE89E64"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>end</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>=</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE7DE79"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>''</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">        termo </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>+=</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> razão</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">    </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF988BC7"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>print</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>(</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE7DE79"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>'PAUSA'</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">    mais </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>=</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color rgb="FF988BC7"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>int</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>(</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF988BC7"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>input</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>(</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE7DE79"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>'Quantos termos você quer mostrar a mais? '</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>))</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>print</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>(</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE7DE79"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>'</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>\n</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE7DE79"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">Progressão finalizada com </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF78D1E1"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>{}</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE7DE79"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> termos mostrados.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>\n</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE7DE79"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>'</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF67E480"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>format</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>(total))</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -37055,10 +37617,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{73331524-72FC-41A3-82E6-4326A0999772}">
-  <dimension ref="A1:G957"/>
+  <dimension ref="A1:G979"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A927" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B953" sqref="B953"/>
+    <sheetView tabSelected="1" topLeftCell="A957" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="A959" sqref="A959:A979"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -42478,8 +43040,180 @@
       <c r="A957" s="54"/>
       <c r="B957" s="42"/>
     </row>
+    <row r="958" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="959" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A959" s="52" t="s">
+        <v>708</v>
+      </c>
+      <c r="B959" s="31" t="s">
+        <v>709</v>
+      </c>
+    </row>
+    <row r="960" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A960" s="53"/>
+      <c r="B960" s="40"/>
+    </row>
+    <row r="961" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A961" s="53"/>
+      <c r="B961" s="11" t="s">
+        <v>696</v>
+      </c>
+    </row>
+    <row r="962" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A962" s="53"/>
+      <c r="B962" s="11" t="s">
+        <v>697</v>
+      </c>
+    </row>
+    <row r="963" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A963" s="53"/>
+      <c r="B963" s="11" t="s">
+        <v>696</v>
+      </c>
+    </row>
+    <row r="964" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A964" s="53"/>
+      <c r="B964" s="7" t="s">
+        <v>698</v>
+      </c>
+    </row>
+    <row r="965" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A965" s="53"/>
+      <c r="B965" s="7" t="s">
+        <v>699</v>
+      </c>
+    </row>
+    <row r="966" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A966" s="53"/>
+      <c r="B966" s="7" t="s">
+        <v>700</v>
+      </c>
+    </row>
+    <row r="967" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A967" s="53"/>
+      <c r="B967" s="7" t="s">
+        <v>701</v>
+      </c>
+    </row>
+    <row r="968" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A968" s="53"/>
+      <c r="B968" s="7" t="s">
+        <v>710</v>
+      </c>
+    </row>
+    <row r="969" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A969" s="53"/>
+      <c r="B969" s="7" t="s">
+        <v>711</v>
+      </c>
+    </row>
+    <row r="970" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A970" s="53"/>
+      <c r="B970" s="34" t="s">
+        <v>712</v>
+      </c>
+    </row>
+    <row r="971" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A971" s="53"/>
+      <c r="B971" s="7" t="s">
+        <v>713</v>
+      </c>
+    </row>
+    <row r="972" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A972" s="53"/>
+      <c r="B972" s="7" t="s">
+        <v>714</v>
+      </c>
+    </row>
+    <row r="973" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A973" s="53"/>
+      <c r="B973" s="7" t="s">
+        <v>715</v>
+      </c>
+    </row>
+    <row r="974" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A974" s="53"/>
+      <c r="B974" s="7" t="s">
+        <v>716</v>
+      </c>
+    </row>
+    <row r="975" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A975" s="53"/>
+      <c r="B975" s="7" t="s">
+        <v>498</v>
+      </c>
+    </row>
+    <row r="976" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A976" s="53"/>
+      <c r="B976" s="7" t="s">
+        <v>717</v>
+      </c>
+    </row>
+    <row r="977" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A977" s="53"/>
+      <c r="B977" s="7" t="s">
+        <v>718</v>
+      </c>
+    </row>
+    <row r="978" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A978" s="53"/>
+      <c r="B978" s="11" t="s">
+        <v>719</v>
+      </c>
+    </row>
+    <row r="979" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A979" s="54"/>
+      <c r="B979" s="42"/>
+    </row>
   </sheetData>
-  <mergeCells count="62">
+  <mergeCells count="63">
+    <mergeCell ref="A959:A979"/>
+    <mergeCell ref="A940:A957"/>
+    <mergeCell ref="A858:A902"/>
+    <mergeCell ref="A832:A856"/>
+    <mergeCell ref="A792:A819"/>
+    <mergeCell ref="A503:A521"/>
+    <mergeCell ref="A652:A665"/>
+    <mergeCell ref="A757:A772"/>
+    <mergeCell ref="A720:A755"/>
+    <mergeCell ref="A686:A700"/>
+    <mergeCell ref="A563:A584"/>
+    <mergeCell ref="A637:A644"/>
+    <mergeCell ref="A674:A684"/>
+    <mergeCell ref="A702:A718"/>
+    <mergeCell ref="A523:A544"/>
+    <mergeCell ref="A667:A672"/>
+    <mergeCell ref="A646:A650"/>
+    <mergeCell ref="A586:A635"/>
+    <mergeCell ref="A546:A561"/>
+    <mergeCell ref="A774:A790"/>
+    <mergeCell ref="A276:A295"/>
+    <mergeCell ref="A356:A364"/>
+    <mergeCell ref="A330:A342"/>
+    <mergeCell ref="A311:A318"/>
+    <mergeCell ref="A490:A501"/>
+    <mergeCell ref="A454:A465"/>
+    <mergeCell ref="A467:A488"/>
+    <mergeCell ref="A297:A309"/>
+    <mergeCell ref="A104:A109"/>
+    <mergeCell ref="A56:A62"/>
+    <mergeCell ref="A48:A54"/>
+    <mergeCell ref="A97:A102"/>
+    <mergeCell ref="A88:A95"/>
+    <mergeCell ref="A81:A86"/>
+    <mergeCell ref="A64:A78"/>
+    <mergeCell ref="A2:A6"/>
+    <mergeCell ref="A37:A46"/>
+    <mergeCell ref="A29:A35"/>
+    <mergeCell ref="A16:A27"/>
+    <mergeCell ref="A8:A14"/>
+    <mergeCell ref="A118:A124"/>
+    <mergeCell ref="A126:A132"/>
+    <mergeCell ref="A189:A196"/>
+    <mergeCell ref="A174:A187"/>
+    <mergeCell ref="A159:A172"/>
+    <mergeCell ref="A146:A156"/>
+    <mergeCell ref="A134:A144"/>
     <mergeCell ref="A904:A938"/>
     <mergeCell ref="A821:A830"/>
     <mergeCell ref="A111:A116"/>
@@ -42496,52 +43230,6 @@
     <mergeCell ref="A230:A237"/>
     <mergeCell ref="A239:A246"/>
     <mergeCell ref="A198:A215"/>
-    <mergeCell ref="A118:A124"/>
-    <mergeCell ref="A126:A132"/>
-    <mergeCell ref="A189:A196"/>
-    <mergeCell ref="A174:A187"/>
-    <mergeCell ref="A159:A172"/>
-    <mergeCell ref="A146:A156"/>
-    <mergeCell ref="A134:A144"/>
-    <mergeCell ref="A2:A6"/>
-    <mergeCell ref="A37:A46"/>
-    <mergeCell ref="A29:A35"/>
-    <mergeCell ref="A16:A27"/>
-    <mergeCell ref="A8:A14"/>
-    <mergeCell ref="A104:A109"/>
-    <mergeCell ref="A56:A62"/>
-    <mergeCell ref="A48:A54"/>
-    <mergeCell ref="A97:A102"/>
-    <mergeCell ref="A88:A95"/>
-    <mergeCell ref="A81:A86"/>
-    <mergeCell ref="A64:A78"/>
-    <mergeCell ref="A586:A635"/>
-    <mergeCell ref="A546:A561"/>
-    <mergeCell ref="A774:A790"/>
-    <mergeCell ref="A276:A295"/>
-    <mergeCell ref="A356:A364"/>
-    <mergeCell ref="A330:A342"/>
-    <mergeCell ref="A311:A318"/>
-    <mergeCell ref="A490:A501"/>
-    <mergeCell ref="A454:A465"/>
-    <mergeCell ref="A467:A488"/>
-    <mergeCell ref="A297:A309"/>
-    <mergeCell ref="A940:A957"/>
-    <mergeCell ref="A858:A902"/>
-    <mergeCell ref="A832:A856"/>
-    <mergeCell ref="A792:A819"/>
-    <mergeCell ref="A503:A521"/>
-    <mergeCell ref="A652:A665"/>
-    <mergeCell ref="A757:A772"/>
-    <mergeCell ref="A720:A755"/>
-    <mergeCell ref="A686:A700"/>
-    <mergeCell ref="A563:A584"/>
-    <mergeCell ref="A637:A644"/>
-    <mergeCell ref="A674:A684"/>
-    <mergeCell ref="A702:A718"/>
-    <mergeCell ref="A523:A544"/>
-    <mergeCell ref="A667:A672"/>
-    <mergeCell ref="A646:A650"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Atualizado o ex067 e planilha
</commit_message>
<xml_diff>
--- a/detalhesPython.xlsx
+++ b/detalhesPython.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Thiago Henrique\Documents\EstudosT\python\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4771D25-31E4-4062-BB82-98309FACA904}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9E6D652-FE95-40CA-9773-5189A15A4002}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="15" windowWidth="29040" windowHeight="15990" xr2:uid="{ECBDB9F7-0FAD-476C-A4A4-7948F29B869E}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="913" uniqueCount="776">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="924" uniqueCount="783">
   <si>
     <t>Descrição</t>
   </si>
@@ -38876,6 +38876,580 @@
         <family val="3"/>
       </rPr>
       <t>!'</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>)</t>
+    </r>
+  </si>
+  <si>
+    <t>Faça um programa que mostre a tabuada de vários números, um de cada vez, para cada valor digitado pelo usuário. O programa será interrompido quando o número solicitado for negativo.</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">    num </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>=</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color rgb="FF988BC7"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>int</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>(</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF988BC7"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>input</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>(</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE7DE79"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>'</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>\n</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE7DE79"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>Quer ver a tabuada de qual valor? '</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>))</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">    </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF988BC7"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>print</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>(</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE7DE79"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>'-'</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>*</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF78D1E1"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>35</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">    </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>if</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> num </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>&lt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF78D1E1"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>0</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>:</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">    </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>for</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> c </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>in</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF988BC7"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>range</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>(</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF78D1E1"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>1</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF78D1E1"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>11</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>):</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">        </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF988BC7"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>print</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>(</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>f</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE7DE79"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>'</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF78D1E1"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>{</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>num</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF78D1E1"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>}</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE7DE79"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> x </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF78D1E1"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>{</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>c</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF78D1E1"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>}</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE7DE79"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> = </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF78D1E1"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>{</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">num </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>*</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> c</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF78D1E1"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>}</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE7DE79"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>'</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>print</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>(</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE7DE79"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>'</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>\n</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE7DE79"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>Programa Tabuada ENCERRADO. Volte sempre!</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>\n</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE7DE79"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>'</t>
     </r>
     <r>
       <rPr>
@@ -40156,10 +40730,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{73331524-72FC-41A3-82E6-4326A0999772}">
-  <dimension ref="A1:G1061"/>
+  <dimension ref="A1:G1075"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A1036" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A1051" sqref="A1051:A1061"/>
+    <sheetView tabSelected="1" topLeftCell="A1042" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="A1063" sqref="A1063:A1075"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -46164,8 +46738,135 @@
       <c r="A1061" s="58"/>
       <c r="B1061" s="42"/>
     </row>
+    <row r="1062" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="1063" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1063" s="56" t="s">
+        <v>751</v>
+      </c>
+      <c r="B1063" s="55" t="s">
+        <v>776</v>
+      </c>
+    </row>
+    <row r="1064" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1064" s="57"/>
+      <c r="B1064" s="40"/>
+    </row>
+    <row r="1065" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1065" s="57"/>
+      <c r="B1065" s="34" t="s">
+        <v>770</v>
+      </c>
+    </row>
+    <row r="1066" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1066" s="57"/>
+      <c r="B1066" s="7" t="s">
+        <v>777</v>
+      </c>
+    </row>
+    <row r="1067" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1067" s="57"/>
+      <c r="B1067" s="7" t="s">
+        <v>778</v>
+      </c>
+    </row>
+    <row r="1068" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1068" s="57"/>
+      <c r="B1068" s="7" t="s">
+        <v>779</v>
+      </c>
+    </row>
+    <row r="1069" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1069" s="57"/>
+      <c r="B1069" s="7" t="s">
+        <v>773</v>
+      </c>
+    </row>
+    <row r="1070" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1070" s="57"/>
+      <c r="B1070" s="7" t="s">
+        <v>780</v>
+      </c>
+    </row>
+    <row r="1071" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1071" s="57"/>
+      <c r="B1071" s="7" t="s">
+        <v>781</v>
+      </c>
+    </row>
+    <row r="1072" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1072" s="57"/>
+      <c r="B1072" s="7" t="s">
+        <v>778</v>
+      </c>
+    </row>
+    <row r="1073" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1073" s="57"/>
+      <c r="B1073" s="11" t="s">
+        <v>782</v>
+      </c>
+    </row>
+    <row r="1074" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1074" s="57"/>
+      <c r="B1074" s="7"/>
+    </row>
+    <row r="1075" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1075" s="58"/>
+      <c r="B1075" s="42"/>
+    </row>
   </sheetData>
-  <mergeCells count="67">
+  <mergeCells count="68">
+    <mergeCell ref="A1063:A1075"/>
+    <mergeCell ref="A1031:A1049"/>
+    <mergeCell ref="A1002:A1029"/>
+    <mergeCell ref="A959:A979"/>
+    <mergeCell ref="A940:A957"/>
+    <mergeCell ref="A858:A902"/>
+    <mergeCell ref="A832:A856"/>
+    <mergeCell ref="A981:A1000"/>
+    <mergeCell ref="A792:A819"/>
+    <mergeCell ref="A904:A938"/>
+    <mergeCell ref="A821:A830"/>
+    <mergeCell ref="A674:A684"/>
+    <mergeCell ref="A702:A718"/>
+    <mergeCell ref="A774:A790"/>
+    <mergeCell ref="A276:A295"/>
+    <mergeCell ref="A356:A364"/>
+    <mergeCell ref="A330:A342"/>
+    <mergeCell ref="A311:A318"/>
+    <mergeCell ref="A490:A501"/>
+    <mergeCell ref="A454:A465"/>
+    <mergeCell ref="A467:A488"/>
+    <mergeCell ref="A297:A309"/>
+    <mergeCell ref="A503:A521"/>
+    <mergeCell ref="A652:A665"/>
+    <mergeCell ref="A757:A772"/>
+    <mergeCell ref="A720:A755"/>
+    <mergeCell ref="A686:A700"/>
+    <mergeCell ref="A563:A584"/>
+    <mergeCell ref="A637:A644"/>
+    <mergeCell ref="A523:A544"/>
+    <mergeCell ref="A667:A672"/>
+    <mergeCell ref="A646:A650"/>
+    <mergeCell ref="A586:A635"/>
+    <mergeCell ref="A546:A561"/>
+    <mergeCell ref="A104:A109"/>
+    <mergeCell ref="A56:A62"/>
+    <mergeCell ref="A48:A54"/>
+    <mergeCell ref="A97:A102"/>
+    <mergeCell ref="A88:A95"/>
+    <mergeCell ref="A81:A86"/>
+    <mergeCell ref="A64:A78"/>
+    <mergeCell ref="A2:A6"/>
+    <mergeCell ref="A37:A46"/>
+    <mergeCell ref="A29:A35"/>
+    <mergeCell ref="A16:A27"/>
+    <mergeCell ref="A8:A14"/>
+    <mergeCell ref="A126:A132"/>
+    <mergeCell ref="A189:A196"/>
+    <mergeCell ref="A174:A187"/>
+    <mergeCell ref="A159:A172"/>
+    <mergeCell ref="A146:A156"/>
+    <mergeCell ref="A134:A144"/>
     <mergeCell ref="A1051:A1061"/>
     <mergeCell ref="A111:A116"/>
     <mergeCell ref="A217:A228"/>
@@ -46182,57 +46883,6 @@
     <mergeCell ref="A239:A246"/>
     <mergeCell ref="A198:A215"/>
     <mergeCell ref="A118:A124"/>
-    <mergeCell ref="A126:A132"/>
-    <mergeCell ref="A189:A196"/>
-    <mergeCell ref="A174:A187"/>
-    <mergeCell ref="A159:A172"/>
-    <mergeCell ref="A146:A156"/>
-    <mergeCell ref="A134:A144"/>
-    <mergeCell ref="A2:A6"/>
-    <mergeCell ref="A37:A46"/>
-    <mergeCell ref="A29:A35"/>
-    <mergeCell ref="A16:A27"/>
-    <mergeCell ref="A8:A14"/>
-    <mergeCell ref="A104:A109"/>
-    <mergeCell ref="A56:A62"/>
-    <mergeCell ref="A48:A54"/>
-    <mergeCell ref="A97:A102"/>
-    <mergeCell ref="A88:A95"/>
-    <mergeCell ref="A81:A86"/>
-    <mergeCell ref="A64:A78"/>
-    <mergeCell ref="A563:A584"/>
-    <mergeCell ref="A637:A644"/>
-    <mergeCell ref="A523:A544"/>
-    <mergeCell ref="A667:A672"/>
-    <mergeCell ref="A646:A650"/>
-    <mergeCell ref="A586:A635"/>
-    <mergeCell ref="A546:A561"/>
-    <mergeCell ref="A674:A684"/>
-    <mergeCell ref="A702:A718"/>
-    <mergeCell ref="A774:A790"/>
-    <mergeCell ref="A276:A295"/>
-    <mergeCell ref="A356:A364"/>
-    <mergeCell ref="A330:A342"/>
-    <mergeCell ref="A311:A318"/>
-    <mergeCell ref="A490:A501"/>
-    <mergeCell ref="A454:A465"/>
-    <mergeCell ref="A467:A488"/>
-    <mergeCell ref="A297:A309"/>
-    <mergeCell ref="A503:A521"/>
-    <mergeCell ref="A652:A665"/>
-    <mergeCell ref="A757:A772"/>
-    <mergeCell ref="A720:A755"/>
-    <mergeCell ref="A686:A700"/>
-    <mergeCell ref="A832:A856"/>
-    <mergeCell ref="A981:A1000"/>
-    <mergeCell ref="A792:A819"/>
-    <mergeCell ref="A904:A938"/>
-    <mergeCell ref="A821:A830"/>
-    <mergeCell ref="A1031:A1049"/>
-    <mergeCell ref="A1002:A1029"/>
-    <mergeCell ref="A959:A979"/>
-    <mergeCell ref="A940:A957"/>
-    <mergeCell ref="A858:A902"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Atualizado o ex069 e planilha
</commit_message>
<xml_diff>
--- a/detalhesPython.xlsx
+++ b/detalhesPython.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Thiago Henrique\Documents\EstudosT\python\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9E6D652-FE95-40CA-9773-5189A15A4002}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A100C61-A28E-4EFD-8A71-645AA754CA8D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="15" windowWidth="29040" windowHeight="15990" xr2:uid="{ECBDB9F7-0FAD-476C-A4A4-7948F29B869E}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="924" uniqueCount="783">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="988" uniqueCount="833">
   <si>
     <t>Descrição</t>
   </si>
@@ -39460,6 +39460,3174 @@
       </rPr>
       <t>)</t>
     </r>
+  </si>
+  <si>
+    <t>ex067</t>
+  </si>
+  <si>
+    <t>ex068</t>
+  </si>
+  <si>
+    <t>Faça um programa que jogue par ou ímpar com o computador. O jogo só será interrompido quando o jogador perder, mostrando o total de vitórias consecutivas que ele conquistou no final do jogo.</t>
+  </si>
+  <si>
+    <r>
+      <t>print</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>(</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE7DE79"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>'=-'</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>*</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF78D1E1"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>15</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>print</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>(</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE7DE79"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>'VAMOS JOGAR PAR OU ÍMPAR'</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF67E480"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>center</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>(</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF78D1E1"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>30</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>))</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">v </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>=</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF78D1E1"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>0</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">    computador </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>=</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF67E480"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>randint</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>(</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF78D1E1"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>0</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF78D1E1"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>10</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">    jogador </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>=</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color rgb="FF988BC7"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>int</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>(</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF988BC7"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>input</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>(</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE7DE79"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>'Digite um valor: '</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>))</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">    total </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>=</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> computador </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> jogador</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">    tipo </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>=</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE7DE79"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>' '</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">    </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>while</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> tipo </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>not</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>in</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE7DE79"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>'PI'</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>:</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">        tipo </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>=</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color rgb="FF988BC7"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>str</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>(</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF988BC7"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>input</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>(</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE7DE79"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>'Par ou Ímpar? [P/I] '</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>)).</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF67E480"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>strip</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>().</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF67E480"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>upper</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>()[</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF78D1E1"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>0</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>]</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">    </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF988BC7"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>print</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>(</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE7DE79"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>'-'</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>*</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF78D1E1"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>55</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">    </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF988BC7"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>print</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>(</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>f</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE7DE79"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">'Você jogou </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF78D1E1"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>{</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>jogador</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF78D1E1"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>}</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE7DE79"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> e o Computador </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF78D1E1"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>{</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>computador</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF78D1E1"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>}</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE7DE79"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">. Total de </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF78D1E1"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>{</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>total</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF78D1E1"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>}</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE7DE79"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> '</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">, </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color rgb="FFE89E64"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>end</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>=</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE7DE79"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>''</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">    </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF988BC7"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>print</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>(</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE7DE79"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>'DEU PAR'</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>if</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> total </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>%</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF78D1E1"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>2</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>==</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF78D1E1"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>0</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>else</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE7DE79"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>'DEU IMPAR'</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">    </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>if</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> tipo  </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>==</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE7DE79"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>'P'</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>:</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">        </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>if</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> total </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>%</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF78D1E1"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>2</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>==</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF78D1E1"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>0</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>:</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">            </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF988BC7"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>print</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>(</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE7DE79"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>'Você VENCEU!'</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">            v </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>+=</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF78D1E1"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>1</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">            </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF988BC7"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>print</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>(</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE7DE79"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>'Você PERDEU..'</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">            </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>break</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">    </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>elif</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> tipo </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>==</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE7DE79"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>'I'</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>:</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">        </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>if</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> total </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>%</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF78D1E1"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>2</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>==</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF78D1E1"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>1</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>:</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">    </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF988BC7"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>print</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>(</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE7DE79"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>'Vamos jogar novamente...'</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">    </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF988BC7"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>print</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>(</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE7DE79"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>'=-'</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>*</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF78D1E1"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>16</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>print</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>(</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE7DE79"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>'=-'</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>*</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF78D1E1"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>16</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>print</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>(</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>f</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE7DE79"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">'GAME OVER! Você venceu </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF78D1E1"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>{</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>v</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF78D1E1"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>}</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE7DE79"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> vezes.'</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>)</t>
+    </r>
+  </si>
+  <si>
+    <t>ex069</t>
+  </si>
+  <si>
+    <t>Crie um programa que leia a idade e o sexo de várias pessoas. A cada pessoa cadastrada, o programa deverá perguntar se o usuário quer ou não continuar. No final, mostre: A) quantas pessoas tem mais de 18 anos. B) quantos homens foram cadastrados. C) quantas mulheres tem menos de 20 anos.</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">tot18 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>=</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> totH </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>=</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> totM20 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>=</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF78D1E1"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>0</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">    </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF988BC7"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>print</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>(</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE7DE79"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>'-'</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>*</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF78D1E1"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>30</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">    </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF988BC7"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>print</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>(</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE7DE79"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>'CADASTRE UMA PESSOA'</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF67E480"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>center</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>(</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF78D1E1"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>30</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>))</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">    sexo </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>=</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE7DE79"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>' '</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">    </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>while</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> sexo </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>not</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>in</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE7DE79"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>'MF'</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>:</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">        sexo </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>=</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color rgb="FF988BC7"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>str</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>(</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF988BC7"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>input</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>(</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE7DE79"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>'Sexo: [M/F] '</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>)).</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF67E480"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>strip</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>().</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF67E480"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>upper</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>()[</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF78D1E1"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>0</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>]</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">    </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>if</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> idade </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>&gt;=</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF78D1E1"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>18</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>:</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">        tot18 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>+=</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF78D1E1"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>1</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">    </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>if</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> sexo </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>==</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE7DE79"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>'M'</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>:</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">         totH </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>+=</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF78D1E1"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>1</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">    </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>if</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> sexo </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>==</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE7DE79"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>'F'</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>and</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> idade </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>&lt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF78D1E1"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>20</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>:</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">         totM20 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>+=</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF78D1E1"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>1</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">    resp </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>=</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE7DE79"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>' '</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">    </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>while</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> resp </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>not</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>in</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE7DE79"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>'SN'</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>:</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">        resp </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>=</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color rgb="FF988BC7"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>str</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>(</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF988BC7"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>input</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>(</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE7DE79"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>'Quer continuar? [S/N] '</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>)).</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF67E480"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>strip</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>().</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF67E480"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>upper</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>()[</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF78D1E1"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>0</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>]</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">    </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>if</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> resp </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>==</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE7DE79"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>'N'</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>:</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>print</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>(</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>f</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE7DE79"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>'======= FIM DO PROGRAMA ======='</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF67E480"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>center</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>(</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF78D1E1"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>30</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>))</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>print</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>(</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>f</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE7DE79"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">'Total de pessoas com mais de 18 anos: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF78D1E1"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>{</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>tot18</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF78D1E1"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>}</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE7DE79"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>'</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>print</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>(</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>f</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE7DE79"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">'Ao todo temos </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF78D1E1"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>{</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>totH</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF78D1E1"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>}</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE7DE79"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> homens cadastrados'</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>print</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>(</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>f</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE7DE79"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">'E temos </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF78D1E1"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>{</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>totM20</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF78D1E1"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>}</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE7DE79"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> mulheres com menos de 20 anos'</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>)</t>
+    </r>
+  </si>
+  <si>
+    <t>ex070</t>
   </si>
 </sst>
 </file>
@@ -40730,10 +43898,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{73331524-72FC-41A3-82E6-4326A0999772}">
-  <dimension ref="A1:G1075"/>
+  <dimension ref="A1:G1171"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A1042" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A1063" sqref="A1063:A1075"/>
+    <sheetView tabSelected="1" topLeftCell="A1131" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="A1144" sqref="A1144:A1171"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -46741,7 +49909,7 @@
     <row r="1062" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="1063" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1063" s="56" t="s">
-        <v>751</v>
+        <v>783</v>
       </c>
       <c r="B1063" s="55" t="s">
         <v>776</v>
@@ -46813,19 +49981,554 @@
       <c r="A1075" s="58"/>
       <c r="B1075" s="42"/>
     </row>
+    <row r="1076" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="1077" spans="1:2" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1077" s="56" t="s">
+        <v>784</v>
+      </c>
+      <c r="B1077" s="31" t="s">
+        <v>785</v>
+      </c>
+    </row>
+    <row r="1078" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1078" s="57"/>
+      <c r="B1078" s="40"/>
+    </row>
+    <row r="1079" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1079" s="57"/>
+      <c r="B1079" s="34" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="1080" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1080" s="57"/>
+      <c r="B1080" s="11" t="s">
+        <v>786</v>
+      </c>
+    </row>
+    <row r="1081" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1081" s="57"/>
+      <c r="B1081" s="11" t="s">
+        <v>787</v>
+      </c>
+    </row>
+    <row r="1082" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1082" s="57"/>
+      <c r="B1082" s="11" t="s">
+        <v>786</v>
+      </c>
+    </row>
+    <row r="1083" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1083" s="57"/>
+      <c r="B1083" s="7" t="s">
+        <v>788</v>
+      </c>
+    </row>
+    <row r="1084" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1084" s="57"/>
+      <c r="B1084" s="34" t="s">
+        <v>770</v>
+      </c>
+    </row>
+    <row r="1085" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1085" s="57"/>
+      <c r="B1085" s="7" t="s">
+        <v>789</v>
+      </c>
+    </row>
+    <row r="1086" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1086" s="57"/>
+      <c r="B1086" s="7" t="s">
+        <v>790</v>
+      </c>
+    </row>
+    <row r="1087" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1087" s="57"/>
+      <c r="B1087" s="7" t="s">
+        <v>791</v>
+      </c>
+    </row>
+    <row r="1088" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1088" s="57"/>
+      <c r="B1088" s="7" t="s">
+        <v>792</v>
+      </c>
+    </row>
+    <row r="1089" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1089" s="57"/>
+      <c r="B1089" s="7" t="s">
+        <v>793</v>
+      </c>
+    </row>
+    <row r="1090" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1090" s="57"/>
+      <c r="B1090" s="7" t="s">
+        <v>794</v>
+      </c>
+    </row>
+    <row r="1091" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1091" s="57"/>
+      <c r="B1091" s="7" t="s">
+        <v>795</v>
+      </c>
+    </row>
+    <row r="1092" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1092" s="57"/>
+      <c r="B1092" s="7" t="s">
+        <v>796</v>
+      </c>
+    </row>
+    <row r="1093" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1093" s="57"/>
+      <c r="B1093" s="7" t="s">
+        <v>797</v>
+      </c>
+    </row>
+    <row r="1094" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1094" s="57"/>
+      <c r="B1094" s="7" t="s">
+        <v>795</v>
+      </c>
+    </row>
+    <row r="1095" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1095" s="57"/>
+      <c r="B1095" s="7" t="s">
+        <v>798</v>
+      </c>
+    </row>
+    <row r="1096" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1096" s="57"/>
+      <c r="B1096" s="7" t="s">
+        <v>799</v>
+      </c>
+    </row>
+    <row r="1097" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1097" s="57"/>
+      <c r="B1097" s="7" t="s">
+        <v>800</v>
+      </c>
+    </row>
+    <row r="1098" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1098" s="57"/>
+      <c r="B1098" s="7" t="s">
+        <v>801</v>
+      </c>
+    </row>
+    <row r="1099" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1099" s="57"/>
+      <c r="B1099" s="7" t="s">
+        <v>629</v>
+      </c>
+    </row>
+    <row r="1100" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1100" s="57"/>
+      <c r="B1100" s="7" t="s">
+        <v>802</v>
+      </c>
+    </row>
+    <row r="1101" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1101" s="57"/>
+      <c r="B1101" s="7" t="s">
+        <v>803</v>
+      </c>
+    </row>
+    <row r="1102" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1102" s="57"/>
+      <c r="B1102" s="7" t="s">
+        <v>804</v>
+      </c>
+    </row>
+    <row r="1103" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1103" s="57"/>
+      <c r="B1103" s="7" t="s">
+        <v>805</v>
+      </c>
+    </row>
+    <row r="1104" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1104" s="57"/>
+      <c r="B1104" s="7" t="s">
+        <v>800</v>
+      </c>
+    </row>
+    <row r="1105" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1105" s="57"/>
+      <c r="B1105" s="7" t="s">
+        <v>801</v>
+      </c>
+    </row>
+    <row r="1106" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1106" s="57"/>
+      <c r="B1106" s="7" t="s">
+        <v>629</v>
+      </c>
+    </row>
+    <row r="1107" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1107" s="57"/>
+      <c r="B1107" s="7" t="s">
+        <v>802</v>
+      </c>
+    </row>
+    <row r="1108" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1108" s="57"/>
+      <c r="B1108" s="7" t="s">
+        <v>803</v>
+      </c>
+    </row>
+    <row r="1109" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1109" s="57"/>
+      <c r="B1109" s="7" t="s">
+        <v>806</v>
+      </c>
+    </row>
+    <row r="1110" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1110" s="57"/>
+      <c r="B1110" s="7" t="s">
+        <v>807</v>
+      </c>
+    </row>
+    <row r="1111" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1111" s="57"/>
+      <c r="B1111" s="11" t="s">
+        <v>808</v>
+      </c>
+    </row>
+    <row r="1112" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1112" s="57"/>
+      <c r="B1112" s="11" t="s">
+        <v>809</v>
+      </c>
+    </row>
+    <row r="1113" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1113" s="58"/>
+      <c r="B1113" s="42"/>
+    </row>
+    <row r="1114" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="1115" spans="1:2" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1115" s="56" t="s">
+        <v>810</v>
+      </c>
+      <c r="B1115" s="31" t="s">
+        <v>811</v>
+      </c>
+    </row>
+    <row r="1116" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1116" s="57"/>
+      <c r="B1116" s="40"/>
+    </row>
+    <row r="1117" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1117" s="57"/>
+      <c r="B1117" s="7" t="s">
+        <v>812</v>
+      </c>
+    </row>
+    <row r="1118" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1118" s="57"/>
+      <c r="B1118" s="34" t="s">
+        <v>770</v>
+      </c>
+    </row>
+    <row r="1119" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1119" s="57"/>
+      <c r="B1119" s="7" t="s">
+        <v>813</v>
+      </c>
+    </row>
+    <row r="1120" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1120" s="57"/>
+      <c r="B1120" s="7" t="s">
+        <v>814</v>
+      </c>
+    </row>
+    <row r="1121" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1121" s="57"/>
+      <c r="B1121" s="7" t="s">
+        <v>813</v>
+      </c>
+    </row>
+    <row r="1122" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1122" s="57"/>
+      <c r="B1122" s="7" t="s">
+        <v>593</v>
+      </c>
+    </row>
+    <row r="1123" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1123" s="57"/>
+      <c r="B1123" s="7" t="s">
+        <v>815</v>
+      </c>
+    </row>
+    <row r="1124" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1124" s="57"/>
+      <c r="B1124" s="7" t="s">
+        <v>816</v>
+      </c>
+    </row>
+    <row r="1125" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1125" s="57"/>
+      <c r="B1125" s="7" t="s">
+        <v>817</v>
+      </c>
+    </row>
+    <row r="1126" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1126" s="57"/>
+      <c r="B1126" s="7" t="s">
+        <v>818</v>
+      </c>
+    </row>
+    <row r="1127" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1127" s="57"/>
+      <c r="B1127" s="7" t="s">
+        <v>819</v>
+      </c>
+    </row>
+    <row r="1128" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1128" s="57"/>
+      <c r="B1128" s="7" t="s">
+        <v>820</v>
+      </c>
+    </row>
+    <row r="1129" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1129" s="57"/>
+      <c r="B1129" s="7" t="s">
+        <v>821</v>
+      </c>
+    </row>
+    <row r="1130" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1130" s="57"/>
+      <c r="B1130" s="7" t="s">
+        <v>822</v>
+      </c>
+    </row>
+    <row r="1131" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1131" s="57"/>
+      <c r="B1131" s="7" t="s">
+        <v>823</v>
+      </c>
+    </row>
+    <row r="1132" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1132" s="57"/>
+      <c r="B1132" s="7" t="s">
+        <v>824</v>
+      </c>
+    </row>
+    <row r="1133" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1133" s="57"/>
+      <c r="B1133" s="7" t="s">
+        <v>813</v>
+      </c>
+    </row>
+    <row r="1134" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1134" s="57"/>
+      <c r="B1134" s="7" t="s">
+        <v>825</v>
+      </c>
+    </row>
+    <row r="1135" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1135" s="57"/>
+      <c r="B1135" s="7" t="s">
+        <v>826</v>
+      </c>
+    </row>
+    <row r="1136" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1136" s="57"/>
+      <c r="B1136" s="7" t="s">
+        <v>827</v>
+      </c>
+    </row>
+    <row r="1137" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1137" s="57"/>
+      <c r="B1137" s="7" t="s">
+        <v>773</v>
+      </c>
+    </row>
+    <row r="1138" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1138" s="57"/>
+      <c r="B1138" s="11" t="s">
+        <v>828</v>
+      </c>
+    </row>
+    <row r="1139" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1139" s="57"/>
+      <c r="B1139" s="11" t="s">
+        <v>829</v>
+      </c>
+    </row>
+    <row r="1140" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1140" s="57"/>
+      <c r="B1140" s="11" t="s">
+        <v>830</v>
+      </c>
+    </row>
+    <row r="1141" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1141" s="57"/>
+      <c r="B1141" s="11" t="s">
+        <v>831</v>
+      </c>
+    </row>
+    <row r="1142" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1142" s="58"/>
+      <c r="B1142" s="42"/>
+    </row>
+    <row r="1143" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="1144" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1144" s="56" t="s">
+        <v>832</v>
+      </c>
+      <c r="B1144" s="31"/>
+    </row>
+    <row r="1145" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1145" s="57"/>
+      <c r="B1145" s="40"/>
+    </row>
+    <row r="1146" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1146" s="57"/>
+      <c r="B1146" s="7"/>
+    </row>
+    <row r="1147" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1147" s="57"/>
+      <c r="B1147" s="34"/>
+    </row>
+    <row r="1148" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1148" s="57"/>
+      <c r="B1148" s="7"/>
+    </row>
+    <row r="1149" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1149" s="57"/>
+      <c r="B1149" s="7"/>
+    </row>
+    <row r="1150" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1150" s="57"/>
+      <c r="B1150" s="7"/>
+    </row>
+    <row r="1151" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1151" s="57"/>
+      <c r="B1151" s="7"/>
+    </row>
+    <row r="1152" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1152" s="57"/>
+      <c r="B1152" s="7"/>
+    </row>
+    <row r="1153" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1153" s="57"/>
+      <c r="B1153" s="7"/>
+    </row>
+    <row r="1154" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1154" s="57"/>
+      <c r="B1154" s="7"/>
+    </row>
+    <row r="1155" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1155" s="57"/>
+      <c r="B1155" s="7"/>
+    </row>
+    <row r="1156" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1156" s="57"/>
+      <c r="B1156" s="7"/>
+    </row>
+    <row r="1157" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1157" s="57"/>
+      <c r="B1157" s="7"/>
+    </row>
+    <row r="1158" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1158" s="57"/>
+      <c r="B1158" s="7"/>
+    </row>
+    <row r="1159" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1159" s="57"/>
+      <c r="B1159" s="7"/>
+    </row>
+    <row r="1160" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1160" s="57"/>
+      <c r="B1160" s="7"/>
+    </row>
+    <row r="1161" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1161" s="57"/>
+      <c r="B1161" s="7"/>
+    </row>
+    <row r="1162" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1162" s="57"/>
+      <c r="B1162" s="7"/>
+    </row>
+    <row r="1163" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1163" s="57"/>
+      <c r="B1163" s="7"/>
+    </row>
+    <row r="1164" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1164" s="57"/>
+      <c r="B1164" s="7"/>
+    </row>
+    <row r="1165" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1165" s="57"/>
+      <c r="B1165" s="7"/>
+    </row>
+    <row r="1166" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1166" s="57"/>
+      <c r="B1166" s="7"/>
+    </row>
+    <row r="1167" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1167" s="57"/>
+      <c r="B1167" s="11"/>
+    </row>
+    <row r="1168" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1168" s="57"/>
+      <c r="B1168" s="11"/>
+    </row>
+    <row r="1169" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1169" s="57"/>
+      <c r="B1169" s="11"/>
+    </row>
+    <row r="1170" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1170" s="57"/>
+      <c r="B1170" s="11"/>
+    </row>
+    <row r="1171" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1171" s="58"/>
+      <c r="B1171" s="42"/>
+    </row>
   </sheetData>
-  <mergeCells count="68">
-    <mergeCell ref="A1063:A1075"/>
-    <mergeCell ref="A1031:A1049"/>
-    <mergeCell ref="A1002:A1029"/>
-    <mergeCell ref="A959:A979"/>
-    <mergeCell ref="A940:A957"/>
-    <mergeCell ref="A858:A902"/>
-    <mergeCell ref="A832:A856"/>
-    <mergeCell ref="A981:A1000"/>
-    <mergeCell ref="A792:A819"/>
-    <mergeCell ref="A904:A938"/>
-    <mergeCell ref="A821:A830"/>
+  <mergeCells count="71">
+    <mergeCell ref="A1077:A1113"/>
+    <mergeCell ref="A1115:A1142"/>
+    <mergeCell ref="A1144:A1171"/>
+    <mergeCell ref="A111:A116"/>
+    <mergeCell ref="A217:A228"/>
+    <mergeCell ref="A248:A260"/>
+    <mergeCell ref="A408:A429"/>
+    <mergeCell ref="A431:A452"/>
+    <mergeCell ref="A380:A392"/>
+    <mergeCell ref="A394:A406"/>
+    <mergeCell ref="A320:A328"/>
+    <mergeCell ref="A366:A378"/>
+    <mergeCell ref="A344:A354"/>
+    <mergeCell ref="A262:A274"/>
+    <mergeCell ref="A230:A237"/>
+    <mergeCell ref="A239:A246"/>
+    <mergeCell ref="A198:A215"/>
+    <mergeCell ref="A118:A124"/>
+    <mergeCell ref="A126:A132"/>
+    <mergeCell ref="A189:A196"/>
+    <mergeCell ref="A174:A187"/>
+    <mergeCell ref="A159:A172"/>
+    <mergeCell ref="A146:A156"/>
+    <mergeCell ref="A134:A144"/>
+    <mergeCell ref="A2:A6"/>
+    <mergeCell ref="A37:A46"/>
+    <mergeCell ref="A29:A35"/>
+    <mergeCell ref="A16:A27"/>
+    <mergeCell ref="A8:A14"/>
+    <mergeCell ref="A104:A109"/>
+    <mergeCell ref="A56:A62"/>
+    <mergeCell ref="A48:A54"/>
+    <mergeCell ref="A97:A102"/>
+    <mergeCell ref="A88:A95"/>
+    <mergeCell ref="A81:A86"/>
+    <mergeCell ref="A64:A78"/>
+    <mergeCell ref="A563:A584"/>
+    <mergeCell ref="A637:A644"/>
+    <mergeCell ref="A523:A544"/>
+    <mergeCell ref="A667:A672"/>
+    <mergeCell ref="A646:A650"/>
+    <mergeCell ref="A586:A635"/>
+    <mergeCell ref="A546:A561"/>
     <mergeCell ref="A674:A684"/>
     <mergeCell ref="A702:A718"/>
     <mergeCell ref="A774:A790"/>
@@ -46842,47 +50545,18 @@
     <mergeCell ref="A757:A772"/>
     <mergeCell ref="A720:A755"/>
     <mergeCell ref="A686:A700"/>
-    <mergeCell ref="A563:A584"/>
-    <mergeCell ref="A637:A644"/>
-    <mergeCell ref="A523:A544"/>
-    <mergeCell ref="A667:A672"/>
-    <mergeCell ref="A646:A650"/>
-    <mergeCell ref="A586:A635"/>
-    <mergeCell ref="A546:A561"/>
-    <mergeCell ref="A104:A109"/>
-    <mergeCell ref="A56:A62"/>
-    <mergeCell ref="A48:A54"/>
-    <mergeCell ref="A97:A102"/>
-    <mergeCell ref="A88:A95"/>
-    <mergeCell ref="A81:A86"/>
-    <mergeCell ref="A64:A78"/>
-    <mergeCell ref="A2:A6"/>
-    <mergeCell ref="A37:A46"/>
-    <mergeCell ref="A29:A35"/>
-    <mergeCell ref="A16:A27"/>
-    <mergeCell ref="A8:A14"/>
-    <mergeCell ref="A126:A132"/>
-    <mergeCell ref="A189:A196"/>
-    <mergeCell ref="A174:A187"/>
-    <mergeCell ref="A159:A172"/>
-    <mergeCell ref="A146:A156"/>
-    <mergeCell ref="A134:A144"/>
+    <mergeCell ref="A858:A902"/>
+    <mergeCell ref="A832:A856"/>
+    <mergeCell ref="A981:A1000"/>
+    <mergeCell ref="A792:A819"/>
+    <mergeCell ref="A904:A938"/>
+    <mergeCell ref="A821:A830"/>
+    <mergeCell ref="A1063:A1075"/>
+    <mergeCell ref="A1031:A1049"/>
+    <mergeCell ref="A1002:A1029"/>
+    <mergeCell ref="A959:A979"/>
+    <mergeCell ref="A940:A957"/>
     <mergeCell ref="A1051:A1061"/>
-    <mergeCell ref="A111:A116"/>
-    <mergeCell ref="A217:A228"/>
-    <mergeCell ref="A248:A260"/>
-    <mergeCell ref="A408:A429"/>
-    <mergeCell ref="A431:A452"/>
-    <mergeCell ref="A380:A392"/>
-    <mergeCell ref="A394:A406"/>
-    <mergeCell ref="A320:A328"/>
-    <mergeCell ref="A366:A378"/>
-    <mergeCell ref="A344:A354"/>
-    <mergeCell ref="A262:A274"/>
-    <mergeCell ref="A230:A237"/>
-    <mergeCell ref="A239:A246"/>
-    <mergeCell ref="A198:A215"/>
-    <mergeCell ref="A118:A124"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Atualizado o ex070 e planilha
</commit_message>
<xml_diff>
--- a/detalhesPython.xlsx
+++ b/detalhesPython.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Thiago Henrique\Documents\EstudosT\python\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A100C61-A28E-4EFD-8A71-645AA754CA8D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F6FD66E8-7FAF-4345-BFE8-1316EC665A59}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="15" windowWidth="29040" windowHeight="15990" xr2:uid="{ECBDB9F7-0FAD-476C-A4A4-7948F29B869E}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="988" uniqueCount="833">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1013" uniqueCount="855">
   <si>
     <t>Descrição</t>
   </si>
@@ -42628,6 +42628,1431 @@
   </si>
   <si>
     <t>ex070</t>
+  </si>
+  <si>
+    <t>Crie um programa que leia o nome e o preço de vários produtos. O programa deverá perguntar se o usuário vai continuar ou não. No final, mostre: A) qual é o total gasto na compra. B) quantos produtos custam mais de R$1000. C) qual é o nome do produto mais barato.</t>
+  </si>
+  <si>
+    <r>
+      <t>print</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>(</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE7DE79"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>'-'</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>*</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF78D1E1"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>40</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>print</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>(</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE7DE79"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>'LOJA SUPER BARATÃO'</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF67E480"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>center</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>(</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF78D1E1"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>40</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>))</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">total </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>=</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> menor </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>=</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> menorvalor </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>=</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> totmil </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>=</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF78D1E1"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>0</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">produtomenorvalor </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>=</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE7DE79"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>''</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">    menor </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>+=</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF78D1E1"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>1</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">    produto </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>=</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color rgb="FF988BC7"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>str</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>(</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF988BC7"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>input</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>(</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE7DE79"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>'Nome do Produto: '</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>)).</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF67E480"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>strip</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>().</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF67E480"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>upper</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>()</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">    valor </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>=</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color rgb="FF988BC7"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>float</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>(</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF988BC7"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>input</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>(</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE7DE79"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>'Preço: R$'</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>))</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">    total </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>+=</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> valor</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">    </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>if</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> valor </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF78D1E1"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>1000</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>:</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">        totmil </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>+=</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF78D1E1"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>1</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">    </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>if</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> menor </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>==</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF78D1E1"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>1</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>or</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> valor </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>&lt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> menorvalor:</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">        menorvalor </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>=</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> valor</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">        produtomenorvalor </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>=</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> produto</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">    continuar </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>=</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE7DE79"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>' '</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">    </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>while</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> continuar </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>not</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>in</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE7DE79"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>'sn'</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>:</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">        continuar </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>=</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color rgb="FF988BC7"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>str</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>(</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF988BC7"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>input</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>(</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE7DE79"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>'Quer continuar? [S/N] '</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>)).</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF67E480"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>strip</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>().</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF67E480"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>lower</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>()[</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF78D1E1"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>0</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>]</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">    </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>if</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> continuar </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>==</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE7DE79"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>'n'</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>:</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>print</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>(</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE7DE79"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>'</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF78D1E1"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>{</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF78D1E1"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>-^40}</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE7DE79"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>'</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF67E480"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>format</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>(</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE7DE79"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>' FIM DO PROGRAMA '</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>))</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>print</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>(</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>f</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE7DE79"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>'O total da compra foi R$</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF78D1E1"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>{</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>total</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>:.2f</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF78D1E1"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>}</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE7DE79"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>'</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>print</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>(</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>f</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE7DE79"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">'Temos </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF78D1E1"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>{</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>totmil</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF78D1E1"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>}</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE7DE79"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> produtos custando mais de R$1000.00'</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>print</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>(</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>f</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE7DE79"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">'E o produto mais barato foi: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF78D1E1"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>{</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>produtomenorvalor</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF78D1E1"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>}</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE7DE79"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> que custa R$</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF78D1E1"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>{</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>menorvalor</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>:.2f</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF78D1E1"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>}</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE7DE79"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>'</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>)</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -43898,10 +45323,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{73331524-72FC-41A3-82E6-4326A0999772}">
-  <dimension ref="A1:G1171"/>
+  <dimension ref="A1:G1170"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A1131" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A1144" sqref="A1144:A1171"/>
+    <sheetView tabSelected="1" topLeftCell="A1125" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="A1144" sqref="A1144:A1170"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -50370,11 +51795,13 @@
       <c r="B1142" s="42"/>
     </row>
     <row r="1143" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="1144" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1144" spans="1:2" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1144" s="56" t="s">
         <v>832</v>
       </c>
-      <c r="B1144" s="31"/>
+      <c r="B1144" s="31" t="s">
+        <v>833</v>
+      </c>
     </row>
     <row r="1145" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1145" s="57"/>
@@ -50382,153 +51809,166 @@
     </row>
     <row r="1146" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1146" s="57"/>
-      <c r="B1146" s="7"/>
+      <c r="B1146" s="11" t="s">
+        <v>834</v>
+      </c>
     </row>
     <row r="1147" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1147" s="57"/>
-      <c r="B1147" s="34"/>
+      <c r="B1147" s="11" t="s">
+        <v>835</v>
+      </c>
     </row>
     <row r="1148" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1148" s="57"/>
-      <c r="B1148" s="7"/>
+      <c r="B1148" s="11" t="s">
+        <v>834</v>
+      </c>
     </row>
     <row r="1149" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1149" s="57"/>
-      <c r="B1149" s="7"/>
+      <c r="B1149" s="7" t="s">
+        <v>836</v>
+      </c>
     </row>
     <row r="1150" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1150" s="57"/>
-      <c r="B1150" s="7"/>
+      <c r="B1150" s="7" t="s">
+        <v>837</v>
+      </c>
     </row>
     <row r="1151" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1151" s="57"/>
-      <c r="B1151" s="7"/>
+      <c r="B1151" s="34" t="s">
+        <v>770</v>
+      </c>
     </row>
     <row r="1152" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1152" s="57"/>
-      <c r="B1152" s="7"/>
+      <c r="B1152" s="7" t="s">
+        <v>838</v>
+      </c>
     </row>
     <row r="1153" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1153" s="57"/>
-      <c r="B1153" s="7"/>
+      <c r="B1153" s="7" t="s">
+        <v>839</v>
+      </c>
     </row>
     <row r="1154" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1154" s="57"/>
-      <c r="B1154" s="7"/>
+      <c r="B1154" s="7" t="s">
+        <v>840</v>
+      </c>
     </row>
     <row r="1155" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1155" s="57"/>
-      <c r="B1155" s="7"/>
+      <c r="B1155" s="7" t="s">
+        <v>841</v>
+      </c>
     </row>
     <row r="1156" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1156" s="57"/>
-      <c r="B1156" s="7"/>
+      <c r="B1156" s="7" t="s">
+        <v>842</v>
+      </c>
     </row>
     <row r="1157" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1157" s="57"/>
-      <c r="B1157" s="7"/>
+      <c r="B1157" s="7" t="s">
+        <v>843</v>
+      </c>
     </row>
     <row r="1158" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1158" s="57"/>
-      <c r="B1158" s="7"/>
+      <c r="B1158" s="7" t="s">
+        <v>844</v>
+      </c>
     </row>
     <row r="1159" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1159" s="57"/>
-      <c r="B1159" s="7"/>
+      <c r="B1159" s="7" t="s">
+        <v>845</v>
+      </c>
     </row>
     <row r="1160" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1160" s="57"/>
-      <c r="B1160" s="7"/>
+      <c r="B1160" s="7" t="s">
+        <v>846</v>
+      </c>
     </row>
     <row r="1161" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1161" s="57"/>
-      <c r="B1161" s="7"/>
+      <c r="B1161" s="7" t="s">
+        <v>847</v>
+      </c>
     </row>
     <row r="1162" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1162" s="57"/>
-      <c r="B1162" s="7"/>
+      <c r="B1162" s="7" t="s">
+        <v>848</v>
+      </c>
     </row>
     <row r="1163" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1163" s="57"/>
-      <c r="B1163" s="7"/>
+      <c r="B1163" s="7" t="s">
+        <v>849</v>
+      </c>
     </row>
     <row r="1164" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1164" s="57"/>
-      <c r="B1164" s="7"/>
+      <c r="B1164" s="7" t="s">
+        <v>850</v>
+      </c>
     </row>
     <row r="1165" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1165" s="57"/>
-      <c r="B1165" s="7"/>
+      <c r="B1165" s="7" t="s">
+        <v>773</v>
+      </c>
     </row>
     <row r="1166" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1166" s="57"/>
-      <c r="B1166" s="7"/>
+      <c r="B1166" s="11" t="s">
+        <v>851</v>
+      </c>
     </row>
     <row r="1167" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1167" s="57"/>
-      <c r="B1167" s="11"/>
+      <c r="B1167" s="11" t="s">
+        <v>852</v>
+      </c>
     </row>
     <row r="1168" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1168" s="57"/>
-      <c r="B1168" s="11"/>
+      <c r="B1168" s="11" t="s">
+        <v>853</v>
+      </c>
     </row>
     <row r="1169" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1169" s="57"/>
-      <c r="B1169" s="11"/>
-    </row>
-    <row r="1170" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1170" s="57"/>
-      <c r="B1170" s="11"/>
-    </row>
-    <row r="1171" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1171" s="58"/>
-      <c r="B1171" s="42"/>
+      <c r="B1169" s="11" t="s">
+        <v>854</v>
+      </c>
+    </row>
+    <row r="1170" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1170" s="58"/>
+      <c r="B1170" s="42"/>
     </row>
   </sheetData>
   <mergeCells count="71">
-    <mergeCell ref="A1077:A1113"/>
-    <mergeCell ref="A1115:A1142"/>
-    <mergeCell ref="A1144:A1171"/>
-    <mergeCell ref="A111:A116"/>
-    <mergeCell ref="A217:A228"/>
-    <mergeCell ref="A248:A260"/>
-    <mergeCell ref="A408:A429"/>
-    <mergeCell ref="A431:A452"/>
-    <mergeCell ref="A380:A392"/>
-    <mergeCell ref="A394:A406"/>
-    <mergeCell ref="A320:A328"/>
-    <mergeCell ref="A366:A378"/>
-    <mergeCell ref="A344:A354"/>
-    <mergeCell ref="A262:A274"/>
-    <mergeCell ref="A230:A237"/>
-    <mergeCell ref="A239:A246"/>
-    <mergeCell ref="A198:A215"/>
-    <mergeCell ref="A118:A124"/>
-    <mergeCell ref="A126:A132"/>
-    <mergeCell ref="A189:A196"/>
-    <mergeCell ref="A174:A187"/>
-    <mergeCell ref="A159:A172"/>
-    <mergeCell ref="A146:A156"/>
-    <mergeCell ref="A134:A144"/>
-    <mergeCell ref="A2:A6"/>
-    <mergeCell ref="A37:A46"/>
-    <mergeCell ref="A29:A35"/>
-    <mergeCell ref="A16:A27"/>
-    <mergeCell ref="A8:A14"/>
-    <mergeCell ref="A104:A109"/>
-    <mergeCell ref="A56:A62"/>
-    <mergeCell ref="A48:A54"/>
-    <mergeCell ref="A97:A102"/>
-    <mergeCell ref="A88:A95"/>
-    <mergeCell ref="A81:A86"/>
-    <mergeCell ref="A64:A78"/>
-    <mergeCell ref="A563:A584"/>
-    <mergeCell ref="A637:A644"/>
-    <mergeCell ref="A523:A544"/>
-    <mergeCell ref="A667:A672"/>
-    <mergeCell ref="A646:A650"/>
-    <mergeCell ref="A586:A635"/>
-    <mergeCell ref="A546:A561"/>
+    <mergeCell ref="A1063:A1075"/>
+    <mergeCell ref="A1031:A1049"/>
+    <mergeCell ref="A1002:A1029"/>
+    <mergeCell ref="A959:A979"/>
+    <mergeCell ref="A940:A957"/>
+    <mergeCell ref="A1051:A1061"/>
+    <mergeCell ref="A858:A902"/>
+    <mergeCell ref="A832:A856"/>
+    <mergeCell ref="A981:A1000"/>
+    <mergeCell ref="A792:A819"/>
+    <mergeCell ref="A904:A938"/>
+    <mergeCell ref="A821:A830"/>
     <mergeCell ref="A674:A684"/>
     <mergeCell ref="A702:A718"/>
     <mergeCell ref="A774:A790"/>
@@ -50545,18 +51985,49 @@
     <mergeCell ref="A757:A772"/>
     <mergeCell ref="A720:A755"/>
     <mergeCell ref="A686:A700"/>
-    <mergeCell ref="A858:A902"/>
-    <mergeCell ref="A832:A856"/>
-    <mergeCell ref="A981:A1000"/>
-    <mergeCell ref="A792:A819"/>
-    <mergeCell ref="A904:A938"/>
-    <mergeCell ref="A821:A830"/>
-    <mergeCell ref="A1063:A1075"/>
-    <mergeCell ref="A1031:A1049"/>
-    <mergeCell ref="A1002:A1029"/>
-    <mergeCell ref="A959:A979"/>
-    <mergeCell ref="A940:A957"/>
-    <mergeCell ref="A1051:A1061"/>
+    <mergeCell ref="A563:A584"/>
+    <mergeCell ref="A637:A644"/>
+    <mergeCell ref="A523:A544"/>
+    <mergeCell ref="A667:A672"/>
+    <mergeCell ref="A646:A650"/>
+    <mergeCell ref="A586:A635"/>
+    <mergeCell ref="A546:A561"/>
+    <mergeCell ref="A104:A109"/>
+    <mergeCell ref="A56:A62"/>
+    <mergeCell ref="A48:A54"/>
+    <mergeCell ref="A97:A102"/>
+    <mergeCell ref="A88:A95"/>
+    <mergeCell ref="A81:A86"/>
+    <mergeCell ref="A64:A78"/>
+    <mergeCell ref="A2:A6"/>
+    <mergeCell ref="A37:A46"/>
+    <mergeCell ref="A29:A35"/>
+    <mergeCell ref="A16:A27"/>
+    <mergeCell ref="A8:A14"/>
+    <mergeCell ref="A198:A215"/>
+    <mergeCell ref="A118:A124"/>
+    <mergeCell ref="A126:A132"/>
+    <mergeCell ref="A189:A196"/>
+    <mergeCell ref="A174:A187"/>
+    <mergeCell ref="A159:A172"/>
+    <mergeCell ref="A146:A156"/>
+    <mergeCell ref="A134:A144"/>
+    <mergeCell ref="A1077:A1113"/>
+    <mergeCell ref="A1115:A1142"/>
+    <mergeCell ref="A1144:A1170"/>
+    <mergeCell ref="A111:A116"/>
+    <mergeCell ref="A217:A228"/>
+    <mergeCell ref="A248:A260"/>
+    <mergeCell ref="A408:A429"/>
+    <mergeCell ref="A431:A452"/>
+    <mergeCell ref="A380:A392"/>
+    <mergeCell ref="A394:A406"/>
+    <mergeCell ref="A320:A328"/>
+    <mergeCell ref="A366:A378"/>
+    <mergeCell ref="A344:A354"/>
+    <mergeCell ref="A262:A274"/>
+    <mergeCell ref="A230:A237"/>
+    <mergeCell ref="A239:A246"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Atualizado o ex071 e planilha
</commit_message>
<xml_diff>
--- a/detalhesPython.xlsx
+++ b/detalhesPython.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Thiago Henrique\Documents\EstudosT\python\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F6FD66E8-7FAF-4345-BFE8-1316EC665A59}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4391611B-3F16-41E8-9C7A-C93914A3D8A5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="15" windowWidth="29040" windowHeight="15990" xr2:uid="{ECBDB9F7-0FAD-476C-A4A4-7948F29B869E}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1013" uniqueCount="855">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1040" uniqueCount="877">
   <si>
     <t>Descrição</t>
   </si>
@@ -44043,6 +44043,1022 @@
         <family val="3"/>
       </rPr>
       <t>'</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>)</t>
+    </r>
+  </si>
+  <si>
+    <t>ex071</t>
+  </si>
+  <si>
+    <t>Crie um programa que simule o funcionamento de um caixa eletrônico. No início, pergunte ao usuário qual será o valor a ser sacado (número inteiro) e o programa vai informar quantas cédulas de cada valor serão entregues.  OBS: considere que o caixa possui cédulas de R$50, R$20, R$10 e R$1.</t>
+  </si>
+  <si>
+    <r>
+      <t>print</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>(</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE7DE79"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>'='</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>*</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF78D1E1"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>40</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>print</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>(</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE7DE79"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>'</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF78D1E1"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>{</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>:^40</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF78D1E1"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>}</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE7DE79"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>'</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF67E480"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>format</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>(</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE7DE79"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>'BANCO CAMPONÊZ'</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>))</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">valor </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>=</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color rgb="FF988BC7"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>int</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>(</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF988BC7"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>input</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>(</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE7DE79"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>'Qual valor quer sacar: R$'</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>))</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">total </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>=</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> valor</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">ced </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>=</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF78D1E1"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>50</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">totced </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>=</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF78D1E1"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>0</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">    </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>if</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> total </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>&gt;=</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> ced:</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">        total </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>-=</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> ced</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">        totced </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>+=</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF78D1E1"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>1</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">        </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>if</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> totced </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF78D1E1"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>0</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>:</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">            </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF988BC7"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>print</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>(</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>f</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE7DE79"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">'Total de </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF78D1E1"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>{</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>totced</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF78D1E1"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>}</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE7DE79"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> cédulas de R$</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF78D1E1"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>{</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>ced</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF78D1E1"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>}</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE7DE79"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>'</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">        </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>if</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> ced </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>==</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF78D1E1"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>50</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>:</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">            ced </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>=</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF78D1E1"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>20</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">        </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>elif</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> ced </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>==</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF78D1E1"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>20</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>:</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">            ced </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>=</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF78D1E1"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>10</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">        </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>elif</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> ced </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>==</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF78D1E1"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>10</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>:</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">            ced </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>=</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF78D1E1"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>1</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">        totced </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>=</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF78D1E1"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>0</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">        </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>if</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> total </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF79C6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>==</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF78D1E1"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>0</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>:</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>print</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E1E6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>(</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE7DE79"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>'Volte sempre ao BANCO CAMPONÊZ! Tenha um ótimo dia!'</t>
     </r>
     <r>
       <rPr>
@@ -45323,10 +46339,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{73331524-72FC-41A3-82E6-4326A0999772}">
-  <dimension ref="A1:G1170"/>
+  <dimension ref="A1:G1199"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A1125" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A1144" sqref="A1144:A1170"/>
+    <sheetView tabSelected="1" topLeftCell="A1160" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="A1172" sqref="A1172:A1199"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -51955,20 +52971,219 @@
       <c r="A1170" s="58"/>
       <c r="B1170" s="42"/>
     </row>
+    <row r="1171" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="1172" spans="1:2" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1172" s="56" t="s">
+        <v>855</v>
+      </c>
+      <c r="B1172" s="31" t="s">
+        <v>856</v>
+      </c>
+    </row>
+    <row r="1173" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1173" s="57"/>
+      <c r="B1173" s="40"/>
+    </row>
+    <row r="1174" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1174" s="57"/>
+      <c r="B1174" s="11" t="s">
+        <v>857</v>
+      </c>
+    </row>
+    <row r="1175" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1175" s="57"/>
+      <c r="B1175" s="11" t="s">
+        <v>858</v>
+      </c>
+    </row>
+    <row r="1176" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1176" s="57"/>
+      <c r="B1176" s="11" t="s">
+        <v>857</v>
+      </c>
+    </row>
+    <row r="1177" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1177" s="57"/>
+      <c r="B1177" s="7" t="s">
+        <v>859</v>
+      </c>
+    </row>
+    <row r="1178" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1178" s="57"/>
+      <c r="B1178" s="7" t="s">
+        <v>860</v>
+      </c>
+    </row>
+    <row r="1179" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1179" s="57"/>
+      <c r="B1179" s="7" t="s">
+        <v>861</v>
+      </c>
+    </row>
+    <row r="1180" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1180" s="57"/>
+      <c r="B1180" s="7" t="s">
+        <v>862</v>
+      </c>
+    </row>
+    <row r="1181" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1181" s="57"/>
+      <c r="B1181" s="34" t="s">
+        <v>770</v>
+      </c>
+    </row>
+    <row r="1182" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1182" s="57"/>
+      <c r="B1182" s="7" t="s">
+        <v>863</v>
+      </c>
+    </row>
+    <row r="1183" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1183" s="57"/>
+      <c r="B1183" s="7" t="s">
+        <v>864</v>
+      </c>
+    </row>
+    <row r="1184" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1184" s="57"/>
+      <c r="B1184" s="7" t="s">
+        <v>865</v>
+      </c>
+    </row>
+    <row r="1185" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1185" s="57"/>
+      <c r="B1185" s="7" t="s">
+        <v>473</v>
+      </c>
+    </row>
+    <row r="1186" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1186" s="57"/>
+      <c r="B1186" s="7" t="s">
+        <v>866</v>
+      </c>
+    </row>
+    <row r="1187" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1187" s="57"/>
+      <c r="B1187" s="7" t="s">
+        <v>867</v>
+      </c>
+    </row>
+    <row r="1188" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1188" s="57"/>
+      <c r="B1188" s="7" t="s">
+        <v>868</v>
+      </c>
+    </row>
+    <row r="1189" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1189" s="57"/>
+      <c r="B1189" s="7" t="s">
+        <v>869</v>
+      </c>
+    </row>
+    <row r="1190" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1190" s="57"/>
+      <c r="B1190" s="7" t="s">
+        <v>870</v>
+      </c>
+    </row>
+    <row r="1191" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1191" s="57"/>
+      <c r="B1191" s="7" t="s">
+        <v>871</v>
+      </c>
+    </row>
+    <row r="1192" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1192" s="57"/>
+      <c r="B1192" s="7" t="s">
+        <v>872</v>
+      </c>
+    </row>
+    <row r="1193" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1193" s="57"/>
+      <c r="B1193" s="7" t="s">
+        <v>873</v>
+      </c>
+    </row>
+    <row r="1194" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1194" s="57"/>
+      <c r="B1194" s="7" t="s">
+        <v>874</v>
+      </c>
+    </row>
+    <row r="1195" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1195" s="57"/>
+      <c r="B1195" s="7" t="s">
+        <v>875</v>
+      </c>
+    </row>
+    <row r="1196" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1196" s="57"/>
+      <c r="B1196" s="7" t="s">
+        <v>803</v>
+      </c>
+    </row>
+    <row r="1197" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1197" s="57"/>
+      <c r="B1197" s="11" t="s">
+        <v>857</v>
+      </c>
+    </row>
+    <row r="1198" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1198" s="57"/>
+      <c r="B1198" s="11" t="s">
+        <v>876</v>
+      </c>
+    </row>
+    <row r="1199" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1199" s="58"/>
+      <c r="B1199" s="42"/>
+    </row>
   </sheetData>
-  <mergeCells count="71">
-    <mergeCell ref="A1063:A1075"/>
-    <mergeCell ref="A1031:A1049"/>
-    <mergeCell ref="A1002:A1029"/>
-    <mergeCell ref="A959:A979"/>
-    <mergeCell ref="A940:A957"/>
-    <mergeCell ref="A1051:A1061"/>
-    <mergeCell ref="A858:A902"/>
-    <mergeCell ref="A832:A856"/>
-    <mergeCell ref="A981:A1000"/>
-    <mergeCell ref="A792:A819"/>
-    <mergeCell ref="A904:A938"/>
-    <mergeCell ref="A821:A830"/>
+  <mergeCells count="72">
+    <mergeCell ref="A1172:A1199"/>
+    <mergeCell ref="A1077:A1113"/>
+    <mergeCell ref="A1115:A1142"/>
+    <mergeCell ref="A1144:A1170"/>
+    <mergeCell ref="A111:A116"/>
+    <mergeCell ref="A217:A228"/>
+    <mergeCell ref="A248:A260"/>
+    <mergeCell ref="A408:A429"/>
+    <mergeCell ref="A431:A452"/>
+    <mergeCell ref="A380:A392"/>
+    <mergeCell ref="A394:A406"/>
+    <mergeCell ref="A320:A328"/>
+    <mergeCell ref="A366:A378"/>
+    <mergeCell ref="A344:A354"/>
+    <mergeCell ref="A262:A274"/>
+    <mergeCell ref="A230:A237"/>
+    <mergeCell ref="A239:A246"/>
+    <mergeCell ref="A198:A215"/>
+    <mergeCell ref="A118:A124"/>
+    <mergeCell ref="A126:A132"/>
+    <mergeCell ref="A189:A196"/>
+    <mergeCell ref="A174:A187"/>
+    <mergeCell ref="A159:A172"/>
+    <mergeCell ref="A146:A156"/>
+    <mergeCell ref="A134:A144"/>
+    <mergeCell ref="A2:A6"/>
+    <mergeCell ref="A37:A46"/>
+    <mergeCell ref="A29:A35"/>
+    <mergeCell ref="A16:A27"/>
+    <mergeCell ref="A8:A14"/>
+    <mergeCell ref="A104:A109"/>
+    <mergeCell ref="A56:A62"/>
+    <mergeCell ref="A48:A54"/>
+    <mergeCell ref="A97:A102"/>
+    <mergeCell ref="A88:A95"/>
+    <mergeCell ref="A81:A86"/>
+    <mergeCell ref="A64:A78"/>
+    <mergeCell ref="A563:A584"/>
+    <mergeCell ref="A637:A644"/>
+    <mergeCell ref="A523:A544"/>
+    <mergeCell ref="A667:A672"/>
+    <mergeCell ref="A646:A650"/>
+    <mergeCell ref="A586:A635"/>
+    <mergeCell ref="A546:A561"/>
     <mergeCell ref="A674:A684"/>
     <mergeCell ref="A702:A718"/>
     <mergeCell ref="A774:A790"/>
@@ -51985,49 +53200,18 @@
     <mergeCell ref="A757:A772"/>
     <mergeCell ref="A720:A755"/>
     <mergeCell ref="A686:A700"/>
-    <mergeCell ref="A563:A584"/>
-    <mergeCell ref="A637:A644"/>
-    <mergeCell ref="A523:A544"/>
-    <mergeCell ref="A667:A672"/>
-    <mergeCell ref="A646:A650"/>
-    <mergeCell ref="A586:A635"/>
-    <mergeCell ref="A546:A561"/>
-    <mergeCell ref="A104:A109"/>
-    <mergeCell ref="A56:A62"/>
-    <mergeCell ref="A48:A54"/>
-    <mergeCell ref="A97:A102"/>
-    <mergeCell ref="A88:A95"/>
-    <mergeCell ref="A81:A86"/>
-    <mergeCell ref="A64:A78"/>
-    <mergeCell ref="A2:A6"/>
-    <mergeCell ref="A37:A46"/>
-    <mergeCell ref="A29:A35"/>
-    <mergeCell ref="A16:A27"/>
-    <mergeCell ref="A8:A14"/>
-    <mergeCell ref="A198:A215"/>
-    <mergeCell ref="A118:A124"/>
-    <mergeCell ref="A126:A132"/>
-    <mergeCell ref="A189:A196"/>
-    <mergeCell ref="A174:A187"/>
-    <mergeCell ref="A159:A172"/>
-    <mergeCell ref="A146:A156"/>
-    <mergeCell ref="A134:A144"/>
-    <mergeCell ref="A1077:A1113"/>
-    <mergeCell ref="A1115:A1142"/>
-    <mergeCell ref="A1144:A1170"/>
-    <mergeCell ref="A111:A116"/>
-    <mergeCell ref="A217:A228"/>
-    <mergeCell ref="A248:A260"/>
-    <mergeCell ref="A408:A429"/>
-    <mergeCell ref="A431:A452"/>
-    <mergeCell ref="A380:A392"/>
-    <mergeCell ref="A394:A406"/>
-    <mergeCell ref="A320:A328"/>
-    <mergeCell ref="A366:A378"/>
-    <mergeCell ref="A344:A354"/>
-    <mergeCell ref="A262:A274"/>
-    <mergeCell ref="A230:A237"/>
-    <mergeCell ref="A239:A246"/>
+    <mergeCell ref="A858:A902"/>
+    <mergeCell ref="A832:A856"/>
+    <mergeCell ref="A981:A1000"/>
+    <mergeCell ref="A792:A819"/>
+    <mergeCell ref="A904:A938"/>
+    <mergeCell ref="A821:A830"/>
+    <mergeCell ref="A1063:A1075"/>
+    <mergeCell ref="A1031:A1049"/>
+    <mergeCell ref="A1002:A1029"/>
+    <mergeCell ref="A959:A979"/>
+    <mergeCell ref="A940:A957"/>
+    <mergeCell ref="A1051:A1061"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>